<commit_message>
Update 9 17 2018
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5502C0-E168-4F2F-98FD-4E2F6F3EDEDF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A3B404-B0A3-4132-8599-6B136A55CCF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4703,63 +4703,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="149">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="144">
     <dxf>
       <fill>
         <patternFill>
@@ -5747,6 +5691,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5993,7 +5958,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8/31/2018</c:v>
+                  <c:v>9/17/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7750,8 +7715,8 @@
   </sheetPr>
   <dimension ref="B1:BT101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X71" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AB90" sqref="AB90"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16055,8 +16020,8 @@
       <c r="J59" s="144" t="s">
         <v>419</v>
       </c>
-      <c r="K59" s="144" t="s">
-        <v>567</v>
+      <c r="K59" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="L59" s="60" t="s">
         <v>483</v>
@@ -20146,127 +20111,127 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AK39 AK46:AK74 AQ14 AM39 AK38:AM38 AK40:AM40 AK2:AM5 AL46:AM55 AL57:AM74 AR4:AR5 AS14:AX14 AY8:AZ8 AY10:BE12 AS2:BB5 BA8:BB9 AR46:BB74 AY14:BB29 R2 AF46:AG74 AF2:AG5 AF38:AG40 AF8:AG12 AF36:AG36 AF33:AG34 AF43:AG44 AF76:AG85 AF14:AG29 AN46:AQ46 AN5:AP5 AN38:BB40 AK34:BB36 AK43:BB44 AN4:AQ4 AK8:AX12 AN48:AQ74 AN47:AP47 AK76:BB85 AL14:AP29 AN2:AR3 V2:V86">
-    <cfRule type="cellIs" dxfId="148" priority="72" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="143" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY9:AZ9">
-    <cfRule type="cellIs" dxfId="147" priority="71" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="142" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE2:BE5 BE8:BE9 BE34:BE36 BE38:BE40 BE43:BE44 BE46:BE74 BE14:BE29 BE76:BE85">
-    <cfRule type="cellIs" dxfId="146" priority="70" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="141" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL39 AL56">
-    <cfRule type="cellIs" dxfId="145" priority="69" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="140" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC2:BC5 BC8:BC9 BC34:BC36 BC38:BC40 BC43:BC44 BC46:BC74 BC14:BC29 BC76:BC85">
-    <cfRule type="cellIs" dxfId="144" priority="67" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="139" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD2:BD5 BD8:BD9 BD34:BD36 BD38:BD40 BD43:BD44 BD46:BD74 BD14:BD29 BD76:BD85">
-    <cfRule type="cellIs" dxfId="143" priority="66" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="138" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK14:AK29 AQ15:AQ29 AR14:AR29 AS15:AX29">
-    <cfRule type="cellIs" dxfId="142" priority="65" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="137" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM56">
-    <cfRule type="cellIs" dxfId="141" priority="61" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="136" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR30">
-    <cfRule type="cellIs" dxfId="140" priority="51" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46 I41:I42 I54:I55 I2:I4 I7:I8 I12 I44 I57 I14:I15 I25 I22:I23 I31:I33 I36 I66:I73">
-    <cfRule type="cellIs" dxfId="139" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="134" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41:N49 N51:N74 N76:N82 M2:N2 N3:N38 M3:M86">
-    <cfRule type="cellIs" dxfId="138" priority="27" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="133" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS2">
-    <cfRule type="cellIs" dxfId="137" priority="24" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="132" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT2">
-    <cfRule type="cellIs" dxfId="136" priority="23" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="131" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:K86 K2:K44">
-    <cfRule type="cellIs" dxfId="135" priority="22" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K46:K58 K2:K44 K60:K86">
+    <cfRule type="cellIs" dxfId="130" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J36 J8:J12 J38:J40 J2:J5 J18 J20:J29 J33:J34 J46:J74">
-    <cfRule type="cellIs" dxfId="134" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="129" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L8:L12 L76:L85 L14:L29 L2:L5 L46:L74">
-    <cfRule type="cellIs" dxfId="133" priority="20" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="128" priority="20" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="132" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="127" priority="19" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="129" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="126" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X86">
-    <cfRule type="cellIs" dxfId="128" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="125" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD86">
-    <cfRule type="cellIs" dxfId="126" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="124" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z86">
-    <cfRule type="cellIs" dxfId="125" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="123" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -20278,49 +20243,49 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O86">
-    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q86">
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S86">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W86">
-    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y86">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA86">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -41183,448 +41148,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="121" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="120" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="119" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="118" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="117" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="116" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="115" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="114" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="113" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="112" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="111" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="110" priority="93">
+    <cfRule type="containsBlanks" dxfId="102" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="109" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="108" priority="91">
+    <cfRule type="containsBlanks" dxfId="100" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="107" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="106" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="105" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="104" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="103" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="102" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="101" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="100" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="99" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="98" priority="69">
+    <cfRule type="containsBlanks" dxfId="90" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="96" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="95" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="94" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="93" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="92" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="91" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="90" priority="63">
+    <cfRule type="containsBlanks" dxfId="82" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="89" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="88" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="87" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="86" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="85" priority="59">
+    <cfRule type="containsBlanks" dxfId="77" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="84" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="83" priority="56">
+    <cfRule type="containsBlanks" dxfId="75" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="82" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="81" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="80" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="79" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="78" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="77" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="76" priority="50">
+    <cfRule type="containsBlanks" dxfId="68" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="75" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="74" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="73" priority="47">
+    <cfRule type="containsBlanks" dxfId="65" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="72" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="71" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="70" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="69" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="68" priority="42">
+    <cfRule type="containsBlanks" dxfId="60" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="67" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="66" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="65" priority="39">
+    <cfRule type="containsBlanks" dxfId="57" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="64" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="63" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="62" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="61" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="60" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="59" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="58" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="57" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="55" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="54" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="53" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="52" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="51" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="50" priority="23">
+    <cfRule type="containsBlanks" dxfId="42" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="49" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="48" priority="19">
+    <cfRule type="containsBlanks" dxfId="40" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="46" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="45" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="44" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="43" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="42" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="41" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="40" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="39" priority="22">
+    <cfRule type="containsBlanks" dxfId="31" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="38" priority="11">
+    <cfRule type="containsBlanks" dxfId="30" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="37" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="35" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="34" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="33" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="30" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="29" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="28" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56520,111 +56485,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="27" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="25" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="24" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="23" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="22" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="21" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="20" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="19" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="17" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="16" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="15" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="14" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="12" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -57948,7 +57913,7 @@
       </c>
       <c r="E3" s="68">
         <f ca="1">TODAY()</f>
-        <v>43343</v>
+        <v>43360</v>
       </c>
       <c r="F3" s="67">
         <v>42551</v>
@@ -58299,7 +58264,7 @@
       <c r="F1" s="1"/>
       <c r="I1" s="34">
         <f ca="1">TODAY()</f>
-        <v>43343</v>
+        <v>43360</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -62364,7 +62329,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update 9 18 2018
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A3B404-B0A3-4132-8599-6B136A55CCF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F451440-0E39-4DA6-AAC0-894609E07BBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5958,7 +5958,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9/17/2018</c:v>
+                  <c:v>9/18/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7715,8 +7715,8 @@
   </sheetPr>
   <dimension ref="B1:BT101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -13114,8 +13114,8 @@
       <c r="J39" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K39" s="144" t="s">
-        <v>567</v>
+      <c r="K39" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="L39" s="25"/>
       <c r="M39" s="144" t="s">
@@ -13281,8 +13281,8 @@
       <c r="J40" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K40" s="144" t="s">
-        <v>567</v>
+      <c r="K40" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="L40" s="25"/>
       <c r="M40" s="144" t="s">
@@ -19782,7 +19782,7 @@
       <c r="J85" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K85" s="144" t="s">
+      <c r="K85" s="179" t="s">
         <v>1116</v>
       </c>
       <c r="L85" s="25"/>
@@ -19951,7 +19951,7 @@
       <c r="J86" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K86" s="144" t="s">
+      <c r="K86" s="179" t="s">
         <v>1116</v>
       </c>
       <c r="L86" s="25"/>
@@ -20188,7 +20188,7 @@
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:K58 K2:K44 K60:K86">
+  <conditionalFormatting sqref="K46:K58 K2:K38 K60:K84 K41:K44">
     <cfRule type="cellIs" dxfId="130" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -57913,7 +57913,7 @@
       </c>
       <c r="E3" s="68">
         <f ca="1">TODAY()</f>
-        <v>43360</v>
+        <v>43361</v>
       </c>
       <c r="F3" s="67">
         <v>42551</v>
@@ -58223,7 +58223,7 @@
   <dimension ref="B1:Y90"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="5520" activePane="bottomLeft"/>
+      <pane ySplit="5470" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -58264,7 +58264,7 @@
       <c r="F1" s="1"/>
       <c r="I1" s="34">
         <f ca="1">TODAY()</f>
-        <v>43360</v>
+        <v>43361</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
Upload IOR Doc Info
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C447F4-540A-4205-9078-FE5F41840409}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81474899-1319-4B7B-AA36-135E98F6D8FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8300" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8373" uniqueCount="1230">
   <si>
     <t>#</t>
   </si>
@@ -3520,9 +3520,6 @@
     <t>test 3</t>
   </si>
   <si>
-    <t>test 4</t>
-  </si>
-  <si>
     <t>test 5</t>
   </si>
   <si>
@@ -3538,21 +3535,12 @@
     <t>CCDsComments</t>
   </si>
   <si>
-    <t>test 6</t>
-  </si>
-  <si>
     <t>commenyts</t>
   </si>
   <si>
     <t>CommissioningReport</t>
   </si>
   <si>
-    <t>dskbclkdbshc</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
     <t>24; 25</t>
   </si>
   <si>
@@ -3593,6 +3581,159 @@
   </si>
   <si>
     <t>62; 63; 64; 65</t>
+  </si>
+  <si>
+    <t>256 files in SharePoint</t>
+  </si>
+  <si>
+    <t>42 files in SharePoint</t>
+  </si>
+  <si>
+    <t>0 files in SharePoint</t>
+  </si>
+  <si>
+    <t>29 files in SharePoint</t>
+  </si>
+  <si>
+    <t>18 files in SharePoint</t>
+  </si>
+  <si>
+    <t>957 files in SharePoint</t>
+  </si>
+  <si>
+    <t>85 files in SharePoint</t>
+  </si>
+  <si>
+    <t>9 files in SharePoint</t>
+  </si>
+  <si>
+    <t>125 files in SharePoint</t>
+  </si>
+  <si>
+    <t>219 files in SharePoint</t>
+  </si>
+  <si>
+    <t>65 files in SharePoint</t>
+  </si>
+  <si>
+    <t>2,177 files in SharePoint</t>
+  </si>
+  <si>
+    <t>281 files in SharePoint</t>
+  </si>
+  <si>
+    <t>37 files in SharePoint</t>
+  </si>
+  <si>
+    <t>68 files in SharePoint</t>
+  </si>
+  <si>
+    <t>3 files in SharePoint</t>
+  </si>
+  <si>
+    <t>87 files in SharePoint</t>
+  </si>
+  <si>
+    <t>28 files in SharePoint total for several Infra projects</t>
+  </si>
+  <si>
+    <t>119 files in SharePoint</t>
+  </si>
+  <si>
+    <t>610 files in SharePoint</t>
+  </si>
+  <si>
+    <t>4 files in SharePoint</t>
+  </si>
+  <si>
+    <t>79 files in SharePoint</t>
+  </si>
+  <si>
+    <t>350 files in SharePoint</t>
+  </si>
+  <si>
+    <t>5 files in SharePoint</t>
+  </si>
+  <si>
+    <t>1 files in SharePoint</t>
+  </si>
+  <si>
+    <t>1,409 files in SharePoint</t>
+  </si>
+  <si>
+    <t>1 file in SharePoint</t>
+  </si>
+  <si>
+    <t>17 files in SharePoint</t>
+  </si>
+  <si>
+    <t>68 files in SharePoint - see N</t>
+  </si>
+  <si>
+    <t>68 files in SharePoint - see S</t>
+  </si>
+  <si>
+    <t>70 files in SharePoint</t>
+  </si>
+  <si>
+    <t>1,943 files in SharePoint</t>
+  </si>
+  <si>
+    <t>1,067 files in SharePoint</t>
+  </si>
+  <si>
+    <t>252 files in SharePoint</t>
+  </si>
+  <si>
+    <t>775 files in SharePoint</t>
+  </si>
+  <si>
+    <t>206 files in SharePoint - combined with 13514</t>
+  </si>
+  <si>
+    <t>638 files in SharePoint</t>
+  </si>
+  <si>
+    <t>314 files in SharePoint</t>
+  </si>
+  <si>
+    <t>175 files in SharePoint</t>
+  </si>
+  <si>
+    <t>201 files in SharePoint</t>
+  </si>
+  <si>
+    <t>40 files in SharePoint</t>
+  </si>
+  <si>
+    <t>see # 13410 (N)</t>
+  </si>
+  <si>
+    <t>multiple projects</t>
+  </si>
+  <si>
+    <t>13 files in SharePoint</t>
+  </si>
+  <si>
+    <t>189 files in SharePoint</t>
+  </si>
+  <si>
+    <t>2 files in SharePoint</t>
+  </si>
+  <si>
+    <t>436 files in SharePoint</t>
+  </si>
+  <si>
+    <t>652 files in SharePoint</t>
+  </si>
+  <si>
+    <t>164 files in SharePoint</t>
+  </si>
+  <si>
+    <t>181 files in SharePoint</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -3813,7 +3954,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3949,6 +4090,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -4141,7 +4288,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="32" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4677,6 +4824,10 @@
     <xf numFmtId="0" fontId="22" fillId="23" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4742,7 +4893,350 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="167">
+  <dxfs count="264">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5912,6 +6406,342 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -6158,7 +6988,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10/11/2018</c:v>
+                  <c:v>10/17/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7915,8 +8745,8 @@
   </sheetPr>
   <dimension ref="B1:BT101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8038,22 +8868,22 @@
         <v>1153</v>
       </c>
       <c r="W1" s="143" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="X1" s="143" t="s">
         <v>1154</v>
       </c>
       <c r="Y1" s="18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="Z1" s="18" t="s">
         <v>1160</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="AA1" s="143" t="s">
         <v>1161</v>
       </c>
-      <c r="AA1" s="143" t="s">
+      <c r="AB1" s="143" t="s">
         <v>1162</v>
-      </c>
-      <c r="AB1" s="143" t="s">
-        <v>1163</v>
       </c>
       <c r="AC1" s="18" t="s">
         <v>1155</v>
@@ -8236,10 +9066,12 @@
         <v>567</v>
       </c>
       <c r="X2" s="144"/>
-      <c r="Y2" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z2" s="144"/>
+      <c r="Y2" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z2" s="144" t="s">
+        <v>1179</v>
+      </c>
       <c r="AA2" s="144" t="s">
         <v>567</v>
       </c>
@@ -8379,10 +9211,12 @@
         <v>567</v>
       </c>
       <c r="X3" s="144"/>
-      <c r="Y3" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z3" s="144"/>
+      <c r="Y3" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z3" s="144" t="s">
+        <v>1183</v>
+      </c>
       <c r="AA3" s="144" t="s">
         <v>567</v>
       </c>
@@ -8518,10 +9352,12 @@
         <v>567</v>
       </c>
       <c r="X4" s="144"/>
-      <c r="Y4" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z4" s="144"/>
+      <c r="Y4" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z4" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA4" s="144" t="s">
         <v>567</v>
       </c>
@@ -8530,7 +9366,7 @@
         <v>567</v>
       </c>
       <c r="AD4" s="144" t="s">
-        <v>1167</v>
+        <v>1229</v>
       </c>
       <c r="AE4" s="18"/>
       <c r="AF4" s="144"/>
@@ -8661,10 +9497,12 @@
       <c r="X5" s="144" t="s">
         <v>1157</v>
       </c>
-      <c r="Y5" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z5" s="144"/>
+      <c r="Y5" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z5" s="144" t="s">
+        <v>1184</v>
+      </c>
       <c r="AA5" s="144" t="s">
         <v>567</v>
       </c>
@@ -8672,9 +9510,7 @@
       <c r="AC5" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AD5" s="144" t="s">
-        <v>1168</v>
-      </c>
+      <c r="AD5" s="144"/>
       <c r="AE5" s="18"/>
       <c r="AF5" s="144"/>
       <c r="AG5" s="144"/>
@@ -8804,10 +9640,12 @@
         <v>567</v>
       </c>
       <c r="X6" s="144"/>
-      <c r="Y6" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z6" s="144"/>
+      <c r="Y6" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z6" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA6" s="144" t="s">
         <v>567</v>
       </c>
@@ -8953,30 +9791,28 @@
         <v>567</v>
       </c>
       <c r="V7" s="144" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="W7" s="144" t="s">
         <v>567</v>
       </c>
       <c r="X7" s="144"/>
-      <c r="Y7" s="144" t="s">
-        <v>567</v>
+      <c r="Y7" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="Z7" s="144" t="s">
+        <v>1181</v>
+      </c>
+      <c r="AA7" s="144" t="s">
+        <v>567</v>
+      </c>
+      <c r="AB7" s="144" t="s">
         <v>1158</v>
       </c>
-      <c r="AA7" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB7" s="144" t="s">
-        <v>1159</v>
-      </c>
       <c r="AC7" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AD7" s="144" t="s">
-        <v>1164</v>
-      </c>
+      <c r="AD7" s="144"/>
       <c r="AE7" s="18"/>
       <c r="AF7" s="144"/>
       <c r="AG7" s="144"/>
@@ -9102,10 +9938,12 @@
         <v>567</v>
       </c>
       <c r="X8" s="144"/>
-      <c r="Y8" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z8" s="144"/>
+      <c r="Y8" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z8" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA8" s="144" t="s">
         <v>567</v>
       </c>
@@ -9244,7 +10082,9 @@
       <c r="Y9" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z9" s="144"/>
+      <c r="Z9" s="144" t="s">
+        <v>1185</v>
+      </c>
       <c r="AA9" s="144" t="s">
         <v>567</v>
       </c>
@@ -9350,7 +10190,7 @@
         <v>567</v>
       </c>
       <c r="N10" s="144" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="O10" s="144" t="s">
         <v>567</v>
@@ -9378,10 +10218,12 @@
         <v>567</v>
       </c>
       <c r="X10" s="144"/>
-      <c r="Y10" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z10" s="144"/>
+      <c r="Y10" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z10" s="144" t="s">
+        <v>1188</v>
+      </c>
       <c r="AA10" s="144" t="s">
         <v>567</v>
       </c>
@@ -9519,10 +10361,12 @@
         <v>567</v>
       </c>
       <c r="X11" s="144"/>
-      <c r="Y11" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z11" s="144"/>
+      <c r="Y11" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z11" s="144" t="s">
+        <v>1190</v>
+      </c>
       <c r="AA11" s="144" t="s">
         <v>567</v>
       </c>
@@ -9634,7 +10478,7 @@
         <v>170</v>
       </c>
       <c r="N12" s="144" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="O12" s="144" t="s">
         <v>567</v>
@@ -9665,7 +10509,9 @@
       <c r="Y12" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z12" s="144"/>
+      <c r="Z12" s="144" t="s">
+        <v>1191</v>
+      </c>
       <c r="AA12" s="144" t="s">
         <v>567</v>
       </c>
@@ -9802,7 +10648,9 @@
       <c r="Y13" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z13" s="144"/>
+      <c r="Z13" s="144" t="s">
+        <v>1195</v>
+      </c>
       <c r="AA13" s="144" t="s">
         <v>567</v>
       </c>
@@ -9938,10 +10786,12 @@
         <v>567</v>
       </c>
       <c r="X14" s="144"/>
-      <c r="Y14" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z14" s="144"/>
+      <c r="Y14" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z14" s="144" t="s">
+        <v>1197</v>
+      </c>
       <c r="AA14" s="144" t="s">
         <v>567</v>
       </c>
@@ -10073,10 +10923,12 @@
         <v>567</v>
       </c>
       <c r="X15" s="144"/>
-      <c r="Y15" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z15" s="144"/>
+      <c r="Y15" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z15" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA15" s="144" t="s">
         <v>567</v>
       </c>
@@ -10182,7 +11034,7 @@
         <v>166</v>
       </c>
       <c r="N16" s="144" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="O16" s="144" t="s">
         <v>567</v>
@@ -10210,10 +11062,12 @@
         <v>567</v>
       </c>
       <c r="X16" s="144"/>
-      <c r="Y16" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z16" s="144"/>
+      <c r="Y16" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z16" s="144" t="s">
+        <v>1199</v>
+      </c>
       <c r="AA16" s="144" t="s">
         <v>567</v>
       </c>
@@ -10349,10 +11203,12 @@
         <v>567</v>
       </c>
       <c r="X17" s="144"/>
-      <c r="Y17" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z17" s="144"/>
+      <c r="Y17" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z17" s="144" t="s">
+        <v>1203</v>
+      </c>
       <c r="AA17" s="144" t="s">
         <v>567</v>
       </c>
@@ -10488,10 +11344,12 @@
         <v>567</v>
       </c>
       <c r="X18" s="144"/>
-      <c r="Y18" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z18" s="144"/>
+      <c r="Y18" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z18" s="144" t="s">
+        <v>1202</v>
+      </c>
       <c r="AA18" s="144" t="s">
         <v>567</v>
       </c>
@@ -10627,10 +11485,12 @@
         <v>567</v>
       </c>
       <c r="X19" s="144"/>
-      <c r="Y19" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z19" s="144"/>
+      <c r="Y19" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z19" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA19" s="144" t="s">
         <v>567</v>
       </c>
@@ -10766,10 +11626,12 @@
         <v>567</v>
       </c>
       <c r="X20" s="144"/>
-      <c r="Y20" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z20" s="144"/>
+      <c r="Y20" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z20" s="144" t="s">
+        <v>1204</v>
+      </c>
       <c r="AA20" s="144" t="s">
         <v>567</v>
       </c>
@@ -10877,7 +11739,7 @@
         <v>166</v>
       </c>
       <c r="N21" s="144" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="O21" s="144" t="s">
         <v>567</v>
@@ -10908,7 +11770,9 @@
       <c r="Y21" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z21" s="144"/>
+      <c r="Z21" s="144" t="s">
+        <v>1208</v>
+      </c>
       <c r="AA21" s="144" t="s">
         <v>567</v>
       </c>
@@ -11048,10 +11912,12 @@
         <v>567</v>
       </c>
       <c r="X22" s="144"/>
-      <c r="Y22" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z22" s="144"/>
+      <c r="Y22" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z22" s="144" t="s">
+        <v>1205</v>
+      </c>
       <c r="AA22" s="144" t="s">
         <v>567</v>
       </c>
@@ -11183,8 +12049,8 @@
         <v>567</v>
       </c>
       <c r="X23" s="144"/>
-      <c r="Y23" s="144" t="s">
-        <v>567</v>
+      <c r="Y23" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z23" s="144"/>
       <c r="AA23" s="144" t="s">
@@ -11323,7 +12189,9 @@
       <c r="Y24" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z24" s="144"/>
+      <c r="Z24" s="144" t="s">
+        <v>1209</v>
+      </c>
       <c r="AA24" s="144" t="s">
         <v>567</v>
       </c>
@@ -11463,10 +12331,12 @@
         <v>567</v>
       </c>
       <c r="X25" s="144"/>
-      <c r="Y25" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z25" s="144"/>
+      <c r="Y25" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z25" s="144" t="s">
+        <v>1210</v>
+      </c>
       <c r="AA25" s="144" t="s">
         <v>567</v>
       </c>
@@ -11602,10 +12472,12 @@
         <v>567</v>
       </c>
       <c r="X26" s="144"/>
-      <c r="Y26" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z26" s="144"/>
+      <c r="Y26" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z26" s="144" t="s">
+        <v>1211</v>
+      </c>
       <c r="AA26" s="144" t="s">
         <v>567</v>
       </c>
@@ -11744,7 +12616,9 @@
       <c r="Y27" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z27" s="144"/>
+      <c r="Z27" s="144" t="s">
+        <v>1182</v>
+      </c>
       <c r="AA27" s="144" t="s">
         <v>567</v>
       </c>
@@ -11880,10 +12754,12 @@
         <v>567</v>
       </c>
       <c r="X28" s="144"/>
-      <c r="Y28" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z28" s="144"/>
+      <c r="Y28" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z28" s="144" t="s">
+        <v>1212</v>
+      </c>
       <c r="AA28" s="144" t="s">
         <v>567</v>
       </c>
@@ -11995,7 +12871,7 @@
         <v>166</v>
       </c>
       <c r="N29" s="144" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="O29" s="144" t="s">
         <v>567</v>
@@ -12023,10 +12899,12 @@
         <v>567</v>
       </c>
       <c r="X29" s="144"/>
-      <c r="Y29" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z29" s="144"/>
+      <c r="Y29" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z29" s="144" t="s">
+        <v>1213</v>
+      </c>
       <c r="AA29" s="144" t="s">
         <v>567</v>
       </c>
@@ -12138,7 +13016,7 @@
         <v>166</v>
       </c>
       <c r="N30" s="144" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="O30" s="144" t="s">
         <v>567</v>
@@ -12166,10 +13044,12 @@
         <v>567</v>
       </c>
       <c r="X30" s="144"/>
-      <c r="Y30" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z30" s="144"/>
+      <c r="Y30" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z30" s="144" t="s">
+        <v>1215</v>
+      </c>
       <c r="AA30" s="144" t="s">
         <v>567</v>
       </c>
@@ -12306,7 +13186,9 @@
       <c r="Y31" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z31" s="144"/>
+      <c r="Z31" s="144" t="s">
+        <v>1192</v>
+      </c>
       <c r="AA31" s="144" t="s">
         <v>567</v>
       </c>
@@ -12412,7 +13294,7 @@
         <v>166</v>
       </c>
       <c r="N32" s="144" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="O32" s="144" t="s">
         <v>567</v>
@@ -12440,10 +13322,12 @@
         <v>567</v>
       </c>
       <c r="X32" s="144"/>
-      <c r="Y32" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z32" s="144"/>
+      <c r="Y32" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z32" s="144" t="s">
+        <v>1216</v>
+      </c>
       <c r="AA32" s="144" t="s">
         <v>567</v>
       </c>
@@ -12577,10 +13461,12 @@
         <v>567</v>
       </c>
       <c r="X33" s="144"/>
-      <c r="Y33" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z33" s="144"/>
+      <c r="Y33" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z33" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA33" s="144" t="s">
         <v>567</v>
       </c>
@@ -12714,10 +13600,12 @@
         <v>567</v>
       </c>
       <c r="X34" s="144"/>
-      <c r="Y34" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z34" s="144"/>
+      <c r="Y34" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z34" s="144" t="s">
+        <v>1217</v>
+      </c>
       <c r="AA34" s="144" t="s">
         <v>567</v>
       </c>
@@ -12855,10 +13743,12 @@
         <v>567</v>
       </c>
       <c r="X35" s="144"/>
-      <c r="Y35" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z35" s="144"/>
+      <c r="Y35" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z35" s="144" t="s">
+        <v>1218</v>
+      </c>
       <c r="AA35" s="144" t="s">
         <v>567</v>
       </c>
@@ -12995,7 +13885,9 @@
       <c r="Y36" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z36" s="144"/>
+      <c r="Z36" s="144" t="s">
+        <v>1219</v>
+      </c>
       <c r="AA36" s="144" t="s">
         <v>567</v>
       </c>
@@ -13132,7 +14024,9 @@
       <c r="Y37" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z37" s="144"/>
+      <c r="Z37" s="144" t="s">
+        <v>1195</v>
+      </c>
       <c r="AA37" s="144" t="s">
         <v>567</v>
       </c>
@@ -13264,10 +14158,12 @@
         <v>567</v>
       </c>
       <c r="X38" s="144"/>
-      <c r="Y38" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z38" s="144"/>
+      <c r="Y38" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z38" s="144" t="s">
+        <v>1225</v>
+      </c>
       <c r="AA38" s="144" t="s">
         <v>567</v>
       </c>
@@ -13403,8 +14299,8 @@
         <v>567</v>
       </c>
       <c r="X39" s="144"/>
-      <c r="Y39" s="144" t="s">
-        <v>567</v>
+      <c r="Y39" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z39" s="144"/>
       <c r="AA39" s="144" t="s">
@@ -13570,8 +14466,8 @@
         <v>567</v>
       </c>
       <c r="X40" s="144"/>
-      <c r="Y40" s="144" t="s">
-        <v>567</v>
+      <c r="Y40" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z40" s="144"/>
       <c r="AA40" s="144" t="s">
@@ -13707,7 +14603,7 @@
         <v>567</v>
       </c>
       <c r="N41" s="144" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="O41" s="144" t="s">
         <v>567</v>
@@ -13735,10 +14631,12 @@
         <v>567</v>
       </c>
       <c r="X41" s="144"/>
-      <c r="Y41" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z41" s="144"/>
+      <c r="Y41" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z41" s="144" t="s">
+        <v>1196</v>
+      </c>
       <c r="AA41" s="144" t="s">
         <v>567</v>
       </c>
@@ -13869,7 +14767,9 @@
       <c r="Y42" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z42" s="144"/>
+      <c r="Z42" s="144" t="s">
+        <v>1221</v>
+      </c>
       <c r="AA42" s="144" t="s">
         <v>567</v>
       </c>
@@ -14004,7 +14904,9 @@
       <c r="Y43" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z43" s="144"/>
+      <c r="Z43" s="144" t="s">
+        <v>1180</v>
+      </c>
       <c r="AA43" s="144" t="s">
         <v>567</v>
       </c>
@@ -14170,10 +15072,12 @@
         <v>567</v>
       </c>
       <c r="X44" s="144"/>
-      <c r="Y44" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z44" s="144"/>
+      <c r="Y44" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z44" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA44" s="144" t="s">
         <v>567</v>
       </c>
@@ -14279,7 +15183,7 @@
         <v>166</v>
       </c>
       <c r="N45" s="144" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="O45" s="144" t="s">
         <v>567</v>
@@ -14310,7 +15214,9 @@
       <c r="Y45" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z45" s="144"/>
+      <c r="Z45" s="144" t="s">
+        <v>1182</v>
+      </c>
       <c r="AA45" s="144" t="s">
         <v>567</v>
       </c>
@@ -14452,10 +15358,12 @@
         <v>567</v>
       </c>
       <c r="X46" s="144"/>
-      <c r="Y46" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z46" s="144"/>
+      <c r="Y46" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z46" s="144" t="s">
+        <v>1186</v>
+      </c>
       <c r="AA46" s="144" t="s">
         <v>567</v>
       </c>
@@ -14591,10 +15499,12 @@
         <v>567</v>
       </c>
       <c r="X47" s="144"/>
-      <c r="Y47" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z47" s="144"/>
+      <c r="Y47" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z47" s="144" t="s">
+        <v>1187</v>
+      </c>
       <c r="AA47" s="144" t="s">
         <v>567</v>
       </c>
@@ -14732,10 +15642,12 @@
         <v>567</v>
       </c>
       <c r="X48" s="144"/>
-      <c r="Y48" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z48" s="144"/>
+      <c r="Y48" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z48" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA48" s="144" t="s">
         <v>567</v>
       </c>
@@ -14869,10 +15781,12 @@
         <v>567</v>
       </c>
       <c r="X49" s="144"/>
-      <c r="Y49" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z49" s="144"/>
+      <c r="Y49" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="Z49" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA49" s="144" t="s">
         <v>567</v>
       </c>
@@ -15013,7 +15927,9 @@
       <c r="Y50" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z50" s="144"/>
+      <c r="Z50" s="144" t="s">
+        <v>1189</v>
+      </c>
       <c r="AA50" s="144" t="s">
         <v>567</v>
       </c>
@@ -15186,7 +16102,9 @@
       <c r="Y51" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z51" s="144"/>
+      <c r="Z51" s="144" t="s">
+        <v>1192</v>
+      </c>
       <c r="AA51" s="144" t="s">
         <v>567</v>
       </c>
@@ -15296,7 +16214,7 @@
         <v>166</v>
       </c>
       <c r="N52" s="144" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="O52" s="144" t="s">
         <v>567</v>
@@ -15327,7 +16245,9 @@
       <c r="Y52" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z52" s="144"/>
+      <c r="Z52" s="144" t="s">
+        <v>1193</v>
+      </c>
       <c r="AA52" s="144" t="s">
         <v>567</v>
       </c>
@@ -15439,7 +16359,7 @@
         <v>567</v>
       </c>
       <c r="N53" s="144" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="O53" s="144" t="s">
         <v>567</v>
@@ -15467,10 +16387,12 @@
         <v>567</v>
       </c>
       <c r="X53" s="144"/>
-      <c r="Y53" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z53" s="144"/>
+      <c r="Y53" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z53" s="144" t="s">
+        <v>1194</v>
+      </c>
       <c r="AA53" s="144" t="s">
         <v>567</v>
       </c>
@@ -15598,10 +16520,12 @@
         <v>567</v>
       </c>
       <c r="X54" s="144"/>
-      <c r="Y54" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z54" s="144"/>
+      <c r="Y54" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z54" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA54" s="144" t="s">
         <v>567</v>
       </c>
@@ -15745,10 +16669,12 @@
         <v>567</v>
       </c>
       <c r="X55" s="144"/>
-      <c r="Y55" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z55" s="144"/>
+      <c r="Y55" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z55" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA55" s="144" t="s">
         <v>567</v>
       </c>
@@ -15886,10 +16812,12 @@
         <v>567</v>
       </c>
       <c r="X56" s="144"/>
-      <c r="Y56" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z56" s="144"/>
+      <c r="Y56" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z56" s="144" t="s">
+        <v>1198</v>
+      </c>
       <c r="AA56" s="144" t="s">
         <v>567</v>
       </c>
@@ -16021,10 +16949,12 @@
         <v>567</v>
       </c>
       <c r="X57" s="144"/>
-      <c r="Y57" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z57" s="144"/>
+      <c r="Y57" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z57" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA57" s="144" t="s">
         <v>567</v>
       </c>
@@ -16158,10 +17088,12 @@
         <v>567</v>
       </c>
       <c r="X58" s="144"/>
-      <c r="Y58" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z58" s="144"/>
+      <c r="Y58" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z58" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA58" s="144" t="s">
         <v>567</v>
       </c>
@@ -16336,7 +17268,9 @@
       <c r="Y59" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z59" s="144"/>
+      <c r="Z59" s="144" t="s">
+        <v>1200</v>
+      </c>
       <c r="AA59" s="144" t="s">
         <v>567</v>
       </c>
@@ -16474,10 +17408,12 @@
         <v>567</v>
       </c>
       <c r="X60" s="144"/>
-      <c r="Y60" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z60" s="144"/>
+      <c r="Y60" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z60" s="144" t="s">
+        <v>1201</v>
+      </c>
       <c r="AA60" s="144" t="s">
         <v>567</v>
       </c>
@@ -16607,8 +17543,8 @@
         <v>567</v>
       </c>
       <c r="X61" s="144"/>
-      <c r="Y61" s="144" t="s">
-        <v>567</v>
+      <c r="Y61" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z61" s="144"/>
       <c r="AA61" s="144" t="s">
@@ -16742,10 +17678,12 @@
         <v>567</v>
       </c>
       <c r="X62" s="144"/>
-      <c r="Y62" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z62" s="144"/>
+      <c r="Y62" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z62" s="144" t="s">
+        <v>1205</v>
+      </c>
       <c r="AA62" s="144" t="s">
         <v>567</v>
       </c>
@@ -16877,8 +17815,8 @@
         <v>567</v>
       </c>
       <c r="X63" s="144"/>
-      <c r="Y63" s="144" t="s">
-        <v>567</v>
+      <c r="Y63" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z63" s="144"/>
       <c r="AA63" s="144" t="s">
@@ -16982,7 +17920,7 @@
         <v>1116</v>
       </c>
       <c r="N64" s="144" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="O64" s="144" t="s">
         <v>567</v>
@@ -17013,7 +17951,9 @@
       <c r="Y64" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z64" s="144"/>
+      <c r="Z64" s="144" t="s">
+        <v>1207</v>
+      </c>
       <c r="AA64" s="144" t="s">
         <v>567</v>
       </c>
@@ -17121,7 +18061,7 @@
         <v>166</v>
       </c>
       <c r="N65" s="144" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="O65" s="144" t="s">
         <v>567</v>
@@ -17149,10 +18089,12 @@
         <v>567</v>
       </c>
       <c r="X65" s="144"/>
-      <c r="Y65" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z65" s="144"/>
+      <c r="Y65" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z65" s="144" t="s">
+        <v>1206</v>
+      </c>
       <c r="AA65" s="144" t="s">
         <v>567</v>
       </c>
@@ -17290,10 +18232,12 @@
         <v>567</v>
       </c>
       <c r="X66" s="144"/>
-      <c r="Y66" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z66" s="144"/>
+      <c r="Y66" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z66" s="144" t="s">
+        <v>1205</v>
+      </c>
       <c r="AA66" s="144" t="s">
         <v>567</v>
       </c>
@@ -17399,7 +18343,7 @@
         <v>567</v>
       </c>
       <c r="N67" s="144" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="O67" s="144" t="s">
         <v>567</v>
@@ -17427,10 +18371,12 @@
         <v>567</v>
       </c>
       <c r="X67" s="144"/>
-      <c r="Y67" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z67" s="144"/>
+      <c r="Y67" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z67" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA67" s="144" t="s">
         <v>567</v>
       </c>
@@ -17564,10 +18510,12 @@
         <v>567</v>
       </c>
       <c r="X68" s="144"/>
-      <c r="Y68" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z68" s="144"/>
+      <c r="Y68" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="Z68" s="144" t="s">
+        <v>1220</v>
+      </c>
       <c r="AA68" s="144" t="s">
         <v>567</v>
       </c>
@@ -17701,10 +18649,12 @@
         <v>567</v>
       </c>
       <c r="X69" s="144"/>
-      <c r="Y69" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z69" s="144"/>
+      <c r="Y69" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z69" s="144" t="s">
+        <v>1214</v>
+      </c>
       <c r="AA69" s="144" t="s">
         <v>567</v>
       </c>
@@ -17838,10 +18788,12 @@
         <v>567</v>
       </c>
       <c r="X70" s="144"/>
-      <c r="Y70" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z70" s="144"/>
+      <c r="Y70" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z70" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA70" s="144" t="s">
         <v>567</v>
       </c>
@@ -17973,10 +18925,12 @@
         <v>567</v>
       </c>
       <c r="X71" s="144"/>
-      <c r="Y71" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z71" s="144"/>
+      <c r="Y71" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z71" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA71" s="144" t="s">
         <v>567</v>
       </c>
@@ -18108,10 +19062,12 @@
         <v>567</v>
       </c>
       <c r="X72" s="144"/>
-      <c r="Y72" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z72" s="144"/>
+      <c r="Y72" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z72" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA72" s="144" t="s">
         <v>567</v>
       </c>
@@ -18243,10 +19199,12 @@
         <v>567</v>
       </c>
       <c r="X73" s="144"/>
-      <c r="Y73" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z73" s="144"/>
+      <c r="Y73" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z73" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA73" s="144" t="s">
         <v>567</v>
       </c>
@@ -18382,10 +19340,12 @@
         <v>567</v>
       </c>
       <c r="X74" s="144"/>
-      <c r="Y74" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z74" s="144"/>
+      <c r="Y74" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z74" s="144" t="s">
+        <v>1222</v>
+      </c>
       <c r="AA74" s="144" t="s">
         <v>567</v>
       </c>
@@ -18553,10 +19513,12 @@
         <v>567</v>
       </c>
       <c r="X75" s="144"/>
-      <c r="Y75" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z75" s="144"/>
+      <c r="Y75" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z75" s="144" t="s">
+        <v>1223</v>
+      </c>
       <c r="AA75" s="144" t="s">
         <v>567</v>
       </c>
@@ -18722,10 +19684,12 @@
         <v>567</v>
       </c>
       <c r="X76" s="144"/>
-      <c r="Y76" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z76" s="144"/>
+      <c r="Y76" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z76" s="144" t="s">
+        <v>1224</v>
+      </c>
       <c r="AA76" s="144" t="s">
         <v>567</v>
       </c>
@@ -18867,10 +19831,12 @@
         <v>567</v>
       </c>
       <c r="X77" s="144"/>
-      <c r="Y77" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z77" s="144"/>
+      <c r="Y77" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z77" s="144" t="s">
+        <v>1227</v>
+      </c>
       <c r="AA77" s="144" t="s">
         <v>567</v>
       </c>
@@ -19008,10 +19974,12 @@
         <v>567</v>
       </c>
       <c r="X78" s="144"/>
-      <c r="Y78" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z78" s="144"/>
+      <c r="Y78" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z78" s="144" t="s">
+        <v>1226</v>
+      </c>
       <c r="AA78" s="144" t="s">
         <v>567</v>
       </c>
@@ -19145,10 +20113,12 @@
         <v>567</v>
       </c>
       <c r="X79" s="144"/>
-      <c r="Y79" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z79" s="144"/>
+      <c r="Y79" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z79" s="144" t="s">
+        <v>1228</v>
+      </c>
       <c r="AA79" s="144" t="s">
         <v>567</v>
       </c>
@@ -19296,10 +20266,12 @@
         <v>567</v>
       </c>
       <c r="X80" s="144"/>
-      <c r="Y80" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z80" s="144"/>
+      <c r="Y80" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z80" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA80" s="144" t="s">
         <v>567</v>
       </c>
@@ -19433,10 +20405,12 @@
         <v>567</v>
       </c>
       <c r="X81" s="144"/>
-      <c r="Y81" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z81" s="144"/>
+      <c r="Y81" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z81" s="144" t="s">
+        <v>1181</v>
+      </c>
       <c r="AA81" s="144" t="s">
         <v>567</v>
       </c>
@@ -19602,10 +20576,12 @@
         <v>567</v>
       </c>
       <c r="X82" s="144"/>
-      <c r="Y82" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z82" s="144"/>
+      <c r="Y82" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z82" s="144" t="s">
+        <v>1194</v>
+      </c>
       <c r="AA82" s="144" t="s">
         <v>567</v>
       </c>
@@ -19771,8 +20747,8 @@
         <v>567</v>
       </c>
       <c r="X83" s="144"/>
-      <c r="Y83" s="144" t="s">
-        <v>567</v>
+      <c r="Y83" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z83" s="144"/>
       <c r="AA83" s="144" t="s">
@@ -19938,8 +20914,8 @@
         <v>567</v>
       </c>
       <c r="X84" s="144"/>
-      <c r="Y84" s="144" t="s">
-        <v>567</v>
+      <c r="Y84" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z84" s="144"/>
       <c r="AA84" s="144" t="s">
@@ -20107,8 +21083,8 @@
         <v>567</v>
       </c>
       <c r="X85" s="144"/>
-      <c r="Y85" s="144" t="s">
-        <v>567</v>
+      <c r="Y85" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z85" s="144"/>
       <c r="AA85" s="144" t="s">
@@ -20276,8 +21252,8 @@
         <v>567</v>
       </c>
       <c r="X86" s="144"/>
-      <c r="Y86" s="144" t="s">
-        <v>567</v>
+      <c r="Y86" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="Z86" s="144"/>
       <c r="AA86" s="144" t="s">
@@ -20402,312 +21378,888 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AK39 AK46:AK74 AQ14 AM39 AK38:AM38 AK40:AM40 AK2:AM5 AL46:AM55 AL57:AM74 AR4:AR5 AS14:AX14 AY8:AZ8 AY10:BE12 AS2:BB5 BA8:BB9 AR46:BB74 AY14:BB29 R2 AF46:AG74 AF2:AG5 AF38:AG40 AF8:AG12 AF36:AG36 AF33:AG34 AF43:AG44 AF76:AG85 AF14:AG29 AN46:AQ46 AN5:AP5 AN38:BB40 AK34:BB36 AK43:BB44 AN4:AQ4 AK8:AX12 AN48:AQ74 AN47:AP47 AK76:BB85 AL14:AP29 AN2:AR3 V2:V86">
-    <cfRule type="cellIs" dxfId="166" priority="94" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="263" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY9:AZ9">
-    <cfRule type="cellIs" dxfId="165" priority="93" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="262" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE2:BE5 BE8:BE9 BE34:BE36 BE38:BE40 BE43:BE44 BE46:BE74 BE14:BE29 BE76:BE85">
-    <cfRule type="cellIs" dxfId="164" priority="92" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="261" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL39 AL56">
-    <cfRule type="cellIs" dxfId="163" priority="91" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="260" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC2:BC5 BC8:BC9 BC34:BC36 BC38:BC40 BC43:BC44 BC46:BC74 BC14:BC29 BC76:BC85">
-    <cfRule type="cellIs" dxfId="162" priority="89" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="259" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD2:BD5 BD8:BD9 BD34:BD36 BD38:BD40 BD43:BD44 BD46:BD74 BD14:BD29 BD76:BD85">
-    <cfRule type="cellIs" dxfId="161" priority="88" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="258" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK14:AK29 AQ15:AQ29 AR14:AR29 AS15:AX29">
-    <cfRule type="cellIs" dxfId="160" priority="87" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="257" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM56">
-    <cfRule type="cellIs" dxfId="159" priority="83" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="256" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR30">
-    <cfRule type="cellIs" dxfId="158" priority="73" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="255" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46 I41:I42 I54:I55 I2:I4 I7:I8 I12 I44 I57 I14:I15 I25 I22:I23 I31:I33 I36 I66:I73">
-    <cfRule type="cellIs" dxfId="157" priority="60" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="254" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M61:M63 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M23:N23 N22 M65:M67 M25:N25 N24 M36:N38 M69:M80 M82">
-    <cfRule type="cellIs" dxfId="156" priority="49" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="253" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS2">
-    <cfRule type="cellIs" dxfId="155" priority="46" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="252" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT2">
-    <cfRule type="cellIs" dxfId="154" priority="45" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:K58 K2:K38 K60:K82 K41:K44">
-    <cfRule type="cellIs" dxfId="153" priority="44" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="250" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J36 J8:J12 J38:J40 J2:J5 J18 J20:J29 J33:J34 J46:J74">
-    <cfRule type="cellIs" dxfId="152" priority="43" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="249" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L8:L12 L76:L85 L14:L29 L2:L5 L46:L74">
-    <cfRule type="cellIs" dxfId="151" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="248" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="150" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="149" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="246" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X86">
-    <cfRule type="cellIs" dxfId="148" priority="37" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD86">
-    <cfRule type="cellIs" dxfId="147" priority="35" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="244" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z86">
-    <cfRule type="cellIs" dxfId="146" priority="33" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="Z2 Z44:Z45 Z14 Z61 Z22:Z23 Z63 Z66 Z68:Z69 Z74:Z75 Z71 Z37 Z83:Z86 Z39:Z42">
+    <cfRule type="cellIs" dxfId="243" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB86">
-    <cfRule type="cellIs" dxfId="145" priority="31" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="242" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O86">
-    <cfRule type="cellIs" dxfId="144" priority="30" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="241" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q86">
-    <cfRule type="cellIs" dxfId="143" priority="29" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="240" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S86">
-    <cfRule type="cellIs" dxfId="142" priority="28" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="239" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="141" priority="27" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="238" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W86">
-    <cfRule type="cellIs" dxfId="140" priority="26" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="237" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y86">
-    <cfRule type="cellIs" dxfId="139" priority="25" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="Y44:Y45 Y2 Y9 Y51 Y12:Y14 Y53:Y55 Y59:Y60 Y20 Y41:Y42 Y22 Y24 Y27 Y65:Y67 Y31 Y74:Y75 Y36:Y37 Y62 Y71 Y69">
+    <cfRule type="cellIs" dxfId="236" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA86">
-    <cfRule type="cellIs" dxfId="138" priority="24" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="235" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="137" priority="23" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="234" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="cellIs" dxfId="22" priority="22" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="233" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="21" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="232" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="20" priority="20" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="231" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="19" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="230" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="229" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
+    <cfRule type="cellIs" dxfId="228" priority="116" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5">
+    <cfRule type="cellIs" dxfId="227" priority="115" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2">
+    <cfRule type="cellIs" dxfId="226" priority="114" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3">
+    <cfRule type="cellIs" dxfId="225" priority="113" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10">
+    <cfRule type="cellIs" dxfId="224" priority="112" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4">
+    <cfRule type="cellIs" dxfId="223" priority="111" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7">
+    <cfRule type="cellIs" dxfId="222" priority="110" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M8">
+    <cfRule type="cellIs" dxfId="221" priority="109" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N52">
+    <cfRule type="cellIs" dxfId="220" priority="108" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16">
+    <cfRule type="cellIs" dxfId="219" priority="107" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N60">
+    <cfRule type="cellIs" dxfId="218" priority="106" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M14:N14">
+    <cfRule type="cellIs" dxfId="217" priority="105" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M34">
+    <cfRule type="cellIs" dxfId="216" priority="104" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26">
+    <cfRule type="cellIs" dxfId="215" priority="103" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M26">
+    <cfRule type="cellIs" dxfId="214" priority="102" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N28">
+    <cfRule type="cellIs" dxfId="213" priority="101" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M68">
+    <cfRule type="cellIs" dxfId="212" priority="100" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z43">
+    <cfRule type="cellIs" dxfId="211" priority="99" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y43">
+    <cfRule type="cellIs" dxfId="210" priority="98" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z3">
+    <cfRule type="cellIs" dxfId="209" priority="97" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3">
+    <cfRule type="cellIs" dxfId="208" priority="96" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z4">
+    <cfRule type="cellIs" dxfId="207" priority="95" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y4">
+    <cfRule type="cellIs" dxfId="206" priority="94" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z5">
+    <cfRule type="cellIs" dxfId="205" priority="93" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y5">
+    <cfRule type="cellIs" dxfId="204" priority="92" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z6">
+    <cfRule type="cellIs" dxfId="203" priority="91" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y6">
+    <cfRule type="cellIs" dxfId="202" priority="90" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z7">
+    <cfRule type="cellIs" dxfId="201" priority="89" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y7">
+    <cfRule type="cellIs" dxfId="200" priority="88" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z8:Z9">
+    <cfRule type="cellIs" dxfId="199" priority="87" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y8">
+    <cfRule type="cellIs" dxfId="198" priority="86" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z46">
+    <cfRule type="cellIs" dxfId="197" priority="85" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y46">
+    <cfRule type="cellIs" dxfId="196" priority="84" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z47">
+    <cfRule type="cellIs" dxfId="195" priority="83" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y47">
+    <cfRule type="cellIs" dxfId="194" priority="82" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z10">
+    <cfRule type="cellIs" dxfId="193" priority="81" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y10">
+    <cfRule type="cellIs" dxfId="192" priority="80" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z48">
+    <cfRule type="cellIs" dxfId="191" priority="79" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y48">
+    <cfRule type="cellIs" dxfId="190" priority="78" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z49">
+    <cfRule type="cellIs" dxfId="189" priority="77" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y49">
+    <cfRule type="cellIs" dxfId="188" priority="76" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z50">
+    <cfRule type="cellIs" dxfId="187" priority="75" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y50">
+    <cfRule type="cellIs" dxfId="186" priority="73" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z11:Z13">
+    <cfRule type="cellIs" dxfId="71" priority="72" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y11">
+    <cfRule type="cellIs" dxfId="70" priority="71" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z51">
+    <cfRule type="cellIs" dxfId="69" priority="70" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y52">
+    <cfRule type="cellIs" dxfId="68" priority="69" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z52:Z54">
+    <cfRule type="cellIs" dxfId="67" priority="68" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z56">
+    <cfRule type="cellIs" dxfId="66" priority="67" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y56">
+    <cfRule type="cellIs" dxfId="65" priority="66" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z57:Z58">
+    <cfRule type="cellIs" dxfId="64" priority="65" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y57:Y58">
+    <cfRule type="cellIs" dxfId="63" priority="64" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z15:Z16">
+    <cfRule type="cellIs" dxfId="62" priority="63" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15:Y16">
+    <cfRule type="cellIs" dxfId="61" priority="62" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z59:Z60">
+    <cfRule type="cellIs" dxfId="60" priority="61" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z55">
+    <cfRule type="cellIs" dxfId="59" priority="60" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y19">
+    <cfRule type="cellIs" dxfId="58" priority="59" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z19">
+    <cfRule type="cellIs" dxfId="57" priority="58" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y18">
+    <cfRule type="cellIs" dxfId="56" priority="57" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z18">
+    <cfRule type="cellIs" dxfId="55" priority="56" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y17">
+    <cfRule type="cellIs" dxfId="54" priority="55" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z17">
+    <cfRule type="cellIs" dxfId="53" priority="54" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y86">
+    <cfRule type="cellIs" dxfId="52" priority="53" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y40">
+    <cfRule type="cellIs" dxfId="51" priority="52" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z20">
+    <cfRule type="cellIs" dxfId="50" priority="51" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z62">
+    <cfRule type="cellIs" dxfId="49" priority="50" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z21">
+    <cfRule type="cellIs" dxfId="47" priority="48" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z64:Z65">
+    <cfRule type="cellIs" dxfId="45" priority="46" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y21">
+    <cfRule type="cellIs" dxfId="44" priority="45" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y64">
+    <cfRule type="cellIs" dxfId="43" priority="44" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y23">
+    <cfRule type="cellIs" dxfId="42" priority="43" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z24">
+    <cfRule type="cellIs" dxfId="41" priority="42" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y25">
+    <cfRule type="cellIs" dxfId="40" priority="41" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z25">
+    <cfRule type="cellIs" dxfId="39" priority="40" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z67">
+    <cfRule type="cellIs" dxfId="38" priority="39" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y26">
+    <cfRule type="cellIs" dxfId="37" priority="38" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z26:Z27">
+    <cfRule type="cellIs" dxfId="36" priority="37" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y28:Y30">
+    <cfRule type="cellIs" dxfId="35" priority="36" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z28:Z31">
+    <cfRule type="cellIs" dxfId="34" priority="35" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y72">
+    <cfRule type="cellIs" dxfId="33" priority="34" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z72">
+    <cfRule type="cellIs" dxfId="32" priority="33" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y73">
+    <cfRule type="cellIs" dxfId="31" priority="32" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z73">
+    <cfRule type="cellIs" dxfId="30" priority="31" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y32">
+    <cfRule type="cellIs" dxfId="29" priority="30" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z32">
+    <cfRule type="cellIs" dxfId="28" priority="29" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y33">
+    <cfRule type="cellIs" dxfId="27" priority="28" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z33">
+    <cfRule type="cellIs" dxfId="26" priority="27" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y34:Y35">
+    <cfRule type="cellIs" dxfId="25" priority="26" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z34:Z36">
+    <cfRule type="cellIs" dxfId="24" priority="25" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y61">
+    <cfRule type="cellIs" dxfId="23" priority="24" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y63">
+    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z70">
+    <cfRule type="cellIs" dxfId="21" priority="22" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y70">
+    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y68">
+    <cfRule type="cellIs" dxfId="19" priority="20" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z76">
+    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y76">
+    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z78">
     <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
+  <conditionalFormatting sqref="Y78">
     <cfRule type="cellIs" dxfId="15" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
+  <conditionalFormatting sqref="Z38">
     <cfRule type="cellIs" dxfId="14" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
+  <conditionalFormatting sqref="Y38">
     <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10">
+  <conditionalFormatting sqref="Z77">
     <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4">
+  <conditionalFormatting sqref="Y77">
     <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7">
+  <conditionalFormatting sqref="Z79">
     <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
+  <conditionalFormatting sqref="Y79">
     <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
+  <conditionalFormatting sqref="Z80">
     <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
+  <conditionalFormatting sqref="Y80">
     <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N60">
+  <conditionalFormatting sqref="Z81">
     <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:N14">
+  <conditionalFormatting sqref="Y81">
     <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M34">
+  <conditionalFormatting sqref="Z82">
     <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
+  <conditionalFormatting sqref="Y82">
     <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
+  <conditionalFormatting sqref="Y83">
     <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
+  <conditionalFormatting sqref="Y84:Y85">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M68">
+  <conditionalFormatting sqref="Y39">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -41571,448 +43123,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="136" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="185" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="135" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="184" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="134" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="183" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="133" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="182" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="132" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="181" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="131" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="180" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="130" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="179" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="129" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="178" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="128" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="177" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="127" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="176" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="126" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="175" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="125" priority="93">
+    <cfRule type="containsBlanks" dxfId="174" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="124" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="173" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="123" priority="91">
+    <cfRule type="containsBlanks" dxfId="172" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="122" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="171" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="121" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="170" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="120" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="169" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="119" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="168" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="118" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="167" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="117" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="166" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="116" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="165" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="115" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="164" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="114" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="163" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="113" priority="69">
+    <cfRule type="containsBlanks" dxfId="162" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="161" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="111" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="160" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="110" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="159" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="109" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="158" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="108" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="157" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="107" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="156" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="106" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="155" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="105" priority="63">
+    <cfRule type="containsBlanks" dxfId="154" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="104" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="153" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="103" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="152" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="102" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="151" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="101" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="150" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="100" priority="59">
+    <cfRule type="containsBlanks" dxfId="149" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="99" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="148" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="98" priority="56">
+    <cfRule type="containsBlanks" dxfId="147" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="97" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="146" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="96" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="145" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="95" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="144" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="94" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="143" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="93" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="142" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="92" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="141" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="91" priority="50">
+    <cfRule type="containsBlanks" dxfId="140" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="90" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="139" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="89" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="138" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="88" priority="47">
+    <cfRule type="containsBlanks" dxfId="137" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="87" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="136" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="86" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="135" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="85" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="134" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="84" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="133" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="83" priority="42">
+    <cfRule type="containsBlanks" dxfId="132" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="82" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="131" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="81" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="130" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="80" priority="39">
+    <cfRule type="containsBlanks" dxfId="129" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="79" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="128" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="78" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="127" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="77" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="126" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="76" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="125" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="75" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="124" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="74" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="123" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="73" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="122" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="72" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="121" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="71" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="120" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="70" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="119" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="69" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="118" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="68" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="117" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="67" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="116" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="66" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="115" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="65" priority="23">
+    <cfRule type="containsBlanks" dxfId="114" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="64" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="63" priority="19">
+    <cfRule type="containsBlanks" dxfId="112" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="61" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="110" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="60" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="59" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="108" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="58" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="57" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="106" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="56" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="55" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="104" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="54" priority="22">
+    <cfRule type="containsBlanks" dxfId="103" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="53" priority="11">
+    <cfRule type="containsBlanks" dxfId="102" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="52" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="101" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="51" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="100" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="50" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="99" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="49" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="97" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="46" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="95" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="93" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42142,34 +43694,34 @@
       <c r="D19" s="138"/>
       <c r="E19" s="138"/>
       <c r="F19" s="138"/>
-      <c r="G19" s="184" t="s">
+      <c r="G19" s="185" t="s">
         <v>717</v>
       </c>
-      <c r="H19" s="185"/>
-      <c r="I19" s="185"/>
-      <c r="J19" s="185"/>
-      <c r="K19" s="186"/>
-      <c r="M19" s="184" t="s">
+      <c r="H19" s="186"/>
+      <c r="I19" s="186"/>
+      <c r="J19" s="186"/>
+      <c r="K19" s="187"/>
+      <c r="M19" s="185" t="s">
         <v>718</v>
       </c>
-      <c r="N19" s="185"/>
-      <c r="O19" s="185"/>
-      <c r="P19" s="185"/>
-      <c r="Q19" s="186"/>
-      <c r="S19" s="184" t="s">
+      <c r="N19" s="186"/>
+      <c r="O19" s="186"/>
+      <c r="P19" s="186"/>
+      <c r="Q19" s="187"/>
+      <c r="S19" s="185" t="s">
         <v>716</v>
       </c>
-      <c r="T19" s="185"/>
-      <c r="U19" s="185"/>
-      <c r="V19" s="185"/>
-      <c r="W19" s="186"/>
-      <c r="Y19" s="184" t="s">
+      <c r="T19" s="186"/>
+      <c r="U19" s="186"/>
+      <c r="V19" s="186"/>
+      <c r="W19" s="187"/>
+      <c r="Y19" s="185" t="s">
         <v>724</v>
       </c>
-      <c r="Z19" s="185"/>
-      <c r="AA19" s="185"/>
-      <c r="AB19" s="185"/>
-      <c r="AC19" s="186"/>
+      <c r="Z19" s="186"/>
+      <c r="AA19" s="186"/>
+      <c r="AB19" s="186"/>
+      <c r="AC19" s="187"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="139"/>
@@ -42178,26 +43730,26 @@
       <c r="D20" s="138"/>
       <c r="E20" s="138"/>
       <c r="F20" s="138"/>
-      <c r="G20" s="187"/>
-      <c r="H20" s="188"/>
-      <c r="I20" s="188"/>
-      <c r="J20" s="188"/>
-      <c r="K20" s="189"/>
-      <c r="M20" s="187"/>
-      <c r="N20" s="188"/>
-      <c r="O20" s="188"/>
-      <c r="P20" s="188"/>
-      <c r="Q20" s="189"/>
-      <c r="S20" s="187"/>
-      <c r="T20" s="188"/>
-      <c r="U20" s="188"/>
-      <c r="V20" s="188"/>
-      <c r="W20" s="189"/>
-      <c r="Y20" s="187"/>
-      <c r="Z20" s="188"/>
-      <c r="AA20" s="188"/>
-      <c r="AB20" s="188"/>
-      <c r="AC20" s="189"/>
+      <c r="G20" s="188"/>
+      <c r="H20" s="189"/>
+      <c r="I20" s="189"/>
+      <c r="J20" s="189"/>
+      <c r="K20" s="190"/>
+      <c r="M20" s="188"/>
+      <c r="N20" s="189"/>
+      <c r="O20" s="189"/>
+      <c r="P20" s="189"/>
+      <c r="Q20" s="190"/>
+      <c r="S20" s="188"/>
+      <c r="T20" s="189"/>
+      <c r="U20" s="189"/>
+      <c r="V20" s="189"/>
+      <c r="W20" s="190"/>
+      <c r="Y20" s="188"/>
+      <c r="Z20" s="189"/>
+      <c r="AA20" s="189"/>
+      <c r="AB20" s="189"/>
+      <c r="AC20" s="190"/>
     </row>
     <row r="21" spans="1:29" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="139"/>
@@ -42206,26 +43758,26 @@
       <c r="D21" s="138"/>
       <c r="E21" s="138"/>
       <c r="F21" s="138"/>
-      <c r="G21" s="190"/>
-      <c r="H21" s="191"/>
-      <c r="I21" s="191"/>
-      <c r="J21" s="191"/>
-      <c r="K21" s="192"/>
-      <c r="M21" s="190"/>
-      <c r="N21" s="191"/>
-      <c r="O21" s="191"/>
-      <c r="P21" s="191"/>
-      <c r="Q21" s="192"/>
-      <c r="S21" s="190"/>
-      <c r="T21" s="191"/>
-      <c r="U21" s="191"/>
-      <c r="V21" s="191"/>
-      <c r="W21" s="192"/>
-      <c r="Y21" s="190"/>
-      <c r="Z21" s="191"/>
-      <c r="AA21" s="191"/>
-      <c r="AB21" s="191"/>
-      <c r="AC21" s="192"/>
+      <c r="G21" s="191"/>
+      <c r="H21" s="192"/>
+      <c r="I21" s="192"/>
+      <c r="J21" s="192"/>
+      <c r="K21" s="193"/>
+      <c r="M21" s="191"/>
+      <c r="N21" s="192"/>
+      <c r="O21" s="192"/>
+      <c r="P21" s="192"/>
+      <c r="Q21" s="193"/>
+      <c r="S21" s="191"/>
+      <c r="T21" s="192"/>
+      <c r="U21" s="192"/>
+      <c r="V21" s="192"/>
+      <c r="W21" s="193"/>
+      <c r="Y21" s="191"/>
+      <c r="Z21" s="192"/>
+      <c r="AA21" s="192"/>
+      <c r="AB21" s="192"/>
+      <c r="AC21" s="193"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -42248,95 +43800,95 @@
     </row>
     <row r="40" spans="1:29" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:29" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="184" t="s">
+      <c r="A41" s="185" t="s">
         <v>719</v>
       </c>
-      <c r="B41" s="185"/>
-      <c r="C41" s="185"/>
-      <c r="D41" s="185"/>
-      <c r="E41" s="186"/>
-      <c r="G41" s="184" t="s">
+      <c r="B41" s="186"/>
+      <c r="C41" s="186"/>
+      <c r="D41" s="186"/>
+      <c r="E41" s="187"/>
+      <c r="G41" s="185" t="s">
         <v>722</v>
       </c>
-      <c r="H41" s="185"/>
-      <c r="I41" s="185"/>
-      <c r="J41" s="185"/>
-      <c r="K41" s="186"/>
-      <c r="M41" s="184" t="s">
+      <c r="H41" s="186"/>
+      <c r="I41" s="186"/>
+      <c r="J41" s="186"/>
+      <c r="K41" s="187"/>
+      <c r="M41" s="185" t="s">
         <v>723</v>
       </c>
-      <c r="N41" s="185"/>
-      <c r="O41" s="185"/>
-      <c r="P41" s="185"/>
-      <c r="Q41" s="186"/>
-      <c r="S41" s="184" t="s">
+      <c r="N41" s="186"/>
+      <c r="O41" s="186"/>
+      <c r="P41" s="186"/>
+      <c r="Q41" s="187"/>
+      <c r="S41" s="185" t="s">
         <v>729</v>
       </c>
-      <c r="T41" s="185"/>
-      <c r="U41" s="185"/>
-      <c r="V41" s="185"/>
-      <c r="W41" s="186"/>
-      <c r="Y41" s="184" t="s">
+      <c r="T41" s="186"/>
+      <c r="U41" s="186"/>
+      <c r="V41" s="186"/>
+      <c r="W41" s="187"/>
+      <c r="Y41" s="185" t="s">
         <v>731</v>
       </c>
-      <c r="Z41" s="185"/>
-      <c r="AA41" s="185"/>
-      <c r="AB41" s="185"/>
-      <c r="AC41" s="186"/>
+      <c r="Z41" s="186"/>
+      <c r="AA41" s="186"/>
+      <c r="AB41" s="186"/>
+      <c r="AC41" s="187"/>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A42" s="187"/>
-      <c r="B42" s="188"/>
-      <c r="C42" s="188"/>
-      <c r="D42" s="188"/>
-      <c r="E42" s="189"/>
-      <c r="G42" s="187"/>
-      <c r="H42" s="188"/>
-      <c r="I42" s="188"/>
-      <c r="J42" s="188"/>
-      <c r="K42" s="189"/>
-      <c r="M42" s="187"/>
-      <c r="N42" s="188"/>
-      <c r="O42" s="188"/>
-      <c r="P42" s="188"/>
-      <c r="Q42" s="189"/>
-      <c r="S42" s="187"/>
-      <c r="T42" s="188"/>
-      <c r="U42" s="188"/>
-      <c r="V42" s="188"/>
-      <c r="W42" s="189"/>
-      <c r="Y42" s="187"/>
-      <c r="Z42" s="188"/>
-      <c r="AA42" s="188"/>
-      <c r="AB42" s="188"/>
-      <c r="AC42" s="189"/>
+      <c r="A42" s="188"/>
+      <c r="B42" s="189"/>
+      <c r="C42" s="189"/>
+      <c r="D42" s="189"/>
+      <c r="E42" s="190"/>
+      <c r="G42" s="188"/>
+      <c r="H42" s="189"/>
+      <c r="I42" s="189"/>
+      <c r="J42" s="189"/>
+      <c r="K42" s="190"/>
+      <c r="M42" s="188"/>
+      <c r="N42" s="189"/>
+      <c r="O42" s="189"/>
+      <c r="P42" s="189"/>
+      <c r="Q42" s="190"/>
+      <c r="S42" s="188"/>
+      <c r="T42" s="189"/>
+      <c r="U42" s="189"/>
+      <c r="V42" s="189"/>
+      <c r="W42" s="190"/>
+      <c r="Y42" s="188"/>
+      <c r="Z42" s="189"/>
+      <c r="AA42" s="189"/>
+      <c r="AB42" s="189"/>
+      <c r="AC42" s="190"/>
     </row>
     <row r="43" spans="1:29" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="190"/>
-      <c r="B43" s="191"/>
-      <c r="C43" s="191"/>
-      <c r="D43" s="191"/>
-      <c r="E43" s="192"/>
-      <c r="G43" s="190"/>
-      <c r="H43" s="191"/>
-      <c r="I43" s="191"/>
-      <c r="J43" s="191"/>
-      <c r="K43" s="192"/>
-      <c r="M43" s="190"/>
-      <c r="N43" s="191"/>
-      <c r="O43" s="191"/>
-      <c r="P43" s="191"/>
-      <c r="Q43" s="192"/>
-      <c r="S43" s="190"/>
-      <c r="T43" s="191"/>
-      <c r="U43" s="191"/>
-      <c r="V43" s="191"/>
-      <c r="W43" s="192"/>
-      <c r="Y43" s="190"/>
-      <c r="Z43" s="191"/>
-      <c r="AA43" s="191"/>
-      <c r="AB43" s="191"/>
-      <c r="AC43" s="192"/>
+      <c r="A43" s="191"/>
+      <c r="B43" s="192"/>
+      <c r="C43" s="192"/>
+      <c r="D43" s="192"/>
+      <c r="E43" s="193"/>
+      <c r="G43" s="191"/>
+      <c r="H43" s="192"/>
+      <c r="I43" s="192"/>
+      <c r="J43" s="192"/>
+      <c r="K43" s="193"/>
+      <c r="M43" s="191"/>
+      <c r="N43" s="192"/>
+      <c r="O43" s="192"/>
+      <c r="P43" s="192"/>
+      <c r="Q43" s="193"/>
+      <c r="S43" s="191"/>
+      <c r="T43" s="192"/>
+      <c r="U43" s="192"/>
+      <c r="V43" s="192"/>
+      <c r="W43" s="193"/>
+      <c r="Y43" s="191"/>
+      <c r="Z43" s="192"/>
+      <c r="AA43" s="192"/>
+      <c r="AB43" s="192"/>
+      <c r="AC43" s="193"/>
     </row>
     <row r="45" spans="1:29" s="138" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45"/>
@@ -42421,98 +43973,98 @@
       <c r="L63" s="138"/>
     </row>
     <row r="64" spans="1:29" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="184" t="s">
+      <c r="A64" s="185" t="s">
         <v>734</v>
       </c>
-      <c r="B64" s="185"/>
-      <c r="C64" s="185"/>
-      <c r="D64" s="185"/>
-      <c r="E64" s="186"/>
-      <c r="G64" s="184" t="s">
+      <c r="B64" s="186"/>
+      <c r="C64" s="186"/>
+      <c r="D64" s="186"/>
+      <c r="E64" s="187"/>
+      <c r="G64" s="185" t="s">
         <v>735</v>
       </c>
-      <c r="H64" s="185"/>
-      <c r="I64" s="185"/>
-      <c r="J64" s="185"/>
-      <c r="K64" s="186"/>
+      <c r="H64" s="186"/>
+      <c r="I64" s="186"/>
+      <c r="J64" s="186"/>
+      <c r="K64" s="187"/>
       <c r="L64" s="138"/>
-      <c r="M64" s="193" t="s">
+      <c r="M64" s="194" t="s">
         <v>739</v>
       </c>
-      <c r="N64" s="194"/>
-      <c r="O64" s="194"/>
-      <c r="P64" s="194"/>
-      <c r="Q64" s="195"/>
-      <c r="S64" s="193" t="s">
+      <c r="N64" s="195"/>
+      <c r="O64" s="195"/>
+      <c r="P64" s="195"/>
+      <c r="Q64" s="196"/>
+      <c r="S64" s="194" t="s">
         <v>740</v>
       </c>
-      <c r="T64" s="194"/>
-      <c r="U64" s="194"/>
-      <c r="V64" s="194"/>
-      <c r="W64" s="195"/>
-      <c r="Y64" s="193" t="s">
+      <c r="T64" s="195"/>
+      <c r="U64" s="195"/>
+      <c r="V64" s="195"/>
+      <c r="W64" s="196"/>
+      <c r="Y64" s="194" t="s">
         <v>741</v>
       </c>
-      <c r="Z64" s="194"/>
-      <c r="AA64" s="194"/>
-      <c r="AB64" s="194"/>
-      <c r="AC64" s="195"/>
+      <c r="Z64" s="195"/>
+      <c r="AA64" s="195"/>
+      <c r="AB64" s="195"/>
+      <c r="AC64" s="196"/>
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A65" s="187"/>
-      <c r="B65" s="188"/>
-      <c r="C65" s="188"/>
-      <c r="D65" s="188"/>
-      <c r="E65" s="189"/>
-      <c r="G65" s="187"/>
-      <c r="H65" s="188"/>
-      <c r="I65" s="188"/>
-      <c r="J65" s="188"/>
-      <c r="K65" s="189"/>
+      <c r="A65" s="188"/>
+      <c r="B65" s="189"/>
+      <c r="C65" s="189"/>
+      <c r="D65" s="189"/>
+      <c r="E65" s="190"/>
+      <c r="G65" s="188"/>
+      <c r="H65" s="189"/>
+      <c r="I65" s="189"/>
+      <c r="J65" s="189"/>
+      <c r="K65" s="190"/>
       <c r="L65" s="138"/>
-      <c r="M65" s="196"/>
-      <c r="N65" s="197"/>
-      <c r="O65" s="197"/>
-      <c r="P65" s="197"/>
-      <c r="Q65" s="198"/>
-      <c r="S65" s="196"/>
-      <c r="T65" s="197"/>
-      <c r="U65" s="197"/>
-      <c r="V65" s="197"/>
-      <c r="W65" s="198"/>
-      <c r="Y65" s="196"/>
-      <c r="Z65" s="197"/>
-      <c r="AA65" s="197"/>
-      <c r="AB65" s="197"/>
-      <c r="AC65" s="198"/>
+      <c r="M65" s="197"/>
+      <c r="N65" s="198"/>
+      <c r="O65" s="198"/>
+      <c r="P65" s="198"/>
+      <c r="Q65" s="199"/>
+      <c r="S65" s="197"/>
+      <c r="T65" s="198"/>
+      <c r="U65" s="198"/>
+      <c r="V65" s="198"/>
+      <c r="W65" s="199"/>
+      <c r="Y65" s="197"/>
+      <c r="Z65" s="198"/>
+      <c r="AA65" s="198"/>
+      <c r="AB65" s="198"/>
+      <c r="AC65" s="199"/>
     </row>
     <row r="66" spans="1:29" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="190"/>
-      <c r="B66" s="191"/>
-      <c r="C66" s="191"/>
-      <c r="D66" s="191"/>
-      <c r="E66" s="192"/>
-      <c r="G66" s="190"/>
-      <c r="H66" s="191"/>
-      <c r="I66" s="191"/>
-      <c r="J66" s="191"/>
-      <c r="K66" s="192"/>
+      <c r="A66" s="191"/>
+      <c r="B66" s="192"/>
+      <c r="C66" s="192"/>
+      <c r="D66" s="192"/>
+      <c r="E66" s="193"/>
+      <c r="G66" s="191"/>
+      <c r="H66" s="192"/>
+      <c r="I66" s="192"/>
+      <c r="J66" s="192"/>
+      <c r="K66" s="193"/>
       <c r="L66" s="138"/>
-      <c r="M66" s="199"/>
-      <c r="N66" s="200"/>
-      <c r="O66" s="200"/>
-      <c r="P66" s="200"/>
-      <c r="Q66" s="201"/>
-      <c r="S66" s="199"/>
-      <c r="T66" s="200"/>
-      <c r="U66" s="200"/>
-      <c r="V66" s="200"/>
-      <c r="W66" s="201"/>
-      <c r="Y66" s="199"/>
-      <c r="Z66" s="200"/>
-      <c r="AA66" s="200"/>
-      <c r="AB66" s="200"/>
-      <c r="AC66" s="201"/>
+      <c r="M66" s="200"/>
+      <c r="N66" s="201"/>
+      <c r="O66" s="201"/>
+      <c r="P66" s="201"/>
+      <c r="Q66" s="202"/>
+      <c r="S66" s="200"/>
+      <c r="T66" s="201"/>
+      <c r="U66" s="201"/>
+      <c r="V66" s="201"/>
+      <c r="W66" s="202"/>
+      <c r="Y66" s="200"/>
+      <c r="Z66" s="201"/>
+      <c r="AA66" s="201"/>
+      <c r="AB66" s="201"/>
+      <c r="AC66" s="202"/>
     </row>
     <row r="69" spans="1:29" ht="24" x14ac:dyDescent="0.3">
       <c r="D69" s="142" t="s">
@@ -56908,111 +58460,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="42" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="40" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="89" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="39" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="88" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="38" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="87" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="37" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="36" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="85" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="35" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="84" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="34" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="83" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="33" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="82" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="32" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="81" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="31" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="80" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="29" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="78" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="27" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="26" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="25" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -58305,13 +59857,13 @@
       <c r="C1" s="74" t="s">
         <v>477</v>
       </c>
-      <c r="F1" s="202" t="s">
+      <c r="F1" s="203" t="s">
         <v>476</v>
       </c>
-      <c r="G1" s="202"/>
-      <c r="H1" s="202"/>
-      <c r="I1" s="202"/>
-      <c r="J1" s="202"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
+      <c r="I1" s="203"/>
+      <c r="J1" s="203"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D2" s="69" t="s">
@@ -58336,7 +59888,7 @@
       </c>
       <c r="E3" s="68">
         <f ca="1">TODAY()</f>
-        <v>43384</v>
+        <v>43390</v>
       </c>
       <c r="F3" s="67">
         <v>42551</v>
@@ -58646,7 +60198,7 @@
   <dimension ref="B1:Y90"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="5475" activePane="bottomLeft"/>
+      <pane ySplit="5535" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -58687,7 +60239,7 @@
       <c r="F1" s="1"/>
       <c r="I1" s="34">
         <f ca="1">TODAY()</f>
-        <v>43384</v>
+        <v>43390</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -62752,7 +64304,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="23" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
update LEED info per 10-17-2018 controls meeting
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81474899-1319-4B7B-AA36-135E98F6D8FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2B5A4A-E6EC-4B2F-AFAD-77916FD09BE1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8373" uniqueCount="1230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8384" uniqueCount="1231">
   <si>
     <t>#</t>
   </si>
@@ -3734,6 +3734,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>per 10/17/2018 controls meeting</t>
   </si>
 </sst>
 </file>
@@ -4893,504 +4896,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="264">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="263">
     <dxf>
       <fill>
         <patternFill>
@@ -6193,6 +5699,496 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8745,8 +8741,8 @@
   </sheetPr>
   <dimension ref="B1:BT101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8759,7 +8755,7 @@
     <col min="6" max="6" width="22.08984375" customWidth="1"/>
     <col min="7" max="7" width="3.26953125" style="1" customWidth="1"/>
     <col min="8" max="9" width="3.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.90625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" style="1" customWidth="1"/>
     <col min="11" max="11" width="3.6328125" style="1" customWidth="1"/>
     <col min="12" max="12" width="5.26953125" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.26953125" style="2" customWidth="1"/>
@@ -13125,7 +13121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:72" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:72" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B31" s="19" t="s">
         <v>86</v>
       </c>
@@ -13145,10 +13141,12 @@
       <c r="H31" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J31" s="144"/>
+      <c r="I31" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J31" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K31" s="144" t="s">
         <v>567</v>
       </c>
@@ -15296,7 +15294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:72" s="24" customFormat="1" ht="40" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:72" s="24" customFormat="1" ht="56" x14ac:dyDescent="0.25">
       <c r="B46" s="19" t="s">
         <v>4</v>
       </c>
@@ -15316,10 +15314,12 @@
       <c r="H46" s="144" t="s">
         <v>1129</v>
       </c>
-      <c r="I46" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J46" s="144"/>
+      <c r="I46" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J46" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K46" s="180" t="s">
         <v>1112</v>
       </c>
@@ -16462,7 +16462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:72" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:72" s="24" customFormat="1" ht="56" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>4</v>
       </c>
@@ -16482,10 +16482,12 @@
       <c r="H54" s="144" t="s">
         <v>168</v>
       </c>
-      <c r="I54" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J54" s="144"/>
+      <c r="I54" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J54" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K54" s="144" t="s">
         <v>567</v>
       </c>
@@ -16611,7 +16613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:72" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:72" s="24" customFormat="1" ht="56" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>4</v>
       </c>
@@ -16631,10 +16633,12 @@
       <c r="H55" s="144" t="s">
         <v>167</v>
       </c>
-      <c r="I55" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J55" s="144"/>
+      <c r="I55" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J55" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K55" s="144" t="s">
         <v>567</v>
       </c>
@@ -16891,7 +16895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:72" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:72" s="24" customFormat="1" ht="56" x14ac:dyDescent="0.25">
       <c r="B57" s="19" t="s">
         <v>4</v>
       </c>
@@ -16911,10 +16915,12 @@
       <c r="H57" s="144" t="s">
         <v>164</v>
       </c>
-      <c r="I57" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J57" s="144"/>
+      <c r="I57" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J57" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K57" s="144" t="s">
         <v>567</v>
       </c>
@@ -18170,7 +18176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:72" s="24" customFormat="1" ht="40" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:72" s="24" customFormat="1" ht="56" x14ac:dyDescent="0.25">
       <c r="B66" s="19" t="s">
         <v>4</v>
       </c>
@@ -18190,10 +18196,12 @@
       <c r="H66" s="144" t="s">
         <v>1133</v>
       </c>
-      <c r="I66" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J66" s="144"/>
+      <c r="I66" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J66" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K66" s="144" t="s">
         <v>567</v>
       </c>
@@ -18311,7 +18319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:72" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:72" s="24" customFormat="1" ht="56" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
         <v>4</v>
       </c>
@@ -18331,10 +18339,12 @@
       <c r="H67" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="I67" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J67" s="144"/>
+      <c r="I67" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J67" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K67" s="144" t="s">
         <v>567</v>
       </c>
@@ -18730,7 +18740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:72" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:72" s="24" customFormat="1" ht="56" x14ac:dyDescent="0.25">
       <c r="B70" s="19" t="s">
         <v>4</v>
       </c>
@@ -18750,10 +18760,12 @@
       <c r="H70" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="I70" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J70" s="144"/>
+      <c r="I70" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J70" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K70" s="144" t="s">
         <v>567</v>
       </c>
@@ -18887,10 +18899,12 @@
       <c r="H71" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="I71" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J71" s="144"/>
+      <c r="I71" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J71" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K71" s="144" t="s">
         <v>567</v>
       </c>
@@ -19024,10 +19038,12 @@
       <c r="H72" s="144" t="s">
         <v>1134</v>
       </c>
-      <c r="I72" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J72" s="144"/>
+      <c r="I72" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J72" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K72" s="144" t="s">
         <v>567</v>
       </c>
@@ -19141,7 +19157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:72" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:72" s="24" customFormat="1" ht="56" x14ac:dyDescent="0.25">
       <c r="B73" s="19" t="s">
         <v>4</v>
       </c>
@@ -19161,10 +19177,12 @@
       <c r="H73" s="144" t="s">
         <v>1135</v>
       </c>
-      <c r="I73" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="J73" s="144"/>
+      <c r="I73" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J73" s="144" t="s">
+        <v>1230</v>
+      </c>
       <c r="K73" s="144" t="s">
         <v>567</v>
       </c>
@@ -21378,888 +21396,894 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AK39 AK46:AK74 AQ14 AM39 AK38:AM38 AK40:AM40 AK2:AM5 AL46:AM55 AL57:AM74 AR4:AR5 AS14:AX14 AY8:AZ8 AY10:BE12 AS2:BB5 BA8:BB9 AR46:BB74 AY14:BB29 R2 AF46:AG74 AF2:AG5 AF38:AG40 AF8:AG12 AF36:AG36 AF33:AG34 AF43:AG44 AF76:AG85 AF14:AG29 AN46:AQ46 AN5:AP5 AN38:BB40 AK34:BB36 AK43:BB44 AN4:AQ4 AK8:AX12 AN48:AQ74 AN47:AP47 AK76:BB85 AL14:AP29 AN2:AR3 V2:V86">
-    <cfRule type="cellIs" dxfId="263" priority="193" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="262" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY9:AZ9">
-    <cfRule type="cellIs" dxfId="262" priority="192" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="261" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE2:BE5 BE8:BE9 BE34:BE36 BE38:BE40 BE43:BE44 BE46:BE74 BE14:BE29 BE76:BE85">
-    <cfRule type="cellIs" dxfId="261" priority="191" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="260" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL39 AL56">
-    <cfRule type="cellIs" dxfId="260" priority="190" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="259" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC2:BC5 BC8:BC9 BC34:BC36 BC38:BC40 BC43:BC44 BC46:BC74 BC14:BC29 BC76:BC85">
-    <cfRule type="cellIs" dxfId="259" priority="188" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="258" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD2:BD5 BD8:BD9 BD34:BD36 BD38:BD40 BD43:BD44 BD46:BD74 BD14:BD29 BD76:BD85">
-    <cfRule type="cellIs" dxfId="258" priority="187" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="257" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK14:AK29 AQ15:AQ29 AR14:AR29 AS15:AX29">
-    <cfRule type="cellIs" dxfId="257" priority="186" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="256" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM56">
-    <cfRule type="cellIs" dxfId="256" priority="182" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="255" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR30">
-    <cfRule type="cellIs" dxfId="255" priority="172" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="254" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46 I41:I42 I54:I55 I2:I4 I7:I8 I12 I44 I57 I14:I15 I25 I22:I23 I31:I33 I36 I66:I73">
-    <cfRule type="cellIs" dxfId="254" priority="159" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="I41:I42 I2:I4 I7:I8 I12 I44 I14:I15 I25 I22:I23 I32:I33 I36 I68:I69">
+    <cfRule type="cellIs" dxfId="253" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M61:M63 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M23:N23 N22 M65:M67 M25:N25 N24 M36:N38 M69:M80 M82">
-    <cfRule type="cellIs" dxfId="253" priority="148" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="252" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS2">
-    <cfRule type="cellIs" dxfId="252" priority="145" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT2">
-    <cfRule type="cellIs" dxfId="251" priority="144" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="250" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:K58 K2:K38 K60:K82 K41:K44">
-    <cfRule type="cellIs" dxfId="250" priority="143" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="249" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J36 J8:J12 J38:J40 J2:J5 J18 J20:J29 J33:J34 J46:J74">
-    <cfRule type="cellIs" dxfId="249" priority="142" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="248" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L8:L12 L76:L85 L14:L29 L2:L5 L46:L74">
-    <cfRule type="cellIs" dxfId="248" priority="141" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="247" priority="140" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="246" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="246" priority="137" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X86">
-    <cfRule type="cellIs" dxfId="245" priority="136" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="244" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD86">
-    <cfRule type="cellIs" dxfId="244" priority="134" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="243" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2 Z44:Z45 Z14 Z61 Z22:Z23 Z63 Z66 Z68:Z69 Z74:Z75 Z71 Z37 Z83:Z86 Z39:Z42">
-    <cfRule type="cellIs" dxfId="243" priority="132" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="242" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB86">
-    <cfRule type="cellIs" dxfId="242" priority="130" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="241" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O86">
-    <cfRule type="cellIs" dxfId="241" priority="129" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="240" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q86">
-    <cfRule type="cellIs" dxfId="240" priority="128" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="239" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S86">
-    <cfRule type="cellIs" dxfId="239" priority="127" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="238" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="238" priority="126" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="237" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W86">
-    <cfRule type="cellIs" dxfId="237" priority="125" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="236" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y44:Y45 Y2 Y9 Y51 Y12:Y14 Y53:Y55 Y59:Y60 Y20 Y41:Y42 Y22 Y24 Y27 Y65:Y67 Y31 Y74:Y75 Y36:Y37 Y62 Y71 Y69">
-    <cfRule type="cellIs" dxfId="236" priority="124" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="235" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA86">
-    <cfRule type="cellIs" dxfId="235" priority="123" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="234" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="234" priority="122" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="233" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="cellIs" dxfId="233" priority="121" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="232" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="232" priority="120" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="231" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="231" priority="119" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="230" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="230" priority="118" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="229" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="cellIs" dxfId="229" priority="117" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="228" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
-    <cfRule type="cellIs" dxfId="228" priority="116" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="227" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="227" priority="115" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="226" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="226" priority="114" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="225" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="225" priority="113" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="224" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="224" priority="112" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="223" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="cellIs" dxfId="223" priority="111" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="222" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="222" priority="110" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="221" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="221" priority="109" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="220" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="220" priority="108" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="219" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="219" priority="107" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="218" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60">
-    <cfRule type="cellIs" dxfId="218" priority="106" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="217" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:N14">
-    <cfRule type="cellIs" dxfId="217" priority="105" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="216" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="216" priority="104" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="215" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="215" priority="103" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="214" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
-    <cfRule type="cellIs" dxfId="214" priority="102" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="213" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="cellIs" dxfId="213" priority="101" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="212" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="cellIs" dxfId="212" priority="100" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="211" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z43">
-    <cfRule type="cellIs" dxfId="211" priority="99" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="210" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y43">
-    <cfRule type="cellIs" dxfId="210" priority="98" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="209" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3">
-    <cfRule type="cellIs" dxfId="209" priority="97" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="208" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3">
-    <cfRule type="cellIs" dxfId="208" priority="96" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="207" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z4">
-    <cfRule type="cellIs" dxfId="207" priority="95" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="206" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y4">
-    <cfRule type="cellIs" dxfId="206" priority="94" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="205" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5">
-    <cfRule type="cellIs" dxfId="205" priority="93" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="204" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y5">
-    <cfRule type="cellIs" dxfId="204" priority="92" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="203" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z6">
-    <cfRule type="cellIs" dxfId="203" priority="91" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="202" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y6">
-    <cfRule type="cellIs" dxfId="202" priority="90" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="201" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z7">
-    <cfRule type="cellIs" dxfId="201" priority="89" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="200" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y7">
-    <cfRule type="cellIs" dxfId="200" priority="88" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="199" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z8:Z9">
-    <cfRule type="cellIs" dxfId="199" priority="87" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="198" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y8">
-    <cfRule type="cellIs" dxfId="198" priority="86" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="197" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46">
-    <cfRule type="cellIs" dxfId="197" priority="85" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="196" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y46">
-    <cfRule type="cellIs" dxfId="196" priority="84" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="195" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z47">
-    <cfRule type="cellIs" dxfId="195" priority="83" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="194" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y47">
-    <cfRule type="cellIs" dxfId="194" priority="82" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="193" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z10">
-    <cfRule type="cellIs" dxfId="193" priority="81" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="192" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10">
-    <cfRule type="cellIs" dxfId="192" priority="80" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="191" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z48">
-    <cfRule type="cellIs" dxfId="191" priority="79" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="190" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y48">
-    <cfRule type="cellIs" dxfId="190" priority="78" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="189" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z49">
-    <cfRule type="cellIs" dxfId="189" priority="77" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="188" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y49">
-    <cfRule type="cellIs" dxfId="188" priority="76" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="187" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z50">
-    <cfRule type="cellIs" dxfId="187" priority="75" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="186" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y50">
-    <cfRule type="cellIs" dxfId="186" priority="73" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="185" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z11:Z13">
-    <cfRule type="cellIs" dxfId="71" priority="72" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="184" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y11">
-    <cfRule type="cellIs" dxfId="70" priority="71" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="183" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z51">
-    <cfRule type="cellIs" dxfId="69" priority="70" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="182" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y52">
-    <cfRule type="cellIs" dxfId="68" priority="69" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="181" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z52:Z54">
-    <cfRule type="cellIs" dxfId="67" priority="68" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="180" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z56">
-    <cfRule type="cellIs" dxfId="66" priority="67" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="179" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y56">
-    <cfRule type="cellIs" dxfId="65" priority="66" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="178" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z57:Z58">
-    <cfRule type="cellIs" dxfId="64" priority="65" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="177" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y57:Y58">
-    <cfRule type="cellIs" dxfId="63" priority="64" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="176" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z15:Z16">
-    <cfRule type="cellIs" dxfId="62" priority="63" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="175" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y15:Y16">
-    <cfRule type="cellIs" dxfId="61" priority="62" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="174" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z59:Z60">
-    <cfRule type="cellIs" dxfId="60" priority="61" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="173" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z55">
-    <cfRule type="cellIs" dxfId="59" priority="60" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="172" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y19">
-    <cfRule type="cellIs" dxfId="58" priority="59" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="171" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z19">
-    <cfRule type="cellIs" dxfId="57" priority="58" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="170" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y18">
-    <cfRule type="cellIs" dxfId="56" priority="57" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="169" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z18">
-    <cfRule type="cellIs" dxfId="55" priority="56" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="168" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y17">
-    <cfRule type="cellIs" dxfId="54" priority="55" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="167" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17">
-    <cfRule type="cellIs" dxfId="53" priority="54" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="166" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y86">
-    <cfRule type="cellIs" dxfId="52" priority="53" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="165" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y40">
-    <cfRule type="cellIs" dxfId="51" priority="52" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="164" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z20">
-    <cfRule type="cellIs" dxfId="50" priority="51" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="163" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z62">
-    <cfRule type="cellIs" dxfId="49" priority="50" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="162" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z21">
-    <cfRule type="cellIs" dxfId="47" priority="48" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="161" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z64:Z65">
-    <cfRule type="cellIs" dxfId="45" priority="46" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="160" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y21">
-    <cfRule type="cellIs" dxfId="44" priority="45" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="159" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y64">
-    <cfRule type="cellIs" dxfId="43" priority="44" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="158" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y23">
-    <cfRule type="cellIs" dxfId="42" priority="43" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="157" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z24">
-    <cfRule type="cellIs" dxfId="41" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="156" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y25">
-    <cfRule type="cellIs" dxfId="40" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="155" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="cellIs" dxfId="39" priority="40" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="154" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z67">
-    <cfRule type="cellIs" dxfId="38" priority="39" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="153" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y26">
-    <cfRule type="cellIs" dxfId="37" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="152" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26:Z27">
-    <cfRule type="cellIs" dxfId="36" priority="37" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="151" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y28:Y30">
-    <cfRule type="cellIs" dxfId="35" priority="36" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="150" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z28:Z31">
-    <cfRule type="cellIs" dxfId="34" priority="35" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="149" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y72">
-    <cfRule type="cellIs" dxfId="33" priority="34" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="148" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z72">
-    <cfRule type="cellIs" dxfId="32" priority="33" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="147" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y73">
-    <cfRule type="cellIs" dxfId="31" priority="32" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="146" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z73">
-    <cfRule type="cellIs" dxfId="30" priority="31" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="145" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y32">
-    <cfRule type="cellIs" dxfId="29" priority="30" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="144" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z32">
-    <cfRule type="cellIs" dxfId="28" priority="29" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="143" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y33">
-    <cfRule type="cellIs" dxfId="27" priority="28" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="142" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z33">
-    <cfRule type="cellIs" dxfId="26" priority="27" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="141" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y34:Y35">
-    <cfRule type="cellIs" dxfId="25" priority="26" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="140" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34:Z36">
-    <cfRule type="cellIs" dxfId="24" priority="25" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="139" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y61">
-    <cfRule type="cellIs" dxfId="23" priority="24" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="138" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y63">
-    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="137" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z70">
-    <cfRule type="cellIs" dxfId="21" priority="22" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="136" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y70">
-    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y68">
-    <cfRule type="cellIs" dxfId="19" priority="20" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="134" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z76">
-    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="133" priority="20" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y76">
-    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="132" priority="19" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z78">
-    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="131" priority="18" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y78">
-    <cfRule type="cellIs" dxfId="15" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="130" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z38">
-    <cfRule type="cellIs" dxfId="14" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="129" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y38">
-    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="128" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z77">
-    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="127" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y77">
-    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="126" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z79">
-    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="125" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y79">
-    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z80">
-    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y80">
-    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z81">
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y81">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z82">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y82">
-    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y83">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y84:Y85">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y39">
+    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -43123,448 +43147,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="185" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="114" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="184" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="113" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="183" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="112" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="182" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="111" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="181" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="110" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="180" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="109" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="179" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="108" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="178" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="107" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="177" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="106" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="176" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="105" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="175" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="104" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="174" priority="93">
+    <cfRule type="containsBlanks" dxfId="103" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="173" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="102" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="172" priority="91">
+    <cfRule type="containsBlanks" dxfId="101" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="171" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="100" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="170" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="99" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="169" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="98" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="168" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="97" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="167" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="96" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="166" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="95" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="165" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="94" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="164" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="93" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="163" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="92" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="162" priority="69">
+    <cfRule type="containsBlanks" dxfId="91" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="160" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="89" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="159" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="88" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="158" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="87" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="157" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="86" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="156" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="85" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="155" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="84" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="154" priority="63">
+    <cfRule type="containsBlanks" dxfId="83" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="153" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="82" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="152" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="81" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="151" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="80" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="150" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="79" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="149" priority="59">
+    <cfRule type="containsBlanks" dxfId="78" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="148" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="77" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="147" priority="56">
+    <cfRule type="containsBlanks" dxfId="76" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="146" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="75" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="145" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="74" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="144" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="73" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="143" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="72" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="142" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="71" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="141" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="70" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="140" priority="50">
+    <cfRule type="containsBlanks" dxfId="69" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="139" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="68" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="138" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="67" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="137" priority="47">
+    <cfRule type="containsBlanks" dxfId="66" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="136" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="65" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="135" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="64" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="134" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="63" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="133" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="62" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="132" priority="42">
+    <cfRule type="containsBlanks" dxfId="61" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="131" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="60" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="130" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="59" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="129" priority="39">
+    <cfRule type="containsBlanks" dxfId="58" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="128" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="57" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="127" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="56" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="126" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="55" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="125" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="124" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="53" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="123" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="52" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="122" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="121" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="50" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="120" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="49" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="119" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="118" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="47" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="117" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="46" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="116" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="115" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="44" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="114" priority="23">
+    <cfRule type="containsBlanks" dxfId="43" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="113" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="112" priority="19">
+    <cfRule type="containsBlanks" dxfId="41" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="40" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="110" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="109" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="108" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="107" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="106" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="105" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="104" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="103" priority="22">
+    <cfRule type="containsBlanks" dxfId="32" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="102" priority="11">
+    <cfRule type="containsBlanks" dxfId="31" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="101" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="100" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="99" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="98" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="97" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="96" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="95" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="94" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="93" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="92" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58460,111 +58484,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="91" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="89" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="88" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="87" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="86" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="85" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="84" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="83" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="82" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="81" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="80" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="79" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="78" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="77" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="76" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="75" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="74" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="73" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -64304,7 +64328,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="72" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
Formating fixes to charts etc
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B718097-DE34-407B-8A08-15FA0A49509D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89959B4-5EB3-43AC-A51A-8AF9EE0E02A2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8898" uniqueCount="1296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8900" uniqueCount="1297">
   <si>
     <t>#</t>
   </si>
@@ -3933,6 +3933,9 @@
   </si>
   <si>
     <t>MinutesComments</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -5043,6 +5046,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5100,10 +5107,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -5113,20 +5116,6 @@
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="286">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7115,6 +7104,20 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7361,7 +7364,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11/26/2018</c:v>
+                  <c:v>12/7/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9118,8 +9121,8 @@
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9244,34 +9247,34 @@
       <c r="T1" s="18" t="s">
         <v>1151</v>
       </c>
-      <c r="U1" s="205" t="s">
+      <c r="U1" s="186" t="s">
         <v>1111</v>
       </c>
-      <c r="V1" s="205" t="s">
+      <c r="V1" s="186" t="s">
         <v>1295</v>
       </c>
-      <c r="W1" s="205" t="s">
+      <c r="W1" s="186" t="s">
         <v>1290</v>
       </c>
-      <c r="X1" s="205" t="s">
+      <c r="X1" s="186" t="s">
         <v>1291</v>
       </c>
-      <c r="Y1" s="205" t="s">
+      <c r="Y1" s="186" t="s">
         <v>144</v>
       </c>
-      <c r="Z1" s="205" t="s">
+      <c r="Z1" s="186" t="s">
         <v>1292</v>
       </c>
-      <c r="AA1" s="205" t="s">
+      <c r="AA1" s="186" t="s">
         <v>707</v>
       </c>
-      <c r="AB1" s="205" t="s">
+      <c r="AB1" s="186" t="s">
         <v>1293</v>
       </c>
-      <c r="AC1" s="205" t="s">
+      <c r="AC1" s="186" t="s">
         <v>728</v>
       </c>
-      <c r="AD1" s="205" t="s">
+      <c r="AD1" s="186" t="s">
         <v>1294</v>
       </c>
       <c r="AE1" s="18" t="s">
@@ -9661,8 +9664,8 @@
       <c r="Y3" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z3" s="144">
-        <v>1</v>
+      <c r="Z3" s="144" t="s">
+        <v>1296</v>
       </c>
       <c r="AA3" s="144" t="s">
         <v>567</v>
@@ -9832,8 +9835,8 @@
       <c r="Y4" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="Z4" s="144">
-        <v>1</v>
+      <c r="Z4" s="144" t="s">
+        <v>1296</v>
       </c>
       <c r="AA4" s="144" t="s">
         <v>567</v>
@@ -25373,13 +25376,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -46242,448 +46245,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="115" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="114" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="113" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="112" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="111" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="110" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="109" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="108" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="107" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="106" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="105" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="104" priority="93">
+    <cfRule type="containsBlanks" dxfId="102" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="103" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="102" priority="91">
+    <cfRule type="containsBlanks" dxfId="100" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="101" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="100" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="99" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="98" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="97" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="96" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="95" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="94" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="93" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="92" priority="69">
+    <cfRule type="containsBlanks" dxfId="90" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="90" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="89" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="88" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="87" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="86" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="85" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="84" priority="63">
+    <cfRule type="containsBlanks" dxfId="82" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="83" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="82" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="81" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="80" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="79" priority="59">
+    <cfRule type="containsBlanks" dxfId="77" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="78" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="77" priority="56">
+    <cfRule type="containsBlanks" dxfId="75" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="76" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="75" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="74" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="73" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="72" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="71" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="70" priority="50">
+    <cfRule type="containsBlanks" dxfId="68" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="69" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="68" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="67" priority="47">
+    <cfRule type="containsBlanks" dxfId="65" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="66" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="65" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="64" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="63" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="62" priority="42">
+    <cfRule type="containsBlanks" dxfId="60" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="61" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="60" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="59" priority="39">
+    <cfRule type="containsBlanks" dxfId="57" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="58" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="57" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="56" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="55" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="54" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="53" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="52" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="51" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="50" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="49" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="48" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="47" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="46" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="44" priority="23">
+    <cfRule type="containsBlanks" dxfId="42" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="43" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="42" priority="19">
+    <cfRule type="containsBlanks" dxfId="40" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="40" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="39" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="37" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="36" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="34" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="33" priority="22">
+    <cfRule type="containsBlanks" dxfId="31" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="32" priority="11">
+    <cfRule type="containsBlanks" dxfId="30" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="31" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46813,34 +46816,34 @@
       <c r="D19" s="138"/>
       <c r="E19" s="138"/>
       <c r="F19" s="138"/>
-      <c r="G19" s="186" t="s">
+      <c r="G19" s="187" t="s">
         <v>717</v>
       </c>
-      <c r="H19" s="187"/>
-      <c r="I19" s="187"/>
-      <c r="J19" s="187"/>
-      <c r="K19" s="188"/>
-      <c r="M19" s="186" t="s">
+      <c r="H19" s="188"/>
+      <c r="I19" s="188"/>
+      <c r="J19" s="188"/>
+      <c r="K19" s="189"/>
+      <c r="M19" s="187" t="s">
         <v>718</v>
       </c>
-      <c r="N19" s="187"/>
-      <c r="O19" s="187"/>
-      <c r="P19" s="187"/>
-      <c r="Q19" s="188"/>
-      <c r="S19" s="186" t="s">
+      <c r="N19" s="188"/>
+      <c r="O19" s="188"/>
+      <c r="P19" s="188"/>
+      <c r="Q19" s="189"/>
+      <c r="S19" s="187" t="s">
         <v>716</v>
       </c>
-      <c r="T19" s="187"/>
-      <c r="U19" s="187"/>
-      <c r="V19" s="187"/>
-      <c r="W19" s="188"/>
-      <c r="Y19" s="186" t="s">
+      <c r="T19" s="188"/>
+      <c r="U19" s="188"/>
+      <c r="V19" s="188"/>
+      <c r="W19" s="189"/>
+      <c r="Y19" s="187" t="s">
         <v>724</v>
       </c>
-      <c r="Z19" s="187"/>
-      <c r="AA19" s="187"/>
-      <c r="AB19" s="187"/>
-      <c r="AC19" s="188"/>
+      <c r="Z19" s="188"/>
+      <c r="AA19" s="188"/>
+      <c r="AB19" s="188"/>
+      <c r="AC19" s="189"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="139"/>
@@ -46849,26 +46852,26 @@
       <c r="D20" s="138"/>
       <c r="E20" s="138"/>
       <c r="F20" s="138"/>
-      <c r="G20" s="189"/>
-      <c r="H20" s="190"/>
-      <c r="I20" s="190"/>
-      <c r="J20" s="190"/>
-      <c r="K20" s="191"/>
-      <c r="M20" s="189"/>
-      <c r="N20" s="190"/>
-      <c r="O20" s="190"/>
-      <c r="P20" s="190"/>
-      <c r="Q20" s="191"/>
-      <c r="S20" s="189"/>
-      <c r="T20" s="190"/>
-      <c r="U20" s="190"/>
-      <c r="V20" s="190"/>
-      <c r="W20" s="191"/>
-      <c r="Y20" s="189"/>
-      <c r="Z20" s="190"/>
-      <c r="AA20" s="190"/>
-      <c r="AB20" s="190"/>
-      <c r="AC20" s="191"/>
+      <c r="G20" s="190"/>
+      <c r="H20" s="191"/>
+      <c r="I20" s="191"/>
+      <c r="J20" s="191"/>
+      <c r="K20" s="192"/>
+      <c r="M20" s="190"/>
+      <c r="N20" s="191"/>
+      <c r="O20" s="191"/>
+      <c r="P20" s="191"/>
+      <c r="Q20" s="192"/>
+      <c r="S20" s="190"/>
+      <c r="T20" s="191"/>
+      <c r="U20" s="191"/>
+      <c r="V20" s="191"/>
+      <c r="W20" s="192"/>
+      <c r="Y20" s="190"/>
+      <c r="Z20" s="191"/>
+      <c r="AA20" s="191"/>
+      <c r="AB20" s="191"/>
+      <c r="AC20" s="192"/>
     </row>
     <row r="21" spans="1:29" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="139"/>
@@ -46877,26 +46880,26 @@
       <c r="D21" s="138"/>
       <c r="E21" s="138"/>
       <c r="F21" s="138"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="193"/>
-      <c r="I21" s="193"/>
-      <c r="J21" s="193"/>
-      <c r="K21" s="194"/>
-      <c r="M21" s="192"/>
-      <c r="N21" s="193"/>
-      <c r="O21" s="193"/>
-      <c r="P21" s="193"/>
-      <c r="Q21" s="194"/>
-      <c r="S21" s="192"/>
-      <c r="T21" s="193"/>
-      <c r="U21" s="193"/>
-      <c r="V21" s="193"/>
-      <c r="W21" s="194"/>
-      <c r="Y21" s="192"/>
-      <c r="Z21" s="193"/>
-      <c r="AA21" s="193"/>
-      <c r="AB21" s="193"/>
-      <c r="AC21" s="194"/>
+      <c r="G21" s="193"/>
+      <c r="H21" s="194"/>
+      <c r="I21" s="194"/>
+      <c r="J21" s="194"/>
+      <c r="K21" s="195"/>
+      <c r="M21" s="193"/>
+      <c r="N21" s="194"/>
+      <c r="O21" s="194"/>
+      <c r="P21" s="194"/>
+      <c r="Q21" s="195"/>
+      <c r="S21" s="193"/>
+      <c r="T21" s="194"/>
+      <c r="U21" s="194"/>
+      <c r="V21" s="194"/>
+      <c r="W21" s="195"/>
+      <c r="Y21" s="193"/>
+      <c r="Z21" s="194"/>
+      <c r="AA21" s="194"/>
+      <c r="AB21" s="194"/>
+      <c r="AC21" s="195"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -46919,95 +46922,95 @@
     </row>
     <row r="40" spans="1:29" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:29" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="186" t="s">
+      <c r="A41" s="187" t="s">
         <v>719</v>
       </c>
-      <c r="B41" s="187"/>
-      <c r="C41" s="187"/>
-      <c r="D41" s="187"/>
-      <c r="E41" s="188"/>
-      <c r="G41" s="186" t="s">
+      <c r="B41" s="188"/>
+      <c r="C41" s="188"/>
+      <c r="D41" s="188"/>
+      <c r="E41" s="189"/>
+      <c r="G41" s="187" t="s">
         <v>722</v>
       </c>
-      <c r="H41" s="187"/>
-      <c r="I41" s="187"/>
-      <c r="J41" s="187"/>
-      <c r="K41" s="188"/>
-      <c r="M41" s="186" t="s">
+      <c r="H41" s="188"/>
+      <c r="I41" s="188"/>
+      <c r="J41" s="188"/>
+      <c r="K41" s="189"/>
+      <c r="M41" s="187" t="s">
         <v>723</v>
       </c>
-      <c r="N41" s="187"/>
-      <c r="O41" s="187"/>
-      <c r="P41" s="187"/>
-      <c r="Q41" s="188"/>
-      <c r="S41" s="186" t="s">
+      <c r="N41" s="188"/>
+      <c r="O41" s="188"/>
+      <c r="P41" s="188"/>
+      <c r="Q41" s="189"/>
+      <c r="S41" s="187" t="s">
         <v>729</v>
       </c>
-      <c r="T41" s="187"/>
-      <c r="U41" s="187"/>
-      <c r="V41" s="187"/>
-      <c r="W41" s="188"/>
-      <c r="Y41" s="186" t="s">
+      <c r="T41" s="188"/>
+      <c r="U41" s="188"/>
+      <c r="V41" s="188"/>
+      <c r="W41" s="189"/>
+      <c r="Y41" s="187" t="s">
         <v>731</v>
       </c>
-      <c r="Z41" s="187"/>
-      <c r="AA41" s="187"/>
-      <c r="AB41" s="187"/>
-      <c r="AC41" s="188"/>
+      <c r="Z41" s="188"/>
+      <c r="AA41" s="188"/>
+      <c r="AB41" s="188"/>
+      <c r="AC41" s="189"/>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A42" s="189"/>
-      <c r="B42" s="190"/>
-      <c r="C42" s="190"/>
-      <c r="D42" s="190"/>
-      <c r="E42" s="191"/>
-      <c r="G42" s="189"/>
-      <c r="H42" s="190"/>
-      <c r="I42" s="190"/>
-      <c r="J42" s="190"/>
-      <c r="K42" s="191"/>
-      <c r="M42" s="189"/>
-      <c r="N42" s="190"/>
-      <c r="O42" s="190"/>
-      <c r="P42" s="190"/>
-      <c r="Q42" s="191"/>
-      <c r="S42" s="189"/>
-      <c r="T42" s="190"/>
-      <c r="U42" s="190"/>
-      <c r="V42" s="190"/>
-      <c r="W42" s="191"/>
-      <c r="Y42" s="189"/>
-      <c r="Z42" s="190"/>
-      <c r="AA42" s="190"/>
-      <c r="AB42" s="190"/>
-      <c r="AC42" s="191"/>
+      <c r="A42" s="190"/>
+      <c r="B42" s="191"/>
+      <c r="C42" s="191"/>
+      <c r="D42" s="191"/>
+      <c r="E42" s="192"/>
+      <c r="G42" s="190"/>
+      <c r="H42" s="191"/>
+      <c r="I42" s="191"/>
+      <c r="J42" s="191"/>
+      <c r="K42" s="192"/>
+      <c r="M42" s="190"/>
+      <c r="N42" s="191"/>
+      <c r="O42" s="191"/>
+      <c r="P42" s="191"/>
+      <c r="Q42" s="192"/>
+      <c r="S42" s="190"/>
+      <c r="T42" s="191"/>
+      <c r="U42" s="191"/>
+      <c r="V42" s="191"/>
+      <c r="W42" s="192"/>
+      <c r="Y42" s="190"/>
+      <c r="Z42" s="191"/>
+      <c r="AA42" s="191"/>
+      <c r="AB42" s="191"/>
+      <c r="AC42" s="192"/>
     </row>
     <row r="43" spans="1:29" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="192"/>
-      <c r="B43" s="193"/>
-      <c r="C43" s="193"/>
-      <c r="D43" s="193"/>
-      <c r="E43" s="194"/>
-      <c r="G43" s="192"/>
-      <c r="H43" s="193"/>
-      <c r="I43" s="193"/>
-      <c r="J43" s="193"/>
-      <c r="K43" s="194"/>
-      <c r="M43" s="192"/>
-      <c r="N43" s="193"/>
-      <c r="O43" s="193"/>
-      <c r="P43" s="193"/>
-      <c r="Q43" s="194"/>
-      <c r="S43" s="192"/>
-      <c r="T43" s="193"/>
-      <c r="U43" s="193"/>
-      <c r="V43" s="193"/>
-      <c r="W43" s="194"/>
-      <c r="Y43" s="192"/>
-      <c r="Z43" s="193"/>
-      <c r="AA43" s="193"/>
-      <c r="AB43" s="193"/>
-      <c r="AC43" s="194"/>
+      <c r="A43" s="193"/>
+      <c r="B43" s="194"/>
+      <c r="C43" s="194"/>
+      <c r="D43" s="194"/>
+      <c r="E43" s="195"/>
+      <c r="G43" s="193"/>
+      <c r="H43" s="194"/>
+      <c r="I43" s="194"/>
+      <c r="J43" s="194"/>
+      <c r="K43" s="195"/>
+      <c r="M43" s="193"/>
+      <c r="N43" s="194"/>
+      <c r="O43" s="194"/>
+      <c r="P43" s="194"/>
+      <c r="Q43" s="195"/>
+      <c r="S43" s="193"/>
+      <c r="T43" s="194"/>
+      <c r="U43" s="194"/>
+      <c r="V43" s="194"/>
+      <c r="W43" s="195"/>
+      <c r="Y43" s="193"/>
+      <c r="Z43" s="194"/>
+      <c r="AA43" s="194"/>
+      <c r="AB43" s="194"/>
+      <c r="AC43" s="195"/>
     </row>
     <row r="45" spans="1:29" s="138" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45"/>
@@ -47092,98 +47095,98 @@
       <c r="L63" s="138"/>
     </row>
     <row r="64" spans="1:29" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="186" t="s">
+      <c r="A64" s="187" t="s">
         <v>734</v>
       </c>
-      <c r="B64" s="187"/>
-      <c r="C64" s="187"/>
-      <c r="D64" s="187"/>
-      <c r="E64" s="188"/>
-      <c r="G64" s="186" t="s">
+      <c r="B64" s="188"/>
+      <c r="C64" s="188"/>
+      <c r="D64" s="188"/>
+      <c r="E64" s="189"/>
+      <c r="G64" s="187" t="s">
         <v>735</v>
       </c>
-      <c r="H64" s="187"/>
-      <c r="I64" s="187"/>
-      <c r="J64" s="187"/>
-      <c r="K64" s="188"/>
+      <c r="H64" s="188"/>
+      <c r="I64" s="188"/>
+      <c r="J64" s="188"/>
+      <c r="K64" s="189"/>
       <c r="L64" s="138"/>
-      <c r="M64" s="195" t="s">
+      <c r="M64" s="196" t="s">
         <v>739</v>
       </c>
-      <c r="N64" s="196"/>
-      <c r="O64" s="196"/>
-      <c r="P64" s="196"/>
-      <c r="Q64" s="197"/>
-      <c r="S64" s="195" t="s">
+      <c r="N64" s="197"/>
+      <c r="O64" s="197"/>
+      <c r="P64" s="197"/>
+      <c r="Q64" s="198"/>
+      <c r="S64" s="196" t="s">
         <v>740</v>
       </c>
-      <c r="T64" s="196"/>
-      <c r="U64" s="196"/>
-      <c r="V64" s="196"/>
-      <c r="W64" s="197"/>
-      <c r="Y64" s="195" t="s">
+      <c r="T64" s="197"/>
+      <c r="U64" s="197"/>
+      <c r="V64" s="197"/>
+      <c r="W64" s="198"/>
+      <c r="Y64" s="196" t="s">
         <v>741</v>
       </c>
-      <c r="Z64" s="196"/>
-      <c r="AA64" s="196"/>
-      <c r="AB64" s="196"/>
-      <c r="AC64" s="197"/>
+      <c r="Z64" s="197"/>
+      <c r="AA64" s="197"/>
+      <c r="AB64" s="197"/>
+      <c r="AC64" s="198"/>
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A65" s="189"/>
-      <c r="B65" s="190"/>
-      <c r="C65" s="190"/>
-      <c r="D65" s="190"/>
-      <c r="E65" s="191"/>
-      <c r="G65" s="189"/>
-      <c r="H65" s="190"/>
-      <c r="I65" s="190"/>
-      <c r="J65" s="190"/>
-      <c r="K65" s="191"/>
+      <c r="A65" s="190"/>
+      <c r="B65" s="191"/>
+      <c r="C65" s="191"/>
+      <c r="D65" s="191"/>
+      <c r="E65" s="192"/>
+      <c r="G65" s="190"/>
+      <c r="H65" s="191"/>
+      <c r="I65" s="191"/>
+      <c r="J65" s="191"/>
+      <c r="K65" s="192"/>
       <c r="L65" s="138"/>
-      <c r="M65" s="198"/>
-      <c r="N65" s="199"/>
-      <c r="O65" s="199"/>
-      <c r="P65" s="199"/>
-      <c r="Q65" s="200"/>
-      <c r="S65" s="198"/>
-      <c r="T65" s="199"/>
-      <c r="U65" s="199"/>
-      <c r="V65" s="199"/>
-      <c r="W65" s="200"/>
-      <c r="Y65" s="198"/>
-      <c r="Z65" s="199"/>
-      <c r="AA65" s="199"/>
-      <c r="AB65" s="199"/>
-      <c r="AC65" s="200"/>
+      <c r="M65" s="199"/>
+      <c r="N65" s="200"/>
+      <c r="O65" s="200"/>
+      <c r="P65" s="200"/>
+      <c r="Q65" s="201"/>
+      <c r="S65" s="199"/>
+      <c r="T65" s="200"/>
+      <c r="U65" s="200"/>
+      <c r="V65" s="200"/>
+      <c r="W65" s="201"/>
+      <c r="Y65" s="199"/>
+      <c r="Z65" s="200"/>
+      <c r="AA65" s="200"/>
+      <c r="AB65" s="200"/>
+      <c r="AC65" s="201"/>
     </row>
     <row r="66" spans="1:29" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="192"/>
-      <c r="B66" s="193"/>
-      <c r="C66" s="193"/>
-      <c r="D66" s="193"/>
-      <c r="E66" s="194"/>
-      <c r="G66" s="192"/>
-      <c r="H66" s="193"/>
-      <c r="I66" s="193"/>
-      <c r="J66" s="193"/>
-      <c r="K66" s="194"/>
+      <c r="A66" s="193"/>
+      <c r="B66" s="194"/>
+      <c r="C66" s="194"/>
+      <c r="D66" s="194"/>
+      <c r="E66" s="195"/>
+      <c r="G66" s="193"/>
+      <c r="H66" s="194"/>
+      <c r="I66" s="194"/>
+      <c r="J66" s="194"/>
+      <c r="K66" s="195"/>
       <c r="L66" s="138"/>
-      <c r="M66" s="201"/>
-      <c r="N66" s="202"/>
-      <c r="O66" s="202"/>
-      <c r="P66" s="202"/>
-      <c r="Q66" s="203"/>
-      <c r="S66" s="201"/>
-      <c r="T66" s="202"/>
-      <c r="U66" s="202"/>
-      <c r="V66" s="202"/>
-      <c r="W66" s="203"/>
-      <c r="Y66" s="201"/>
-      <c r="Z66" s="202"/>
-      <c r="AA66" s="202"/>
-      <c r="AB66" s="202"/>
-      <c r="AC66" s="203"/>
+      <c r="M66" s="202"/>
+      <c r="N66" s="203"/>
+      <c r="O66" s="203"/>
+      <c r="P66" s="203"/>
+      <c r="Q66" s="204"/>
+      <c r="S66" s="202"/>
+      <c r="T66" s="203"/>
+      <c r="U66" s="203"/>
+      <c r="V66" s="203"/>
+      <c r="W66" s="204"/>
+      <c r="Y66" s="202"/>
+      <c r="Z66" s="203"/>
+      <c r="AA66" s="203"/>
+      <c r="AB66" s="203"/>
+      <c r="AC66" s="204"/>
     </row>
     <row r="69" spans="1:29" ht="24" x14ac:dyDescent="0.3">
       <c r="D69" s="142" t="s">
@@ -61579,111 +61582,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="21" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="18" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="16" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="10" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -62976,13 +62979,13 @@
       <c r="C1" s="74" t="s">
         <v>477</v>
       </c>
-      <c r="F1" s="204" t="s">
+      <c r="F1" s="205" t="s">
         <v>476</v>
       </c>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
-      <c r="I1" s="204"/>
-      <c r="J1" s="204"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="205"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D2" s="69" t="s">
@@ -63007,7 +63010,7 @@
       </c>
       <c r="E3" s="68">
         <f ca="1">TODAY()</f>
-        <v>43430</v>
+        <v>43441</v>
       </c>
       <c r="F3" s="67">
         <v>42551</v>
@@ -63317,7 +63320,7 @@
   <dimension ref="B1:Y90"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="7905" activePane="bottomLeft"/>
+      <pane ySplit="7910" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -63358,7 +63361,7 @@
       <c r="F1" s="1"/>
       <c r="I1" s="34">
         <f ca="1">TODAY()</f>
-        <v>43430</v>
+        <v>43441</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -67423,7 +67426,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
11220 added some submittal detail
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E28853-9437-43AF-B545-1B7EDEE7D262}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3484130B-394E-4B8A-A68E-097FCC202CAB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8903" uniqueCount="1300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8904" uniqueCount="1301">
   <si>
     <t>#</t>
   </si>
@@ -3945,6 +3945,9 @@
   </si>
   <si>
     <t>2018-12-11: only some plumbing warranties on SP</t>
+  </si>
+  <si>
+    <t>2018-12-11: takeoffs done for P,M,some E</t>
   </si>
 </sst>
 </file>
@@ -9131,7 +9134,7 @@
   <dimension ref="B1:CD101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16965,9 +16968,11 @@
       </c>
       <c r="AL45" s="144"/>
       <c r="AM45" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AN45" s="144"/>
+        <v>1112</v>
+      </c>
+      <c r="AN45" s="144" t="s">
+        <v>1300</v>
+      </c>
       <c r="AO45" s="18"/>
       <c r="AP45" s="146">
         <v>40544</v>

</xml_diff>

<commit_message>
Update click-bat legend notes on index
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3484130B-394E-4B8A-A68E-097FCC202CAB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2879D70D-3272-410D-9CA8-2330C3CC969E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7376,7 +7376,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12/11/2018</c:v>
+                  <c:v>12/12/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9134,7 +9134,7 @@
   <dimension ref="B1:CD101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16938,7 +16938,7 @@
         <v>1299</v>
       </c>
       <c r="AA45" s="144" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="AB45" s="144" t="s">
         <v>1297</v>
@@ -63024,7 +63024,7 @@
       </c>
       <c r="E3" s="68">
         <f ca="1">TODAY()</f>
-        <v>43445</v>
+        <v>43446</v>
       </c>
       <c r="F3" s="67">
         <v>42551</v>
@@ -63375,7 +63375,7 @@
       <c r="F1" s="1"/>
       <c r="I1" s="34">
         <f ca="1">TODAY()</f>
-        <v>43445</v>
+        <v>43446</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
updated submittal review based on files in SP on project not equip level
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2879D70D-3272-410D-9CA8-2330C3CC969E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B91A69-AF37-43C2-952B-F631C5769361}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8904" uniqueCount="1301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8927" uniqueCount="1318">
   <si>
     <t>#</t>
   </si>
@@ -3938,9 +3938,6 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>tagged with "trade" in SP</t>
-  </si>
-  <si>
     <t>2018-12-11: only some plumbing O&amp;Ms on SP</t>
   </si>
   <si>
@@ -3948,6 +3945,60 @@
   </si>
   <si>
     <t>2018-12-11: takeoffs done for P,M,some E</t>
+  </si>
+  <si>
+    <t>finishing early 2019</t>
+  </si>
+  <si>
+    <t>scheduled for 2019</t>
+  </si>
+  <si>
+    <t>only 3 submittals in SP</t>
+  </si>
+  <si>
+    <t>do have restroom submittals (proj #15355)</t>
+  </si>
+  <si>
+    <t>finished in 2018</t>
+  </si>
+  <si>
+    <t>1 submittal only in SP</t>
+  </si>
+  <si>
+    <t>only a handful of submittals on SP; No Elec of HVAC</t>
+  </si>
+  <si>
+    <t>only 1 submittal in SP</t>
+  </si>
+  <si>
+    <t>~10 submittals in SP; no HVAC, etc</t>
+  </si>
+  <si>
+    <t>some submittals for 12kV project in SP</t>
+  </si>
+  <si>
+    <t>several submittals in SP, but no Elec of Plumbing</t>
+  </si>
+  <si>
+    <t>only ~5 submittals in SP; no HVAC of plumbing</t>
+  </si>
+  <si>
+    <t>see Prop N #13110</t>
+  </si>
+  <si>
+    <t>see Cont Ed SP site</t>
+  </si>
+  <si>
+    <t>see Prop N #13150</t>
+  </si>
+  <si>
+    <t>see Prop N #13410</t>
+  </si>
+  <si>
+    <t>no submittals in SP, but building expected to be leased (in 2019)</t>
+  </si>
+  <si>
+    <t>see Prop S #14215</t>
   </si>
 </sst>
 </file>
@@ -5127,7 +5178,224 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="286">
+  <dxfs count="317">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7376,7 +7644,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12/12/2018</c:v>
+                  <c:v>1/7/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9133,8 +9401,8 @@
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9147,23 +9415,23 @@
     <col min="6" max="6" width="22.08984375" customWidth="1"/>
     <col min="7" max="7" width="3.26953125" style="1" customWidth="1"/>
     <col min="8" max="9" width="3.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.26953125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.7265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="7.26953125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.81640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="7.26953125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="9.08984375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="7.26953125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.81640625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.26953125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.81640625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.26953125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6328125" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.08984375" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="7.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="7.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.08984375" style="2" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="10.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="8.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="11.81640625" style="2" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="8.26953125" style="1" customWidth="1"/>
     <col min="28" max="28" width="11.81640625" style="2" customWidth="1"/>
     <col min="29" max="29" width="8.26953125" style="1" customWidth="1"/>
@@ -9277,10 +9545,10 @@
       <c r="Z1" s="186" t="s">
         <v>1292</v>
       </c>
-      <c r="AA1" s="186" t="s">
+      <c r="AA1" s="18" t="s">
         <v>707</v>
       </c>
-      <c r="AB1" s="186" t="s">
+      <c r="AB1" s="18" t="s">
         <v>1293</v>
       </c>
       <c r="AC1" s="186" t="s">
@@ -9504,12 +9772,10 @@
       <c r="Z2" s="144">
         <v>1</v>
       </c>
-      <c r="AA2" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB2" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA2" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB2" s="144"/>
       <c r="AC2" s="144" t="s">
         <v>567</v>
       </c>
@@ -9679,12 +9945,10 @@
       <c r="Z3" s="144" t="s">
         <v>1296</v>
       </c>
-      <c r="AA3" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB3" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA3" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB3" s="144"/>
       <c r="AC3" s="144" t="s">
         <v>567</v>
       </c>
@@ -9850,11 +10114,11 @@
       <c r="Z4" s="144" t="s">
         <v>1296</v>
       </c>
-      <c r="AA4" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB4" s="144">
-        <v>1</v>
+      <c r="AA4" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB4" s="144" t="s">
+        <v>1300</v>
       </c>
       <c r="AC4" s="144" t="s">
         <v>567</v>
@@ -10023,12 +10287,10 @@
       <c r="Z5" s="144">
         <v>1</v>
       </c>
-      <c r="AA5" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB5" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA5" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB5" s="144"/>
       <c r="AC5" s="144" t="s">
         <v>567</v>
       </c>
@@ -10198,12 +10460,10 @@
       <c r="Z6" s="144">
         <v>1</v>
       </c>
-      <c r="AA6" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB6" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA6" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB6" s="144"/>
       <c r="AC6" s="144" t="s">
         <v>567</v>
       </c>
@@ -10385,11 +10645,11 @@
       <c r="Z7" s="144">
         <v>1</v>
       </c>
-      <c r="AA7" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB7" s="144">
-        <v>1</v>
+      <c r="AA7" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB7" s="144" t="s">
+        <v>1300</v>
       </c>
       <c r="AC7" s="144" t="s">
         <v>567</v>
@@ -10558,11 +10818,11 @@
       <c r="Z8" s="144">
         <v>1</v>
       </c>
-      <c r="AA8" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB8" s="144">
-        <v>1</v>
+      <c r="AA8" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB8" s="144" t="s">
+        <v>1300</v>
       </c>
       <c r="AC8" s="144" t="s">
         <v>567</v>
@@ -10729,12 +10989,10 @@
       <c r="Z9" s="144">
         <v>1</v>
       </c>
-      <c r="AA9" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB9" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA9" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB9" s="144"/>
       <c r="AC9" s="144" t="s">
         <v>567</v>
       </c>
@@ -10901,9 +11159,7 @@
       <c r="AA10" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AB10" s="144">
-        <v>1</v>
-      </c>
+      <c r="AB10" s="144"/>
       <c r="AC10" s="144" t="s">
         <v>567</v>
       </c>
@@ -11073,11 +11329,11 @@
       <c r="Z11" s="144">
         <v>1</v>
       </c>
-      <c r="AA11" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB11" s="144">
-        <v>1</v>
+      <c r="AA11" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB11" s="144" t="s">
+        <v>1302</v>
       </c>
       <c r="AC11" s="144" t="s">
         <v>567</v>
@@ -11251,8 +11507,8 @@
       <c r="AA12" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AB12" s="144">
-        <v>1</v>
+      <c r="AB12" s="144" t="s">
+        <v>1300</v>
       </c>
       <c r="AC12" s="144" t="s">
         <v>567</v>
@@ -11417,12 +11673,10 @@
       <c r="Z13" s="144">
         <v>1</v>
       </c>
-      <c r="AA13" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB13" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA13" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB13" s="144"/>
       <c r="AC13" s="144" t="s">
         <v>567</v>
       </c>
@@ -11588,12 +11842,10 @@
       <c r="Z14" s="144">
         <v>1</v>
       </c>
-      <c r="AA14" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB14" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA14" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB14" s="144"/>
       <c r="AC14" s="144" t="s">
         <v>567</v>
       </c>
@@ -11758,8 +12010,8 @@
       <c r="AA15" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AB15" s="144">
-        <v>1</v>
+      <c r="AB15" s="144" t="s">
+        <v>1300</v>
       </c>
       <c r="AC15" s="144" t="s">
         <v>567</v>
@@ -11927,8 +12179,8 @@
       <c r="AA16" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AB16" s="144">
-        <v>1</v>
+      <c r="AB16" s="144" t="s">
+        <v>1303</v>
       </c>
       <c r="AC16" s="144" t="s">
         <v>567</v>
@@ -12095,12 +12347,10 @@
       <c r="Z17" s="144">
         <v>1</v>
       </c>
-      <c r="AA17" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB17" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA17" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB17" s="144"/>
       <c r="AC17" s="144" t="s">
         <v>567</v>
       </c>
@@ -12266,12 +12516,10 @@
       <c r="Z18" s="144">
         <v>1</v>
       </c>
-      <c r="AA18" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB18" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA18" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB18" s="144"/>
       <c r="AC18" s="144" t="s">
         <v>567</v>
       </c>
@@ -12437,12 +12685,10 @@
       <c r="Z19" s="144">
         <v>1</v>
       </c>
-      <c r="AA19" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB19" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA19" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB19" s="144"/>
       <c r="AC19" s="144" t="s">
         <v>567</v>
       </c>
@@ -12608,11 +12854,11 @@
       <c r="Z20" s="144">
         <v>1</v>
       </c>
-      <c r="AA20" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB20" s="144">
-        <v>1</v>
+      <c r="AA20" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB20" s="144" t="s">
+        <v>1305</v>
       </c>
       <c r="AC20" s="144" t="s">
         <v>567</v>
@@ -12779,11 +13025,11 @@
       <c r="Z21" s="144">
         <v>1</v>
       </c>
-      <c r="AA21" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB21" s="144">
-        <v>1</v>
+      <c r="AA21" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB21" s="144" t="s">
+        <v>1306</v>
       </c>
       <c r="AC21" s="144" t="s">
         <v>567</v>
@@ -12954,12 +13200,10 @@
       <c r="Z22" s="144">
         <v>1</v>
       </c>
-      <c r="AA22" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB22" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA22" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB22" s="144"/>
       <c r="AC22" s="144" t="s">
         <v>567</v>
       </c>
@@ -13081,8 +13325,8 @@
         <v>567</v>
       </c>
       <c r="L23" s="19"/>
-      <c r="M23" s="144" t="s">
-        <v>567</v>
+      <c r="M23" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="N23" s="144"/>
       <c r="O23" s="25" t="s">
@@ -13121,12 +13365,10 @@
       <c r="Z23" s="144">
         <v>1</v>
       </c>
-      <c r="AA23" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB23" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA23" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB23" s="144"/>
       <c r="AC23" s="144" t="s">
         <v>567</v>
       </c>
@@ -13288,12 +13530,10 @@
       <c r="Z24" s="144">
         <v>1</v>
       </c>
-      <c r="AA24" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB24" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA24" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB24" s="144"/>
       <c r="AC24" s="144" t="s">
         <v>567</v>
       </c>
@@ -13463,11 +13703,11 @@
       <c r="Z25" s="144">
         <v>1</v>
       </c>
-      <c r="AA25" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB25" s="144">
-        <v>1</v>
+      <c r="AA25" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB25" s="144" t="s">
+        <v>1308</v>
       </c>
       <c r="AC25" s="144" t="s">
         <v>567</v>
@@ -13634,12 +13874,10 @@
       <c r="Z26" s="144">
         <v>1</v>
       </c>
-      <c r="AA26" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB26" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA26" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB26" s="144"/>
       <c r="AC26" s="144" t="s">
         <v>567</v>
       </c>
@@ -13805,12 +14043,10 @@
       <c r="Z27" s="144">
         <v>1</v>
       </c>
-      <c r="AA27" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB27" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA27" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB27" s="144"/>
       <c r="AC27" s="144" t="s">
         <v>567</v>
       </c>
@@ -13976,11 +14212,11 @@
       <c r="Z28" s="144">
         <v>1</v>
       </c>
-      <c r="AA28" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB28" s="144">
-        <v>1</v>
+      <c r="AA28" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB28" s="144" t="s">
+        <v>1305</v>
       </c>
       <c r="AC28" s="144" t="s">
         <v>567</v>
@@ -14151,12 +14387,10 @@
       <c r="Z29" s="144">
         <v>1</v>
       </c>
-      <c r="AA29" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB29" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA29" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB29" s="144"/>
       <c r="AC29" s="144" t="s">
         <v>567</v>
       </c>
@@ -14326,12 +14560,10 @@
       <c r="Z30" s="144">
         <v>1</v>
       </c>
-      <c r="AA30" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB30" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA30" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB30" s="144"/>
       <c r="AC30" s="144" t="s">
         <v>567</v>
       </c>
@@ -14497,12 +14729,10 @@
       <c r="Z31" s="144">
         <v>1</v>
       </c>
-      <c r="AA31" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB31" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA31" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB31" s="144"/>
       <c r="AC31" s="144" t="s">
         <v>567</v>
       </c>
@@ -14594,7 +14824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B32" s="19" t="s">
         <v>86</v>
       </c>
@@ -14666,11 +14896,11 @@
       <c r="Z32" s="144">
         <v>1</v>
       </c>
-      <c r="AA32" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB32" s="144">
-        <v>1</v>
+      <c r="AA32" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB32" s="144" t="s">
+        <v>1310</v>
       </c>
       <c r="AC32" s="144" t="s">
         <v>567</v>
@@ -14835,12 +15065,10 @@
       <c r="Z33" s="144">
         <v>1</v>
       </c>
-      <c r="AA33" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB33" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA33" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB33" s="144"/>
       <c r="AC33" s="144" t="s">
         <v>567</v>
       </c>
@@ -15004,11 +15232,11 @@
       <c r="Z34" s="144">
         <v>1</v>
       </c>
-      <c r="AA34" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB34" s="144">
-        <v>1</v>
+      <c r="AA34" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB34" s="144" t="s">
+        <v>1311</v>
       </c>
       <c r="AC34" s="144" t="s">
         <v>567</v>
@@ -15177,12 +15405,10 @@
       <c r="Z35" s="144">
         <v>1</v>
       </c>
-      <c r="AA35" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB35" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA35" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB35" s="144"/>
       <c r="AC35" s="144" t="s">
         <v>567</v>
       </c>
@@ -15346,11 +15572,11 @@
       <c r="Z36" s="144">
         <v>1</v>
       </c>
-      <c r="AA36" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB36" s="144">
-        <v>1</v>
+      <c r="AA36" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB36" s="144" t="s">
+        <v>1313</v>
       </c>
       <c r="AC36" s="144" t="s">
         <v>567</v>
@@ -15515,12 +15741,10 @@
       <c r="Z37" s="144">
         <v>1</v>
       </c>
-      <c r="AA37" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB37" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA37" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB37" s="144"/>
       <c r="AC37" s="144" t="s">
         <v>567</v>
       </c>
@@ -15682,12 +15906,10 @@
       <c r="Z38" s="144">
         <v>1</v>
       </c>
-      <c r="AA38" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB38" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA38" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB38" s="144"/>
       <c r="AC38" s="144" t="s">
         <v>567</v>
       </c>
@@ -15851,12 +16073,10 @@
       <c r="Z39" s="144">
         <v>1</v>
       </c>
-      <c r="AA39" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB39" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA39" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB39" s="144"/>
       <c r="AC39" s="144" t="s">
         <v>567</v>
       </c>
@@ -16046,12 +16266,10 @@
       <c r="Z40" s="144">
         <v>1</v>
       </c>
-      <c r="AA40" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB40" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA40" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB40" s="144"/>
       <c r="AC40" s="144" t="s">
         <v>567</v>
       </c>
@@ -16242,9 +16460,7 @@
       <c r="AA41" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AB41" s="144">
-        <v>1</v>
-      </c>
+      <c r="AB41" s="144"/>
       <c r="AC41" s="144" t="s">
         <v>567</v>
       </c>
@@ -16403,8 +16619,8 @@
       <c r="AA42" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AB42" s="144">
-        <v>1</v>
+      <c r="AB42" s="144" t="s">
+        <v>1309</v>
       </c>
       <c r="AC42" s="144" t="s">
         <v>567</v>
@@ -16567,12 +16783,10 @@
       <c r="Z43" s="144">
         <v>1</v>
       </c>
-      <c r="AA43" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB43" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA43" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB43" s="144"/>
       <c r="AC43" s="144" t="s">
         <v>567</v>
       </c>
@@ -16771,8 +16985,8 @@
       <c r="AA44" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AB44" s="144">
-        <v>1</v>
+      <c r="AB44" s="144" t="s">
+        <v>1301</v>
       </c>
       <c r="AC44" s="144" t="s">
         <v>567</v>
@@ -16929,20 +17143,18 @@
         <v>170</v>
       </c>
       <c r="X45" s="144" t="s">
+        <v>1297</v>
+      </c>
+      <c r="Y45" s="144" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z45" s="144" t="s">
         <v>1298</v>
       </c>
-      <c r="Y45" s="144" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z45" s="144" t="s">
-        <v>1299</v>
-      </c>
-      <c r="AA45" s="144" t="s">
-        <v>170</v>
-      </c>
-      <c r="AB45" s="144" t="s">
-        <v>1297</v>
-      </c>
+      <c r="AA45" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB45" s="144"/>
       <c r="AC45" s="144" t="s">
         <v>567</v>
       </c>
@@ -16971,7 +17183,7 @@
         <v>1112</v>
       </c>
       <c r="AN45" s="144" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="AO45" s="18"/>
       <c r="AP45" s="146">
@@ -17118,12 +17330,10 @@
       <c r="Z46" s="144">
         <v>1</v>
       </c>
-      <c r="AA46" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB46" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA46" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB46" s="144"/>
       <c r="AC46" s="144" t="s">
         <v>567</v>
       </c>
@@ -17289,12 +17499,10 @@
       <c r="Z47" s="144">
         <v>1</v>
       </c>
-      <c r="AA47" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB47" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA47" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB47" s="144"/>
       <c r="AC47" s="144" t="s">
         <v>567</v>
       </c>
@@ -17462,12 +17670,10 @@
       <c r="Z48" s="144">
         <v>1</v>
       </c>
-      <c r="AA48" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB48" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA48" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB48" s="144"/>
       <c r="AC48" s="144" t="s">
         <v>567</v>
       </c>
@@ -17631,12 +17837,10 @@
       <c r="Z49" s="144">
         <v>1</v>
       </c>
-      <c r="AA49" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB49" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA49" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB49" s="144"/>
       <c r="AC49" s="144" t="s">
         <v>567</v>
       </c>
@@ -17804,12 +18008,10 @@
       <c r="Z50" s="144">
         <v>1</v>
       </c>
-      <c r="AA50" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB50" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA50" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB50" s="144"/>
       <c r="AC50" s="144" t="s">
         <v>567</v>
       </c>
@@ -18009,12 +18211,10 @@
       <c r="Z51" s="144">
         <v>1</v>
       </c>
-      <c r="AA51" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB51" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA51" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB51" s="144"/>
       <c r="AC51" s="144" t="s">
         <v>567</v>
       </c>
@@ -18182,12 +18382,10 @@
       <c r="Z52" s="144">
         <v>1</v>
       </c>
-      <c r="AA52" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB52" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA52" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB52" s="144"/>
       <c r="AC52" s="144" t="s">
         <v>567</v>
       </c>
@@ -18357,11 +18555,11 @@
       <c r="Z53" s="144">
         <v>1</v>
       </c>
-      <c r="AA53" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB53" s="144">
-        <v>1</v>
+      <c r="AA53" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB53" s="144" t="s">
+        <v>1304</v>
       </c>
       <c r="AC53" s="144" t="s">
         <v>567</v>
@@ -18522,12 +18720,10 @@
       <c r="Z54" s="144">
         <v>1</v>
       </c>
-      <c r="AA54" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB54" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA54" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB54" s="144"/>
       <c r="AC54" s="144" t="s">
         <v>567</v>
       </c>
@@ -18703,12 +18899,10 @@
       <c r="Z55" s="144">
         <v>1</v>
       </c>
-      <c r="AA55" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB55" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA55" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB55" s="144"/>
       <c r="AC55" s="144" t="s">
         <v>567</v>
       </c>
@@ -18876,12 +19070,10 @@
       <c r="Z56" s="144">
         <v>1</v>
       </c>
-      <c r="AA56" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB56" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA56" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB56" s="144"/>
       <c r="AC56" s="144" t="s">
         <v>567</v>
       </c>
@@ -19045,12 +19237,10 @@
       <c r="Z57" s="144">
         <v>1</v>
       </c>
-      <c r="AA57" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB57" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA57" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB57" s="144"/>
       <c r="AC57" s="144" t="s">
         <v>567</v>
       </c>
@@ -19214,12 +19404,10 @@
       <c r="Z58" s="144">
         <v>1</v>
       </c>
-      <c r="AA58" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB58" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA58" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB58" s="144"/>
       <c r="AC58" s="144" t="s">
         <v>567</v>
       </c>
@@ -19421,12 +19609,10 @@
       <c r="Z59" s="144">
         <v>1</v>
       </c>
-      <c r="AA59" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB59" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA59" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB59" s="144"/>
       <c r="AC59" s="144" t="s">
         <v>567</v>
       </c>
@@ -19594,12 +19780,10 @@
       <c r="Z60" s="144">
         <v>1</v>
       </c>
-      <c r="AA60" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB60" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA60" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB60" s="144"/>
       <c r="AC60" s="144" t="s">
         <v>567</v>
       </c>
@@ -19719,8 +19903,8 @@
         <v>567</v>
       </c>
       <c r="L61" s="19"/>
-      <c r="M61" s="144" t="s">
-        <v>567</v>
+      <c r="M61" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="N61" s="144"/>
       <c r="O61" s="19" t="s">
@@ -19759,11 +19943,11 @@
       <c r="Z61" s="144">
         <v>1</v>
       </c>
-      <c r="AA61" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB61" s="144">
-        <v>1</v>
+      <c r="AA61" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB61" s="144" t="s">
+        <v>1312</v>
       </c>
       <c r="AC61" s="144" t="s">
         <v>567</v>
@@ -19926,12 +20110,10 @@
       <c r="Z62" s="144">
         <v>1</v>
       </c>
-      <c r="AA62" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB62" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA62" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB62" s="144"/>
       <c r="AC62" s="144" t="s">
         <v>567</v>
       </c>
@@ -20053,8 +20235,8 @@
         <v>567</v>
       </c>
       <c r="L63" s="19"/>
-      <c r="M63" s="144" t="s">
-        <v>567</v>
+      <c r="M63" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="N63" s="144"/>
       <c r="O63" s="185" t="s">
@@ -20091,12 +20273,10 @@
       <c r="Z63" s="144">
         <v>1</v>
       </c>
-      <c r="AA63" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB63" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA63" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB63" s="144"/>
       <c r="AC63" s="144" t="s">
         <v>567</v>
       </c>
@@ -20254,11 +20434,11 @@
       <c r="Z64" s="144">
         <v>1</v>
       </c>
-      <c r="AA64" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB64" s="144">
-        <v>1</v>
+      <c r="AA64" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB64" s="144" t="s">
+        <v>1314</v>
       </c>
       <c r="AC64" s="144" t="s">
         <v>567</v>
@@ -20425,12 +20605,10 @@
       <c r="Z65" s="144">
         <v>1</v>
       </c>
-      <c r="AA65" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB65" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA65" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB65" s="144"/>
       <c r="AC65" s="144" t="s">
         <v>567</v>
       </c>
@@ -20600,11 +20778,11 @@
       <c r="Z66" s="144">
         <v>1</v>
       </c>
-      <c r="AA66" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB66" s="144">
-        <v>1</v>
+      <c r="AA66" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB66" s="144" t="s">
+        <v>1307</v>
       </c>
       <c r="AC66" s="144" t="s">
         <v>567</v>
@@ -20771,12 +20949,10 @@
       <c r="Z67" s="144">
         <v>1</v>
       </c>
-      <c r="AA67" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB67" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA67" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB67" s="144"/>
       <c r="AC67" s="144" t="s">
         <v>567</v>
       </c>
@@ -20940,11 +21116,11 @@
       <c r="Z68" s="144">
         <v>1</v>
       </c>
-      <c r="AA68" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB68" s="144">
-        <v>1</v>
+      <c r="AA68" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB68" s="144" t="s">
+        <v>1315</v>
       </c>
       <c r="AC68" s="144" t="s">
         <v>567</v>
@@ -21112,9 +21288,7 @@
       <c r="AA69" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="AB69" s="144">
-        <v>1</v>
-      </c>
+      <c r="AB69" s="144"/>
       <c r="AC69" s="144" t="s">
         <v>567</v>
       </c>
@@ -21280,12 +21454,10 @@
       <c r="Z70" s="144">
         <v>1</v>
       </c>
-      <c r="AA70" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB70" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA70" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB70" s="144"/>
       <c r="AC70" s="144" t="s">
         <v>567</v>
       </c>
@@ -21449,12 +21621,10 @@
       <c r="Z71" s="144">
         <v>1</v>
       </c>
-      <c r="AA71" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB71" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA71" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB71" s="144"/>
       <c r="AC71" s="144" t="s">
         <v>567</v>
       </c>
@@ -21618,12 +21788,10 @@
       <c r="Z72" s="144">
         <v>1</v>
       </c>
-      <c r="AA72" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB72" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA72" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB72" s="144"/>
       <c r="AC72" s="144" t="s">
         <v>567</v>
       </c>
@@ -21787,12 +21955,10 @@
       <c r="Z73" s="144">
         <v>1</v>
       </c>
-      <c r="AA73" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB73" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA73" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB73" s="144"/>
       <c r="AC73" s="144" t="s">
         <v>567</v>
       </c>
@@ -21958,12 +22124,10 @@
       <c r="Z74" s="144">
         <v>1</v>
       </c>
-      <c r="AA74" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB74" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA74" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB74" s="144"/>
       <c r="AC74" s="144" t="s">
         <v>567</v>
       </c>
@@ -22163,11 +22327,11 @@
       <c r="Z75" s="144">
         <v>1</v>
       </c>
-      <c r="AA75" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB75" s="144">
-        <v>1</v>
+      <c r="AA75" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB75" s="144" t="s">
+        <v>1317</v>
       </c>
       <c r="AC75" s="144" t="s">
         <v>567</v>
@@ -22364,12 +22528,10 @@
       <c r="Z76" s="144">
         <v>1</v>
       </c>
-      <c r="AA76" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB76" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA76" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB76" s="144"/>
       <c r="AC76" s="144" t="s">
         <v>567</v>
       </c>
@@ -22541,11 +22703,11 @@
       <c r="Z77" s="144">
         <v>1</v>
       </c>
-      <c r="AA77" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB77" s="144">
-        <v>1</v>
+      <c r="AA77" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB77" s="144" t="s">
+        <v>1302</v>
       </c>
       <c r="AC77" s="144" t="s">
         <v>567</v>
@@ -22714,12 +22876,10 @@
       <c r="Z78" s="144">
         <v>1</v>
       </c>
-      <c r="AA78" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB78" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA78" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB78" s="144"/>
       <c r="AC78" s="144" t="s">
         <v>567</v>
       </c>
@@ -22883,12 +23043,10 @@
       <c r="Z79" s="144">
         <v>1</v>
       </c>
-      <c r="AA79" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB79" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA79" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB79" s="144"/>
       <c r="AC79" s="144" t="s">
         <v>567</v>
       </c>
@@ -23066,11 +23224,11 @@
       <c r="Z80" s="144">
         <v>1</v>
       </c>
-      <c r="AA80" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB80" s="144">
-        <v>1</v>
+      <c r="AA80" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AB80" s="144" t="s">
+        <v>1316</v>
       </c>
       <c r="AC80" s="144" t="s">
         <v>567</v>
@@ -23235,12 +23393,10 @@
       <c r="Z81" s="144">
         <v>1</v>
       </c>
-      <c r="AA81" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB81" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA81" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB81" s="144"/>
       <c r="AC81" s="144" t="s">
         <v>567</v>
       </c>
@@ -23436,12 +23592,10 @@
       <c r="Z82" s="144">
         <v>1</v>
       </c>
-      <c r="AA82" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB82" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA82" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB82" s="144"/>
       <c r="AC82" s="144" t="s">
         <v>567</v>
       </c>
@@ -23635,12 +23789,10 @@
       <c r="Z83" s="144">
         <v>1</v>
       </c>
-      <c r="AA83" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB83" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA83" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB83" s="144"/>
       <c r="AC83" s="144" t="s">
         <v>567</v>
       </c>
@@ -23830,12 +23982,10 @@
       <c r="Z84" s="144">
         <v>1</v>
       </c>
-      <c r="AA84" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB84" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA84" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB84" s="144"/>
       <c r="AC84" s="144" t="s">
         <v>567</v>
       </c>
@@ -24027,12 +24177,10 @@
       <c r="Z85" s="144">
         <v>1</v>
       </c>
-      <c r="AA85" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB85" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA85" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB85" s="144"/>
       <c r="AC85" s="144" t="s">
         <v>567</v>
       </c>
@@ -24224,12 +24372,10 @@
       <c r="Z86" s="144">
         <v>1</v>
       </c>
-      <c r="AA86" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="AB86" s="144">
-        <v>1</v>
-      </c>
+      <c r="AA86" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AB86" s="144"/>
       <c r="AC86" s="144" t="s">
         <v>567</v>
       </c>
@@ -24370,1033 +24516,1195 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
-    <cfRule type="cellIs" dxfId="285" priority="218" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="316" priority="245" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI9:BJ9">
-    <cfRule type="cellIs" dxfId="284" priority="217" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="315" priority="244" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="283" priority="216" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="314" priority="243" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="282" priority="215" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="313" priority="242" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
-    <cfRule type="cellIs" dxfId="281" priority="213" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="312" priority="240" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="280" priority="212" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="311" priority="239" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="279" priority="211" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="310" priority="238" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="278" priority="207" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="309" priority="234" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="277" priority="197" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="308" priority="224" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I4 I7:I8 I12 I44 I14:I15 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="276" priority="184" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="307" priority="211" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M61:M63 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M23:N23 N22 M65:M67 M25:N25 N24 M36:N38 M69:M80 M82">
-    <cfRule type="cellIs" dxfId="275" priority="173" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
+    <cfRule type="cellIs" dxfId="306" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
-    <cfRule type="cellIs" dxfId="274" priority="170" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="305" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD2">
-    <cfRule type="cellIs" dxfId="273" priority="169" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="304" priority="196" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:K58 K2:K38 K60:K61 K41:K44 K63:K74 K76:K82">
-    <cfRule type="cellIs" dxfId="272" priority="168" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="303" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J36 J8:J12 J38:J40 J2:J5 J18 J20:J29 J33:J34 J46:J74">
-    <cfRule type="cellIs" dxfId="271" priority="167" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="302" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L8:L12 L76:L85 L14:L29 L2:L5 L46:L61 L63:L74">
-    <cfRule type="cellIs" dxfId="270" priority="166" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="301" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="269" priority="165" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="300" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="268" priority="162" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="299" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="267" priority="161" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="298" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="266" priority="159" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="297" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="265" priority="157" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="296" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
-    <cfRule type="cellIs" dxfId="264" priority="155" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="295" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
-    <cfRule type="cellIs" dxfId="263" priority="154" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="294" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q86">
-    <cfRule type="cellIs" dxfId="262" priority="153" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="293" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S86">
-    <cfRule type="cellIs" dxfId="261" priority="152" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="292" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AE86">
-    <cfRule type="cellIs" dxfId="260" priority="151" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="291" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG2:AG86">
-    <cfRule type="cellIs" dxfId="259" priority="150" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="290" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
-    <cfRule type="cellIs" dxfId="258" priority="149" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="289" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK2:AK86">
-    <cfRule type="cellIs" dxfId="257" priority="148" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="288" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM2:AM86">
-    <cfRule type="cellIs" dxfId="256" priority="147" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="287" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="cellIs" dxfId="255" priority="146" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="286" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="254" priority="145" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="285" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="253" priority="144" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="284" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="252" priority="143" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="283" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="cellIs" dxfId="251" priority="142" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="282" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
-    <cfRule type="cellIs" dxfId="250" priority="141" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="281" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="249" priority="140" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="280" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="248" priority="139" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="279" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="247" priority="138" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="278" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="246" priority="137" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="277" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="cellIs" dxfId="245" priority="136" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="276" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="244" priority="135" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="275" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="243" priority="134" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="274" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="242" priority="133" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="273" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="241" priority="132" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="272" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60">
-    <cfRule type="cellIs" dxfId="240" priority="131" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="271" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:N14">
-    <cfRule type="cellIs" dxfId="239" priority="130" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="270" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="238" priority="129" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="269" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="237" priority="128" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="268" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
-    <cfRule type="cellIs" dxfId="236" priority="127" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="267" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="cellIs" dxfId="235" priority="126" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="266" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="cellIs" dxfId="234" priority="125" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="265" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ43">
-    <cfRule type="cellIs" dxfId="233" priority="124" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="264" priority="151" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI43">
-    <cfRule type="cellIs" dxfId="232" priority="123" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="263" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3">
-    <cfRule type="cellIs" dxfId="231" priority="122" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="262" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="cellIs" dxfId="230" priority="121" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="261" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ4">
-    <cfRule type="cellIs" dxfId="229" priority="120" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="260" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI4">
-    <cfRule type="cellIs" dxfId="228" priority="119" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="259" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ5">
-    <cfRule type="cellIs" dxfId="227" priority="118" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="258" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI5">
-    <cfRule type="cellIs" dxfId="226" priority="117" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="257" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ6">
-    <cfRule type="cellIs" dxfId="225" priority="116" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="256" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6">
-    <cfRule type="cellIs" dxfId="224" priority="115" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="255" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ7">
-    <cfRule type="cellIs" dxfId="223" priority="114" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="254" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI7">
-    <cfRule type="cellIs" dxfId="222" priority="113" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="253" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:AJ9">
-    <cfRule type="cellIs" dxfId="221" priority="112" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="252" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI8">
-    <cfRule type="cellIs" dxfId="220" priority="111" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ46">
-    <cfRule type="cellIs" dxfId="219" priority="110" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="250" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI46">
-    <cfRule type="cellIs" dxfId="218" priority="109" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="249" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ47">
-    <cfRule type="cellIs" dxfId="217" priority="108" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="248" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI47">
-    <cfRule type="cellIs" dxfId="216" priority="107" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10">
-    <cfRule type="cellIs" dxfId="215" priority="106" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="246" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI10">
-    <cfRule type="cellIs" dxfId="214" priority="105" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ48">
-    <cfRule type="cellIs" dxfId="213" priority="104" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="244" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI48">
-    <cfRule type="cellIs" dxfId="212" priority="103" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="243" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ49">
-    <cfRule type="cellIs" dxfId="211" priority="102" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="242" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="210" priority="101" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="241" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="209" priority="100" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="240" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI50">
-    <cfRule type="cellIs" dxfId="208" priority="98" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="239" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11:AJ13">
-    <cfRule type="cellIs" dxfId="207" priority="97" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="238" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI11">
-    <cfRule type="cellIs" dxfId="206" priority="96" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="237" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ51">
-    <cfRule type="cellIs" dxfId="205" priority="95" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="236" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI52">
-    <cfRule type="cellIs" dxfId="204" priority="94" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="235" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ52:AJ54">
-    <cfRule type="cellIs" dxfId="203" priority="93" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="234" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ56">
-    <cfRule type="cellIs" dxfId="202" priority="92" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="233" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI56">
-    <cfRule type="cellIs" dxfId="201" priority="91" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="232" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ57:AJ58">
-    <cfRule type="cellIs" dxfId="200" priority="90" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="231" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI57:AI58">
-    <cfRule type="cellIs" dxfId="199" priority="89" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="230" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ15:AJ16">
-    <cfRule type="cellIs" dxfId="198" priority="88" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="229" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI15:AI16">
-    <cfRule type="cellIs" dxfId="197" priority="87" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="228" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ59:AJ60">
-    <cfRule type="cellIs" dxfId="196" priority="86" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="227" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ55">
-    <cfRule type="cellIs" dxfId="195" priority="85" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="226" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="cellIs" dxfId="194" priority="84" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="225" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="cellIs" dxfId="193" priority="83" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="224" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI18">
-    <cfRule type="cellIs" dxfId="192" priority="82" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="223" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="191" priority="81" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="222" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI17">
-    <cfRule type="cellIs" dxfId="190" priority="80" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="221" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ17">
-    <cfRule type="cellIs" dxfId="189" priority="79" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="220" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI86">
-    <cfRule type="cellIs" dxfId="188" priority="78" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="219" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI40">
-    <cfRule type="cellIs" dxfId="187" priority="77" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="218" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="186" priority="76" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="217" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="185" priority="75" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="216" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="184" priority="73" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="215" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
-    <cfRule type="cellIs" dxfId="183" priority="71" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="214" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21">
-    <cfRule type="cellIs" dxfId="182" priority="70" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="213" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI64">
-    <cfRule type="cellIs" dxfId="181" priority="69" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="212" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI23">
-    <cfRule type="cellIs" dxfId="180" priority="68" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="211" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ24">
-    <cfRule type="cellIs" dxfId="179" priority="67" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="210" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI25">
-    <cfRule type="cellIs" dxfId="178" priority="66" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="209" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ25">
-    <cfRule type="cellIs" dxfId="177" priority="65" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="208" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ67">
-    <cfRule type="cellIs" dxfId="176" priority="64" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="207" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI26">
-    <cfRule type="cellIs" dxfId="175" priority="63" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="206" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ26:AJ27">
-    <cfRule type="cellIs" dxfId="174" priority="62" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="205" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI28:AI30">
-    <cfRule type="cellIs" dxfId="173" priority="61" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="204" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28:AJ31">
-    <cfRule type="cellIs" dxfId="172" priority="60" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="203" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI72">
-    <cfRule type="cellIs" dxfId="171" priority="59" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="202" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ72">
-    <cfRule type="cellIs" dxfId="170" priority="58" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="201" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI73">
-    <cfRule type="cellIs" dxfId="169" priority="57" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="200" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ73">
-    <cfRule type="cellIs" dxfId="168" priority="56" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="199" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI32">
-    <cfRule type="cellIs" dxfId="167" priority="55" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="198" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="cellIs" dxfId="166" priority="54" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="197" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI33">
-    <cfRule type="cellIs" dxfId="165" priority="53" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="196" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ33">
-    <cfRule type="cellIs" dxfId="164" priority="52" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="195" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI34:AI35">
-    <cfRule type="cellIs" dxfId="163" priority="51" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="194" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ34:AJ36">
-    <cfRule type="cellIs" dxfId="162" priority="50" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="193" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI61">
-    <cfRule type="cellIs" dxfId="161" priority="49" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="192" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI63">
-    <cfRule type="cellIs" dxfId="160" priority="48" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="191" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ70">
-    <cfRule type="cellIs" dxfId="159" priority="47" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="190" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI70">
-    <cfRule type="cellIs" dxfId="158" priority="46" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="189" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI68">
-    <cfRule type="cellIs" dxfId="157" priority="45" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="188" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ76">
-    <cfRule type="cellIs" dxfId="156" priority="44" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="187" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI76">
-    <cfRule type="cellIs" dxfId="155" priority="43" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="186" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ78">
-    <cfRule type="cellIs" dxfId="154" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="185" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI78">
-    <cfRule type="cellIs" dxfId="153" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="184" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38">
-    <cfRule type="cellIs" dxfId="152" priority="40" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="183" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38">
-    <cfRule type="cellIs" dxfId="151" priority="39" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="182" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ77">
-    <cfRule type="cellIs" dxfId="150" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="181" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI77">
-    <cfRule type="cellIs" dxfId="149" priority="37" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="180" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ79">
-    <cfRule type="cellIs" dxfId="148" priority="36" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="179" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI79">
-    <cfRule type="cellIs" dxfId="147" priority="35" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="178" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ80">
-    <cfRule type="cellIs" dxfId="146" priority="34" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="177" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80">
-    <cfRule type="cellIs" dxfId="145" priority="33" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="176" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ81">
-    <cfRule type="cellIs" dxfId="144" priority="32" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="175" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI81">
-    <cfRule type="cellIs" dxfId="143" priority="31" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="174" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ82">
-    <cfRule type="cellIs" dxfId="142" priority="30" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="173" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI82">
-    <cfRule type="cellIs" dxfId="141" priority="29" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="172" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI83">
-    <cfRule type="cellIs" dxfId="140" priority="28" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="171" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI84:AI85">
-    <cfRule type="cellIs" dxfId="139" priority="27" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="170" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI39">
-    <cfRule type="cellIs" dxfId="138" priority="26" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="169" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="cellIs" dxfId="137" priority="25" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="168" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O61">
-    <cfRule type="cellIs" dxfId="136" priority="24" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="167" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54">
-    <cfRule type="cellIs" dxfId="135" priority="23" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="166" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O57">
-    <cfRule type="cellIs" dxfId="134" priority="22" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="165" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O58">
-    <cfRule type="cellIs" dxfId="133" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="164" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O67">
-    <cfRule type="cellIs" dxfId="132" priority="20" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="163" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71">
-    <cfRule type="cellIs" dxfId="131" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="162" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72">
-    <cfRule type="cellIs" dxfId="130" priority="18" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="161" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="129" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="160" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="128" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="159" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="cellIs" dxfId="127" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="158" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="126" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="157" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L75">
-    <cfRule type="cellIs" dxfId="125" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="156" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI12">
-    <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="155" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2">
-    <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="154" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W86">
-    <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="153" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="152" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA2:AA86">
-    <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
+    <cfRule type="cellIs" dxfId="151" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2">
-    <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="150" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y86">
-    <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="149" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2">
-    <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="148" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="147" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="146" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="145" priority="28" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
+    <cfRule type="cellIs" dxfId="30" priority="27" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA48">
+    <cfRule type="cellIs" dxfId="29" priority="26" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA11">
+    <cfRule type="cellIs" dxfId="28" priority="25" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA51">
+    <cfRule type="cellIs" dxfId="27" priority="24" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA52">
+    <cfRule type="cellIs" dxfId="25" priority="23" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA53">
+    <cfRule type="cellIs" dxfId="24" priority="22" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA57 AA54:AA55">
+    <cfRule type="cellIs" dxfId="23" priority="21" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA20">
+    <cfRule type="cellIs" dxfId="22" priority="20" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA21">
+    <cfRule type="cellIs" dxfId="21" priority="19" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA66">
+    <cfRule type="cellIs" dxfId="20" priority="18" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA25">
+    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA26">
+    <cfRule type="cellIs" dxfId="18" priority="16" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA28">
+    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA32">
+    <cfRule type="cellIs" dxfId="16" priority="14" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA34">
+    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA27">
+    <cfRule type="cellIs" dxfId="13" priority="12" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA33 AA31">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA61 M61">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA62">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA63 M63">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA65">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA67">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA68">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA70:AA73">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA77">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA74 AA38">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA37">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -46259,448 +46567,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="144" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="143" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="142" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="141" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="140" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="139" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="138" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="137" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="136" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="135" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="134" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="102" priority="93">
+    <cfRule type="containsBlanks" dxfId="133" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="132" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="100" priority="91">
+    <cfRule type="containsBlanks" dxfId="131" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="130" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="129" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="128" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="127" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="126" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="125" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="124" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="123" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="122" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="90" priority="69">
+    <cfRule type="containsBlanks" dxfId="121" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="120" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="119" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="118" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="117" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="116" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="115" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="114" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="82" priority="63">
+    <cfRule type="containsBlanks" dxfId="113" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="77" priority="59">
+    <cfRule type="containsBlanks" dxfId="108" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="107" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="75" priority="56">
+    <cfRule type="containsBlanks" dxfId="106" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="105" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="104" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="103" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="102" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="101" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="100" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="68" priority="50">
+    <cfRule type="containsBlanks" dxfId="99" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="98" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="97" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="65" priority="47">
+    <cfRule type="containsBlanks" dxfId="96" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="60" priority="42">
+    <cfRule type="containsBlanks" dxfId="91" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="90" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="57" priority="39">
+    <cfRule type="containsBlanks" dxfId="88" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="87" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="86" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="85" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="84" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="83" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="82" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="79" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="78" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="77" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="76" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="75" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="74" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="42" priority="23">
+    <cfRule type="containsBlanks" dxfId="73" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="72" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="40" priority="19">
+    <cfRule type="containsBlanks" dxfId="71" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="70" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="68" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="65" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="64" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="31" priority="22">
+    <cfRule type="containsBlanks" dxfId="62" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="30" priority="11">
+    <cfRule type="containsBlanks" dxfId="61" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="60" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="59" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="57" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="56" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="54" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61596,111 +61904,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="48" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="47" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="45" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="44" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -63024,7 +63332,7 @@
       </c>
       <c r="E3" s="68">
         <f ca="1">TODAY()</f>
-        <v>43446</v>
+        <v>43472</v>
       </c>
       <c r="F3" s="67">
         <v>42551</v>
@@ -63375,7 +63683,7 @@
       <c r="F1" s="1"/>
       <c r="I1" s="34">
         <f ca="1">TODAY()</f>
-        <v>43446</v>
+        <v>43472</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -67440,7 +67748,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update soils report data based on what is on SP
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B91A69-AF37-43C2-952B-F631C5769361}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCE6E7D-934E-49D1-8DC8-E614B6CE50B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8927" uniqueCount="1318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8957" uniqueCount="1334">
   <si>
     <t>#</t>
   </si>
@@ -3999,6 +3999,54 @@
   </si>
   <si>
     <t>see Prop S #14215</t>
+  </si>
+  <si>
+    <t>Central Plant soils report</t>
+  </si>
+  <si>
+    <t>see Prop N #11110</t>
+  </si>
+  <si>
+    <t>project finished in early 2019</t>
+  </si>
+  <si>
+    <t>not applicable?</t>
+  </si>
+  <si>
+    <t>to construct in 2019</t>
+  </si>
+  <si>
+    <t>see Prop S #11220</t>
+  </si>
+  <si>
+    <t>temporary</t>
+  </si>
+  <si>
+    <t>project to finish early 2019</t>
+  </si>
+  <si>
+    <t>no soils report needed?</t>
+  </si>
+  <si>
+    <t>13410; 13130</t>
+  </si>
+  <si>
+    <t>see also Prop S #13110</t>
+  </si>
+  <si>
+    <t>see also Prop N #13110</t>
+  </si>
+  <si>
+    <t>site not to be owned by SDCCD</t>
+  </si>
+  <si>
+    <t>see Prop S #13410; 13130</t>
+  </si>
+  <si>
+    <t>includes fault hazard eval</t>
+  </si>
+  <si>
+    <t>building built in 1930's or 1940;s</t>
   </si>
 </sst>
 </file>
@@ -5178,147 +5226,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="317">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="324">
     <dxf>
       <fill>
         <patternFill>
@@ -7398,6 +7306,195 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7644,7 +7741,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1/7/2019</c:v>
+                  <c:v>1/8/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9401,8 +9498,8 @@
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9413,8 +9510,8 @@
     <col min="4" max="4" width="8.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.26953125" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="22.08984375" customWidth="1"/>
-    <col min="7" max="7" width="3.26953125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="3.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="1.36328125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="3.453125" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="10.1796875" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="6.6328125" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="10.08984375" style="1" hidden="1" customWidth="1"/>
@@ -9424,14 +9521,14 @@
     <col min="16" max="16" width="10.81640625" style="2" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="7.26953125" style="2" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="9.08984375" style="2" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="7.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="10.81640625" style="2" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="7.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="10.81640625" style="2" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="8.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="7.26953125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.26953125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="10.81640625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.26953125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.81640625" style="2" customWidth="1"/>
     <col min="27" max="27" width="8.26953125" style="1" customWidth="1"/>
     <col min="28" max="28" width="11.81640625" style="2" customWidth="1"/>
     <col min="29" max="29" width="8.26953125" style="1" customWidth="1"/>
@@ -9748,12 +9845,10 @@
       <c r="R2" s="144">
         <v>1</v>
       </c>
-      <c r="S2" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T2" s="144">
-        <v>1</v>
-      </c>
+      <c r="S2" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T2" s="144"/>
       <c r="U2" s="144" t="s">
         <v>567</v>
       </c>
@@ -9921,11 +10016,11 @@
       <c r="R3" s="144">
         <v>1</v>
       </c>
-      <c r="S3" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T3" s="144">
-        <v>1</v>
+      <c r="S3" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T3" s="144" t="s">
+        <v>1319</v>
       </c>
       <c r="U3" s="144" t="s">
         <v>567</v>
@@ -10093,8 +10188,8 @@
       <c r="S4" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="T4" s="144">
-        <v>1</v>
+      <c r="T4" s="144" t="s">
+        <v>1320</v>
       </c>
       <c r="U4" s="144" t="s">
         <v>567</v>
@@ -10263,12 +10358,10 @@
       <c r="R5" s="144">
         <v>1</v>
       </c>
-      <c r="S5" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T5" s="144">
-        <v>1</v>
-      </c>
+      <c r="S5" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T5" s="144"/>
       <c r="U5" s="144" t="s">
         <v>567</v>
       </c>
@@ -10436,11 +10529,11 @@
       <c r="R6" s="144">
         <v>1</v>
       </c>
-      <c r="S6" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T6" s="144">
-        <v>1</v>
+      <c r="S6" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T6" s="144" t="s">
+        <v>1321</v>
       </c>
       <c r="U6" s="144" t="s">
         <v>567</v>
@@ -10624,8 +10717,8 @@
       <c r="S7" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="T7" s="144">
-        <v>1</v>
+      <c r="T7" s="144" t="s">
+        <v>1320</v>
       </c>
       <c r="U7" s="144" t="s">
         <v>567</v>
@@ -10797,8 +10890,8 @@
       <c r="S8" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="T8" s="144">
-        <v>1</v>
+      <c r="T8" s="144" t="s">
+        <v>1320</v>
       </c>
       <c r="U8" s="144" t="s">
         <v>567</v>
@@ -10965,11 +11058,11 @@
       <c r="R9" s="144">
         <v>1</v>
       </c>
-      <c r="S9" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T9" s="144">
-        <v>1</v>
+      <c r="S9" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T9" s="144" t="s">
+        <v>1321</v>
       </c>
       <c r="U9" s="144" t="s">
         <v>567</v>
@@ -11132,11 +11225,11 @@
       <c r="R10" s="144">
         <v>1</v>
       </c>
-      <c r="S10" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T10" s="144">
-        <v>1</v>
+      <c r="S10" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T10" s="144" t="s">
+        <v>1318</v>
       </c>
       <c r="U10" s="144" t="s">
         <v>567</v>
@@ -11305,12 +11398,10 @@
       <c r="R11" s="144">
         <v>1</v>
       </c>
-      <c r="S11" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T11" s="144">
-        <v>1</v>
-      </c>
+      <c r="S11" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T11" s="144"/>
       <c r="U11" s="144" t="s">
         <v>567</v>
       </c>
@@ -11480,12 +11571,10 @@
       <c r="R12" s="144">
         <v>1</v>
       </c>
-      <c r="S12" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T12" s="144">
-        <v>1</v>
-      </c>
+      <c r="S12" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T12" s="144"/>
       <c r="U12" s="144" t="s">
         <v>567</v>
       </c>
@@ -11649,11 +11738,11 @@
       <c r="R13" s="144">
         <v>1</v>
       </c>
-      <c r="S13" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T13" s="144">
-        <v>1</v>
+      <c r="S13" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T13" s="144" t="s">
+        <v>1326</v>
       </c>
       <c r="U13" s="144" t="s">
         <v>567</v>
@@ -11818,12 +11907,10 @@
       <c r="R14" s="144">
         <v>1</v>
       </c>
-      <c r="S14" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T14" s="144">
-        <v>1</v>
-      </c>
+      <c r="S14" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T14" s="144"/>
       <c r="U14" s="144" t="s">
         <v>567</v>
       </c>
@@ -11986,8 +12073,8 @@
       <c r="S15" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="T15" s="144">
-        <v>1</v>
+      <c r="T15" s="144" t="s">
+        <v>1325</v>
       </c>
       <c r="U15" s="144" t="s">
         <v>567</v>
@@ -12152,12 +12239,10 @@
       <c r="R16" s="144">
         <v>1</v>
       </c>
-      <c r="S16" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T16" s="144">
-        <v>1</v>
-      </c>
+      <c r="S16" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T16" s="144"/>
       <c r="U16" s="144" t="s">
         <v>567</v>
       </c>
@@ -12323,11 +12408,11 @@
       <c r="R17" s="144">
         <v>1</v>
       </c>
-      <c r="S17" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T17" s="144">
-        <v>1</v>
+      <c r="S17" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T17" s="144" t="s">
+        <v>1324</v>
       </c>
       <c r="U17" s="144" t="s">
         <v>567</v>
@@ -12492,11 +12577,11 @@
       <c r="R18" s="144">
         <v>1</v>
       </c>
-      <c r="S18" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T18" s="144">
-        <v>1</v>
+      <c r="S18" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T18" s="144" t="s">
+        <v>1324</v>
       </c>
       <c r="U18" s="144" t="s">
         <v>567</v>
@@ -12615,7 +12700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>86</v>
       </c>
@@ -12661,12 +12746,10 @@
       <c r="R19" s="144">
         <v>1</v>
       </c>
-      <c r="S19" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T19" s="144">
-        <v>1</v>
-      </c>
+      <c r="S19" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T19" s="144"/>
       <c r="U19" s="144" t="s">
         <v>567</v>
       </c>
@@ -12830,11 +12913,11 @@
       <c r="R20" s="144">
         <v>1</v>
       </c>
-      <c r="S20" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T20" s="144">
-        <v>1</v>
+      <c r="S20" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T20" s="144" t="s">
+        <v>1328</v>
       </c>
       <c r="U20" s="144" t="s">
         <v>567</v>
@@ -13001,12 +13084,10 @@
       <c r="R21" s="144">
         <v>1</v>
       </c>
-      <c r="S21" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T21" s="144">
-        <v>1</v>
-      </c>
+      <c r="S21" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T21" s="144"/>
       <c r="U21" s="144" t="s">
         <v>567</v>
       </c>
@@ -13176,12 +13257,10 @@
       <c r="R22" s="144">
         <v>1</v>
       </c>
-      <c r="S22" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T22" s="144">
-        <v>1</v>
-      </c>
+      <c r="S22" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T22" s="144"/>
       <c r="U22" s="144" t="s">
         <v>567</v>
       </c>
@@ -13295,7 +13374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
         <v>86</v>
       </c>
@@ -13341,11 +13420,11 @@
       <c r="R23" s="144">
         <v>1</v>
       </c>
-      <c r="S23" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T23" s="144">
-        <v>1</v>
+      <c r="S23" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T23" s="144" t="s">
+        <v>1330</v>
       </c>
       <c r="U23" s="144" t="s">
         <v>567</v>
@@ -13506,12 +13585,10 @@
       <c r="R24" s="144">
         <v>1</v>
       </c>
-      <c r="S24" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T24" s="144">
-        <v>1</v>
-      </c>
+      <c r="S24" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T24" s="144"/>
       <c r="U24" s="144" t="s">
         <v>567</v>
       </c>
@@ -13679,12 +13756,10 @@
       <c r="R25" s="144">
         <v>1</v>
       </c>
-      <c r="S25" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T25" s="144">
-        <v>1</v>
-      </c>
+      <c r="S25" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T25" s="144"/>
       <c r="U25" s="144" t="s">
         <v>567</v>
       </c>
@@ -13850,12 +13925,10 @@
       <c r="R26" s="144">
         <v>1</v>
       </c>
-      <c r="S26" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T26" s="144">
-        <v>1</v>
-      </c>
+      <c r="S26" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T26" s="144"/>
       <c r="U26" s="144" t="s">
         <v>567</v>
       </c>
@@ -14019,11 +14092,11 @@
       <c r="R27" s="144">
         <v>1</v>
       </c>
-      <c r="S27" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T27" s="144">
-        <v>1</v>
+      <c r="S27" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T27" s="144" t="s">
+        <v>1331</v>
       </c>
       <c r="U27" s="144" t="s">
         <v>567</v>
@@ -14188,12 +14261,10 @@
       <c r="R28" s="144">
         <v>1</v>
       </c>
-      <c r="S28" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T28" s="144">
-        <v>1</v>
-      </c>
+      <c r="S28" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T28" s="144"/>
       <c r="U28" s="144" t="s">
         <v>567</v>
       </c>
@@ -14363,12 +14434,10 @@
       <c r="R29" s="144">
         <v>1</v>
       </c>
-      <c r="S29" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T29" s="144">
-        <v>1</v>
-      </c>
+      <c r="S29" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T29" s="144"/>
       <c r="U29" s="144" t="s">
         <v>567</v>
       </c>
@@ -14536,12 +14605,10 @@
       <c r="R30" s="144">
         <v>1</v>
       </c>
-      <c r="S30" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T30" s="144">
-        <v>1</v>
-      </c>
+      <c r="S30" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T30" s="144"/>
       <c r="U30" s="144" t="s">
         <v>567</v>
       </c>
@@ -14659,7 +14726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B31" s="19" t="s">
         <v>86</v>
       </c>
@@ -14705,12 +14772,10 @@
       <c r="R31" s="144">
         <v>1</v>
       </c>
-      <c r="S31" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T31" s="144">
-        <v>1</v>
-      </c>
+      <c r="S31" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T31" s="144"/>
       <c r="U31" s="144" t="s">
         <v>567</v>
       </c>
@@ -14872,12 +14937,10 @@
       <c r="R32" s="144">
         <v>1</v>
       </c>
-      <c r="S32" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T32" s="144">
-        <v>1</v>
-      </c>
+      <c r="S32" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T32" s="144"/>
       <c r="U32" s="144" t="s">
         <v>567</v>
       </c>
@@ -15041,12 +15104,10 @@
       <c r="R33" s="144">
         <v>1</v>
       </c>
-      <c r="S33" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T33" s="144">
-        <v>1</v>
-      </c>
+      <c r="S33" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T33" s="144"/>
       <c r="U33" s="144" t="s">
         <v>567</v>
       </c>
@@ -15208,12 +15269,10 @@
       <c r="R34" s="144">
         <v>1</v>
       </c>
-      <c r="S34" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T34" s="144">
-        <v>1</v>
-      </c>
+      <c r="S34" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T34" s="144"/>
       <c r="U34" s="144" t="s">
         <v>567</v>
       </c>
@@ -15381,12 +15440,10 @@
       <c r="R35" s="144">
         <v>1</v>
       </c>
-      <c r="S35" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T35" s="144">
-        <v>1</v>
-      </c>
+      <c r="S35" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T35" s="144"/>
       <c r="U35" s="144" t="s">
         <v>567</v>
       </c>
@@ -15548,11 +15605,11 @@
       <c r="R36" s="144">
         <v>1</v>
       </c>
-      <c r="S36" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T36" s="144">
-        <v>1</v>
+      <c r="S36" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T36" s="144" t="s">
+        <v>1313</v>
       </c>
       <c r="U36" s="144" t="s">
         <v>567</v>
@@ -15717,12 +15774,10 @@
       <c r="R37" s="144">
         <v>1</v>
       </c>
-      <c r="S37" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T37" s="144">
-        <v>1</v>
-      </c>
+      <c r="S37" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T37" s="144"/>
       <c r="U37" s="144" t="s">
         <v>567</v>
       </c>
@@ -15882,12 +15937,10 @@
       <c r="R38" s="144">
         <v>1</v>
       </c>
-      <c r="S38" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T38" s="144">
-        <v>1</v>
-      </c>
+      <c r="S38" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T38" s="144"/>
       <c r="U38" s="144" t="s">
         <v>567</v>
       </c>
@@ -16005,7 +16058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
         <v>86</v>
       </c>
@@ -16049,12 +16102,10 @@
       <c r="R39" s="144">
         <v>1</v>
       </c>
-      <c r="S39" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T39" s="144">
-        <v>1</v>
-      </c>
+      <c r="S39" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T39" s="144"/>
       <c r="U39" s="144" t="s">
         <v>567</v>
       </c>
@@ -16198,7 +16249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B40" s="19" t="s">
         <v>86</v>
       </c>
@@ -16242,12 +16293,10 @@
       <c r="R40" s="144">
         <v>1</v>
       </c>
-      <c r="S40" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T40" s="144">
-        <v>1</v>
-      </c>
+      <c r="S40" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T40" s="144"/>
       <c r="U40" s="144" t="s">
         <v>567</v>
       </c>
@@ -16433,11 +16482,11 @@
       <c r="R41" s="144">
         <v>1</v>
       </c>
-      <c r="S41" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T41" s="144">
-        <v>1</v>
+      <c r="S41" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T41" s="144" t="s">
+        <v>1318</v>
       </c>
       <c r="U41" s="144" t="s">
         <v>567</v>
@@ -16592,12 +16641,10 @@
       <c r="R42" s="144">
         <v>1</v>
       </c>
-      <c r="S42" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T42" s="144">
-        <v>1</v>
-      </c>
+      <c r="S42" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T42" s="144"/>
       <c r="U42" s="144" t="s">
         <v>567</v>
       </c>
@@ -16759,11 +16806,11 @@
       <c r="R43" s="144">
         <v>1</v>
       </c>
-      <c r="S43" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T43" s="144">
-        <v>1</v>
+      <c r="S43" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T43" s="144" t="s">
+        <v>1323</v>
       </c>
       <c r="U43" s="144" t="s">
         <v>567</v>
@@ -16914,7 +16961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B44" s="19" t="s">
         <v>4</v>
       </c>
@@ -16961,8 +17008,8 @@
       <c r="S44" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="T44" s="144">
-        <v>1</v>
+      <c r="T44" s="144" t="s">
+        <v>1322</v>
       </c>
       <c r="U44" s="144" t="s">
         <v>567</v>
@@ -17127,12 +17174,10 @@
       <c r="R45" s="144">
         <v>1</v>
       </c>
-      <c r="S45" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T45" s="144">
-        <v>1</v>
-      </c>
+      <c r="S45" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T45" s="144"/>
       <c r="U45" s="144" t="s">
         <v>567</v>
       </c>
@@ -17306,11 +17351,11 @@
       <c r="R46" s="144">
         <v>1</v>
       </c>
-      <c r="S46" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T46" s="144">
-        <v>1</v>
+      <c r="S46" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T46" s="144" t="s">
+        <v>1321</v>
       </c>
       <c r="U46" s="144" t="s">
         <v>567</v>
@@ -17475,12 +17520,10 @@
       <c r="R47" s="144">
         <v>1</v>
       </c>
-      <c r="S47" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T47" s="144">
-        <v>1</v>
-      </c>
+      <c r="S47" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T47" s="144"/>
       <c r="U47" s="144" t="s">
         <v>567</v>
       </c>
@@ -17646,11 +17689,11 @@
       <c r="R48" s="144">
         <v>1</v>
       </c>
-      <c r="S48" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T48" s="144">
-        <v>1</v>
+      <c r="S48" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T48" s="144" t="s">
+        <v>1321</v>
       </c>
       <c r="U48" s="144" t="s">
         <v>567</v>
@@ -17769,7 +17812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>4</v>
       </c>
@@ -17813,11 +17856,11 @@
       <c r="R49" s="144">
         <v>1</v>
       </c>
-      <c r="S49" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T49" s="144">
-        <v>1</v>
+      <c r="S49" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T49" s="144" t="s">
+        <v>1324</v>
       </c>
       <c r="U49" s="144" t="s">
         <v>567</v>
@@ -17984,12 +18027,10 @@
       <c r="R50" s="144">
         <v>1</v>
       </c>
-      <c r="S50" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T50" s="144">
-        <v>1</v>
-      </c>
+      <c r="S50" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T50" s="144"/>
       <c r="U50" s="144" t="s">
         <v>567</v>
       </c>
@@ -18187,12 +18228,10 @@
       <c r="R51" s="144">
         <v>1</v>
       </c>
-      <c r="S51" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T51" s="144">
-        <v>1</v>
-      </c>
+      <c r="S51" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T51" s="144"/>
       <c r="U51" s="144" t="s">
         <v>567</v>
       </c>
@@ -18358,12 +18397,10 @@
       <c r="R52" s="144">
         <v>1</v>
       </c>
-      <c r="S52" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T52" s="144">
-        <v>1</v>
-      </c>
+      <c r="S52" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T52" s="144"/>
       <c r="U52" s="144" t="s">
         <v>567</v>
       </c>
@@ -18531,12 +18568,10 @@
       <c r="R53" s="144">
         <v>1</v>
       </c>
-      <c r="S53" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T53" s="144">
-        <v>1</v>
-      </c>
+      <c r="S53" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T53" s="144"/>
       <c r="U53" s="144" t="s">
         <v>567</v>
       </c>
@@ -18696,11 +18731,11 @@
       <c r="R54" s="144">
         <v>1</v>
       </c>
-      <c r="S54" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T54" s="144">
-        <v>1</v>
+      <c r="S54" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T54" s="144" t="s">
+        <v>1326</v>
       </c>
       <c r="U54" s="144" t="s">
         <v>567</v>
@@ -18875,12 +18910,10 @@
       <c r="R55" s="144">
         <v>1</v>
       </c>
-      <c r="S55" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T55" s="144">
-        <v>1</v>
-      </c>
+      <c r="S55" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T55" s="144"/>
       <c r="U55" s="144" t="s">
         <v>567</v>
       </c>
@@ -19046,12 +19079,10 @@
       <c r="R56" s="144">
         <v>1</v>
       </c>
-      <c r="S56" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T56" s="144">
-        <v>1</v>
-      </c>
+      <c r="S56" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T56" s="144"/>
       <c r="U56" s="144" t="s">
         <v>567</v>
       </c>
@@ -19213,12 +19244,10 @@
       <c r="R57" s="144">
         <v>1</v>
       </c>
-      <c r="S57" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T57" s="144">
-        <v>1</v>
-      </c>
+      <c r="S57" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T57" s="144"/>
       <c r="U57" s="144" t="s">
         <v>567</v>
       </c>
@@ -19334,7 +19363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B58" s="19" t="s">
         <v>4</v>
       </c>
@@ -19380,12 +19409,10 @@
       <c r="R58" s="144">
         <v>1</v>
       </c>
-      <c r="S58" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T58" s="144">
-        <v>1</v>
-      </c>
+      <c r="S58" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T58" s="144"/>
       <c r="U58" s="144" t="s">
         <v>567</v>
       </c>
@@ -19585,12 +19612,10 @@
       <c r="R59" s="144">
         <v>1</v>
       </c>
-      <c r="S59" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T59" s="144">
-        <v>1</v>
-      </c>
+      <c r="S59" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T59" s="144"/>
       <c r="U59" s="144" t="s">
         <v>567</v>
       </c>
@@ -19756,12 +19781,10 @@
       <c r="R60" s="144">
         <v>1</v>
       </c>
-      <c r="S60" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T60" s="144">
-        <v>1</v>
-      </c>
+      <c r="S60" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T60" s="144"/>
       <c r="U60" s="144" t="s">
         <v>567</v>
       </c>
@@ -19919,11 +19942,11 @@
       <c r="R61" s="144">
         <v>1</v>
       </c>
-      <c r="S61" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T61" s="144">
-        <v>1</v>
+      <c r="S61" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T61" s="144" t="s">
+        <v>1329</v>
       </c>
       <c r="U61" s="144" t="s">
         <v>567</v>
@@ -20086,11 +20109,11 @@
       <c r="R62" s="144">
         <v>1</v>
       </c>
-      <c r="S62" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T62" s="144">
-        <v>1</v>
+      <c r="S62" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T62" s="144" t="s">
+        <v>1314</v>
       </c>
       <c r="U62" s="144" t="s">
         <v>567</v>
@@ -20205,7 +20228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B63" s="19" t="s">
         <v>4</v>
       </c>
@@ -20249,11 +20272,11 @@
       <c r="R63" s="144">
         <v>1</v>
       </c>
-      <c r="S63" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T63" s="144">
-        <v>1</v>
+      <c r="S63" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T63" s="144" t="s">
+        <v>1314</v>
       </c>
       <c r="U63" s="144" t="s">
         <v>567</v>
@@ -20410,11 +20433,11 @@
       <c r="R64" s="144">
         <v>1</v>
       </c>
-      <c r="S64" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T64" s="144">
-        <v>1</v>
+      <c r="S64" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T64" s="144" t="s">
+        <v>1314</v>
       </c>
       <c r="U64" s="144" t="s">
         <v>567</v>
@@ -20581,12 +20604,10 @@
       <c r="R65" s="144">
         <v>1</v>
       </c>
-      <c r="S65" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T65" s="144">
-        <v>1</v>
-      </c>
+      <c r="S65" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T65" s="144"/>
       <c r="U65" s="144" t="s">
         <v>567</v>
       </c>
@@ -20754,12 +20775,10 @@
       <c r="R66" s="144">
         <v>1</v>
       </c>
-      <c r="S66" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T66" s="144">
-        <v>1</v>
-      </c>
+      <c r="S66" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T66" s="144"/>
       <c r="U66" s="144" t="s">
         <v>567</v>
       </c>
@@ -20877,7 +20896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
         <v>4</v>
       </c>
@@ -20928,9 +20947,7 @@
       <c r="S67" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="T67" s="144">
-        <v>1</v>
-      </c>
+      <c r="T67" s="144"/>
       <c r="U67" s="144" t="s">
         <v>567</v>
       </c>
@@ -21051,8 +21068,8 @@
       <c r="C68" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="27">
-        <v>13410</v>
+      <c r="D68" s="27" t="s">
+        <v>1327</v>
       </c>
       <c r="E68" s="27"/>
       <c r="F68" s="20" t="s">
@@ -21092,11 +21109,11 @@
       <c r="R68" s="144">
         <v>1</v>
       </c>
-      <c r="S68" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T68" s="144">
-        <v>1</v>
+      <c r="S68" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T68" s="144" t="s">
+        <v>1315</v>
       </c>
       <c r="U68" s="144" t="s">
         <v>567</v>
@@ -21261,12 +21278,10 @@
       <c r="R69" s="144">
         <v>1</v>
       </c>
-      <c r="S69" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T69" s="144">
-        <v>1</v>
-      </c>
+      <c r="S69" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T69" s="144"/>
       <c r="U69" s="144" t="s">
         <v>567</v>
       </c>
@@ -21384,7 +21399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B70" s="19" t="s">
         <v>4</v>
       </c>
@@ -21430,12 +21445,10 @@
       <c r="R70" s="144">
         <v>1</v>
       </c>
-      <c r="S70" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T70" s="144">
-        <v>1</v>
-      </c>
+      <c r="S70" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T70" s="144"/>
       <c r="U70" s="144" t="s">
         <v>567</v>
       </c>
@@ -21597,12 +21610,10 @@
       <c r="R71" s="144">
         <v>1</v>
       </c>
-      <c r="S71" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T71" s="144">
-        <v>1</v>
-      </c>
+      <c r="S71" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T71" s="144"/>
       <c r="U71" s="144" t="s">
         <v>567</v>
       </c>
@@ -21767,9 +21778,7 @@
       <c r="S72" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="T72" s="144">
-        <v>1</v>
-      </c>
+      <c r="T72" s="144"/>
       <c r="U72" s="144" t="s">
         <v>567</v>
       </c>
@@ -21931,12 +21940,10 @@
       <c r="R73" s="144">
         <v>1</v>
       </c>
-      <c r="S73" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T73" s="144">
-        <v>1</v>
-      </c>
+      <c r="S73" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T73" s="144"/>
       <c r="U73" s="144" t="s">
         <v>567</v>
       </c>
@@ -22100,12 +22107,10 @@
       <c r="R74" s="144">
         <v>1</v>
       </c>
-      <c r="S74" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T74" s="144">
-        <v>1</v>
-      </c>
+      <c r="S74" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T74" s="144"/>
       <c r="U74" s="144" t="s">
         <v>567</v>
       </c>
@@ -22255,7 +22260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B75" s="19" t="s">
         <v>4</v>
       </c>
@@ -22303,12 +22308,10 @@
       <c r="R75" s="144">
         <v>1</v>
       </c>
-      <c r="S75" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T75" s="144">
-        <v>1</v>
-      </c>
+      <c r="S75" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T75" s="144"/>
       <c r="U75" s="144" t="s">
         <v>567</v>
       </c>
@@ -22504,12 +22507,10 @@
       <c r="R76" s="144">
         <v>1</v>
       </c>
-      <c r="S76" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T76" s="144">
-        <v>1</v>
-      </c>
+      <c r="S76" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T76" s="144"/>
       <c r="U76" s="144" t="s">
         <v>567</v>
       </c>
@@ -22679,12 +22680,10 @@
       <c r="R77" s="144">
         <v>1</v>
       </c>
-      <c r="S77" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T77" s="144">
-        <v>1</v>
-      </c>
+      <c r="S77" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T77" s="144"/>
       <c r="U77" s="144" t="s">
         <v>567</v>
       </c>
@@ -22852,12 +22851,10 @@
       <c r="R78" s="144">
         <v>1</v>
       </c>
-      <c r="S78" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T78" s="144">
-        <v>1</v>
-      </c>
+      <c r="S78" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T78" s="144"/>
       <c r="U78" s="144" t="s">
         <v>567</v>
       </c>
@@ -23019,11 +23016,11 @@
       <c r="R79" s="144">
         <v>1</v>
       </c>
-      <c r="S79" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T79" s="144">
-        <v>1</v>
+      <c r="S79" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="T79" s="144" t="s">
+        <v>1332</v>
       </c>
       <c r="U79" s="144" t="s">
         <v>567</v>
@@ -23200,11 +23197,11 @@
       <c r="R80" s="144">
         <v>1</v>
       </c>
-      <c r="S80" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T80" s="144">
-        <v>1</v>
+      <c r="S80" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T80" s="144" t="s">
+        <v>1333</v>
       </c>
       <c r="U80" s="144" t="s">
         <v>567</v>
@@ -23323,7 +23320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B81" s="19" t="s">
         <v>4</v>
       </c>
@@ -23369,12 +23366,10 @@
       <c r="R81" s="144">
         <v>1</v>
       </c>
-      <c r="S81" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T81" s="144">
-        <v>1</v>
-      </c>
+      <c r="S81" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T81" s="144"/>
       <c r="U81" s="144" t="s">
         <v>567</v>
       </c>
@@ -23568,12 +23563,10 @@
       <c r="R82" s="144">
         <v>1</v>
       </c>
-      <c r="S82" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T82" s="144">
-        <v>1</v>
-      </c>
+      <c r="S82" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="T82" s="144"/>
       <c r="U82" s="144" t="s">
         <v>567</v>
       </c>
@@ -23721,7 +23714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B83" s="19" t="s">
         <v>4</v>
       </c>
@@ -23765,12 +23758,10 @@
       <c r="R83" s="144">
         <v>1</v>
       </c>
-      <c r="S83" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T83" s="144">
-        <v>1</v>
-      </c>
+      <c r="S83" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T83" s="144"/>
       <c r="U83" s="144" t="s">
         <v>567</v>
       </c>
@@ -23958,12 +23949,10 @@
       <c r="R84" s="144">
         <v>1</v>
       </c>
-      <c r="S84" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T84" s="144">
-        <v>1</v>
-      </c>
+      <c r="S84" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T84" s="144"/>
       <c r="U84" s="144" t="s">
         <v>567</v>
       </c>
@@ -24109,7 +24098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B85" s="19" t="s">
         <v>4</v>
       </c>
@@ -24153,12 +24142,10 @@
       <c r="R85" s="144">
         <v>1</v>
       </c>
-      <c r="S85" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T85" s="144">
-        <v>1</v>
-      </c>
+      <c r="S85" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T85" s="144"/>
       <c r="U85" s="144" t="s">
         <v>567</v>
       </c>
@@ -24304,7 +24291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B86" s="19" t="s">
         <v>4</v>
       </c>
@@ -24348,12 +24335,10 @@
       <c r="R86" s="144">
         <v>1</v>
       </c>
-      <c r="S86" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="T86" s="144">
-        <v>1</v>
-      </c>
+      <c r="S86" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="T86" s="144"/>
       <c r="U86" s="144" t="s">
         <v>567</v>
       </c>
@@ -24516,1194 +24501,1260 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
+    <cfRule type="cellIs" dxfId="323" priority="256" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BI9:BJ9">
+    <cfRule type="cellIs" dxfId="322" priority="255" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
+    <cfRule type="cellIs" dxfId="321" priority="254" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AV39 AV56">
+    <cfRule type="cellIs" dxfId="320" priority="253" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
+    <cfRule type="cellIs" dxfId="319" priority="251" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
+    <cfRule type="cellIs" dxfId="318" priority="250" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
+    <cfRule type="cellIs" dxfId="317" priority="249" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW56">
     <cfRule type="cellIs" dxfId="316" priority="245" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BI9:BJ9">
-    <cfRule type="cellIs" dxfId="315" priority="244" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="314" priority="243" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="313" priority="242" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
-    <cfRule type="cellIs" dxfId="312" priority="240" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="311" priority="239" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="310" priority="238" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="309" priority="234" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="308" priority="224" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="315" priority="235" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I4 I7:I8 I12 I44 I14:I15 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="307" priority="211" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="314" priority="222" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
+    <cfRule type="cellIs" dxfId="313" priority="211" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CC2">
+    <cfRule type="cellIs" dxfId="312" priority="208" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CD2">
+    <cfRule type="cellIs" dxfId="311" priority="207" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46:K58 K2:K38 K60:K61 K41:K44 K63:K74 K76:K82">
+    <cfRule type="cellIs" dxfId="310" priority="206" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J36 J8:J12 J38:J40 J2:J5 J18 J20:J29 J33:J34 J46:J74">
+    <cfRule type="cellIs" dxfId="309" priority="205" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L8:L12 L76:L85 L14:L29 L2:L5 L46:L61 L63:L74">
+    <cfRule type="cellIs" dxfId="308" priority="204" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="cellIs" dxfId="307" priority="203" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2">
     <cfRule type="cellIs" dxfId="306" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CC2">
-    <cfRule type="cellIs" dxfId="305" priority="197" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AH2:AH86">
+    <cfRule type="cellIs" dxfId="305" priority="199" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CD2">
-    <cfRule type="cellIs" dxfId="304" priority="196" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AN2:AN86">
+    <cfRule type="cellIs" dxfId="304" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:K58 K2:K38 K60:K61 K41:K44 K63:K74 K76:K82">
+  <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
     <cfRule type="cellIs" dxfId="303" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J36 J8:J12 J38:J40 J2:J5 J18 J20:J29 J33:J34 J46:J74">
-    <cfRule type="cellIs" dxfId="302" priority="194" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L8:L12 L76:L85 L14:L29 L2:L5 L46:L61 L63:L74">
-    <cfRule type="cellIs" dxfId="301" priority="193" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="300" priority="192" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="299" priority="189" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="298" priority="188" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="297" priority="186" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="296" priority="184" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
-    <cfRule type="cellIs" dxfId="295" priority="182" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="302" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
-    <cfRule type="cellIs" dxfId="294" priority="181" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="301" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q86">
-    <cfRule type="cellIs" dxfId="293" priority="180" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="300" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S86">
-    <cfRule type="cellIs" dxfId="292" priority="179" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S4 S6:S8 S50 S44 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
+    <cfRule type="cellIs" dxfId="299" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AE86">
-    <cfRule type="cellIs" dxfId="291" priority="178" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="298" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG2:AG86">
-    <cfRule type="cellIs" dxfId="290" priority="177" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="297" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
-    <cfRule type="cellIs" dxfId="289" priority="176" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="296" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK2:AK86">
-    <cfRule type="cellIs" dxfId="288" priority="175" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="295" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM2:AM86">
-    <cfRule type="cellIs" dxfId="287" priority="174" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="294" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="cellIs" dxfId="286" priority="173" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="293" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="285" priority="172" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="292" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="284" priority="171" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="291" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="283" priority="170" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="290" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="cellIs" dxfId="282" priority="169" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="289" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
-    <cfRule type="cellIs" dxfId="281" priority="168" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="288" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="280" priority="167" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="287" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="279" priority="166" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="286" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="278" priority="165" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="285" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="277" priority="164" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="284" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="cellIs" dxfId="276" priority="163" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="283" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="275" priority="162" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="282" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="274" priority="161" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="281" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="273" priority="160" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="280" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="272" priority="159" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="279" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60">
-    <cfRule type="cellIs" dxfId="271" priority="158" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="278" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:N14">
-    <cfRule type="cellIs" dxfId="270" priority="157" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="277" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="269" priority="156" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="276" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="268" priority="155" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="275" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
-    <cfRule type="cellIs" dxfId="267" priority="154" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="274" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="cellIs" dxfId="266" priority="153" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="273" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="cellIs" dxfId="265" priority="152" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="272" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ43">
-    <cfRule type="cellIs" dxfId="264" priority="151" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="271" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI43">
-    <cfRule type="cellIs" dxfId="263" priority="150" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="270" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3">
-    <cfRule type="cellIs" dxfId="262" priority="149" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="269" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="cellIs" dxfId="261" priority="148" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="268" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ4">
-    <cfRule type="cellIs" dxfId="260" priority="147" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="267" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI4">
-    <cfRule type="cellIs" dxfId="259" priority="146" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="266" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ5">
-    <cfRule type="cellIs" dxfId="258" priority="145" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="265" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI5">
-    <cfRule type="cellIs" dxfId="257" priority="144" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="264" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ6">
-    <cfRule type="cellIs" dxfId="256" priority="143" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="263" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6">
-    <cfRule type="cellIs" dxfId="255" priority="142" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="262" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ7">
-    <cfRule type="cellIs" dxfId="254" priority="141" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="261" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI7">
-    <cfRule type="cellIs" dxfId="253" priority="140" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="260" priority="151" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:AJ9">
-    <cfRule type="cellIs" dxfId="252" priority="139" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="259" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI8">
-    <cfRule type="cellIs" dxfId="251" priority="138" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="258" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ46">
-    <cfRule type="cellIs" dxfId="250" priority="137" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="257" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI46">
-    <cfRule type="cellIs" dxfId="249" priority="136" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="256" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ47">
-    <cfRule type="cellIs" dxfId="248" priority="135" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="255" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI47">
-    <cfRule type="cellIs" dxfId="247" priority="134" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="254" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10">
-    <cfRule type="cellIs" dxfId="246" priority="133" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="253" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI10">
-    <cfRule type="cellIs" dxfId="245" priority="132" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="252" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ48">
-    <cfRule type="cellIs" dxfId="244" priority="131" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI48">
-    <cfRule type="cellIs" dxfId="243" priority="130" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="250" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ49">
-    <cfRule type="cellIs" dxfId="242" priority="129" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="249" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="241" priority="128" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="248" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="240" priority="127" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI50">
-    <cfRule type="cellIs" dxfId="239" priority="125" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="246" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11:AJ13">
-    <cfRule type="cellIs" dxfId="238" priority="124" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI11">
-    <cfRule type="cellIs" dxfId="237" priority="123" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="244" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ51">
-    <cfRule type="cellIs" dxfId="236" priority="122" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="243" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI52">
-    <cfRule type="cellIs" dxfId="235" priority="121" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="242" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ52:AJ54">
-    <cfRule type="cellIs" dxfId="234" priority="120" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="241" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ56">
-    <cfRule type="cellIs" dxfId="233" priority="119" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="240" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI56">
-    <cfRule type="cellIs" dxfId="232" priority="118" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="239" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ57:AJ58">
-    <cfRule type="cellIs" dxfId="231" priority="117" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="238" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI57:AI58">
-    <cfRule type="cellIs" dxfId="230" priority="116" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="237" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ15:AJ16">
-    <cfRule type="cellIs" dxfId="229" priority="115" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="236" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI15:AI16">
-    <cfRule type="cellIs" dxfId="228" priority="114" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="235" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ59:AJ60">
-    <cfRule type="cellIs" dxfId="227" priority="113" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="234" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ55">
-    <cfRule type="cellIs" dxfId="226" priority="112" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="233" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="cellIs" dxfId="225" priority="111" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="232" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="cellIs" dxfId="224" priority="110" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="231" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI18">
-    <cfRule type="cellIs" dxfId="223" priority="109" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="230" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="222" priority="108" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="229" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI17">
-    <cfRule type="cellIs" dxfId="221" priority="107" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="228" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ17">
-    <cfRule type="cellIs" dxfId="220" priority="106" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="227" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI86">
-    <cfRule type="cellIs" dxfId="219" priority="105" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="226" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI40">
-    <cfRule type="cellIs" dxfId="218" priority="104" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="225" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="217" priority="103" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="224" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="216" priority="102" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="223" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="215" priority="100" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="222" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
-    <cfRule type="cellIs" dxfId="214" priority="98" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="221" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21">
-    <cfRule type="cellIs" dxfId="213" priority="97" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="220" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI64">
-    <cfRule type="cellIs" dxfId="212" priority="96" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="219" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI23">
-    <cfRule type="cellIs" dxfId="211" priority="95" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="218" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ24">
-    <cfRule type="cellIs" dxfId="210" priority="94" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="217" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI25">
-    <cfRule type="cellIs" dxfId="209" priority="93" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="216" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ25">
-    <cfRule type="cellIs" dxfId="208" priority="92" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="215" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ67">
-    <cfRule type="cellIs" dxfId="207" priority="91" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="214" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI26">
-    <cfRule type="cellIs" dxfId="206" priority="90" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="213" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ26:AJ27">
-    <cfRule type="cellIs" dxfId="205" priority="89" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="212" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI28:AI30">
-    <cfRule type="cellIs" dxfId="204" priority="88" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="211" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28:AJ31">
-    <cfRule type="cellIs" dxfId="203" priority="87" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="210" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI72">
-    <cfRule type="cellIs" dxfId="202" priority="86" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="209" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ72">
-    <cfRule type="cellIs" dxfId="201" priority="85" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="208" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI73">
-    <cfRule type="cellIs" dxfId="200" priority="84" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="207" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ73">
-    <cfRule type="cellIs" dxfId="199" priority="83" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="206" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI32">
-    <cfRule type="cellIs" dxfId="198" priority="82" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="205" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="cellIs" dxfId="197" priority="81" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="204" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI33">
-    <cfRule type="cellIs" dxfId="196" priority="80" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="203" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ33">
-    <cfRule type="cellIs" dxfId="195" priority="79" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="202" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI34:AI35">
-    <cfRule type="cellIs" dxfId="194" priority="78" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="201" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ34:AJ36">
-    <cfRule type="cellIs" dxfId="193" priority="77" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="200" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI61">
-    <cfRule type="cellIs" dxfId="192" priority="76" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="199" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI63">
-    <cfRule type="cellIs" dxfId="191" priority="75" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="198" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ70">
-    <cfRule type="cellIs" dxfId="190" priority="74" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="197" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI70">
-    <cfRule type="cellIs" dxfId="189" priority="73" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="196" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI68">
-    <cfRule type="cellIs" dxfId="188" priority="72" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="195" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ76">
-    <cfRule type="cellIs" dxfId="187" priority="71" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="194" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI76">
-    <cfRule type="cellIs" dxfId="186" priority="70" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="193" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ78">
-    <cfRule type="cellIs" dxfId="185" priority="69" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="192" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI78">
-    <cfRule type="cellIs" dxfId="184" priority="68" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="191" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38">
-    <cfRule type="cellIs" dxfId="183" priority="67" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="190" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38">
-    <cfRule type="cellIs" dxfId="182" priority="66" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="189" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ77">
-    <cfRule type="cellIs" dxfId="181" priority="65" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="188" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI77">
-    <cfRule type="cellIs" dxfId="180" priority="64" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="187" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ79">
-    <cfRule type="cellIs" dxfId="179" priority="63" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="186" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI79">
-    <cfRule type="cellIs" dxfId="178" priority="62" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="185" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ80">
-    <cfRule type="cellIs" dxfId="177" priority="61" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="184" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80">
-    <cfRule type="cellIs" dxfId="176" priority="60" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="183" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ81">
-    <cfRule type="cellIs" dxfId="175" priority="59" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="182" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI81">
-    <cfRule type="cellIs" dxfId="174" priority="58" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="181" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ82">
-    <cfRule type="cellIs" dxfId="173" priority="57" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="180" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI82">
-    <cfRule type="cellIs" dxfId="172" priority="56" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="179" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI83">
-    <cfRule type="cellIs" dxfId="171" priority="55" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="178" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI84:AI85">
-    <cfRule type="cellIs" dxfId="170" priority="54" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="177" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI39">
-    <cfRule type="cellIs" dxfId="169" priority="53" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="176" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="cellIs" dxfId="168" priority="52" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="175" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O61">
-    <cfRule type="cellIs" dxfId="167" priority="51" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="174" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54">
-    <cfRule type="cellIs" dxfId="166" priority="50" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="173" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O57">
-    <cfRule type="cellIs" dxfId="165" priority="49" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="172" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O58">
-    <cfRule type="cellIs" dxfId="164" priority="48" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="171" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O67">
-    <cfRule type="cellIs" dxfId="163" priority="47" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="170" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71">
-    <cfRule type="cellIs" dxfId="162" priority="46" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="169" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72">
-    <cfRule type="cellIs" dxfId="161" priority="45" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="168" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="160" priority="44" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="167" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="159" priority="43" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="166" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="cellIs" dxfId="158" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="165" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="157" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="164" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L75">
-    <cfRule type="cellIs" dxfId="156" priority="39" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="163" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI12">
-    <cfRule type="cellIs" dxfId="155" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="162" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2">
-    <cfRule type="cellIs" dxfId="154" priority="37" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="161" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W86">
-    <cfRule type="cellIs" dxfId="153" priority="36" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="160" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="cellIs" dxfId="152" priority="35" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="159" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
-    <cfRule type="cellIs" dxfId="151" priority="34" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="158" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2">
-    <cfRule type="cellIs" dxfId="150" priority="33" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="157" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y86">
-    <cfRule type="cellIs" dxfId="149" priority="32" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="156" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2">
-    <cfRule type="cellIs" dxfId="148" priority="31" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="155" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="147" priority="30" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="154" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="cellIs" dxfId="146" priority="29" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="153" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="145" priority="28" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="152" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
-    <cfRule type="cellIs" dxfId="30" priority="27" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="151" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA48">
-    <cfRule type="cellIs" dxfId="29" priority="26" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="150" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA11">
-    <cfRule type="cellIs" dxfId="28" priority="25" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="149" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA51">
-    <cfRule type="cellIs" dxfId="27" priority="24" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="148" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA52">
-    <cfRule type="cellIs" dxfId="25" priority="23" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="147" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA53">
-    <cfRule type="cellIs" dxfId="24" priority="22" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="146" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57 AA54:AA55">
-    <cfRule type="cellIs" dxfId="23" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="145" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA20">
-    <cfRule type="cellIs" dxfId="22" priority="20" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="144" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA21">
-    <cfRule type="cellIs" dxfId="21" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="143" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA66">
-    <cfRule type="cellIs" dxfId="20" priority="18" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="142" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA25">
-    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="141" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA26">
-    <cfRule type="cellIs" dxfId="18" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="140" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA28">
-    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="139" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA32">
-    <cfRule type="cellIs" dxfId="16" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="138" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA34">
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="137" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27">
-    <cfRule type="cellIs" dxfId="13" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="136" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA33 AA31">
-    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA61 M61">
-    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="134" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA62">
-    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="133" priority="20" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA63 M63">
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="132" priority="19" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA65">
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="131" priority="18" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA67">
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="130" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA68">
-    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="129" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA70:AA73">
+    <cfRule type="cellIs" dxfId="128" priority="15" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA77">
+    <cfRule type="cellIs" dxfId="127" priority="14" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA74 AA38">
+    <cfRule type="cellIs" dxfId="126" priority="13" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA37">
+    <cfRule type="cellIs" dxfId="125" priority="12" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S9">
+    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S46">
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S48">
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S18">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S54">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S55">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S57">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S76">
     <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA77">
+  <conditionalFormatting sqref="S78">
     <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA74 AA38">
+  <conditionalFormatting sqref="S81">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA37">
+  <conditionalFormatting sqref="S82">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -46567,448 +46618,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="144" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="124" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="143" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="123" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="142" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="122" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="141" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="121" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="140" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="120" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="139" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="119" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="138" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="118" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="137" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="117" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="136" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="116" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="135" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="115" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="134" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="114" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="133" priority="93">
+    <cfRule type="containsBlanks" dxfId="113" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="132" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="112" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="131" priority="91">
+    <cfRule type="containsBlanks" dxfId="111" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="130" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="129" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="128" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="127" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="126" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="125" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="124" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="104" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="123" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="122" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="102" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="121" priority="69">
+    <cfRule type="containsBlanks" dxfId="101" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="100" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="119" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="118" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="117" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="116" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="115" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="114" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="113" priority="63">
+    <cfRule type="containsBlanks" dxfId="93" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="112" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="92" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="111" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="91" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="110" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="90" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="109" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="108" priority="59">
+    <cfRule type="containsBlanks" dxfId="88" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="107" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="87" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="106" priority="56">
+    <cfRule type="containsBlanks" dxfId="86" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="105" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="85" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="104" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="84" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="103" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="83" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="102" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="82" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="101" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="100" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="99" priority="50">
+    <cfRule type="containsBlanks" dxfId="79" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="98" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="78" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="97" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="77" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="96" priority="47">
+    <cfRule type="containsBlanks" dxfId="76" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="95" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="75" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="94" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="74" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="93" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="73" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="92" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="72" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="91" priority="42">
+    <cfRule type="containsBlanks" dxfId="71" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="90" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="70" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="89" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="88" priority="39">
+    <cfRule type="containsBlanks" dxfId="68" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="87" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="67" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="86" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="85" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="65" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="84" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="64" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="83" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="63" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="82" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="62" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="81" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="61" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="80" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="60" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="79" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="59" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="78" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="77" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="57" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="76" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="56" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="75" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="55" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="74" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="54" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="73" priority="23">
+    <cfRule type="containsBlanks" dxfId="53" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="72" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="52" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="71" priority="19">
+    <cfRule type="containsBlanks" dxfId="51" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="50" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="69" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="68" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="48" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="66" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="46" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="65" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="64" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="62" priority="22">
+    <cfRule type="containsBlanks" dxfId="42" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="61" priority="11">
+    <cfRule type="containsBlanks" dxfId="41" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="60" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="40" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="59" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="57" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="56" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="54" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61904,111 +61955,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="50" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="48" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="47" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="46" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="45" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="44" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="43" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="42" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="41" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="40" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="39" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="37" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="36" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="35" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="34" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="33" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -63332,7 +63383,7 @@
       </c>
       <c r="E3" s="68">
         <f ca="1">TODAY()</f>
-        <v>43472</v>
+        <v>43473</v>
       </c>
       <c r="F3" s="67">
         <v>42551</v>
@@ -63642,7 +63693,7 @@
   <dimension ref="B1:Y90"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="7905" activePane="bottomLeft"/>
+      <pane ySplit="7820" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -63683,7 +63734,7 @@
       <c r="F1" s="1"/>
       <c r="I1" s="34">
         <f ca="1">TODAY()</f>
-        <v>43472</v>
+        <v>43473</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -67748,7 +67799,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
update some of record drawings on program level
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCE6E7D-934E-49D1-8DC8-E614B6CE50B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855296D1-CC41-4068-AA5F-F7233E928EC1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8957" uniqueCount="1334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8959" uniqueCount="1336">
   <si>
     <t>#</t>
   </si>
@@ -4047,6 +4047,12 @@
   </si>
   <si>
     <t>building built in 1930's or 1940;s</t>
+  </si>
+  <si>
+    <t>central plant and signage as-builts saved digitally in SP</t>
+  </si>
+  <si>
+    <t>Mesa-031; Restroom as-builts in digital</t>
   </si>
 </sst>
 </file>
@@ -5356,83 +5362,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -6099,6 +6028,83 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9498,8 +9504,8 @@
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="CF6" sqref="CF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9513,57 +9519,60 @@
     <col min="7" max="7" width="1.36328125" style="1" customWidth="1"/>
     <col min="8" max="9" width="3.453125" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="10.1796875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6328125" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.08984375" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.26953125" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="9.7265625" style="2" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="7.26953125" style="2" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="10.81640625" style="2" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="7.26953125" style="2" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="9.08984375" style="2" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="7.26953125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.81640625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.26953125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.81640625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="8.26953125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="8.26953125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.81640625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="8.26953125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="11.81640625" style="2" customWidth="1"/>
-    <col min="31" max="33" width="8" style="1" customWidth="1"/>
-    <col min="34" max="34" width="16.7265625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="8" style="1" customWidth="1"/>
-    <col min="36" max="36" width="16.7265625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="8" style="1" customWidth="1"/>
-    <col min="38" max="38" width="16.7265625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="8" style="1" customWidth="1"/>
-    <col min="40" max="40" width="16.7265625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="2.26953125" style="1" customWidth="1"/>
-    <col min="42" max="42" width="7.26953125" style="1" customWidth="1"/>
-    <col min="43" max="43" width="8" style="1" customWidth="1"/>
-    <col min="44" max="45" width="7.26953125" style="2" customWidth="1"/>
-    <col min="46" max="46" width="2.26953125" style="1" customWidth="1"/>
-    <col min="47" max="49" width="8.81640625" style="1" customWidth="1"/>
-    <col min="50" max="52" width="7.26953125" style="1" customWidth="1"/>
-    <col min="53" max="54" width="8.81640625" style="1" customWidth="1"/>
-    <col min="55" max="57" width="8.26953125" style="1" customWidth="1"/>
-    <col min="58" max="59" width="9.26953125" style="1" customWidth="1"/>
-    <col min="60" max="67" width="7.26953125" style="1" customWidth="1"/>
-    <col min="68" max="68" width="9.81640625" style="1" customWidth="1"/>
-    <col min="69" max="69" width="3" style="1" customWidth="1"/>
-    <col min="70" max="70" width="8.7265625" style="1"/>
-    <col min="71" max="71" width="9.26953125" style="1" customWidth="1"/>
-    <col min="72" max="72" width="2.7265625" style="1" customWidth="1"/>
-    <col min="73" max="73" width="8.1796875" style="1" customWidth="1"/>
-    <col min="74" max="74" width="7.7265625" style="1" customWidth="1"/>
-    <col min="75" max="75" width="4.54296875" style="1" customWidth="1"/>
-    <col min="76" max="76" width="3" style="1" customWidth="1"/>
-    <col min="78" max="78" width="6.26953125" style="1" customWidth="1"/>
-    <col min="80" max="81" width="7.26953125" style="1" customWidth="1"/>
-    <col min="82" max="82" width="7.26953125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="10.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="10.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="8.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="11.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="8.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="11.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="8.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="11.81640625" style="2" hidden="1" customWidth="1"/>
+    <col min="31" max="33" width="8" style="1" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="16.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="8" style="1" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="16.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="8" style="1" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="16.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="8" style="1" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="16.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="2.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="8" style="1" hidden="1" customWidth="1"/>
+    <col min="44" max="45" width="7.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="2.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="47" max="49" width="8.81640625" style="1" hidden="1" customWidth="1"/>
+    <col min="50" max="52" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="53" max="54" width="8.81640625" style="1" hidden="1" customWidth="1"/>
+    <col min="55" max="57" width="8.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="58" max="59" width="9.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="60" max="67" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="9.81640625" style="1" hidden="1" customWidth="1"/>
+    <col min="69" max="69" width="3" style="1" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="9.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="2.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="73" max="73" width="8.1796875" style="1" hidden="1" customWidth="1"/>
+    <col min="74" max="74" width="7.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="75" max="75" width="4.54296875" style="1" hidden="1" customWidth="1"/>
+    <col min="76" max="76" width="3" style="1" hidden="1" customWidth="1"/>
+    <col min="77" max="77" width="0" hidden="1" customWidth="1"/>
+    <col min="78" max="78" width="6.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="79" max="79" width="0" hidden="1" customWidth="1"/>
+    <col min="80" max="81" width="7.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="82" max="82" width="7.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="83" max="83" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:82" s="33" customFormat="1" ht="38" x14ac:dyDescent="0.25">
@@ -9821,8 +9830,8 @@
       <c r="J2" s="145" t="s">
         <v>418</v>
       </c>
-      <c r="K2" s="144" t="s">
-        <v>567</v>
+      <c r="K2" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L2" s="60" t="s">
         <v>484</v>
@@ -9992,8 +10001,8 @@
       <c r="J3" s="145" t="s">
         <v>418</v>
       </c>
-      <c r="K3" s="144" t="s">
-        <v>567</v>
+      <c r="K3" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L3" s="60" t="s">
         <v>484</v>
@@ -10334,8 +10343,8 @@
       <c r="J5" s="145" t="s">
         <v>419</v>
       </c>
-      <c r="K5" s="144" t="s">
-        <v>567</v>
+      <c r="K5" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L5" s="60" t="s">
         <v>494</v>
@@ -10505,8 +10514,8 @@
       <c r="J6" s="144" t="s">
         <v>419</v>
       </c>
-      <c r="K6" s="144" t="s">
-        <v>567</v>
+      <c r="K6" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L6" s="60" t="s">
         <v>491</v>
@@ -11034,8 +11043,8 @@
       <c r="J9" s="144" t="s">
         <v>419</v>
       </c>
-      <c r="K9" s="144" t="s">
-        <v>567</v>
+      <c r="K9" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L9" s="60" t="s">
         <v>495</v>
@@ -11714,8 +11723,8 @@
       <c r="J13" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="144" t="s">
-        <v>567</v>
+      <c r="K13" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L13" s="60" t="s">
         <v>490</v>
@@ -11885,8 +11894,8 @@
       <c r="J14" s="144" t="s">
         <v>419</v>
       </c>
-      <c r="K14" s="144" t="s">
-        <v>567</v>
+      <c r="K14" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L14" s="19"/>
       <c r="M14" s="56" t="s">
@@ -12219,7 +12228,7 @@
         <v>567</v>
       </c>
       <c r="L16" s="60" t="s">
-        <v>501</v>
+        <v>1335</v>
       </c>
       <c r="M16" s="60" t="s">
         <v>166</v>
@@ -12388,8 +12397,8 @@
       <c r="J17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="144" t="s">
-        <v>567</v>
+      <c r="K17" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L17" s="19"/>
       <c r="M17" s="144" t="s">
@@ -12555,8 +12564,8 @@
       <c r="J18" s="144" t="s">
         <v>1140</v>
       </c>
-      <c r="K18" s="144" t="s">
-        <v>567</v>
+      <c r="K18" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="56" t="s">
@@ -12726,8 +12735,8 @@
       <c r="J19" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="144" t="s">
-        <v>567</v>
+      <c r="K19" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="144" t="s">
@@ -16465,7 +16474,9 @@
       <c r="K41" s="144" t="s">
         <v>567</v>
       </c>
-      <c r="L41" s="19"/>
+      <c r="L41" s="19" t="s">
+        <v>1334</v>
+      </c>
       <c r="M41" s="144" t="s">
         <v>567</v>
       </c>
@@ -18006,7 +18017,7 @@
       <c r="K50" s="180" t="s">
         <v>1112</v>
       </c>
-      <c r="L50" s="25" t="s">
+      <c r="L50" s="19" t="s">
         <v>1146</v>
       </c>
       <c r="M50" s="60" t="s">
@@ -18180,7 +18191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>4</v>
       </c>
@@ -18206,10 +18217,12 @@
       <c r="J51" s="144" t="s">
         <v>418</v>
       </c>
-      <c r="K51" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="L51" s="19"/>
+      <c r="K51" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="L51" s="19" t="s">
+        <v>1146</v>
+      </c>
       <c r="M51" s="60" t="s">
         <v>166</v>
       </c>
@@ -18373,8 +18386,8 @@
       <c r="J52" s="144" t="s">
         <v>418</v>
       </c>
-      <c r="K52" s="144" t="s">
-        <v>567</v>
+      <c r="K52" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L52" s="60" t="s">
         <v>481</v>
@@ -18546,8 +18559,8 @@
       <c r="J53" s="144" t="s">
         <v>1140</v>
       </c>
-      <c r="K53" s="144" t="s">
-        <v>567</v>
+      <c r="K53" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L53" s="19"/>
       <c r="M53" s="144" t="s">
@@ -18711,8 +18724,8 @@
       <c r="J54" s="144" t="s">
         <v>1229</v>
       </c>
-      <c r="K54" s="144" t="s">
-        <v>567</v>
+      <c r="K54" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L54" s="19"/>
       <c r="M54" s="144" t="s">
@@ -18890,8 +18903,8 @@
       <c r="J55" s="144" t="s">
         <v>1229</v>
       </c>
-      <c r="K55" s="144" t="s">
-        <v>567</v>
+      <c r="K55" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L55" s="19"/>
       <c r="M55" s="144" t="s">
@@ -19055,8 +19068,8 @@
       <c r="J56" s="144" t="s">
         <v>418</v>
       </c>
-      <c r="K56" s="144" t="s">
-        <v>567</v>
+      <c r="K56" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L56" s="60" t="s">
         <v>482</v>
@@ -19224,8 +19237,8 @@
       <c r="J57" s="144" t="s">
         <v>1229</v>
       </c>
-      <c r="K57" s="144" t="s">
-        <v>567</v>
+      <c r="K57" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L57" s="19"/>
       <c r="M57" s="144" t="s">
@@ -19389,8 +19402,8 @@
       <c r="J58" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K58" s="144" t="s">
-        <v>567</v>
+      <c r="K58" s="179" t="s">
+        <v>1116</v>
       </c>
       <c r="L58" s="25"/>
       <c r="M58" s="144" t="s">
@@ -19759,8 +19772,8 @@
       <c r="J60" s="144" t="s">
         <v>419</v>
       </c>
-      <c r="K60" s="144" t="s">
-        <v>567</v>
+      <c r="K60" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="L60" s="19"/>
       <c r="M60" s="60" t="s">
@@ -24578,7 +24591,7 @@
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:K58 K2:K38 K60:K61 K41:K44 K63:K74 K76:K82">
+  <conditionalFormatting sqref="K41:K44 K63:K74 K76:K82 K20:K38 K46:K57 K60:K61 K2:K18">
     <cfRule type="cellIs" dxfId="310" priority="206" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -25695,67 +25708,67 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S46">
-    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S48">
-    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S18">
-    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54">
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S55">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S57">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S76">
-    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S78">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S81">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S82">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -46618,448 +46631,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="124" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="123" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="122" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="121" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="120" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="119" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="118" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="117" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="116" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="115" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="114" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="113" priority="93">
+    <cfRule type="containsBlanks" dxfId="102" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="112" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="111" priority="91">
+    <cfRule type="containsBlanks" dxfId="100" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="110" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="109" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="108" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="107" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="106" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="105" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="104" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="103" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="102" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="101" priority="69">
+    <cfRule type="containsBlanks" dxfId="90" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="99" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="98" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="97" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="96" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="95" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="94" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="93" priority="63">
+    <cfRule type="containsBlanks" dxfId="82" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="92" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="91" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="90" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="89" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="88" priority="59">
+    <cfRule type="containsBlanks" dxfId="77" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="87" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="86" priority="56">
+    <cfRule type="containsBlanks" dxfId="75" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="85" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="84" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="83" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="82" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="81" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="80" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="79" priority="50">
+    <cfRule type="containsBlanks" dxfId="68" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="78" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="77" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="76" priority="47">
+    <cfRule type="containsBlanks" dxfId="65" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="75" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="74" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="73" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="72" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="71" priority="42">
+    <cfRule type="containsBlanks" dxfId="60" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="70" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="69" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="68" priority="39">
+    <cfRule type="containsBlanks" dxfId="57" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="67" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="66" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="65" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="64" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="63" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="62" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="61" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="60" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="59" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="58" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="57" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="56" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="55" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="54" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="53" priority="23">
+    <cfRule type="containsBlanks" dxfId="42" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="52" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="51" priority="19">
+    <cfRule type="containsBlanks" dxfId="40" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="49" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="48" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="47" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="46" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="45" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="43" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="42" priority="22">
+    <cfRule type="containsBlanks" dxfId="31" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="41" priority="11">
+    <cfRule type="containsBlanks" dxfId="30" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="40" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="37" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61955,111 +61968,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="30" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="28" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="27" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="26" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="25" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="24" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="23" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="22" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="21" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="20" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="19" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="18" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="15" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="13" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -67799,7 +67812,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
dsa approved mesa facilities support
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9570A7-2537-409D-A5CA-1E0B18250EDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45A4C33-24A4-49F0-8AA2-C51139197B31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32770" yWindow="32770" windowWidth="20520" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8959" uniqueCount="1340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8966" uniqueCount="1342">
   <si>
     <t>#</t>
   </si>
@@ -4046,9 +4046,6 @@
     <t>04-111402; 04-114653</t>
   </si>
   <si>
-    <t>04-113884 (final DSA invoice being routed in SDCCD 1/9/19)</t>
-  </si>
-  <si>
     <t>04-103471 (1/9/19 pending $500 reopen fee and final invoice payment)</t>
   </si>
   <si>
@@ -4065,6 +4062,15 @@
   </si>
   <si>
     <t>Certified (still "no" 1/9/19)</t>
+  </si>
+  <si>
+    <t>digital files on SP of M and E only; confirm hardcopy location</t>
+  </si>
+  <si>
+    <t>only MEPF on SP digital; no A etc</t>
+  </si>
+  <si>
+    <t>04-113884</t>
   </si>
 </sst>
 </file>
@@ -5244,14 +5250,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="325">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="329">
     <dxf>
       <fill>
         <patternFill>
@@ -7520,6 +7519,41 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7766,7 +7800,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1/9/2019</c:v>
+                  <c:v>2/8/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9524,7 +9558,7 @@
   <dimension ref="B1:CD101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9848,7 +9882,7 @@
         <v>170</v>
       </c>
       <c r="J2" s="145" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="K2" s="56" t="s">
         <v>170</v>
@@ -10019,7 +10053,7 @@
         <v>170</v>
       </c>
       <c r="J3" s="145" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="K3" s="56" t="s">
         <v>170</v>
@@ -11912,7 +11946,7 @@
         <v>170</v>
       </c>
       <c r="J14" s="144" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="K14" s="56" t="s">
         <v>170</v>
@@ -12558,7 +12592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>86</v>
       </c>
@@ -12729,7 +12763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>86</v>
       </c>
@@ -12920,10 +12954,12 @@
       <c r="J20" s="144" t="s">
         <v>420</v>
       </c>
-      <c r="K20" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="L20" s="19"/>
+      <c r="K20" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>1142</v>
+      </c>
       <c r="M20" s="60" t="s">
         <v>166</v>
       </c>
@@ -13091,10 +13127,12 @@
       <c r="J21" s="144" t="s">
         <v>419</v>
       </c>
-      <c r="K21" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="L21" s="19"/>
+      <c r="K21" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>1142</v>
+      </c>
       <c r="M21" s="60" t="s">
         <v>166</v>
       </c>
@@ -13238,7 +13276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B22" s="19" t="s">
         <v>86</v>
       </c>
@@ -13564,7 +13602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
         <v>86</v>
       </c>
@@ -13590,8 +13628,8 @@
       <c r="J24" s="144" t="s">
         <v>419</v>
       </c>
-      <c r="K24" s="144" t="s">
-        <v>567</v>
+      <c r="K24" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="L24" s="60" t="s">
         <v>499</v>
@@ -13759,7 +13797,7 @@
         <v>170</v>
       </c>
       <c r="J25" s="144" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="K25" s="144" t="s">
         <v>567</v>
@@ -13906,7 +13944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
         <v>86</v>
       </c>
@@ -13932,10 +13970,12 @@
       <c r="J26" s="144" t="s">
         <v>419</v>
       </c>
-      <c r="K26" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="L26" s="19"/>
+      <c r="K26" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="L26" s="19" t="s">
+        <v>1340</v>
+      </c>
       <c r="M26" s="56" t="s">
         <v>170</v>
       </c>
@@ -14099,10 +14139,12 @@
       <c r="J27" s="144" t="s">
         <v>418</v>
       </c>
-      <c r="K27" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="L27" s="19"/>
+      <c r="K27" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="L27" s="19" t="s">
+        <v>1142</v>
+      </c>
       <c r="M27" s="60" t="s">
         <v>166</v>
       </c>
@@ -14584,7 +14626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B30" s="19" t="s">
         <v>86</v>
       </c>
@@ -14755,7 +14797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B31" s="19" t="s">
         <v>86</v>
       </c>
@@ -14942,7 +14984,7 @@
         <v>170</v>
       </c>
       <c r="J32" s="144" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="K32" s="144" t="s">
         <v>567</v>
@@ -15087,7 +15129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B33" s="19" t="s">
         <v>86</v>
       </c>
@@ -15445,7 +15487,7 @@
         <v>170</v>
       </c>
       <c r="J35" s="145" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="K35" s="144" t="s">
         <v>567</v>
@@ -15610,7 +15652,7 @@
         <v>170</v>
       </c>
       <c r="J36" s="144" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="K36" s="144" t="s">
         <v>567</v>
@@ -15918,7 +15960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
         <v>86</v>
       </c>
@@ -16087,7 +16129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
         <v>86</v>
       </c>
@@ -16278,7 +16320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B40" s="19" t="s">
         <v>86</v>
       </c>
@@ -16485,7 +16527,7 @@
         <v>170</v>
       </c>
       <c r="H41" s="144" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="I41" s="144" t="s">
         <v>567</v>
@@ -16630,7 +16672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B42" s="19" t="s">
         <v>86</v>
       </c>
@@ -16992,7 +17034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B44" s="19" t="s">
         <v>4</v>
       </c>
@@ -17503,7 +17545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B47" s="19" t="s">
         <v>4</v>
       </c>
@@ -17843,7 +17885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>4</v>
       </c>
@@ -18380,7 +18422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:82" s="24" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:82" s="24" customFormat="1" ht="32" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
         <v>4</v>
       </c>
@@ -18553,7 +18595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:82" s="24" customFormat="1" ht="32" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>4</v>
       </c>
@@ -18567,11 +18609,11 @@
       <c r="F53" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G53" s="56" t="s">
-        <v>170</v>
-      </c>
-      <c r="H53" s="144" t="s">
-        <v>1333</v>
+      <c r="G53" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="H53" s="184" t="s">
+        <v>1341</v>
       </c>
       <c r="I53" s="179" t="s">
         <v>1116</v>
@@ -18718,7 +18760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>4</v>
       </c>
@@ -18897,7 +18939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>4</v>
       </c>
@@ -19231,7 +19273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B57" s="19" t="s">
         <v>4</v>
       </c>
@@ -19396,7 +19438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B58" s="19" t="s">
         <v>4</v>
       </c>
@@ -19595,7 +19637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B59" s="19" t="s">
         <v>4</v>
       </c>
@@ -19766,7 +19808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B60" s="19" t="s">
         <v>4</v>
       </c>
@@ -19929,7 +19971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B61" s="19" t="s">
         <v>4</v>
       </c>
@@ -19955,10 +19997,12 @@
       <c r="J61" s="144" t="s">
         <v>1135</v>
       </c>
-      <c r="K61" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="L61" s="19"/>
+      <c r="K61" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="L61" s="19" t="s">
+        <v>1308</v>
+      </c>
       <c r="M61" s="179" t="s">
         <v>1116</v>
       </c>
@@ -20261,7 +20305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B63" s="19" t="s">
         <v>4</v>
       </c>
@@ -20418,7 +20462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B64" s="19" t="s">
         <v>4</v>
       </c>
@@ -20444,10 +20488,12 @@
       <c r="J64" s="144" t="s">
         <v>1137</v>
       </c>
-      <c r="K64" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="L64" s="19"/>
+      <c r="K64" s="179" t="s">
+        <v>1116</v>
+      </c>
+      <c r="L64" s="19" t="s">
+        <v>1310</v>
+      </c>
       <c r="M64" s="179" t="s">
         <v>1116</v>
       </c>
@@ -20587,7 +20633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B65" s="19" t="s">
         <v>4</v>
       </c>
@@ -20613,8 +20659,8 @@
       <c r="J65" s="144" t="s">
         <v>420</v>
       </c>
-      <c r="K65" s="144" t="s">
-        <v>567</v>
+      <c r="K65" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="L65" s="60" t="s">
         <v>498</v>
@@ -20776,7 +20822,7 @@
         <v>170</v>
       </c>
       <c r="H66" s="144" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="I66" s="179" t="s">
         <v>1116</v>
@@ -20784,8 +20830,8 @@
       <c r="J66" s="144" t="s">
         <v>1225</v>
       </c>
-      <c r="K66" s="144" t="s">
-        <v>567</v>
+      <c r="K66" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="L66" s="60" t="s">
         <v>486</v>
@@ -20929,7 +20975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:82" s="24" customFormat="1" ht="32" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
         <v>4</v>
       </c>
@@ -20955,10 +21001,12 @@
       <c r="J67" s="144" t="s">
         <v>1225</v>
       </c>
-      <c r="K67" s="144" t="s">
-        <v>567</v>
-      </c>
-      <c r="L67" s="19"/>
+      <c r="K67" s="180" t="s">
+        <v>1112</v>
+      </c>
+      <c r="L67" s="19" t="s">
+        <v>1339</v>
+      </c>
       <c r="M67" s="144" t="s">
         <v>567</v>
       </c>
@@ -21094,7 +21142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B68" s="19" t="s">
         <v>4</v>
       </c>
@@ -21267,7 +21315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B69" s="19" t="s">
         <v>4</v>
       </c>
@@ -21432,7 +21480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B70" s="19" t="s">
         <v>4</v>
       </c>
@@ -21927,7 +21975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B73" s="19" t="s">
         <v>4</v>
       </c>
@@ -22092,7 +22140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B74" s="19" t="s">
         <v>4</v>
       </c>
@@ -22293,7 +22341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B75" s="19" t="s">
         <v>4</v>
       </c>
@@ -22667,7 +22715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:82" s="24" customFormat="1" ht="64" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B77" s="19" t="s">
         <v>4</v>
       </c>
@@ -22836,7 +22884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="B78" s="19" t="s">
         <v>4</v>
       </c>
@@ -23202,7 +23250,7 @@
         <v>170</v>
       </c>
       <c r="H80" s="144" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="I80" s="179" t="s">
         <v>1116</v>
@@ -23353,7 +23401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B81" s="19" t="s">
         <v>4</v>
       </c>
@@ -23747,7 +23795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B83" s="19" t="s">
         <v>4</v>
       </c>
@@ -24131,7 +24179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B85" s="19" t="s">
         <v>4</v>
       </c>
@@ -24324,7 +24372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
       <c r="B86" s="19" t="s">
         <v>4</v>
       </c>
@@ -24534,1267 +24582,1291 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
-    <cfRule type="cellIs" dxfId="324" priority="257" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="328" priority="261" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI9:BJ9">
-    <cfRule type="cellIs" dxfId="323" priority="256" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="327" priority="260" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="322" priority="255" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="326" priority="259" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="321" priority="254" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="325" priority="258" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
-    <cfRule type="cellIs" dxfId="320" priority="252" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="324" priority="256" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="319" priority="251" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="323" priority="255" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="318" priority="250" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="322" priority="254" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="317" priority="246" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="321" priority="250" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="316" priority="236" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="320" priority="240" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I4 I7:I8 I12 I44 I14:I15 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="315" priority="223" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="319" priority="227" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="314" priority="212" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="318" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
+    <cfRule type="cellIs" dxfId="317" priority="213" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CD2">
+    <cfRule type="cellIs" dxfId="316" priority="212" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K41:K44 K63 K76:K82 K22:K23 K46:K57 K60 K2:K18 K68:K74 K25 K28:K38">
+    <cfRule type="cellIs" dxfId="315" priority="211" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J8:J12 J38:J40 J18 J33:J34 J46:J74 J2:J5 J20:J29 J36">
+    <cfRule type="cellIs" dxfId="314" priority="210" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L8:L12 L76:L85 L2:L5 L46:L61 L63:L66 L14:L26 L68:L74 L28:L29">
     <cfRule type="cellIs" dxfId="313" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CD2">
+  <conditionalFormatting sqref="I35">
     <cfRule type="cellIs" dxfId="312" priority="208" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K44 K63:K74 K76:K82 K20:K38 K46:K57 K60:K61 K2:K18">
-    <cfRule type="cellIs" dxfId="311" priority="207" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J8:J12 J38:J40 J18 J33:J34 J46:J74 J2:J5 J20:J29 J36">
-    <cfRule type="cellIs" dxfId="310" priority="206" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L8:L12 L76:L85 L14:L29 L2:L5 L46:L61 L63:L74">
-    <cfRule type="cellIs" dxfId="309" priority="205" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="308" priority="204" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="307" priority="201" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="311" priority="205" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="306" priority="200" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="310" priority="204" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="305" priority="198" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="309" priority="202" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="304" priority="196" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="308" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
+    <cfRule type="cellIs" dxfId="307" priority="198" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+    <cfRule type="cellIs" dxfId="306" priority="197" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q86">
+    <cfRule type="cellIs" dxfId="305" priority="196" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4 S6:S8 S50 S44 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
+    <cfRule type="cellIs" dxfId="304" priority="195" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2:AE86">
     <cfRule type="cellIs" dxfId="303" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+  <conditionalFormatting sqref="AG2:AG86">
     <cfRule type="cellIs" dxfId="302" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q86">
+  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
     <cfRule type="cellIs" dxfId="301" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4 S6:S8 S50 S44 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
+  <conditionalFormatting sqref="AK2:AK86">
     <cfRule type="cellIs" dxfId="300" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE86">
+  <conditionalFormatting sqref="AM2:AM86">
     <cfRule type="cellIs" dxfId="299" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG86">
+  <conditionalFormatting sqref="N46">
     <cfRule type="cellIs" dxfId="298" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
+  <conditionalFormatting sqref="N9">
     <cfRule type="cellIs" dxfId="297" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK86">
+  <conditionalFormatting sqref="N6">
     <cfRule type="cellIs" dxfId="296" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AM86">
+  <conditionalFormatting sqref="N48">
     <cfRule type="cellIs" dxfId="295" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46">
+  <conditionalFormatting sqref="N45">
     <cfRule type="cellIs" dxfId="294" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9">
+  <conditionalFormatting sqref="N50">
     <cfRule type="cellIs" dxfId="293" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6">
+  <conditionalFormatting sqref="N5">
     <cfRule type="cellIs" dxfId="292" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N48">
+  <conditionalFormatting sqref="N2">
     <cfRule type="cellIs" dxfId="291" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N45">
+  <conditionalFormatting sqref="N3">
     <cfRule type="cellIs" dxfId="290" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N10">
     <cfRule type="cellIs" dxfId="289" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
+  <conditionalFormatting sqref="M4">
     <cfRule type="cellIs" dxfId="288" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
+  <conditionalFormatting sqref="M7">
     <cfRule type="cellIs" dxfId="287" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
+  <conditionalFormatting sqref="M8">
     <cfRule type="cellIs" dxfId="286" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10">
+  <conditionalFormatting sqref="N52">
     <cfRule type="cellIs" dxfId="285" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4">
+  <conditionalFormatting sqref="N16">
     <cfRule type="cellIs" dxfId="284" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7">
+  <conditionalFormatting sqref="N60">
     <cfRule type="cellIs" dxfId="283" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
+  <conditionalFormatting sqref="M14:N14">
     <cfRule type="cellIs" dxfId="282" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
+  <conditionalFormatting sqref="M34">
     <cfRule type="cellIs" dxfId="281" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
+  <conditionalFormatting sqref="N26">
     <cfRule type="cellIs" dxfId="280" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N60">
+  <conditionalFormatting sqref="M26">
     <cfRule type="cellIs" dxfId="279" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:N14">
+  <conditionalFormatting sqref="N28">
     <cfRule type="cellIs" dxfId="278" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M34">
+  <conditionalFormatting sqref="M68">
     <cfRule type="cellIs" dxfId="277" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
+  <conditionalFormatting sqref="AJ43">
     <cfRule type="cellIs" dxfId="276" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
+  <conditionalFormatting sqref="AI43">
     <cfRule type="cellIs" dxfId="275" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
+  <conditionalFormatting sqref="AJ3">
     <cfRule type="cellIs" dxfId="274" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M68">
+  <conditionalFormatting sqref="AI3">
     <cfRule type="cellIs" dxfId="273" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ43">
+  <conditionalFormatting sqref="AJ4">
     <cfRule type="cellIs" dxfId="272" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI43">
+  <conditionalFormatting sqref="AI4">
     <cfRule type="cellIs" dxfId="271" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ3">
+  <conditionalFormatting sqref="AJ5">
     <cfRule type="cellIs" dxfId="270" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI3">
+  <conditionalFormatting sqref="AI5">
     <cfRule type="cellIs" dxfId="269" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ4">
+  <conditionalFormatting sqref="AJ6">
     <cfRule type="cellIs" dxfId="268" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI4">
+  <conditionalFormatting sqref="AI6">
     <cfRule type="cellIs" dxfId="267" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ5">
+  <conditionalFormatting sqref="AJ7">
     <cfRule type="cellIs" dxfId="266" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI5">
+  <conditionalFormatting sqref="AI7">
     <cfRule type="cellIs" dxfId="265" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ6">
+  <conditionalFormatting sqref="AJ8:AJ9">
     <cfRule type="cellIs" dxfId="264" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI6">
+  <conditionalFormatting sqref="AI8">
     <cfRule type="cellIs" dxfId="263" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ7">
+  <conditionalFormatting sqref="AJ46">
     <cfRule type="cellIs" dxfId="262" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI7">
+  <conditionalFormatting sqref="AI46">
     <cfRule type="cellIs" dxfId="261" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ8:AJ9">
+  <conditionalFormatting sqref="AJ47">
     <cfRule type="cellIs" dxfId="260" priority="151" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI8">
+  <conditionalFormatting sqref="AI47">
     <cfRule type="cellIs" dxfId="259" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ46">
+  <conditionalFormatting sqref="AJ10">
     <cfRule type="cellIs" dxfId="258" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI46">
+  <conditionalFormatting sqref="AI10">
     <cfRule type="cellIs" dxfId="257" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ47">
+  <conditionalFormatting sqref="AJ48">
     <cfRule type="cellIs" dxfId="256" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI47">
+  <conditionalFormatting sqref="AI48">
     <cfRule type="cellIs" dxfId="255" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ10">
+  <conditionalFormatting sqref="AJ49">
     <cfRule type="cellIs" dxfId="254" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI10">
+  <conditionalFormatting sqref="AI49">
     <cfRule type="cellIs" dxfId="253" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ48">
+  <conditionalFormatting sqref="AJ50">
     <cfRule type="cellIs" dxfId="252" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI48">
-    <cfRule type="cellIs" dxfId="251" priority="142" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI50">
+    <cfRule type="cellIs" dxfId="251" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ49">
-    <cfRule type="cellIs" dxfId="250" priority="141" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ11:AJ13">
+    <cfRule type="cellIs" dxfId="250" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="249" priority="140" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI11">
+    <cfRule type="cellIs" dxfId="249" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="248" priority="139" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ51">
+    <cfRule type="cellIs" dxfId="248" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI50">
+  <conditionalFormatting sqref="AI52">
     <cfRule type="cellIs" dxfId="247" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11:AJ13">
+  <conditionalFormatting sqref="AJ52:AJ54">
     <cfRule type="cellIs" dxfId="246" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI11">
+  <conditionalFormatting sqref="AJ56">
     <cfRule type="cellIs" dxfId="245" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ51">
+  <conditionalFormatting sqref="AI56">
     <cfRule type="cellIs" dxfId="244" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI52">
+  <conditionalFormatting sqref="AJ57:AJ58">
     <cfRule type="cellIs" dxfId="243" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ52:AJ54">
+  <conditionalFormatting sqref="AI57:AI58">
     <cfRule type="cellIs" dxfId="242" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ56">
+  <conditionalFormatting sqref="AJ15:AJ16">
     <cfRule type="cellIs" dxfId="241" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI56">
+  <conditionalFormatting sqref="AI15:AI16">
     <cfRule type="cellIs" dxfId="240" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ57:AJ58">
+  <conditionalFormatting sqref="AJ59:AJ60">
     <cfRule type="cellIs" dxfId="239" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI57:AI58">
+  <conditionalFormatting sqref="AJ55">
     <cfRule type="cellIs" dxfId="238" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15:AJ16">
+  <conditionalFormatting sqref="AI19">
     <cfRule type="cellIs" dxfId="237" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI15:AI16">
+  <conditionalFormatting sqref="AJ19">
     <cfRule type="cellIs" dxfId="236" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ59:AJ60">
+  <conditionalFormatting sqref="AI18">
     <cfRule type="cellIs" dxfId="235" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ55">
+  <conditionalFormatting sqref="AJ18">
     <cfRule type="cellIs" dxfId="234" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI19">
+  <conditionalFormatting sqref="AI17">
     <cfRule type="cellIs" dxfId="233" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19">
+  <conditionalFormatting sqref="AJ17">
     <cfRule type="cellIs" dxfId="232" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI18">
+  <conditionalFormatting sqref="AI86">
     <cfRule type="cellIs" dxfId="231" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ18">
+  <conditionalFormatting sqref="AI40">
     <cfRule type="cellIs" dxfId="230" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI17">
+  <conditionalFormatting sqref="AJ20">
     <cfRule type="cellIs" dxfId="229" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ17">
+  <conditionalFormatting sqref="AJ62">
     <cfRule type="cellIs" dxfId="228" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI86">
-    <cfRule type="cellIs" dxfId="227" priority="117" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI40">
-    <cfRule type="cellIs" dxfId="226" priority="116" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="225" priority="115" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="224" priority="114" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="223" priority="112" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="227" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
+    <cfRule type="cellIs" dxfId="226" priority="114" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI21">
+    <cfRule type="cellIs" dxfId="225" priority="113" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI64">
+    <cfRule type="cellIs" dxfId="224" priority="112" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI23">
+    <cfRule type="cellIs" dxfId="223" priority="111" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ24">
     <cfRule type="cellIs" dxfId="222" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI21">
+  <conditionalFormatting sqref="AI25">
     <cfRule type="cellIs" dxfId="221" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI64">
+  <conditionalFormatting sqref="AJ25">
     <cfRule type="cellIs" dxfId="220" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI23">
+  <conditionalFormatting sqref="AJ67">
     <cfRule type="cellIs" dxfId="219" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ24">
+  <conditionalFormatting sqref="AI26">
     <cfRule type="cellIs" dxfId="218" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI25">
+  <conditionalFormatting sqref="AJ26:AJ27">
     <cfRule type="cellIs" dxfId="217" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ25">
+  <conditionalFormatting sqref="AI28:AI30">
     <cfRule type="cellIs" dxfId="216" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ67">
+  <conditionalFormatting sqref="AJ28:AJ31">
     <cfRule type="cellIs" dxfId="215" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI26">
+  <conditionalFormatting sqref="AI72">
     <cfRule type="cellIs" dxfId="214" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ26:AJ27">
+  <conditionalFormatting sqref="AJ72">
     <cfRule type="cellIs" dxfId="213" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI28:AI30">
+  <conditionalFormatting sqref="AI73">
     <cfRule type="cellIs" dxfId="212" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ28:AJ31">
+  <conditionalFormatting sqref="AJ73">
     <cfRule type="cellIs" dxfId="211" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI72">
+  <conditionalFormatting sqref="AI32">
     <cfRule type="cellIs" dxfId="210" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ72">
+  <conditionalFormatting sqref="AJ32">
     <cfRule type="cellIs" dxfId="209" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI73">
+  <conditionalFormatting sqref="AI33">
     <cfRule type="cellIs" dxfId="208" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ73">
+  <conditionalFormatting sqref="AJ33">
     <cfRule type="cellIs" dxfId="207" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI32">
+  <conditionalFormatting sqref="AI34:AI35">
     <cfRule type="cellIs" dxfId="206" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ32">
+  <conditionalFormatting sqref="AJ34:AJ36">
     <cfRule type="cellIs" dxfId="205" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI33">
+  <conditionalFormatting sqref="AI61">
     <cfRule type="cellIs" dxfId="204" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ33">
+  <conditionalFormatting sqref="AI63">
     <cfRule type="cellIs" dxfId="203" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI34:AI35">
+  <conditionalFormatting sqref="AJ70">
     <cfRule type="cellIs" dxfId="202" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ34:AJ36">
+  <conditionalFormatting sqref="AI70">
     <cfRule type="cellIs" dxfId="201" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI61">
+  <conditionalFormatting sqref="AI68">
     <cfRule type="cellIs" dxfId="200" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI63">
+  <conditionalFormatting sqref="AJ76">
     <cfRule type="cellIs" dxfId="199" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ70">
+  <conditionalFormatting sqref="AI76">
     <cfRule type="cellIs" dxfId="198" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI70">
+  <conditionalFormatting sqref="AJ78">
     <cfRule type="cellIs" dxfId="197" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI68">
+  <conditionalFormatting sqref="AI78">
     <cfRule type="cellIs" dxfId="196" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ76">
+  <conditionalFormatting sqref="AJ38">
     <cfRule type="cellIs" dxfId="195" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI76">
+  <conditionalFormatting sqref="AI38">
     <cfRule type="cellIs" dxfId="194" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ78">
+  <conditionalFormatting sqref="AJ77">
     <cfRule type="cellIs" dxfId="193" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI78">
+  <conditionalFormatting sqref="AI77">
     <cfRule type="cellIs" dxfId="192" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ38">
+  <conditionalFormatting sqref="AJ79">
     <cfRule type="cellIs" dxfId="191" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI38">
+  <conditionalFormatting sqref="AI79">
     <cfRule type="cellIs" dxfId="190" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ77">
+  <conditionalFormatting sqref="AJ80">
     <cfRule type="cellIs" dxfId="189" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI77">
+  <conditionalFormatting sqref="AI80">
     <cfRule type="cellIs" dxfId="188" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ79">
+  <conditionalFormatting sqref="AJ81">
     <cfRule type="cellIs" dxfId="187" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI79">
+  <conditionalFormatting sqref="AI81">
     <cfRule type="cellIs" dxfId="186" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ80">
+  <conditionalFormatting sqref="AJ82">
     <cfRule type="cellIs" dxfId="185" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI80">
+  <conditionalFormatting sqref="AI82">
     <cfRule type="cellIs" dxfId="184" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ81">
+  <conditionalFormatting sqref="AI83">
     <cfRule type="cellIs" dxfId="183" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI81">
+  <conditionalFormatting sqref="AI84:AI85">
     <cfRule type="cellIs" dxfId="182" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ82">
+  <conditionalFormatting sqref="AI39">
     <cfRule type="cellIs" dxfId="181" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI82">
+  <conditionalFormatting sqref="J31">
     <cfRule type="cellIs" dxfId="180" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI83">
+  <conditionalFormatting sqref="O61">
     <cfRule type="cellIs" dxfId="179" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI84:AI85">
+  <conditionalFormatting sqref="O54">
     <cfRule type="cellIs" dxfId="178" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI39">
+  <conditionalFormatting sqref="O57">
     <cfRule type="cellIs" dxfId="177" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
+  <conditionalFormatting sqref="O58">
     <cfRule type="cellIs" dxfId="176" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O61">
+  <conditionalFormatting sqref="O67">
     <cfRule type="cellIs" dxfId="175" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O54">
+  <conditionalFormatting sqref="O71">
     <cfRule type="cellIs" dxfId="174" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O57">
+  <conditionalFormatting sqref="O72">
     <cfRule type="cellIs" dxfId="173" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O58">
+  <conditionalFormatting sqref="O80">
     <cfRule type="cellIs" dxfId="172" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O67">
+  <conditionalFormatting sqref="O82">
     <cfRule type="cellIs" dxfId="171" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O71">
+  <conditionalFormatting sqref="K62">
     <cfRule type="cellIs" dxfId="170" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O72">
+  <conditionalFormatting sqref="L62">
     <cfRule type="cellIs" dxfId="169" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="168" priority="56" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L75">
+    <cfRule type="cellIs" dxfId="168" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="167" priority="55" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI12">
+    <cfRule type="cellIs" dxfId="167" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="cellIs" dxfId="166" priority="54" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="X2">
+    <cfRule type="cellIs" dxfId="166" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="165" priority="53" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="W2:W86">
+    <cfRule type="cellIs" dxfId="165" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L75">
+  <conditionalFormatting sqref="AB2">
     <cfRule type="cellIs" dxfId="164" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI12">
+  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
     <cfRule type="cellIs" dxfId="163" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
+  <conditionalFormatting sqref="Z2">
     <cfRule type="cellIs" dxfId="162" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W86">
+  <conditionalFormatting sqref="Y2:Y86">
     <cfRule type="cellIs" dxfId="161" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2">
+  <conditionalFormatting sqref="AD2">
     <cfRule type="cellIs" dxfId="160" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
+  <conditionalFormatting sqref="AC2:AC86">
     <cfRule type="cellIs" dxfId="159" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2">
+  <conditionalFormatting sqref="V2">
     <cfRule type="cellIs" dxfId="158" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y86">
+  <conditionalFormatting sqref="U2:U86">
     <cfRule type="cellIs" dxfId="157" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2">
+  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
     <cfRule type="cellIs" dxfId="156" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC86">
+  <conditionalFormatting sqref="AA48">
     <cfRule type="cellIs" dxfId="155" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2">
+  <conditionalFormatting sqref="AA11">
     <cfRule type="cellIs" dxfId="154" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U86">
+  <conditionalFormatting sqref="AA51">
     <cfRule type="cellIs" dxfId="153" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
+  <conditionalFormatting sqref="AA52">
     <cfRule type="cellIs" dxfId="152" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA48">
+  <conditionalFormatting sqref="AA53">
     <cfRule type="cellIs" dxfId="151" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA11">
+  <conditionalFormatting sqref="AA57 AA54:AA55">
     <cfRule type="cellIs" dxfId="150" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA51">
+  <conditionalFormatting sqref="AA20">
     <cfRule type="cellIs" dxfId="149" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA52">
+  <conditionalFormatting sqref="AA21">
     <cfRule type="cellIs" dxfId="148" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA53">
+  <conditionalFormatting sqref="AA66">
     <cfRule type="cellIs" dxfId="147" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA57 AA54:AA55">
+  <conditionalFormatting sqref="AA25">
     <cfRule type="cellIs" dxfId="146" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA20">
+  <conditionalFormatting sqref="AA26">
     <cfRule type="cellIs" dxfId="145" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA21">
+  <conditionalFormatting sqref="AA28">
     <cfRule type="cellIs" dxfId="144" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA66">
+  <conditionalFormatting sqref="AA32">
     <cfRule type="cellIs" dxfId="143" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA25">
+  <conditionalFormatting sqref="AA34">
     <cfRule type="cellIs" dxfId="142" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA26">
+  <conditionalFormatting sqref="AA27">
     <cfRule type="cellIs" dxfId="141" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA28">
+  <conditionalFormatting sqref="AA33 AA31">
     <cfRule type="cellIs" dxfId="140" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA32">
+  <conditionalFormatting sqref="AA61 M61">
     <cfRule type="cellIs" dxfId="139" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA34">
+  <conditionalFormatting sqref="AA62">
     <cfRule type="cellIs" dxfId="138" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA27">
+  <conditionalFormatting sqref="AA63 M63">
     <cfRule type="cellIs" dxfId="137" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA33 AA31">
+  <conditionalFormatting sqref="AA65">
     <cfRule type="cellIs" dxfId="136" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA61 M61">
+  <conditionalFormatting sqref="AA67">
     <cfRule type="cellIs" dxfId="135" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA62">
+  <conditionalFormatting sqref="AA68">
     <cfRule type="cellIs" dxfId="134" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA63 M63">
+  <conditionalFormatting sqref="AA70:AA73">
     <cfRule type="cellIs" dxfId="133" priority="20" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA65">
+  <conditionalFormatting sqref="AA77">
     <cfRule type="cellIs" dxfId="132" priority="19" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA67">
+  <conditionalFormatting sqref="AA74 AA38">
     <cfRule type="cellIs" dxfId="131" priority="18" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA68">
+  <conditionalFormatting sqref="AA37">
     <cfRule type="cellIs" dxfId="130" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA70:AA73">
+  <conditionalFormatting sqref="S9">
     <cfRule type="cellIs" dxfId="129" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA77">
+  <conditionalFormatting sqref="S46">
     <cfRule type="cellIs" dxfId="128" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA74 AA38">
+  <conditionalFormatting sqref="S48">
     <cfRule type="cellIs" dxfId="127" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA37">
+  <conditionalFormatting sqref="S18">
     <cfRule type="cellIs" dxfId="126" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
+  <conditionalFormatting sqref="S54">
     <cfRule type="cellIs" dxfId="125" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S46">
+  <conditionalFormatting sqref="S55">
     <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48">
+  <conditionalFormatting sqref="S57">
     <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
+  <conditionalFormatting sqref="S76">
     <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S54">
+  <conditionalFormatting sqref="S78">
     <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S55">
+  <conditionalFormatting sqref="S81">
     <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S57">
+  <conditionalFormatting sqref="S82">
     <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S76">
+  <conditionalFormatting sqref="J32">
     <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S78">
+  <conditionalFormatting sqref="K66">
     <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S81">
+  <conditionalFormatting sqref="L67">
     <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S82">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L27">
+    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -46657,448 +46729,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="114" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="113" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="112" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="111" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="110" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="109" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="108" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="107" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="106" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="105" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="104" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="103" priority="93">
+    <cfRule type="containsBlanks" dxfId="102" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="102" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="101" priority="91">
+    <cfRule type="containsBlanks" dxfId="100" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="100" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="99" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="98" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="97" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="96" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="95" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="94" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="93" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="92" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="91" priority="69">
+    <cfRule type="containsBlanks" dxfId="90" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="89" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="88" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="87" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="86" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="85" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="84" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="83" priority="63">
+    <cfRule type="containsBlanks" dxfId="82" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="82" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="81" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="80" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="79" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="78" priority="59">
+    <cfRule type="containsBlanks" dxfId="77" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="77" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="76" priority="56">
+    <cfRule type="containsBlanks" dxfId="75" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="75" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="74" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="73" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="72" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="71" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="70" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="69" priority="50">
+    <cfRule type="containsBlanks" dxfId="68" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="68" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="67" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="66" priority="47">
+    <cfRule type="containsBlanks" dxfId="65" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="65" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="64" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="63" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="62" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="61" priority="42">
+    <cfRule type="containsBlanks" dxfId="60" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="60" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="59" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="58" priority="39">
+    <cfRule type="containsBlanks" dxfId="57" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="57" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="56" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="55" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="53" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="52" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="50" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="49" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="47" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="46" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="44" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="43" priority="23">
+    <cfRule type="containsBlanks" dxfId="42" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="41" priority="19">
+    <cfRule type="containsBlanks" dxfId="40" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="38" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="37" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="34" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="32" priority="22">
+    <cfRule type="containsBlanks" dxfId="31" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="31" priority="11">
+    <cfRule type="containsBlanks" dxfId="30" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61994,111 +62066,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="20" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="18" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="17" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="15" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="14" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="13" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="12" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="10" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -63422,7 +63494,7 @@
       </c>
       <c r="E3" s="68">
         <f ca="1">TODAY()</f>
-        <v>43474</v>
+        <v>43504</v>
       </c>
       <c r="F3" s="67">
         <v>42551</v>
@@ -63732,7 +63804,7 @@
   <dimension ref="B1:Y90"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="7920" activePane="bottomLeft"/>
+      <pane ySplit="7935" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -63773,7 +63845,7 @@
       <c r="F1" s="1"/>
       <c r="I1" s="34">
         <f ca="1">TODAY()</f>
-        <v>43474</v>
+        <v>43504</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -67838,7 +67910,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
dsa cert for city centre seismic
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45A4C33-24A4-49F0-8AA2-C51139197B31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C9D31A-6C73-405D-986F-89E0E5A62F25}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8966" uniqueCount="1342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20710" uniqueCount="1341">
   <si>
     <t>#</t>
   </si>
@@ -4044,9 +4044,6 @@
   </si>
   <si>
     <t>04-111402; 04-114653</t>
-  </si>
-  <si>
-    <t>04-103471 (1/9/19 pending $500 reopen fee and final invoice payment)</t>
   </si>
   <si>
     <t>Certfied: 04-112591, 04-112720, 04-113173; Not Certified: 04-111104/07</t>
@@ -9552,13 +9549,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9858,7 +9855,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="2" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>86</v>
       </c>
@@ -9882,7 +9879,7 @@
         <v>170</v>
       </c>
       <c r="J2" s="145" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="K2" s="56" t="s">
         <v>170</v>
@@ -10029,7 +10026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>86</v>
       </c>
@@ -10053,7 +10050,7 @@
         <v>170</v>
       </c>
       <c r="J3" s="145" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="K3" s="56" t="s">
         <v>170</v>
@@ -10200,7 +10197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>86</v>
       </c>
@@ -10371,7 +10368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>86</v>
       </c>
@@ -10542,7 +10539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>86</v>
       </c>
@@ -10729,7 +10726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>86</v>
       </c>
@@ -10902,7 +10899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
         <v>86</v>
       </c>
@@ -11071,7 +11068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>86</v>
       </c>
@@ -11240,7 +11237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:82" s="24" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:82" s="24" customFormat="1" ht="26.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
         <v>86</v>
       </c>
@@ -11411,7 +11408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
         <v>86</v>
       </c>
@@ -11586,7 +11583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
         <v>86</v>
       </c>
@@ -11751,7 +11748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
         <v>86</v>
       </c>
@@ -11922,7 +11919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
         <v>86</v>
       </c>
@@ -11946,7 +11943,7 @@
         <v>170</v>
       </c>
       <c r="J14" s="144" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="K14" s="56" t="s">
         <v>170</v>
@@ -12085,7 +12082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
         <v>86</v>
       </c>
@@ -12252,7 +12249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:82" s="24" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:82" s="24" customFormat="1" ht="26" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
         <v>86</v>
       </c>
@@ -12425,7 +12422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:82" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:82" s="24" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>86</v>
       </c>
@@ -12592,7 +12589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>86</v>
       </c>
@@ -12763,7 +12760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>86</v>
       </c>
@@ -12928,7 +12925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
         <v>86</v>
       </c>
@@ -13101,7 +13098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="19" t="s">
         <v>86</v>
       </c>
@@ -13276,7 +13273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="19" t="s">
         <v>86</v>
       </c>
@@ -13441,7 +13438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
         <v>86</v>
       </c>
@@ -13602,7 +13599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
         <v>86</v>
       </c>
@@ -13773,7 +13770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
         <v>86</v>
       </c>
@@ -13797,7 +13794,7 @@
         <v>170</v>
       </c>
       <c r="J25" s="144" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="K25" s="144" t="s">
         <v>567</v>
@@ -13944,7 +13941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
         <v>86</v>
       </c>
@@ -13974,7 +13971,7 @@
         <v>170</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="M26" s="56" t="s">
         <v>170</v>
@@ -14113,7 +14110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
         <v>86</v>
       </c>
@@ -14284,7 +14281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
         <v>86</v>
       </c>
@@ -14455,7 +14452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="19" t="s">
         <v>86</v>
       </c>
@@ -14626,7 +14623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="19" t="s">
         <v>86</v>
       </c>
@@ -14797,7 +14794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="19" t="s">
         <v>86</v>
       </c>
@@ -14960,7 +14957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="19" t="s">
         <v>86</v>
       </c>
@@ -14984,7 +14981,7 @@
         <v>170</v>
       </c>
       <c r="J32" s="144" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="K32" s="144" t="s">
         <v>567</v>
@@ -15129,7 +15126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="19" t="s">
         <v>86</v>
       </c>
@@ -15292,7 +15289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="19" t="s">
         <v>86</v>
       </c>
@@ -15463,7 +15460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="19" t="s">
         <v>86</v>
       </c>
@@ -15487,7 +15484,7 @@
         <v>170</v>
       </c>
       <c r="J35" s="145" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="K35" s="144" t="s">
         <v>567</v>
@@ -15628,7 +15625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="19" t="s">
         <v>86</v>
       </c>
@@ -15652,7 +15649,7 @@
         <v>170</v>
       </c>
       <c r="J36" s="144" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="K36" s="144" t="s">
         <v>567</v>
@@ -15799,7 +15796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
         <v>86</v>
       </c>
@@ -15960,7 +15957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
         <v>86</v>
       </c>
@@ -16129,7 +16126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
         <v>86</v>
       </c>
@@ -16320,7 +16317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="19" t="s">
         <v>86</v>
       </c>
@@ -16527,7 +16524,7 @@
         <v>170</v>
       </c>
       <c r="H41" s="144" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="I41" s="144" t="s">
         <v>567</v>
@@ -16833,7 +16830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="19" t="s">
         <v>4</v>
       </c>
@@ -17034,7 +17031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="19" t="s">
         <v>4</v>
       </c>
@@ -17197,7 +17194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="19" t="s">
         <v>4</v>
       </c>
@@ -17374,7 +17371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="19" t="s">
         <v>4</v>
       </c>
@@ -17545,7 +17542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="19" t="s">
         <v>4</v>
       </c>
@@ -17712,7 +17709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="19" t="s">
         <v>4</v>
       </c>
@@ -17885,7 +17882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>4</v>
       </c>
@@ -18050,7 +18047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="19" t="s">
         <v>4</v>
       </c>
@@ -18253,7 +18250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>4</v>
       </c>
@@ -18422,7 +18419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:82" s="24" customFormat="1" ht="32" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:82" s="24" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
         <v>4</v>
       </c>
@@ -18595,7 +18592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>4</v>
       </c>
@@ -18613,7 +18610,7 @@
         <v>166</v>
       </c>
       <c r="H53" s="184" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="I53" s="179" t="s">
         <v>1116</v>
@@ -18760,7 +18757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>4</v>
       </c>
@@ -18939,7 +18936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>4</v>
       </c>
@@ -19104,7 +19101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="19" t="s">
         <v>4</v>
       </c>
@@ -19273,7 +19270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="19" t="s">
         <v>4</v>
       </c>
@@ -19438,7 +19435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="19" t="s">
         <v>4</v>
       </c>
@@ -19637,7 +19634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="19" t="s">
         <v>4</v>
       </c>
@@ -19808,7 +19805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="19" t="s">
         <v>4</v>
       </c>
@@ -19971,7 +19968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="19" t="s">
         <v>4</v>
       </c>
@@ -20136,7 +20133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="19" t="s">
         <v>4</v>
       </c>
@@ -20305,7 +20302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="19" t="s">
         <v>4</v>
       </c>
@@ -20462,7 +20459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="19" t="s">
         <v>4</v>
       </c>
@@ -20822,7 +20819,7 @@
         <v>170</v>
       </c>
       <c r="H66" s="144" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="I66" s="179" t="s">
         <v>1116</v>
@@ -20975,7 +20972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:82" s="24" customFormat="1" ht="32" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:82" s="24" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="19" t="s">
         <v>4</v>
       </c>
@@ -21005,7 +21002,7 @@
         <v>1112</v>
       </c>
       <c r="L67" s="19" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M67" s="144" t="s">
         <v>567</v>
@@ -21142,7 +21139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="19" t="s">
         <v>4</v>
       </c>
@@ -21315,7 +21312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="19" t="s">
         <v>4</v>
       </c>
@@ -21480,7 +21477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="19" t="s">
         <v>4</v>
       </c>
@@ -21645,7 +21642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:82" s="24" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:82" s="24" customFormat="1" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="19" t="s">
         <v>4</v>
       </c>
@@ -21810,7 +21807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:82" s="24" customFormat="1" ht="9.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:82" s="24" customFormat="1" ht="9.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="19" t="s">
         <v>4</v>
       </c>
@@ -21975,7 +21972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="19" t="s">
         <v>4</v>
       </c>
@@ -22140,7 +22137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="19" t="s">
         <v>4</v>
       </c>
@@ -22341,7 +22338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="19" t="s">
         <v>4</v>
       </c>
@@ -22542,7 +22539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="19" t="s">
         <v>4</v>
       </c>
@@ -22715,7 +22712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="19" t="s">
         <v>4</v>
       </c>
@@ -22884,7 +22881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="19" t="s">
         <v>4</v>
       </c>
@@ -23049,7 +23046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:82" s="24" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="19" t="s">
         <v>4</v>
       </c>
@@ -23232,7 +23229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:82" s="24" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:82" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B80" s="19" t="s">
         <v>4</v>
       </c>
@@ -23246,11 +23243,11 @@
       <c r="F80" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G80" s="56" t="s">
-        <v>170</v>
+      <c r="G80" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="H80" s="144" t="s">
-        <v>1333</v>
+        <v>175</v>
       </c>
       <c r="I80" s="179" t="s">
         <v>1116</v>
@@ -23401,7 +23398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="19" t="s">
         <v>4</v>
       </c>
@@ -23598,7 +23595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:82" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:82" s="24" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="19" t="s">
         <v>4</v>
       </c>
@@ -23795,7 +23792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="19" t="s">
         <v>4</v>
       </c>
@@ -23986,7 +23983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:82" s="24" customFormat="1" ht="9.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:82" s="24" customFormat="1" ht="9.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="19" t="s">
         <v>4</v>
       </c>
@@ -24179,7 +24176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="19" t="s">
         <v>4</v>
       </c>
@@ -24372,7 +24369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:82" s="24" customFormat="1" ht="8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:82" s="24" customFormat="1" ht="8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="19" t="s">
         <v>4</v>
       </c>
@@ -24575,7 +24572,13 @@
       <c r="L101" s="181"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:BZ86" xr:uid="{80EDEBF8-D0D6-4190-95E6-3EF458C8A471}"/>
+  <autoFilter ref="B1:BZ86" xr:uid="{80EDEBF8-D0D6-4190-95E6-3EF458C8A471}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="No"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:CA86">
     <sortCondition ref="B2:B86"/>
     <sortCondition ref="D2:D86"/>
@@ -63804,7 +63807,7 @@
   <dimension ref="B1:Y90"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="7935" activePane="bottomLeft"/>
+      <pane ySplit="8025" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>

</xml_diff>

<commit_message>
City ADT buildings DSA certified etc
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EEAC87-FCC7-4C48-8A16-160695164F8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0ECB319-3DA3-4B11-B843-97518106B271}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8980" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20775" uniqueCount="1359">
   <si>
     <t>#</t>
   </si>
@@ -3890,9 +3890,6 @@
     <t>15 photos in SP; 1,346 in IOR SP</t>
   </si>
   <si>
-    <t>MISSING Mechanical &amp; Plumbing in SP</t>
-  </si>
-  <si>
     <t>CE-005</t>
   </si>
   <si>
@@ -4082,9 +4079,6 @@
     <t>04-107524; 04-113290 ("Accepted", although DSA tracker shows a sstill open 2/8/19)</t>
   </si>
   <si>
-    <t>04-114494; also 04-116376 (D Fire Alarm)</t>
-  </si>
-  <si>
     <t>Certfied (04-110878; 04-111010; 04-111216); Not Certified: 04-115435 (Alts to CP)</t>
   </si>
   <si>
@@ -4097,12 +4091,6 @@
     <t>have digital; did not confirm hardcopy yet</t>
   </si>
   <si>
-    <t>&lt;&lt;Appears to be on R Drive &gt;&gt;City-063-067; 083</t>
-  </si>
-  <si>
-    <t>&lt;&lt;appears to be on R drive&gt;&gt; Mesa-024; 030</t>
-  </si>
-  <si>
     <t>&lt;appears to be on R drive&gt;&gt;</t>
   </si>
   <si>
@@ -4118,9 +4106,6 @@
     <t>digital copy in Fac Man SP site; to construct in 2019</t>
   </si>
   <si>
-    <t>dated 12/23/2014</t>
-  </si>
-  <si>
     <t>labor warranties and toilet accessories warranties only on Fac Man SP</t>
   </si>
   <si>
@@ -4128,6 +4113,15 @@
   </si>
   <si>
     <t>combined A-D-T project; did not confirm hardcopy version</t>
+  </si>
+  <si>
+    <t>is digitally in Fac Man SP</t>
+  </si>
+  <si>
+    <t>04-108058; 04-108059; 04-108072; 04-108993; 04-110263</t>
+  </si>
+  <si>
+    <t>04-114494 (Certified); 04-116376 (D Fire Alarm in NOT certified as of 3/4/2019)</t>
   </si>
 </sst>
 </file>
@@ -7865,7 +7859,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/21/2019</c:v>
+                  <c:v>3/4/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9623,7 +9617,7 @@
   <dimension ref="B1:CD101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -9635,7 +9629,7 @@
     <col min="5" max="5" width="6.265625" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="22.06640625" customWidth="1"/>
     <col min="7" max="7" width="4" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="3.46484375" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.19921875" style="1" customWidth="1"/>
     <col min="11" max="11" width="6.59765625" style="1" customWidth="1"/>
@@ -9755,31 +9749,31 @@
         <v>1111</v>
       </c>
       <c r="V1" s="152" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="W1" s="152" t="s">
+        <v>1283</v>
+      </c>
+      <c r="X1" s="152" t="s">
         <v>1284</v>
-      </c>
-      <c r="X1" s="152" t="s">
-        <v>1285</v>
       </c>
       <c r="Y1" s="152" t="s">
         <v>144</v>
       </c>
       <c r="Z1" s="152" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="AA1" s="12" t="s">
         <v>707</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="AC1" s="152" t="s">
         <v>728</v>
       </c>
       <c r="AD1" s="152" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="AE1" s="12" t="s">
         <v>689</v>
@@ -9946,7 +9940,7 @@
         <v>170</v>
       </c>
       <c r="J2" s="119" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="K2" s="52" t="s">
         <v>166</v>
@@ -9986,7 +9980,7 @@
         <v>166</v>
       </c>
       <c r="X2" s="118" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="Y2" s="118" t="s">
         <v>567</v>
@@ -10117,7 +10111,7 @@
         <v>170</v>
       </c>
       <c r="J3" s="119" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="K3" s="52" t="s">
         <v>166</v>
@@ -10147,7 +10141,7 @@
         <v>1112</v>
       </c>
       <c r="T3" s="118" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="U3" s="118" t="s">
         <v>567</v>
@@ -10159,13 +10153,13 @@
         <v>166</v>
       </c>
       <c r="X3" s="118" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="Y3" s="118" t="s">
         <v>567</v>
       </c>
       <c r="Z3" s="118" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="AA3" s="48" t="s">
         <v>170</v>
@@ -10278,11 +10272,11 @@
       <c r="F4" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="48" t="s">
-        <v>170</v>
+      <c r="G4" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H4" s="118" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>567</v>
@@ -10294,7 +10288,7 @@
         <v>166</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>1360</v>
+        <v>1355</v>
       </c>
       <c r="M4" s="13" t="s">
         <v>567</v>
@@ -10318,7 +10312,7 @@
         <v>567</v>
       </c>
       <c r="T4" s="118" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="U4" s="118" t="s">
         <v>567</v>
@@ -10336,13 +10330,13 @@
         <v>567</v>
       </c>
       <c r="Z4" s="118" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="AA4" s="48" t="s">
         <v>170</v>
       </c>
       <c r="AB4" s="118" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AC4" s="118" t="s">
         <v>567</v>
@@ -10455,7 +10449,7 @@
         <v>170</v>
       </c>
       <c r="H5" s="118" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="I5" s="52" t="s">
         <v>166</v>
@@ -10662,7 +10656,7 @@
         <v>170</v>
       </c>
       <c r="T6" s="118" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="U6" s="118" t="s">
         <v>567</v>
@@ -10674,13 +10668,13 @@
         <v>166</v>
       </c>
       <c r="X6" s="118" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="Y6" s="118" t="s">
         <v>567</v>
       </c>
       <c r="Z6" s="118" t="s">
-        <v>1358</v>
+        <v>1353</v>
       </c>
       <c r="AA6" s="52" t="s">
         <v>166</v>
@@ -10696,13 +10690,13 @@
         <v>567</v>
       </c>
       <c r="AF6" s="118" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="AG6" s="52" t="s">
         <v>166</v>
       </c>
       <c r="AH6" s="118" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="AI6" s="48" t="s">
         <v>170</v>
@@ -10811,11 +10805,11 @@
       <c r="F7" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="48" t="s">
-        <v>170</v>
+      <c r="G7" s="146" t="s">
+        <v>1112</v>
       </c>
       <c r="H7" s="118" t="s">
-        <v>1345</v>
+        <v>1358</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>567</v>
@@ -10827,7 +10821,7 @@
         <v>166</v>
       </c>
       <c r="L7" s="52" t="s">
-        <v>1359</v>
+        <v>1354</v>
       </c>
       <c r="M7" s="13" t="s">
         <v>567</v>
@@ -10851,7 +10845,7 @@
         <v>567</v>
       </c>
       <c r="T7" s="118" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="U7" s="118" t="s">
         <v>567</v>
@@ -10875,7 +10869,7 @@
         <v>170</v>
       </c>
       <c r="AB7" s="118" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AC7" s="118" t="s">
         <v>567</v>
@@ -10986,11 +10980,11 @@
       <c r="F8" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="48" t="s">
-        <v>170</v>
+      <c r="G8" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H8" s="118" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>567</v>
@@ -11002,7 +10996,7 @@
         <v>166</v>
       </c>
       <c r="L8" s="52" t="s">
-        <v>1359</v>
+        <v>1354</v>
       </c>
       <c r="M8" s="13" t="s">
         <v>567</v>
@@ -11026,7 +11020,7 @@
         <v>567</v>
       </c>
       <c r="T8" s="118" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="U8" s="118" t="s">
         <v>567</v>
@@ -11050,7 +11044,7 @@
         <v>170</v>
       </c>
       <c r="AB8" s="118" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AC8" s="118" t="s">
         <v>567</v>
@@ -11169,11 +11163,11 @@
       <c r="J9" s="118" t="s">
         <v>419</v>
       </c>
-      <c r="K9" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L9" s="146" t="s">
-        <v>1350</v>
+      <c r="K9" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L9" s="52" t="s">
+        <v>495</v>
       </c>
       <c r="M9" s="52" t="s">
         <v>166</v>
@@ -11197,7 +11191,7 @@
         <v>170</v>
       </c>
       <c r="T9" s="118" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="U9" s="118" t="s">
         <v>567</v>
@@ -11231,10 +11225,12 @@
         <v>567</v>
       </c>
       <c r="AF9" s="118"/>
-      <c r="AG9" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="AH9" s="118"/>
+      <c r="AG9" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH9" s="118" t="s">
+        <v>1356</v>
+      </c>
       <c r="AI9" s="118" t="s">
         <v>567</v>
       </c>
@@ -11330,7 +11326,7 @@
         <v>170</v>
       </c>
       <c r="H10" s="118" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="I10" s="145" t="s">
         <v>1116</v>
@@ -11364,7 +11360,7 @@
         <v>166</v>
       </c>
       <c r="T10" s="118" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="U10" s="118" t="s">
         <v>567</v>
@@ -11509,12 +11505,10 @@
       <c r="J11" s="118" t="s">
         <v>419</v>
       </c>
-      <c r="K11" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>1281</v>
-      </c>
+      <c r="K11" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L11" s="13"/>
       <c r="M11" s="48" t="s">
         <v>170</v>
       </c>
@@ -11559,7 +11553,7 @@
         <v>170</v>
       </c>
       <c r="AB11" s="118" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>567</v>
@@ -11676,7 +11670,7 @@
         <v>170</v>
       </c>
       <c r="H12" s="118" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="I12" s="13" t="s">
         <v>567</v>
@@ -11732,7 +11726,7 @@
         <v>567</v>
       </c>
       <c r="AB12" s="118" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AC12" s="118" t="s">
         <v>567</v>
@@ -11849,11 +11843,11 @@
       <c r="J13" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L13" s="146" t="s">
-        <v>1351</v>
+      <c r="K13" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>490</v>
       </c>
       <c r="M13" s="52" t="s">
         <v>166</v>
@@ -11877,7 +11871,7 @@
         <v>170</v>
       </c>
       <c r="T13" s="118" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="U13" s="118" t="s">
         <v>567</v>
@@ -12018,13 +12012,13 @@
         <v>170</v>
       </c>
       <c r="J14" s="118" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="K14" s="146" t="s">
         <v>1112</v>
       </c>
       <c r="L14" s="146" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="M14" s="48" t="s">
         <v>170</v>
@@ -12177,7 +12171,7 @@
         <v>170</v>
       </c>
       <c r="H15" s="118" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>567</v>
@@ -12211,7 +12205,7 @@
         <v>567</v>
       </c>
       <c r="T15" s="118" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="U15" s="118" t="s">
         <v>567</v>
@@ -12235,7 +12229,7 @@
         <v>567</v>
       </c>
       <c r="AB15" s="118" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AC15" s="118" t="s">
         <v>567</v>
@@ -12356,7 +12350,7 @@
         <v>567</v>
       </c>
       <c r="L16" s="52" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="M16" s="52" t="s">
         <v>166</v>
@@ -12402,7 +12396,7 @@
         <v>567</v>
       </c>
       <c r="AB16" s="118" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="AC16" s="118" t="s">
         <v>567</v>
@@ -12549,7 +12543,7 @@
         <v>1112</v>
       </c>
       <c r="T17" s="118" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="U17" s="118" t="s">
         <v>567</v>
@@ -12718,7 +12712,7 @@
         <v>1112</v>
       </c>
       <c r="T18" s="118" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="U18" s="118" t="s">
         <v>567</v>
@@ -13020,7 +13014,7 @@
         <v>170</v>
       </c>
       <c r="H20" s="118" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="I20" s="52" t="s">
         <v>166</v>
@@ -13056,7 +13050,7 @@
         <v>166</v>
       </c>
       <c r="T20" s="118" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="U20" s="118" t="s">
         <v>567</v>
@@ -13080,7 +13074,7 @@
         <v>170</v>
       </c>
       <c r="AB20" s="118" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="AC20" s="118" t="s">
         <v>567</v>
@@ -13251,7 +13245,7 @@
         <v>170</v>
       </c>
       <c r="AB21" s="118" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="AC21" s="118" t="s">
         <v>567</v>
@@ -13380,7 +13374,7 @@
         <v>1112</v>
       </c>
       <c r="L22" s="146" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="M22" s="52" t="s">
         <v>166</v>
@@ -13567,7 +13561,7 @@
         <v>1116</v>
       </c>
       <c r="T23" s="118" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="U23" s="118" t="s">
         <v>567</v>
@@ -13873,13 +13867,13 @@
         <v>170</v>
       </c>
       <c r="J25" s="118" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="K25" s="146" t="s">
         <v>1112</v>
       </c>
       <c r="L25" s="146" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="M25" s="52" t="s">
         <v>166</v>
@@ -13925,7 +13919,7 @@
         <v>170</v>
       </c>
       <c r="AB25" s="118" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="AC25" s="118" t="s">
         <v>567</v>
@@ -14050,7 +14044,7 @@
         <v>170</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="M26" s="48" t="s">
         <v>170</v>
@@ -14243,7 +14237,7 @@
         <v>166</v>
       </c>
       <c r="T27" s="118" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="U27" s="118" t="s">
         <v>567</v>
@@ -14378,7 +14372,7 @@
         <v>166</v>
       </c>
       <c r="H28" s="118" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="I28" s="52" t="s">
         <v>166</v>
@@ -14434,7 +14428,7 @@
         <v>170</v>
       </c>
       <c r="AB28" s="118" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="AC28" s="118" t="s">
         <v>567</v>
@@ -15060,13 +15054,13 @@
         <v>170</v>
       </c>
       <c r="J32" s="118" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="K32" s="146" t="s">
         <v>1112</v>
       </c>
       <c r="L32" s="146" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="M32" s="52" t="s">
         <v>166</v>
@@ -15112,7 +15106,7 @@
         <v>170</v>
       </c>
       <c r="AB32" s="118" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="AC32" s="118" t="s">
         <v>567</v>
@@ -15444,7 +15438,7 @@
         <v>170</v>
       </c>
       <c r="AB34" s="118" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="AC34" s="118" t="s">
         <v>567</v>
@@ -15565,7 +15559,7 @@
         <v>170</v>
       </c>
       <c r="J35" s="119" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="K35" s="118" t="s">
         <v>567</v>
@@ -15730,7 +15724,7 @@
         <v>170</v>
       </c>
       <c r="J36" s="118" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="K36" s="118" t="s">
         <v>567</v>
@@ -15758,7 +15752,7 @@
         <v>166</v>
       </c>
       <c r="T36" s="118" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="U36" s="118" t="s">
         <v>567</v>
@@ -15782,7 +15776,7 @@
         <v>166</v>
       </c>
       <c r="AB36" s="118" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="AC36" s="118" t="s">
         <v>567</v>
@@ -16056,7 +16050,7 @@
         <v>170</v>
       </c>
       <c r="H38" s="118" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="I38" s="52" t="s">
         <v>166</v>
@@ -16587,7 +16581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:82" s="18" customFormat="1" ht="63" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:82" s="18" customFormat="1" ht="70.900000000000006" hidden="1" x14ac:dyDescent="0.35">
       <c r="B41" s="13" t="s">
         <v>86</v>
       </c>
@@ -16605,7 +16599,7 @@
         <v>170</v>
       </c>
       <c r="H41" s="118" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="I41" s="118" t="s">
         <v>567</v>
@@ -16615,7 +16609,7 @@
         <v>567</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="M41" s="118" t="s">
         <v>567</v>
@@ -16637,7 +16631,7 @@
         <v>166</v>
       </c>
       <c r="T41" s="118" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="U41" s="118" t="s">
         <v>567</v>
@@ -16768,7 +16762,7 @@
         <v>170</v>
       </c>
       <c r="H42" s="118" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="I42" s="118" t="s">
         <v>567</v>
@@ -16818,7 +16812,7 @@
         <v>567</v>
       </c>
       <c r="AB42" s="118" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="AC42" s="118" t="s">
         <v>567</v>
@@ -16961,7 +16955,7 @@
         <v>1116</v>
       </c>
       <c r="T43" s="118" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="U43" s="118" t="s">
         <v>567</v>
@@ -17130,7 +17124,7 @@
         <v>567</v>
       </c>
       <c r="H44" s="118" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="I44" s="118" t="s">
         <v>567</v>
@@ -17160,7 +17154,7 @@
         <v>166</v>
       </c>
       <c r="T44" s="118" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="U44" s="118" t="s">
         <v>567</v>
@@ -17184,7 +17178,7 @@
         <v>567</v>
       </c>
       <c r="AB44" s="118" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="AC44" s="118" t="s">
         <v>567</v>
@@ -17339,13 +17333,13 @@
         <v>170</v>
       </c>
       <c r="X45" s="118" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y45" s="118" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z45" s="118" t="s">
         <v>1291</v>
-      </c>
-      <c r="Y45" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z45" s="118" t="s">
-        <v>1292</v>
       </c>
       <c r="AA45" s="52" t="s">
         <v>166</v>
@@ -17379,7 +17373,7 @@
         <v>1112</v>
       </c>
       <c r="AN45" s="118" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AO45" s="12"/>
       <c r="AP45" s="120">
@@ -17506,7 +17500,7 @@
         <v>170</v>
       </c>
       <c r="T46" s="118" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="U46" s="118" t="s">
         <v>567</v>
@@ -17844,7 +17838,7 @@
         <v>170</v>
       </c>
       <c r="T48" s="118" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="U48" s="118" t="s">
         <v>567</v>
@@ -18011,7 +18005,7 @@
         <v>1112</v>
       </c>
       <c r="T49" s="118" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="U49" s="118" t="s">
         <v>567</v>
@@ -18500,7 +18494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:82" s="18" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:82" s="18" customFormat="1" ht="39.4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B52" s="13" t="s">
         <v>4</v>
       </c>
@@ -18518,7 +18512,7 @@
         <v>166</v>
       </c>
       <c r="H52" s="118" t="s">
-        <v>165</v>
+        <v>1357</v>
       </c>
       <c r="I52" s="52" t="s">
         <v>166</v>
@@ -18526,8 +18520,8 @@
       <c r="J52" s="118" t="s">
         <v>418</v>
       </c>
-      <c r="K52" s="48" t="s">
-        <v>170</v>
+      <c r="K52" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L52" s="52" t="s">
         <v>481</v>
@@ -18691,7 +18685,7 @@
         <v>166</v>
       </c>
       <c r="H53" s="150" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="I53" s="145" t="s">
         <v>1116</v>
@@ -18747,7 +18741,7 @@
         <v>170</v>
       </c>
       <c r="AB53" s="118" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="AC53" s="118" t="s">
         <v>567</v>
@@ -18888,7 +18882,7 @@
         <v>170</v>
       </c>
       <c r="T54" s="118" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="U54" s="118" t="s">
         <v>567</v>
@@ -19043,12 +19037,10 @@
       <c r="J55" s="118" t="s">
         <v>1223</v>
       </c>
-      <c r="K55" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L55" s="146" t="s">
-        <v>1352</v>
-      </c>
+      <c r="K55" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L55" s="13"/>
       <c r="M55" s="118" t="s">
         <v>567</v>
       </c>
@@ -19214,7 +19206,7 @@
         <v>1112</v>
       </c>
       <c r="L56" s="146" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="M56" s="52" t="s">
         <v>166</v>
@@ -19918,7 +19910,7 @@
         <v>1112</v>
       </c>
       <c r="L60" s="146" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="M60" s="52" t="s">
         <v>166</v>
@@ -20083,7 +20075,7 @@
         <v>1116</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="M61" s="145" t="s">
         <v>1116</v>
@@ -20105,7 +20097,7 @@
         <v>166</v>
       </c>
       <c r="T61" s="118" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="U61" s="118" t="s">
         <v>567</v>
@@ -20129,7 +20121,7 @@
         <v>1116</v>
       </c>
       <c r="AB61" s="118" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="AC61" s="118" t="s">
         <v>567</v>
@@ -20272,7 +20264,7 @@
         <v>1116</v>
       </c>
       <c r="T62" s="118" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="U62" s="118" t="s">
         <v>567</v>
@@ -20435,7 +20427,7 @@
         <v>1116</v>
       </c>
       <c r="T63" s="118" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="U63" s="118" t="s">
         <v>567</v>
@@ -20574,7 +20566,7 @@
         <v>1116</v>
       </c>
       <c r="L64" s="13" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="M64" s="145" t="s">
         <v>1116</v>
@@ -20598,7 +20590,7 @@
         <v>1116</v>
       </c>
       <c r="T64" s="118" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="U64" s="118" t="s">
         <v>567</v>
@@ -20622,7 +20614,7 @@
         <v>1116</v>
       </c>
       <c r="AB64" s="118" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="AC64" s="118" t="s">
         <v>567</v>
@@ -20904,7 +20896,7 @@
         <v>170</v>
       </c>
       <c r="H66" s="118" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="I66" s="145" t="s">
         <v>1116</v>
@@ -20962,7 +20954,7 @@
         <v>170</v>
       </c>
       <c r="AB66" s="118" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="AC66" s="118" t="s">
         <v>567</v>
@@ -21057,7 +21049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:82" s="18" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B67" s="13" t="s">
         <v>4</v>
       </c>
@@ -21087,7 +21079,7 @@
         <v>1112</v>
       </c>
       <c r="L67" s="13" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="M67" s="118" t="s">
         <v>567</v>
@@ -21232,7 +21224,7 @@
         <v>41</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="E68" s="21"/>
       <c r="F68" s="14" t="s">
@@ -21276,7 +21268,7 @@
         <v>166</v>
       </c>
       <c r="T68" s="118" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="U68" s="118" t="s">
         <v>567</v>
@@ -21300,7 +21292,7 @@
         <v>1116</v>
       </c>
       <c r="AB68" s="118" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="AC68" s="118" t="s">
         <v>567</v>
@@ -22453,7 +22445,7 @@
         <v>166</v>
       </c>
       <c r="L75" s="52" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="M75" s="48" t="s">
         <v>170</v>
@@ -22497,7 +22489,7 @@
         <v>1116</v>
       </c>
       <c r="AB75" s="118" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="AC75" s="118" t="s">
         <v>567</v>
@@ -22624,7 +22616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
       <c r="B76" s="13" t="s">
         <v>4</v>
       </c>
@@ -22654,7 +22646,7 @@
         <v>1112</v>
       </c>
       <c r="L76" s="146" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="M76" s="48" t="s">
         <v>170</v>
@@ -22817,7 +22809,7 @@
         <v>1112</v>
       </c>
       <c r="H77" s="118" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="I77" s="52" t="s">
         <v>166</v>
@@ -22871,7 +22863,7 @@
         <v>170</v>
       </c>
       <c r="AB77" s="118" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="AC77" s="118" t="s">
         <v>567</v>
@@ -23133,7 +23125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
       <c r="B79" s="13" t="s">
         <v>4</v>
       </c>
@@ -23163,7 +23155,7 @@
         <v>170</v>
       </c>
       <c r="L79" s="52" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="M79" s="48" t="s">
         <v>170</v>
@@ -23185,7 +23177,7 @@
         <v>166</v>
       </c>
       <c r="T79" s="118" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="U79" s="118" t="s">
         <v>567</v>
@@ -23366,7 +23358,7 @@
         <v>1116</v>
       </c>
       <c r="T80" s="118" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="U80" s="118" t="s">
         <v>567</v>
@@ -23390,7 +23382,7 @@
         <v>1112</v>
       </c>
       <c r="AB80" s="118" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="AC80" s="118" t="s">
         <v>567</v>
@@ -24672,1374 +24664,1368 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
-    <cfRule type="cellIs" dxfId="342" priority="279" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="342" priority="280" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI9:BJ9">
-    <cfRule type="cellIs" dxfId="341" priority="278" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="341" priority="279" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="340" priority="277" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="340" priority="278" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="339" priority="276" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="339" priority="277" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
-    <cfRule type="cellIs" dxfId="338" priority="274" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="338" priority="275" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="337" priority="273" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="337" priority="274" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="336" priority="272" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="336" priority="273" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="335" priority="268" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="335" priority="269" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="334" priority="258" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="334" priority="259" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I4 I7:I8 I12 I44 I14:I15 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="333" priority="245" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="333" priority="246" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="332" priority="234" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="332" priority="235" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
-    <cfRule type="cellIs" dxfId="331" priority="231" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="331" priority="232" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD2">
-    <cfRule type="cellIs" dxfId="330" priority="230" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="330" priority="231" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K44 K63 K77:K82 K23 K68:K74 K28:K31 K46:K57 K9:K18 K60 K33:K38">
-    <cfRule type="cellIs" dxfId="329" priority="229" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K41:K44 K63 K77:K82 K23 K68:K74 K28:K31 K46:K51 K10 K60 K33:K38 K12 K53:K54 K14:K18 K56:K57">
+    <cfRule type="cellIs" dxfId="329" priority="230" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:J15 J76:J85 J43:J44 J8:J12 J38:J40 J18 J33:J34 J46:J74 J2:J5 J20:J29 J36">
-    <cfRule type="cellIs" dxfId="328" priority="228" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="328" priority="229" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L85 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5">
-    <cfRule type="cellIs" dxfId="327" priority="227" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="327" priority="228" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="326" priority="226" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="326" priority="227" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="325" priority="223" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="325" priority="224" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="324" priority="222" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="324" priority="223" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="323" priority="220" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="323" priority="221" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="322" priority="218" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="322" priority="219" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
-    <cfRule type="cellIs" dxfId="321" priority="216" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="321" priority="217" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
-    <cfRule type="cellIs" dxfId="320" priority="215" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="320" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q86">
-    <cfRule type="cellIs" dxfId="319" priority="214" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="319" priority="215" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
-    <cfRule type="cellIs" dxfId="318" priority="213" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="318" priority="214" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AE86">
-    <cfRule type="cellIs" dxfId="317" priority="212" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="317" priority="213" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG5 AG7:AG86">
-    <cfRule type="cellIs" dxfId="316" priority="211" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
+    <cfRule type="cellIs" dxfId="316" priority="212" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
-    <cfRule type="cellIs" dxfId="315" priority="210" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="315" priority="211" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK2:AK86">
-    <cfRule type="cellIs" dxfId="314" priority="209" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="314" priority="210" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM2:AM86">
-    <cfRule type="cellIs" dxfId="313" priority="208" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="313" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="cellIs" dxfId="312" priority="207" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="312" priority="208" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="311" priority="206" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="311" priority="207" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="310" priority="205" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="310" priority="206" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="309" priority="204" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="309" priority="205" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="cellIs" dxfId="308" priority="203" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="308" priority="204" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
-    <cfRule type="cellIs" dxfId="307" priority="202" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="307" priority="203" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="306" priority="201" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="306" priority="202" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="305" priority="200" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="305" priority="201" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="304" priority="199" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="304" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="303" priority="198" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="303" priority="199" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="302" priority="194" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="302" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="301" priority="193" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="301" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60">
-    <cfRule type="cellIs" dxfId="300" priority="192" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="300" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:N14">
-    <cfRule type="cellIs" dxfId="299" priority="191" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="299" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="298" priority="190" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="298" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="297" priority="189" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="297" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
-    <cfRule type="cellIs" dxfId="296" priority="188" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="296" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="cellIs" dxfId="295" priority="187" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="295" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="cellIs" dxfId="294" priority="186" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="294" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ43">
-    <cfRule type="cellIs" dxfId="293" priority="185" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="293" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI43">
-    <cfRule type="cellIs" dxfId="292" priority="184" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="292" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3">
-    <cfRule type="cellIs" dxfId="291" priority="183" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="291" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="cellIs" dxfId="290" priority="182" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="290" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ4">
-    <cfRule type="cellIs" dxfId="289" priority="181" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="289" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI4">
-    <cfRule type="cellIs" dxfId="288" priority="180" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="288" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ5">
-    <cfRule type="cellIs" dxfId="287" priority="179" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="287" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI5">
-    <cfRule type="cellIs" dxfId="286" priority="178" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="286" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ6">
-    <cfRule type="cellIs" dxfId="285" priority="177" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="285" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6">
-    <cfRule type="cellIs" dxfId="284" priority="176" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="284" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ7">
-    <cfRule type="cellIs" dxfId="283" priority="175" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="283" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI7">
-    <cfRule type="cellIs" dxfId="282" priority="174" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="282" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:AJ9">
-    <cfRule type="cellIs" dxfId="281" priority="173" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="281" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI8">
-    <cfRule type="cellIs" dxfId="280" priority="172" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="280" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ46">
-    <cfRule type="cellIs" dxfId="279" priority="171" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="279" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI46">
-    <cfRule type="cellIs" dxfId="278" priority="170" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="278" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ47">
-    <cfRule type="cellIs" dxfId="277" priority="169" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="277" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI47">
-    <cfRule type="cellIs" dxfId="276" priority="168" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="276" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10">
-    <cfRule type="cellIs" dxfId="275" priority="167" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="275" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI10">
-    <cfRule type="cellIs" dxfId="274" priority="166" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="274" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ48">
-    <cfRule type="cellIs" dxfId="273" priority="165" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="273" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI48">
-    <cfRule type="cellIs" dxfId="272" priority="164" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="272" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ49">
-    <cfRule type="cellIs" dxfId="271" priority="163" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="271" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="270" priority="162" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="270" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="269" priority="161" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="269" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI50">
-    <cfRule type="cellIs" dxfId="268" priority="159" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="268" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11:AJ13">
-    <cfRule type="cellIs" dxfId="267" priority="158" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="267" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI11">
-    <cfRule type="cellIs" dxfId="266" priority="157" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="266" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ51">
-    <cfRule type="cellIs" dxfId="265" priority="156" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="265" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI52">
-    <cfRule type="cellIs" dxfId="264" priority="155" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="264" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ52:AJ54">
-    <cfRule type="cellIs" dxfId="263" priority="154" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="263" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ56">
-    <cfRule type="cellIs" dxfId="262" priority="153" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="262" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI56">
-    <cfRule type="cellIs" dxfId="261" priority="152" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="261" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ57:AJ58">
-    <cfRule type="cellIs" dxfId="260" priority="151" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="260" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI57:AI58">
-    <cfRule type="cellIs" dxfId="259" priority="150" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="259" priority="151" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ15:AJ16">
-    <cfRule type="cellIs" dxfId="258" priority="149" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="258" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI15:AI16">
-    <cfRule type="cellIs" dxfId="257" priority="148" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="257" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ59:AJ60">
-    <cfRule type="cellIs" dxfId="256" priority="147" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="256" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ55">
-    <cfRule type="cellIs" dxfId="255" priority="146" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="255" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="cellIs" dxfId="254" priority="145" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="254" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="cellIs" dxfId="253" priority="144" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="253" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI18">
-    <cfRule type="cellIs" dxfId="252" priority="143" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="252" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="251" priority="142" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI17">
-    <cfRule type="cellIs" dxfId="250" priority="141" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="250" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ17">
-    <cfRule type="cellIs" dxfId="249" priority="140" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="249" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI86">
-    <cfRule type="cellIs" dxfId="248" priority="139" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="248" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI40">
-    <cfRule type="cellIs" dxfId="247" priority="138" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="246" priority="137" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="246" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="245" priority="136" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="244" priority="134" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="244" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
-    <cfRule type="cellIs" dxfId="243" priority="132" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="243" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21">
-    <cfRule type="cellIs" dxfId="242" priority="131" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="242" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI64">
-    <cfRule type="cellIs" dxfId="241" priority="130" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="241" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI23">
-    <cfRule type="cellIs" dxfId="240" priority="129" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="240" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ24">
-    <cfRule type="cellIs" dxfId="239" priority="128" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="239" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI25">
-    <cfRule type="cellIs" dxfId="238" priority="127" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="238" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ25">
-    <cfRule type="cellIs" dxfId="237" priority="126" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="237" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ67">
-    <cfRule type="cellIs" dxfId="236" priority="125" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="236" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI26">
-    <cfRule type="cellIs" dxfId="235" priority="124" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="235" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ26:AJ27">
-    <cfRule type="cellIs" dxfId="234" priority="123" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="234" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI28:AI30">
-    <cfRule type="cellIs" dxfId="233" priority="122" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="233" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28:AJ31">
-    <cfRule type="cellIs" dxfId="232" priority="121" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="232" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI72">
-    <cfRule type="cellIs" dxfId="231" priority="120" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="231" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ72">
-    <cfRule type="cellIs" dxfId="230" priority="119" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="230" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI73">
-    <cfRule type="cellIs" dxfId="229" priority="118" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="229" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ73">
-    <cfRule type="cellIs" dxfId="228" priority="117" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="228" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI32">
-    <cfRule type="cellIs" dxfId="227" priority="116" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="227" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="cellIs" dxfId="226" priority="115" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="226" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI33">
-    <cfRule type="cellIs" dxfId="225" priority="114" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="225" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ33">
-    <cfRule type="cellIs" dxfId="224" priority="113" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="224" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI34:AI35">
-    <cfRule type="cellIs" dxfId="223" priority="112" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="223" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ34:AJ36">
-    <cfRule type="cellIs" dxfId="222" priority="111" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="222" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI61">
-    <cfRule type="cellIs" dxfId="221" priority="110" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="221" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI63">
-    <cfRule type="cellIs" dxfId="220" priority="109" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="220" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ70">
-    <cfRule type="cellIs" dxfId="219" priority="108" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="219" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI70">
-    <cfRule type="cellIs" dxfId="218" priority="107" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="218" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI68">
-    <cfRule type="cellIs" dxfId="217" priority="106" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="217" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ76">
-    <cfRule type="cellIs" dxfId="216" priority="105" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="216" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI76">
-    <cfRule type="cellIs" dxfId="215" priority="104" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="215" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ78">
-    <cfRule type="cellIs" dxfId="214" priority="103" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="214" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI78">
-    <cfRule type="cellIs" dxfId="213" priority="102" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="213" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38">
-    <cfRule type="cellIs" dxfId="212" priority="101" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="212" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38">
-    <cfRule type="cellIs" dxfId="211" priority="100" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="211" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ77">
-    <cfRule type="cellIs" dxfId="210" priority="99" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="210" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI77">
-    <cfRule type="cellIs" dxfId="209" priority="98" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="209" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ79">
-    <cfRule type="cellIs" dxfId="208" priority="97" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="208" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI79">
-    <cfRule type="cellIs" dxfId="207" priority="96" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="207" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ80">
-    <cfRule type="cellIs" dxfId="206" priority="95" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="206" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80">
-    <cfRule type="cellIs" dxfId="205" priority="94" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="205" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ81">
-    <cfRule type="cellIs" dxfId="204" priority="93" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="204" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI81">
-    <cfRule type="cellIs" dxfId="203" priority="92" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="203" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ82">
-    <cfRule type="cellIs" dxfId="202" priority="91" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="202" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI82">
-    <cfRule type="cellIs" dxfId="201" priority="90" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="201" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI83">
-    <cfRule type="cellIs" dxfId="200" priority="89" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="200" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI84:AI85">
-    <cfRule type="cellIs" dxfId="199" priority="88" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="199" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI39">
-    <cfRule type="cellIs" dxfId="198" priority="87" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="198" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="cellIs" dxfId="197" priority="86" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="197" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O61">
-    <cfRule type="cellIs" dxfId="196" priority="85" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="196" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54">
-    <cfRule type="cellIs" dxfId="195" priority="84" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="195" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O57">
-    <cfRule type="cellIs" dxfId="194" priority="83" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="194" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O58">
-    <cfRule type="cellIs" dxfId="193" priority="82" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="193" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O67">
-    <cfRule type="cellIs" dxfId="192" priority="81" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="192" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71">
-    <cfRule type="cellIs" dxfId="191" priority="80" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="191" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72">
-    <cfRule type="cellIs" dxfId="190" priority="79" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="190" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="189" priority="78" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="189" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="188" priority="77" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="188" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="cellIs" dxfId="187" priority="76" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="187" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="186" priority="75" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="186" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L75">
-    <cfRule type="cellIs" dxfId="185" priority="73" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="185" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI12">
-    <cfRule type="cellIs" dxfId="184" priority="72" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="184" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2">
-    <cfRule type="cellIs" dxfId="183" priority="71" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="183" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4:W5 W7:W86">
-    <cfRule type="cellIs" dxfId="182" priority="70" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="182" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="cellIs" dxfId="181" priority="69" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="181" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
-    <cfRule type="cellIs" dxfId="180" priority="68" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="180" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2">
-    <cfRule type="cellIs" dxfId="179" priority="67" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="179" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y86">
-    <cfRule type="cellIs" dxfId="178" priority="66" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="178" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2">
-    <cfRule type="cellIs" dxfId="177" priority="65" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="177" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="176" priority="64" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="176" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="cellIs" dxfId="175" priority="63" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="175" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="174" priority="62" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="174" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
-    <cfRule type="cellIs" dxfId="173" priority="61" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="173" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA48">
-    <cfRule type="cellIs" dxfId="172" priority="60" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="172" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA11">
-    <cfRule type="cellIs" dxfId="171" priority="59" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="171" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA51">
-    <cfRule type="cellIs" dxfId="170" priority="58" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="170" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA52">
-    <cfRule type="cellIs" dxfId="169" priority="57" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="169" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA53">
-    <cfRule type="cellIs" dxfId="168" priority="56" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="168" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57 AA54:AA55">
-    <cfRule type="cellIs" dxfId="167" priority="55" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="167" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA20">
-    <cfRule type="cellIs" dxfId="166" priority="54" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="166" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA21">
-    <cfRule type="cellIs" dxfId="165" priority="53" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="165" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA66">
-    <cfRule type="cellIs" dxfId="164" priority="52" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="164" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA25">
-    <cfRule type="cellIs" dxfId="163" priority="51" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="163" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA26">
-    <cfRule type="cellIs" dxfId="162" priority="50" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="162" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA28">
-    <cfRule type="cellIs" dxfId="161" priority="49" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="161" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA32">
-    <cfRule type="cellIs" dxfId="160" priority="48" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="160" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA34">
-    <cfRule type="cellIs" dxfId="159" priority="47" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="159" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27">
-    <cfRule type="cellIs" dxfId="158" priority="46" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="158" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA33 AA31">
-    <cfRule type="cellIs" dxfId="157" priority="45" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="157" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA61 M61">
-    <cfRule type="cellIs" dxfId="156" priority="44" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="156" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA62">
-    <cfRule type="cellIs" dxfId="155" priority="43" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="155" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA63 M63">
-    <cfRule type="cellIs" dxfId="154" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="154" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA65">
-    <cfRule type="cellIs" dxfId="153" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="153" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA67">
-    <cfRule type="cellIs" dxfId="152" priority="40" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="152" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA68">
-    <cfRule type="cellIs" dxfId="151" priority="39" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="151" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA70:AA73">
-    <cfRule type="cellIs" dxfId="150" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="150" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA77">
-    <cfRule type="cellIs" dxfId="149" priority="37" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="149" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA74 AA38">
-    <cfRule type="cellIs" dxfId="148" priority="36" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="148" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37">
-    <cfRule type="cellIs" dxfId="147" priority="35" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="147" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="146" priority="34" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="146" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S46">
-    <cfRule type="cellIs" dxfId="145" priority="33" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="145" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S48">
-    <cfRule type="cellIs" dxfId="144" priority="32" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="144" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S18">
-    <cfRule type="cellIs" dxfId="143" priority="31" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="143" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54">
-    <cfRule type="cellIs" dxfId="142" priority="30" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="142" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S55">
-    <cfRule type="cellIs" dxfId="141" priority="29" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="141" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S57">
-    <cfRule type="cellIs" dxfId="140" priority="28" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="140" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S76">
-    <cfRule type="cellIs" dxfId="139" priority="27" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="139" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S78">
-    <cfRule type="cellIs" dxfId="138" priority="26" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="138" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S81">
-    <cfRule type="cellIs" dxfId="137" priority="25" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="137" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S82">
-    <cfRule type="cellIs" dxfId="136" priority="24" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="136" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="135" priority="23" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="cellIs" dxfId="134" priority="22" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="134" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L67">
-    <cfRule type="cellIs" dxfId="133" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="133" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="132" priority="20" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="132" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="131" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="131" priority="20" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G8">
-    <cfRule type="cellIs" dxfId="130" priority="18" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="129" priority="17" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="130" priority="19" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="128" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="128" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="127" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="127" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="126" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="126" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="cellIs" dxfId="125" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="125" priority="14" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L13">
+    <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L55">
+    <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L56">
+    <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L60">
+    <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K76">
+    <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L76">
+    <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6">
+    <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7">
+    <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8">
+    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L55">
-    <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L60">
-    <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
-    <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L76">
-    <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
-    <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
-    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
     <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -57481,7 +57467,7 @@
       <c r="BD33" s="19"/>
       <c r="BE33" s="63"/>
     </row>
-    <row r="34" spans="2:57" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:57" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B34" s="13" t="s">
         <v>4</v>
       </c>
@@ -57950,7 +57936,7 @@
       <c r="BD38" s="19"/>
       <c r="BE38" s="63"/>
     </row>
-    <row r="39" spans="2:57" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:57" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
         <v>4</v>
       </c>
@@ -63666,7 +63652,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43517</v>
+        <v>43528</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -63976,7 +63962,7 @@
   <dimension ref="B1:Y87"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="7845" activePane="bottomLeft"/>
+      <pane ySplit="7680" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -64015,7 +64001,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43517</v>
+        <v>43528</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
City ADT Leed cert
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F985F7E0-2A8F-43BD-BFDB-1CD3E359D0EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E3DAB7-C47E-43ED-A1FE-753A2BCBBA94}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8979" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8980" uniqueCount="1363">
   <si>
     <t>#</t>
   </si>
@@ -4085,9 +4085,6 @@
     <t>&lt;appears to be on R drive&gt;&gt;</t>
   </si>
   <si>
-    <t>&lt;appears to be on R drive&gt;&gt; Mesa - 046; 050--062; 068-073; 094; 097</t>
-  </si>
-  <si>
     <t>&lt;appears to be on R drive&gt;&gt; Miramar-021; 024-025; 042-043; 045-052</t>
   </si>
   <si>
@@ -4127,7 +4124,16 @@
     <t>Silver (still "no" 3/12/2019)</t>
   </si>
   <si>
-    <t>Certified (still "no" 3/12/2019)</t>
+    <t>updated to Fac Man SP</t>
+  </si>
+  <si>
+    <t>many warranties loaded on SP, but not checked ast equipment-level</t>
+  </si>
+  <si>
+    <t>Gold (61 points) achieved March 2019</t>
+  </si>
+  <si>
+    <t>Gold (62 points) achieved March 2019</t>
   </si>
 </sst>
 </file>
@@ -5217,7 +5223,14 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="342">
+  <dxfs count="344">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7612,6 +7625,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7858,7 +7878,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3/12/2019</c:v>
+                  <c:v>3/19/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9616,7 +9636,8 @@
   <dimension ref="B1:CD101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <pane ySplit="1605" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -9939,7 +9960,7 @@
         <v>170</v>
       </c>
       <c r="J2" s="119" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="K2" s="52" t="s">
         <v>166</v>
@@ -10110,7 +10131,7 @@
         <v>170</v>
       </c>
       <c r="J3" s="119" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="K3" s="52" t="s">
         <v>166</v>
@@ -10277,17 +10298,17 @@
       <c r="H4" s="118" t="s">
         <v>1333</v>
       </c>
-      <c r="I4" s="48" t="s">
-        <v>170</v>
+      <c r="I4" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="J4" s="118" t="s">
-        <v>1359</v>
+        <v>1362</v>
       </c>
       <c r="K4" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="M4" s="13" t="s">
         <v>567</v>
@@ -10673,7 +10694,7 @@
         <v>567</v>
       </c>
       <c r="Z6" s="118" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="AA6" s="52" t="s">
         <v>166</v>
@@ -10695,7 +10716,7 @@
         <v>166</v>
       </c>
       <c r="AH6" s="118" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="AI6" s="48" t="s">
         <v>170</v>
@@ -10808,19 +10829,17 @@
         <v>1112</v>
       </c>
       <c r="H7" s="118" t="s">
-        <v>1355</v>
-      </c>
-      <c r="I7" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="J7" s="118" t="s">
-        <v>1360</v>
-      </c>
+        <v>1354</v>
+      </c>
+      <c r="I7" s="145" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J7" s="118"/>
       <c r="K7" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L7" s="52" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M7" s="13" t="s">
         <v>567</v>
@@ -10985,17 +11004,17 @@
       <c r="H8" s="118" t="s">
         <v>1333</v>
       </c>
-      <c r="I8" s="48" t="s">
-        <v>170</v>
+      <c r="I8" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="J8" s="118" t="s">
-        <v>1359</v>
+        <v>1361</v>
       </c>
       <c r="K8" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L8" s="52" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M8" s="13" t="s">
         <v>567</v>
@@ -11228,7 +11247,7 @@
         <v>166</v>
       </c>
       <c r="AH9" s="118" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="AI9" s="118" t="s">
         <v>567</v>
@@ -11675,7 +11694,7 @@
         <v>170</v>
       </c>
       <c r="J12" s="118" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="K12" s="118" t="s">
         <v>567</v>
@@ -12011,7 +12030,7 @@
         <v>170</v>
       </c>
       <c r="J14" s="118" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="K14" s="146" t="s">
         <v>1112</v>
@@ -12047,17 +12066,17 @@
       <c r="V14" s="118">
         <v>1</v>
       </c>
-      <c r="W14" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X14" s="118">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z14" s="118">
-        <v>1</v>
+      <c r="W14" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="X14" s="118" t="s">
+        <v>1359</v>
+      </c>
+      <c r="Y14" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="Z14" s="118" t="s">
+        <v>1360</v>
       </c>
       <c r="AA14" s="52" t="s">
         <v>166</v>
@@ -12176,7 +12195,7 @@
         <v>170</v>
       </c>
       <c r="J15" s="118" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="K15" s="118" t="s">
         <v>567</v>
@@ -13866,13 +13885,13 @@
         <v>170</v>
       </c>
       <c r="J25" s="118" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="K25" s="146" t="s">
         <v>1112</v>
       </c>
       <c r="L25" s="146" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="M25" s="52" t="s">
         <v>166</v>
@@ -15053,7 +15072,7 @@
         <v>170</v>
       </c>
       <c r="J32" s="118" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="K32" s="146" t="s">
         <v>1112</v>
@@ -15558,7 +15577,7 @@
         <v>170</v>
       </c>
       <c r="J35" s="119" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="K35" s="118" t="s">
         <v>567</v>
@@ -15723,7 +15742,7 @@
         <v>170</v>
       </c>
       <c r="J36" s="118" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="K36" s="118" t="s">
         <v>567</v>
@@ -17153,7 +17172,7 @@
         <v>166</v>
       </c>
       <c r="T44" s="118" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="U44" s="118" t="s">
         <v>567</v>
@@ -18511,7 +18530,7 @@
         <v>166</v>
       </c>
       <c r="H52" s="118" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="I52" s="52" t="s">
         <v>166</v>
@@ -19175,7 +19194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:82" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B56" s="13" t="s">
         <v>4</v>
       </c>
@@ -19201,11 +19220,11 @@
       <c r="J56" s="118" t="s">
         <v>418</v>
       </c>
-      <c r="K56" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L56" s="146" t="s">
-        <v>1346</v>
+      <c r="K56" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>482</v>
       </c>
       <c r="M56" s="52" t="s">
         <v>166</v>
@@ -23154,7 +23173,7 @@
         <v>170</v>
       </c>
       <c r="L79" s="52" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="M79" s="48" t="s">
         <v>170</v>
@@ -24657,1369 +24676,1381 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
+    <cfRule type="cellIs" dxfId="343" priority="282" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BI9:BJ9">
+    <cfRule type="cellIs" dxfId="342" priority="281" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
     <cfRule type="cellIs" dxfId="341" priority="280" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BI9:BJ9">
+  <conditionalFormatting sqref="AV39 AV56">
     <cfRule type="cellIs" dxfId="340" priority="279" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="339" priority="278" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
+    <cfRule type="cellIs" dxfId="339" priority="277" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="338" priority="277" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
+    <cfRule type="cellIs" dxfId="338" priority="276" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
+  <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
     <cfRule type="cellIs" dxfId="337" priority="275" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="336" priority="274" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="335" priority="273" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="334" priority="269" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="336" priority="271" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="333" priority="259" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="335" priority="261" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I3 I44 I14 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="332" priority="246" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="334" priority="248" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="331" priority="235" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="333" priority="237" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
+    <cfRule type="cellIs" dxfId="332" priority="234" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CD2">
+    <cfRule type="cellIs" dxfId="331" priority="233" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K41:K44 K63 K77:K82 K23 K68:K74 K28:K31 K46:K51 K10 K60 K33:K38 K12 K53:K54 K14:K18 K57">
     <cfRule type="cellIs" dxfId="330" priority="232" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CD2">
+  <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
     <cfRule type="cellIs" dxfId="329" priority="231" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K44 K63 K77:K82 K23 K68:K74 K28:K31 K46:K51 K10 K60 K33:K38 K12 K53:K54 K14:K18 K56:K57">
+  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L85 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5">
     <cfRule type="cellIs" dxfId="328" priority="230" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J5 J20:J29 J36 J8:J12 J14:J15">
+  <conditionalFormatting sqref="I35">
     <cfRule type="cellIs" dxfId="327" priority="229" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L85 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5">
-    <cfRule type="cellIs" dxfId="326" priority="228" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="325" priority="227" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="324" priority="224" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="326" priority="226" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="323" priority="223" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="325" priority="225" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="322" priority="221" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="324" priority="223" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="321" priority="219" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="323" priority="221" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
+    <cfRule type="cellIs" dxfId="322" priority="219" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+    <cfRule type="cellIs" dxfId="321" priority="218" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q86">
     <cfRule type="cellIs" dxfId="320" priority="217" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
     <cfRule type="cellIs" dxfId="319" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q86">
+  <conditionalFormatting sqref="AE2:AE86">
     <cfRule type="cellIs" dxfId="318" priority="215" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
+  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
     <cfRule type="cellIs" dxfId="317" priority="214" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE86">
+  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
     <cfRule type="cellIs" dxfId="316" priority="213" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
+  <conditionalFormatting sqref="AK2:AK86">
     <cfRule type="cellIs" dxfId="315" priority="212" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
+  <conditionalFormatting sqref="AM2:AM86">
     <cfRule type="cellIs" dxfId="314" priority="211" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK86">
+  <conditionalFormatting sqref="N46">
     <cfRule type="cellIs" dxfId="313" priority="210" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AM86">
+  <conditionalFormatting sqref="N9">
     <cfRule type="cellIs" dxfId="312" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46">
+  <conditionalFormatting sqref="N6">
     <cfRule type="cellIs" dxfId="311" priority="208" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9">
+  <conditionalFormatting sqref="N48">
     <cfRule type="cellIs" dxfId="310" priority="207" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6">
+  <conditionalFormatting sqref="N45">
     <cfRule type="cellIs" dxfId="309" priority="206" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N48">
+  <conditionalFormatting sqref="N50">
     <cfRule type="cellIs" dxfId="308" priority="205" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N45">
+  <conditionalFormatting sqref="N5">
     <cfRule type="cellIs" dxfId="307" priority="204" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N2">
     <cfRule type="cellIs" dxfId="306" priority="203" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
+  <conditionalFormatting sqref="N3">
     <cfRule type="cellIs" dxfId="305" priority="202" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
+  <conditionalFormatting sqref="N10">
     <cfRule type="cellIs" dxfId="304" priority="201" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="303" priority="200" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N52">
+    <cfRule type="cellIs" dxfId="303" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="302" priority="199" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N16">
+    <cfRule type="cellIs" dxfId="302" priority="196" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
+  <conditionalFormatting sqref="N60">
     <cfRule type="cellIs" dxfId="301" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
+  <conditionalFormatting sqref="M14:N14">
     <cfRule type="cellIs" dxfId="300" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N60">
+  <conditionalFormatting sqref="M34">
     <cfRule type="cellIs" dxfId="299" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:N14">
+  <conditionalFormatting sqref="N26">
     <cfRule type="cellIs" dxfId="298" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M34">
+  <conditionalFormatting sqref="M26">
     <cfRule type="cellIs" dxfId="297" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
+  <conditionalFormatting sqref="N28">
     <cfRule type="cellIs" dxfId="296" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
+  <conditionalFormatting sqref="M68">
     <cfRule type="cellIs" dxfId="295" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
+  <conditionalFormatting sqref="AJ43">
     <cfRule type="cellIs" dxfId="294" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M68">
+  <conditionalFormatting sqref="AI43">
     <cfRule type="cellIs" dxfId="293" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ43">
+  <conditionalFormatting sqref="AJ3">
     <cfRule type="cellIs" dxfId="292" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI43">
+  <conditionalFormatting sqref="AI3">
     <cfRule type="cellIs" dxfId="291" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ3">
+  <conditionalFormatting sqref="AJ4">
     <cfRule type="cellIs" dxfId="290" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI3">
+  <conditionalFormatting sqref="AI4">
     <cfRule type="cellIs" dxfId="289" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ4">
+  <conditionalFormatting sqref="AJ5">
     <cfRule type="cellIs" dxfId="288" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI4">
+  <conditionalFormatting sqref="AI5">
     <cfRule type="cellIs" dxfId="287" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ5">
+  <conditionalFormatting sqref="AJ6">
     <cfRule type="cellIs" dxfId="286" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI5">
+  <conditionalFormatting sqref="AI6">
     <cfRule type="cellIs" dxfId="285" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ6">
+  <conditionalFormatting sqref="AJ7">
     <cfRule type="cellIs" dxfId="284" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI6">
+  <conditionalFormatting sqref="AI7">
     <cfRule type="cellIs" dxfId="283" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ7">
+  <conditionalFormatting sqref="AJ8:AJ9">
     <cfRule type="cellIs" dxfId="282" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI7">
+  <conditionalFormatting sqref="AI8">
     <cfRule type="cellIs" dxfId="281" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ8:AJ9">
+  <conditionalFormatting sqref="AJ46">
     <cfRule type="cellIs" dxfId="280" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI8">
+  <conditionalFormatting sqref="AI46">
     <cfRule type="cellIs" dxfId="279" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ46">
+  <conditionalFormatting sqref="AJ47">
     <cfRule type="cellIs" dxfId="278" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI46">
+  <conditionalFormatting sqref="AI47">
     <cfRule type="cellIs" dxfId="277" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ47">
+  <conditionalFormatting sqref="AJ10">
     <cfRule type="cellIs" dxfId="276" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI47">
+  <conditionalFormatting sqref="AI10">
     <cfRule type="cellIs" dxfId="275" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ10">
+  <conditionalFormatting sqref="AJ48">
     <cfRule type="cellIs" dxfId="274" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI10">
+  <conditionalFormatting sqref="AI48">
     <cfRule type="cellIs" dxfId="273" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ48">
+  <conditionalFormatting sqref="AJ49">
     <cfRule type="cellIs" dxfId="272" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI48">
+  <conditionalFormatting sqref="AI49">
     <cfRule type="cellIs" dxfId="271" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ49">
+  <conditionalFormatting sqref="AJ50">
     <cfRule type="cellIs" dxfId="270" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="269" priority="163" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI50">
+    <cfRule type="cellIs" dxfId="269" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="268" priority="162" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ11:AJ13">
+    <cfRule type="cellIs" dxfId="268" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI50">
+  <conditionalFormatting sqref="AI11">
     <cfRule type="cellIs" dxfId="267" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11:AJ13">
+  <conditionalFormatting sqref="AJ51">
     <cfRule type="cellIs" dxfId="266" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI11">
+  <conditionalFormatting sqref="AI52">
     <cfRule type="cellIs" dxfId="265" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ51">
+  <conditionalFormatting sqref="AJ52:AJ54">
     <cfRule type="cellIs" dxfId="264" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI52">
+  <conditionalFormatting sqref="AJ56">
     <cfRule type="cellIs" dxfId="263" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ52:AJ54">
+  <conditionalFormatting sqref="AI56">
     <cfRule type="cellIs" dxfId="262" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ56">
+  <conditionalFormatting sqref="AJ57:AJ58">
     <cfRule type="cellIs" dxfId="261" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI56">
+  <conditionalFormatting sqref="AI57:AI58">
     <cfRule type="cellIs" dxfId="260" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ57:AJ58">
+  <conditionalFormatting sqref="AJ15:AJ16">
     <cfRule type="cellIs" dxfId="259" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI57:AI58">
+  <conditionalFormatting sqref="AI15:AI16">
     <cfRule type="cellIs" dxfId="258" priority="151" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15:AJ16">
+  <conditionalFormatting sqref="AJ59:AJ60">
     <cfRule type="cellIs" dxfId="257" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI15:AI16">
+  <conditionalFormatting sqref="AJ55">
     <cfRule type="cellIs" dxfId="256" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ59:AJ60">
+  <conditionalFormatting sqref="AI19">
     <cfRule type="cellIs" dxfId="255" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ55">
+  <conditionalFormatting sqref="AJ19">
     <cfRule type="cellIs" dxfId="254" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI19">
+  <conditionalFormatting sqref="AI18">
     <cfRule type="cellIs" dxfId="253" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19">
+  <conditionalFormatting sqref="AJ18">
     <cfRule type="cellIs" dxfId="252" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI18">
+  <conditionalFormatting sqref="AI17">
     <cfRule type="cellIs" dxfId="251" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ18">
+  <conditionalFormatting sqref="AJ17">
     <cfRule type="cellIs" dxfId="250" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI17">
+  <conditionalFormatting sqref="AI86">
     <cfRule type="cellIs" dxfId="249" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ17">
+  <conditionalFormatting sqref="AI40">
     <cfRule type="cellIs" dxfId="248" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI86">
+  <conditionalFormatting sqref="AJ20">
     <cfRule type="cellIs" dxfId="247" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI40">
+  <conditionalFormatting sqref="AJ62">
     <cfRule type="cellIs" dxfId="246" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="245" priority="138" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="244" priority="137" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="243" priority="135" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
+    <cfRule type="cellIs" dxfId="244" priority="135" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI21">
+    <cfRule type="cellIs" dxfId="243" priority="134" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI64">
     <cfRule type="cellIs" dxfId="242" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI21">
+  <conditionalFormatting sqref="AI23">
     <cfRule type="cellIs" dxfId="241" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI64">
+  <conditionalFormatting sqref="AJ24">
     <cfRule type="cellIs" dxfId="240" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI23">
+  <conditionalFormatting sqref="AI25">
     <cfRule type="cellIs" dxfId="239" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ24">
+  <conditionalFormatting sqref="AJ25">
     <cfRule type="cellIs" dxfId="238" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI25">
+  <conditionalFormatting sqref="AJ67">
     <cfRule type="cellIs" dxfId="237" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ25">
+  <conditionalFormatting sqref="AI26">
     <cfRule type="cellIs" dxfId="236" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ67">
+  <conditionalFormatting sqref="AJ26:AJ27">
     <cfRule type="cellIs" dxfId="235" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI26">
+  <conditionalFormatting sqref="AI28:AI30">
     <cfRule type="cellIs" dxfId="234" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ26:AJ27">
+  <conditionalFormatting sqref="AJ28:AJ31">
     <cfRule type="cellIs" dxfId="233" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI28:AI30">
+  <conditionalFormatting sqref="AI72">
     <cfRule type="cellIs" dxfId="232" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ28:AJ31">
+  <conditionalFormatting sqref="AJ72">
     <cfRule type="cellIs" dxfId="231" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI72">
+  <conditionalFormatting sqref="AI73">
     <cfRule type="cellIs" dxfId="230" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ72">
+  <conditionalFormatting sqref="AJ73">
     <cfRule type="cellIs" dxfId="229" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI73">
+  <conditionalFormatting sqref="AI32">
     <cfRule type="cellIs" dxfId="228" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ73">
+  <conditionalFormatting sqref="AJ32">
     <cfRule type="cellIs" dxfId="227" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI32">
+  <conditionalFormatting sqref="AI33">
     <cfRule type="cellIs" dxfId="226" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ32">
+  <conditionalFormatting sqref="AJ33">
     <cfRule type="cellIs" dxfId="225" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI33">
+  <conditionalFormatting sqref="AI34:AI35">
     <cfRule type="cellIs" dxfId="224" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ33">
+  <conditionalFormatting sqref="AJ34:AJ36">
     <cfRule type="cellIs" dxfId="223" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI34:AI35">
+  <conditionalFormatting sqref="AI61">
     <cfRule type="cellIs" dxfId="222" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ34:AJ36">
+  <conditionalFormatting sqref="AI63">
     <cfRule type="cellIs" dxfId="221" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI61">
+  <conditionalFormatting sqref="AJ70">
     <cfRule type="cellIs" dxfId="220" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI63">
+  <conditionalFormatting sqref="AI70">
     <cfRule type="cellIs" dxfId="219" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ70">
+  <conditionalFormatting sqref="AI68">
     <cfRule type="cellIs" dxfId="218" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI70">
+  <conditionalFormatting sqref="AJ76">
     <cfRule type="cellIs" dxfId="217" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI68">
+  <conditionalFormatting sqref="AI76">
     <cfRule type="cellIs" dxfId="216" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ76">
+  <conditionalFormatting sqref="AJ78">
     <cfRule type="cellIs" dxfId="215" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI76">
+  <conditionalFormatting sqref="AI78">
     <cfRule type="cellIs" dxfId="214" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ78">
+  <conditionalFormatting sqref="AJ38">
     <cfRule type="cellIs" dxfId="213" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI78">
+  <conditionalFormatting sqref="AI38">
     <cfRule type="cellIs" dxfId="212" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ38">
+  <conditionalFormatting sqref="AJ77">
     <cfRule type="cellIs" dxfId="211" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI38">
+  <conditionalFormatting sqref="AI77">
     <cfRule type="cellIs" dxfId="210" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ77">
+  <conditionalFormatting sqref="AJ79">
     <cfRule type="cellIs" dxfId="209" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI77">
+  <conditionalFormatting sqref="AI79">
     <cfRule type="cellIs" dxfId="208" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ79">
+  <conditionalFormatting sqref="AJ80">
     <cfRule type="cellIs" dxfId="207" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI79">
+  <conditionalFormatting sqref="AI80">
     <cfRule type="cellIs" dxfId="206" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ80">
+  <conditionalFormatting sqref="AJ81">
     <cfRule type="cellIs" dxfId="205" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI80">
+  <conditionalFormatting sqref="AI81">
     <cfRule type="cellIs" dxfId="204" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ81">
+  <conditionalFormatting sqref="AJ82">
     <cfRule type="cellIs" dxfId="203" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI81">
+  <conditionalFormatting sqref="AI82">
     <cfRule type="cellIs" dxfId="202" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ82">
+  <conditionalFormatting sqref="AI83">
     <cfRule type="cellIs" dxfId="201" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI82">
+  <conditionalFormatting sqref="AI84:AI85">
     <cfRule type="cellIs" dxfId="200" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI83">
+  <conditionalFormatting sqref="AI39">
     <cfRule type="cellIs" dxfId="199" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI84:AI85">
+  <conditionalFormatting sqref="J31">
     <cfRule type="cellIs" dxfId="198" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI39">
+  <conditionalFormatting sqref="O61">
     <cfRule type="cellIs" dxfId="197" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
+  <conditionalFormatting sqref="O54">
     <cfRule type="cellIs" dxfId="196" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O61">
+  <conditionalFormatting sqref="O57">
     <cfRule type="cellIs" dxfId="195" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O54">
+  <conditionalFormatting sqref="O58">
     <cfRule type="cellIs" dxfId="194" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O57">
+  <conditionalFormatting sqref="O67">
     <cfRule type="cellIs" dxfId="193" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O58">
+  <conditionalFormatting sqref="O71">
     <cfRule type="cellIs" dxfId="192" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O67">
+  <conditionalFormatting sqref="O72">
     <cfRule type="cellIs" dxfId="191" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O71">
+  <conditionalFormatting sqref="O80">
     <cfRule type="cellIs" dxfId="190" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O72">
+  <conditionalFormatting sqref="O82">
     <cfRule type="cellIs" dxfId="189" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80">
+  <conditionalFormatting sqref="K62">
     <cfRule type="cellIs" dxfId="188" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82">
+  <conditionalFormatting sqref="L62">
     <cfRule type="cellIs" dxfId="187" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="cellIs" dxfId="186" priority="77" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L75">
+    <cfRule type="cellIs" dxfId="186" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="185" priority="76" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI12">
+    <cfRule type="cellIs" dxfId="185" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L75">
+  <conditionalFormatting sqref="X2">
     <cfRule type="cellIs" dxfId="184" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI12">
+  <conditionalFormatting sqref="W4:W5 W7:W13 W15:W86">
     <cfRule type="cellIs" dxfId="183" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
+  <conditionalFormatting sqref="AB2">
     <cfRule type="cellIs" dxfId="182" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W4:W5 W7:W86">
+  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
     <cfRule type="cellIs" dxfId="181" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2">
+  <conditionalFormatting sqref="Z2">
     <cfRule type="cellIs" dxfId="180" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
+  <conditionalFormatting sqref="Y2:Y13 Y15:Y86">
     <cfRule type="cellIs" dxfId="179" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2">
+  <conditionalFormatting sqref="AD2">
     <cfRule type="cellIs" dxfId="178" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y86">
+  <conditionalFormatting sqref="AC2:AC86">
     <cfRule type="cellIs" dxfId="177" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2">
+  <conditionalFormatting sqref="V2">
     <cfRule type="cellIs" dxfId="176" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC86">
+  <conditionalFormatting sqref="U2:U86">
     <cfRule type="cellIs" dxfId="175" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2">
+  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
     <cfRule type="cellIs" dxfId="174" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U86">
+  <conditionalFormatting sqref="AA48">
     <cfRule type="cellIs" dxfId="173" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
+  <conditionalFormatting sqref="AA11">
     <cfRule type="cellIs" dxfId="172" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA48">
+  <conditionalFormatting sqref="AA51">
     <cfRule type="cellIs" dxfId="171" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA11">
+  <conditionalFormatting sqref="AA52">
     <cfRule type="cellIs" dxfId="170" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA51">
+  <conditionalFormatting sqref="AA53">
     <cfRule type="cellIs" dxfId="169" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA52">
+  <conditionalFormatting sqref="AA57 AA54:AA55">
     <cfRule type="cellIs" dxfId="168" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA53">
+  <conditionalFormatting sqref="AA20">
     <cfRule type="cellIs" dxfId="167" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA57 AA54:AA55">
+  <conditionalFormatting sqref="AA21">
     <cfRule type="cellIs" dxfId="166" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA20">
+  <conditionalFormatting sqref="AA66">
     <cfRule type="cellIs" dxfId="165" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA21">
+  <conditionalFormatting sqref="AA25">
     <cfRule type="cellIs" dxfId="164" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA66">
+  <conditionalFormatting sqref="AA26">
     <cfRule type="cellIs" dxfId="163" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA25">
+  <conditionalFormatting sqref="AA28">
     <cfRule type="cellIs" dxfId="162" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA26">
+  <conditionalFormatting sqref="AA32">
     <cfRule type="cellIs" dxfId="161" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA28">
+  <conditionalFormatting sqref="AA34">
     <cfRule type="cellIs" dxfId="160" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA32">
+  <conditionalFormatting sqref="AA27">
     <cfRule type="cellIs" dxfId="159" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA34">
+  <conditionalFormatting sqref="AA33 AA31">
     <cfRule type="cellIs" dxfId="158" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA27">
+  <conditionalFormatting sqref="AA61 M61">
     <cfRule type="cellIs" dxfId="157" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA33 AA31">
+  <conditionalFormatting sqref="AA62">
     <cfRule type="cellIs" dxfId="156" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA61 M61">
+  <conditionalFormatting sqref="AA63 M63">
     <cfRule type="cellIs" dxfId="155" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA62">
+  <conditionalFormatting sqref="AA65">
     <cfRule type="cellIs" dxfId="154" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA63 M63">
+  <conditionalFormatting sqref="AA67">
     <cfRule type="cellIs" dxfId="153" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA65">
+  <conditionalFormatting sqref="AA68">
     <cfRule type="cellIs" dxfId="152" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA67">
+  <conditionalFormatting sqref="AA70:AA73">
     <cfRule type="cellIs" dxfId="151" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA68">
+  <conditionalFormatting sqref="AA77">
     <cfRule type="cellIs" dxfId="150" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA70:AA73">
+  <conditionalFormatting sqref="AA74 AA38">
     <cfRule type="cellIs" dxfId="149" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA77">
+  <conditionalFormatting sqref="AA37">
     <cfRule type="cellIs" dxfId="148" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA74 AA38">
+  <conditionalFormatting sqref="S9">
     <cfRule type="cellIs" dxfId="147" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA37">
+  <conditionalFormatting sqref="S46">
     <cfRule type="cellIs" dxfId="146" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
+  <conditionalFormatting sqref="S48">
     <cfRule type="cellIs" dxfId="145" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S46">
+  <conditionalFormatting sqref="S18">
     <cfRule type="cellIs" dxfId="144" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48">
+  <conditionalFormatting sqref="S54">
     <cfRule type="cellIs" dxfId="143" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
+  <conditionalFormatting sqref="S55">
     <cfRule type="cellIs" dxfId="142" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S54">
+  <conditionalFormatting sqref="S57">
     <cfRule type="cellIs" dxfId="141" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S55">
+  <conditionalFormatting sqref="S76">
     <cfRule type="cellIs" dxfId="140" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S57">
+  <conditionalFormatting sqref="S78">
     <cfRule type="cellIs" dxfId="139" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S76">
+  <conditionalFormatting sqref="S81">
     <cfRule type="cellIs" dxfId="138" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S78">
+  <conditionalFormatting sqref="S82">
     <cfRule type="cellIs" dxfId="137" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S81">
+  <conditionalFormatting sqref="J32">
     <cfRule type="cellIs" dxfId="136" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S82">
+  <conditionalFormatting sqref="K66">
     <cfRule type="cellIs" dxfId="135" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
+  <conditionalFormatting sqref="L67">
     <cfRule type="cellIs" dxfId="134" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="133" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L67">
+  <conditionalFormatting sqref="L27">
     <cfRule type="cellIs" dxfId="132" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="G7">
     <cfRule type="cellIs" dxfId="131" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="130" priority="20" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G20">
+    <cfRule type="cellIs" dxfId="130" priority="19" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="129" priority="19" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="129" priority="18" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
+  <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" dxfId="128" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
+  <conditionalFormatting sqref="X3">
     <cfRule type="cellIs" dxfId="127" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="126" priority="15" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L13">
+    <cfRule type="cellIs" dxfId="126" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3">
-    <cfRule type="cellIs" dxfId="125" priority="14" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L55">
+    <cfRule type="cellIs" dxfId="125" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
+  <conditionalFormatting sqref="L56">
     <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L55">
+  <conditionalFormatting sqref="L14">
     <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
+  <conditionalFormatting sqref="L60">
     <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
+  <conditionalFormatting sqref="K76">
     <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L60">
+  <conditionalFormatting sqref="L76">
     <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
+  <conditionalFormatting sqref="L6">
     <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76">
+  <conditionalFormatting sqref="L7">
     <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
+  <conditionalFormatting sqref="L8">
     <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
+  <conditionalFormatting sqref="L9">
     <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
+  <conditionalFormatting sqref="Y14">
     <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="J4">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -46881,448 +46912,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="114" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="113" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="112" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="111" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="110" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="109" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="108" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="107" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="106" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="105" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="104" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="102" priority="93">
+    <cfRule type="containsBlanks" dxfId="103" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="102" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="100" priority="91">
+    <cfRule type="containsBlanks" dxfId="101" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="100" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="99" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="98" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="97" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="96" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="95" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="94" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="93" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="92" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="90" priority="69">
+    <cfRule type="containsBlanks" dxfId="91" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="89" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="88" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="87" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="86" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="85" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="84" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="82" priority="63">
+    <cfRule type="containsBlanks" dxfId="83" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="82" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="81" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="80" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="79" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="77" priority="59">
+    <cfRule type="containsBlanks" dxfId="78" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="77" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="75" priority="56">
+    <cfRule type="containsBlanks" dxfId="76" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="75" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="74" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="73" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="72" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="71" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="70" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="68" priority="50">
+    <cfRule type="containsBlanks" dxfId="69" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="68" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="67" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="65" priority="47">
+    <cfRule type="containsBlanks" dxfId="66" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="65" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="64" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="63" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="62" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="60" priority="42">
+    <cfRule type="containsBlanks" dxfId="61" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="60" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="59" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="57" priority="39">
+    <cfRule type="containsBlanks" dxfId="58" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="57" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="56" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="55" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="53" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="52" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="50" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="49" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="47" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="46" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="44" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="42" priority="23">
+    <cfRule type="containsBlanks" dxfId="43" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="40" priority="19">
+    <cfRule type="containsBlanks" dxfId="41" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="40" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="31" priority="22">
+    <cfRule type="containsBlanks" dxfId="32" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="30" priority="11">
+    <cfRule type="containsBlanks" dxfId="31" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -62217,111 +62248,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -63645,7 +63676,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43536</v>
+        <v>43543</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -63955,7 +63986,7 @@
   <dimension ref="B1:Y87"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="7680" activePane="bottomLeft"/>
+      <pane ySplit="7860" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -63994,7 +64025,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43536</v>
+        <v>43543</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -68001,7 +68032,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
more uploads to sharepoint
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E3DAB7-C47E-43ED-A1FE-753A2BCBBA94}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FBE8A8-D79E-4063-A0BA-F9BA8327F938}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8980" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8989" uniqueCount="1377">
   <si>
     <t>#</t>
   </si>
@@ -4085,9 +4085,6 @@
     <t>&lt;appears to be on R drive&gt;&gt;</t>
   </si>
   <si>
-    <t>&lt;appears to be on R drive&gt;&gt; Miramar-021; 024-025; 042-043; 045-052</t>
-  </si>
-  <si>
     <t>&lt;&lt;minimal files on R drive&gt;&gt; CE-008</t>
   </si>
   <si>
@@ -4124,16 +4121,61 @@
     <t>Silver (still "no" 3/12/2019)</t>
   </si>
   <si>
-    <t>updated to Fac Man SP</t>
-  </si>
-  <si>
-    <t>many warranties loaded on SP, but not checked ast equipment-level</t>
-  </si>
-  <si>
     <t>Gold (61 points) achieved March 2019</t>
   </si>
   <si>
     <t>Gold (62 points) achieved March 2019</t>
+  </si>
+  <si>
+    <t>digital in FacMan SP; hardcopy not confirmed</t>
+  </si>
+  <si>
+    <t>updated to Fac Man SP; hardcopies not confirmed</t>
+  </si>
+  <si>
+    <t>many warranties loaded on SP, but not checked at equipment-level</t>
+  </si>
+  <si>
+    <t>many loaded and tagged on FM SP</t>
+  </si>
+  <si>
+    <t>loaded in FM SP</t>
+  </si>
+  <si>
+    <t>in Fac Man SP site; need to confirm hardcopy</t>
+  </si>
+  <si>
+    <t>in FacMan SP site</t>
+  </si>
+  <si>
+    <t>in FacMan SP site; not confirmed hardcopy location</t>
+  </si>
+  <si>
+    <t>parsed digitally in SP; need to confirm hardcopy</t>
+  </si>
+  <si>
+    <t>warranties in Op Manuals</t>
+  </si>
+  <si>
+    <t>minimal submittals only in SP</t>
+  </si>
+  <si>
+    <t>04-110654; 04-110712</t>
+  </si>
+  <si>
+    <t>digital in SP; Miramar-016 (record specs not complete for park structure)</t>
+  </si>
+  <si>
+    <t>as-builts are in SP; Miramar-021; 024-025; 042-043; 045-052</t>
+  </si>
+  <si>
+    <t>Site Piping Plan sheet is password-protected</t>
+  </si>
+  <si>
+    <t>OM's are saved digitally on file, but may not be complete (i.e. Electrical seems short)</t>
+  </si>
+  <si>
+    <t>combined-warranty-file-in-SP</t>
   </si>
 </sst>
 </file>
@@ -5223,14 +5265,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="344">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="346">
     <dxf>
       <fill>
         <patternFill>
@@ -7632,6 +7667,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7878,7 +7934,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3/19/2019</c:v>
+                  <c:v>3/26/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9637,7 +9693,8 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1605" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -9653,7 +9710,7 @@
     <col min="9" max="9" width="3.46484375" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.19921875" style="1" customWidth="1"/>
     <col min="11" max="11" width="6.59765625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.06640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.3984375" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
     <col min="14" max="14" width="9.73046875" style="1" customWidth="1"/>
     <col min="15" max="15" width="7.265625" style="1" customWidth="1"/>
@@ -9960,7 +10017,7 @@
         <v>170</v>
       </c>
       <c r="J2" s="119" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="K2" s="52" t="s">
         <v>166</v>
@@ -10131,7 +10188,7 @@
         <v>170</v>
       </c>
       <c r="J3" s="119" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="K3" s="52" t="s">
         <v>166</v>
@@ -10302,13 +10359,13 @@
         <v>166</v>
       </c>
       <c r="J4" s="118" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
       <c r="K4" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="M4" s="13" t="s">
         <v>567</v>
@@ -10694,7 +10751,7 @@
         <v>567</v>
       </c>
       <c r="Z6" s="118" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="AA6" s="52" t="s">
         <v>166</v>
@@ -10716,7 +10773,7 @@
         <v>166</v>
       </c>
       <c r="AH6" s="118" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="AI6" s="48" t="s">
         <v>170</v>
@@ -10829,7 +10886,7 @@
         <v>1112</v>
       </c>
       <c r="H7" s="118" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="I7" s="145" t="s">
         <v>1116</v>
@@ -10839,7 +10896,7 @@
         <v>166</v>
       </c>
       <c r="L7" s="52" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="M7" s="13" t="s">
         <v>567</v>
@@ -11008,13 +11065,13 @@
         <v>166</v>
       </c>
       <c r="J8" s="118" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
       <c r="K8" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L8" s="52" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="M8" s="13" t="s">
         <v>567</v>
@@ -11247,7 +11304,7 @@
         <v>166</v>
       </c>
       <c r="AH9" s="118" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="AI9" s="118" t="s">
         <v>567</v>
@@ -11694,7 +11751,7 @@
         <v>170</v>
       </c>
       <c r="J12" s="118" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="K12" s="118" t="s">
         <v>567</v>
@@ -12030,13 +12087,13 @@
         <v>170</v>
       </c>
       <c r="J14" s="118" t="s">
-        <v>1356</v>
-      </c>
-      <c r="K14" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L14" s="146" t="s">
-        <v>1345</v>
+        <v>1355</v>
+      </c>
+      <c r="K14" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>1360</v>
       </c>
       <c r="M14" s="48" t="s">
         <v>170</v>
@@ -12070,18 +12127,20 @@
         <v>166</v>
       </c>
       <c r="X14" s="118" t="s">
-        <v>1359</v>
+        <v>1361</v>
       </c>
       <c r="Y14" s="146" t="s">
         <v>1112</v>
       </c>
       <c r="Z14" s="118" t="s">
-        <v>1360</v>
+        <v>1362</v>
       </c>
       <c r="AA14" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="AB14" s="118"/>
+      <c r="AB14" s="118" t="s">
+        <v>1363</v>
+      </c>
       <c r="AC14" s="118" t="s">
         <v>567</v>
       </c>
@@ -12102,10 +12161,12 @@
       <c r="AJ14" s="118" t="s">
         <v>1190</v>
       </c>
-      <c r="AK14" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="AL14" s="118"/>
+      <c r="AK14" s="150" t="s">
+        <v>166</v>
+      </c>
+      <c r="AL14" s="118" t="s">
+        <v>1364</v>
+      </c>
       <c r="AM14" s="118" t="s">
         <v>567</v>
       </c>
@@ -12195,7 +12256,7 @@
         <v>170</v>
       </c>
       <c r="J15" s="118" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="K15" s="118" t="s">
         <v>567</v>
@@ -13040,8 +13101,8 @@
       <c r="J20" s="118" t="s">
         <v>420</v>
       </c>
-      <c r="K20" s="146" t="s">
-        <v>1112</v>
+      <c r="K20" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L20" s="13" t="s">
         <v>1140</v>
@@ -13076,23 +13137,23 @@
       <c r="V20" s="118">
         <v>1</v>
       </c>
-      <c r="W20" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X20" s="118">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z20" s="118">
-        <v>1</v>
+      <c r="W20" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="X20" s="118" t="s">
+        <v>1368</v>
+      </c>
+      <c r="Y20" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="Z20" s="118" t="s">
+        <v>1369</v>
       </c>
       <c r="AA20" s="48" t="s">
         <v>170</v>
       </c>
       <c r="AB20" s="118" t="s">
-        <v>1298</v>
+        <v>1370</v>
       </c>
       <c r="AC20" s="118" t="s">
         <v>567</v>
@@ -13861,7 +13922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:82" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B25" s="13" t="s">
         <v>86</v>
       </c>
@@ -13885,13 +13946,13 @@
         <v>170</v>
       </c>
       <c r="J25" s="118" t="s">
-        <v>1356</v>
-      </c>
-      <c r="K25" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L25" s="146" t="s">
-        <v>1346</v>
+        <v>1355</v>
+      </c>
+      <c r="K25" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>1373</v>
       </c>
       <c r="M25" s="52" t="s">
         <v>166</v>
@@ -14201,7 +14262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -14543,7 +14604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B29" s="13" t="s">
         <v>86</v>
       </c>
@@ -14714,7 +14775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B30" s="13" t="s">
         <v>86</v>
       </c>
@@ -14732,7 +14793,7 @@
         <v>166</v>
       </c>
       <c r="H30" s="118" t="s">
-        <v>447</v>
+        <v>1371</v>
       </c>
       <c r="I30" s="52" t="s">
         <v>166</v>
@@ -14740,11 +14801,11 @@
       <c r="J30" s="118" t="s">
         <v>421</v>
       </c>
-      <c r="K30" s="118" t="s">
-        <v>567</v>
+      <c r="K30" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L30" s="52" t="s">
-        <v>497</v>
+        <v>1372</v>
       </c>
       <c r="M30" s="52" t="s">
         <v>166</v>
@@ -15048,7 +15109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:82" s="18" customFormat="1" ht="39.4" x14ac:dyDescent="0.35">
       <c r="B32" s="13" t="s">
         <v>86</v>
       </c>
@@ -15072,13 +15133,13 @@
         <v>170</v>
       </c>
       <c r="J32" s="118" t="s">
-        <v>1356</v>
-      </c>
-      <c r="K32" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L32" s="146" t="s">
-        <v>1345</v>
+        <v>1355</v>
+      </c>
+      <c r="K32" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>1374</v>
       </c>
       <c r="M32" s="52" t="s">
         <v>166</v>
@@ -15108,17 +15169,17 @@
       <c r="V32" s="118">
         <v>1</v>
       </c>
-      <c r="W32" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X32" s="118">
-        <v>1</v>
-      </c>
-      <c r="Y32" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z32" s="118">
-        <v>1</v>
+      <c r="W32" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="X32" s="118" t="s">
+        <v>1375</v>
+      </c>
+      <c r="Y32" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z32" s="118" t="s">
+        <v>1376</v>
       </c>
       <c r="AA32" s="48" t="s">
         <v>170</v>
@@ -15577,7 +15638,7 @@
         <v>170</v>
       </c>
       <c r="J35" s="119" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="K35" s="118" t="s">
         <v>567</v>
@@ -15742,7 +15803,7 @@
         <v>170</v>
       </c>
       <c r="J36" s="118" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="K36" s="118" t="s">
         <v>567</v>
@@ -17172,7 +17233,7 @@
         <v>166</v>
       </c>
       <c r="T44" s="118" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="U44" s="118" t="s">
         <v>567</v>
@@ -18140,7 +18201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B50" s="13" t="s">
         <v>4</v>
       </c>
@@ -18343,7 +18404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B51" s="13" t="s">
         <v>4</v>
       </c>
@@ -18530,7 +18591,7 @@
         <v>166</v>
       </c>
       <c r="H52" s="118" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="I52" s="52" t="s">
         <v>166</v>
@@ -19898,7 +19959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B60" s="13" t="s">
         <v>4</v>
       </c>
@@ -19924,11 +19985,11 @@
       <c r="J60" s="118" t="s">
         <v>419</v>
       </c>
-      <c r="K60" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L60" s="146" t="s">
-        <v>1345</v>
+      <c r="K60" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L60" s="13" t="s">
+        <v>1367</v>
       </c>
       <c r="M60" s="52" t="s">
         <v>166</v>
@@ -19958,17 +20019,17 @@
       <c r="V60" s="118">
         <v>1</v>
       </c>
-      <c r="W60" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X60" s="118">
-        <v>1</v>
-      </c>
-      <c r="Y60" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z60" s="118">
-        <v>1</v>
+      <c r="W60" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="X60" s="118" t="s">
+        <v>1365</v>
+      </c>
+      <c r="Y60" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z60" s="118" t="s">
+        <v>1366</v>
       </c>
       <c r="AA60" s="52" t="s">
         <v>166</v>
@@ -20123,11 +20184,11 @@
       <c r="V61" s="118">
         <v>1</v>
       </c>
-      <c r="W61" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X61" s="118">
-        <v>1</v>
+      <c r="W61" s="145" t="s">
+        <v>1116</v>
+      </c>
+      <c r="X61" s="13" t="s">
+        <v>1305</v>
       </c>
       <c r="Y61" s="118" t="s">
         <v>567</v>
@@ -23173,7 +23234,7 @@
         <v>170</v>
       </c>
       <c r="L79" s="52" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="M79" s="48" t="s">
         <v>170</v>
@@ -24676,1381 +24737,1393 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
+    <cfRule type="cellIs" dxfId="345" priority="284" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BI9:BJ9">
+    <cfRule type="cellIs" dxfId="344" priority="283" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
     <cfRule type="cellIs" dxfId="343" priority="282" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BI9:BJ9">
+  <conditionalFormatting sqref="AV39 AV56">
     <cfRule type="cellIs" dxfId="342" priority="281" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="341" priority="280" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
+    <cfRule type="cellIs" dxfId="341" priority="279" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="340" priority="279" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
+    <cfRule type="cellIs" dxfId="340" priority="278" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
+  <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
     <cfRule type="cellIs" dxfId="339" priority="277" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="338" priority="276" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="337" priority="275" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="336" priority="271" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="338" priority="273" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="335" priority="261" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="337" priority="263" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I3 I44 I14 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="334" priority="248" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="336" priority="250" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="333" priority="237" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="335" priority="239" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
+    <cfRule type="cellIs" dxfId="334" priority="236" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CD2">
+    <cfRule type="cellIs" dxfId="333" priority="235" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K41:K44 K63 K77:K82 K23 K68:K74 K28:K29 K46:K51 K10 K33:K38 K12 K53:K54 K15:K18 K57 K31">
     <cfRule type="cellIs" dxfId="332" priority="234" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CD2">
+  <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
     <cfRule type="cellIs" dxfId="331" priority="233" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K44 K63 K77:K82 K23 K68:K74 K28:K31 K46:K51 K10 K60 K33:K38 K12 K53:K54 K14:K18 K57">
+  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L85 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5">
     <cfRule type="cellIs" dxfId="330" priority="232" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
+  <conditionalFormatting sqref="I35">
     <cfRule type="cellIs" dxfId="329" priority="231" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L85 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5">
-    <cfRule type="cellIs" dxfId="328" priority="230" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="327" priority="229" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="326" priority="226" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="328" priority="228" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="325" priority="225" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="327" priority="227" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="324" priority="223" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="326" priority="225" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="323" priority="221" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="325" priority="223" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
+    <cfRule type="cellIs" dxfId="324" priority="221" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+    <cfRule type="cellIs" dxfId="323" priority="220" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q86">
     <cfRule type="cellIs" dxfId="322" priority="219" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
     <cfRule type="cellIs" dxfId="321" priority="218" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q86">
+  <conditionalFormatting sqref="AE2:AE86">
     <cfRule type="cellIs" dxfId="320" priority="217" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
+  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
     <cfRule type="cellIs" dxfId="319" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE86">
+  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
     <cfRule type="cellIs" dxfId="318" priority="215" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
+  <conditionalFormatting sqref="AK2:AK13 AK15:AK86">
     <cfRule type="cellIs" dxfId="317" priority="214" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
+  <conditionalFormatting sqref="AM2:AM86">
     <cfRule type="cellIs" dxfId="316" priority="213" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK86">
+  <conditionalFormatting sqref="N46">
     <cfRule type="cellIs" dxfId="315" priority="212" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AM86">
+  <conditionalFormatting sqref="N9">
     <cfRule type="cellIs" dxfId="314" priority="211" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46">
+  <conditionalFormatting sqref="N6">
     <cfRule type="cellIs" dxfId="313" priority="210" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9">
+  <conditionalFormatting sqref="N48">
     <cfRule type="cellIs" dxfId="312" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6">
+  <conditionalFormatting sqref="N45">
     <cfRule type="cellIs" dxfId="311" priority="208" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N48">
+  <conditionalFormatting sqref="N50">
     <cfRule type="cellIs" dxfId="310" priority="207" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N45">
+  <conditionalFormatting sqref="N5">
     <cfRule type="cellIs" dxfId="309" priority="206" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N2">
     <cfRule type="cellIs" dxfId="308" priority="205" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
+  <conditionalFormatting sqref="N3">
     <cfRule type="cellIs" dxfId="307" priority="204" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
+  <conditionalFormatting sqref="N10">
     <cfRule type="cellIs" dxfId="306" priority="203" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="305" priority="202" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N52">
+    <cfRule type="cellIs" dxfId="305" priority="199" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="304" priority="201" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N16">
+    <cfRule type="cellIs" dxfId="304" priority="198" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
+  <conditionalFormatting sqref="N60">
     <cfRule type="cellIs" dxfId="303" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
+  <conditionalFormatting sqref="M14:N14">
     <cfRule type="cellIs" dxfId="302" priority="196" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N60">
+  <conditionalFormatting sqref="M34">
     <cfRule type="cellIs" dxfId="301" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:N14">
+  <conditionalFormatting sqref="N26">
     <cfRule type="cellIs" dxfId="300" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M34">
+  <conditionalFormatting sqref="M26">
     <cfRule type="cellIs" dxfId="299" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
+  <conditionalFormatting sqref="N28">
     <cfRule type="cellIs" dxfId="298" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
+  <conditionalFormatting sqref="M68">
     <cfRule type="cellIs" dxfId="297" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
+  <conditionalFormatting sqref="AJ43">
     <cfRule type="cellIs" dxfId="296" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M68">
+  <conditionalFormatting sqref="AI43">
     <cfRule type="cellIs" dxfId="295" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ43">
+  <conditionalFormatting sqref="AJ3">
     <cfRule type="cellIs" dxfId="294" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI43">
+  <conditionalFormatting sqref="AI3">
     <cfRule type="cellIs" dxfId="293" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ3">
+  <conditionalFormatting sqref="AJ4">
     <cfRule type="cellIs" dxfId="292" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI3">
+  <conditionalFormatting sqref="AI4">
     <cfRule type="cellIs" dxfId="291" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ4">
+  <conditionalFormatting sqref="AJ5">
     <cfRule type="cellIs" dxfId="290" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI4">
+  <conditionalFormatting sqref="AI5">
     <cfRule type="cellIs" dxfId="289" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ5">
+  <conditionalFormatting sqref="AJ6">
     <cfRule type="cellIs" dxfId="288" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI5">
+  <conditionalFormatting sqref="AI6">
     <cfRule type="cellIs" dxfId="287" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ6">
+  <conditionalFormatting sqref="AJ7">
     <cfRule type="cellIs" dxfId="286" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI6">
+  <conditionalFormatting sqref="AI7">
     <cfRule type="cellIs" dxfId="285" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ7">
+  <conditionalFormatting sqref="AJ8:AJ9">
     <cfRule type="cellIs" dxfId="284" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI7">
+  <conditionalFormatting sqref="AI8">
     <cfRule type="cellIs" dxfId="283" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ8:AJ9">
+  <conditionalFormatting sqref="AJ46">
     <cfRule type="cellIs" dxfId="282" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI8">
+  <conditionalFormatting sqref="AI46">
     <cfRule type="cellIs" dxfId="281" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ46">
+  <conditionalFormatting sqref="AJ47">
     <cfRule type="cellIs" dxfId="280" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI46">
+  <conditionalFormatting sqref="AI47">
     <cfRule type="cellIs" dxfId="279" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ47">
+  <conditionalFormatting sqref="AJ10">
     <cfRule type="cellIs" dxfId="278" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI47">
+  <conditionalFormatting sqref="AI10">
     <cfRule type="cellIs" dxfId="277" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ10">
+  <conditionalFormatting sqref="AJ48">
     <cfRule type="cellIs" dxfId="276" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI10">
+  <conditionalFormatting sqref="AI48">
     <cfRule type="cellIs" dxfId="275" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ48">
+  <conditionalFormatting sqref="AJ49">
     <cfRule type="cellIs" dxfId="274" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI48">
+  <conditionalFormatting sqref="AI49">
     <cfRule type="cellIs" dxfId="273" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ49">
+  <conditionalFormatting sqref="AJ50">
     <cfRule type="cellIs" dxfId="272" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="271" priority="165" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI50">
+    <cfRule type="cellIs" dxfId="271" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="270" priority="164" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ11:AJ13">
+    <cfRule type="cellIs" dxfId="270" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI50">
+  <conditionalFormatting sqref="AI11">
     <cfRule type="cellIs" dxfId="269" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11:AJ13">
+  <conditionalFormatting sqref="AJ51">
     <cfRule type="cellIs" dxfId="268" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI11">
+  <conditionalFormatting sqref="AI52">
     <cfRule type="cellIs" dxfId="267" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ51">
+  <conditionalFormatting sqref="AJ52:AJ54">
     <cfRule type="cellIs" dxfId="266" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI52">
+  <conditionalFormatting sqref="AJ56">
     <cfRule type="cellIs" dxfId="265" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ52:AJ54">
+  <conditionalFormatting sqref="AI56">
     <cfRule type="cellIs" dxfId="264" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ56">
+  <conditionalFormatting sqref="AJ57:AJ58">
     <cfRule type="cellIs" dxfId="263" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI56">
+  <conditionalFormatting sqref="AI57:AI58">
     <cfRule type="cellIs" dxfId="262" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ57:AJ58">
+  <conditionalFormatting sqref="AJ15:AJ16">
     <cfRule type="cellIs" dxfId="261" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI57:AI58">
+  <conditionalFormatting sqref="AI15:AI16">
     <cfRule type="cellIs" dxfId="260" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15:AJ16">
+  <conditionalFormatting sqref="AJ59:AJ60">
     <cfRule type="cellIs" dxfId="259" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI15:AI16">
+  <conditionalFormatting sqref="AJ55">
     <cfRule type="cellIs" dxfId="258" priority="151" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ59:AJ60">
+  <conditionalFormatting sqref="AI19">
     <cfRule type="cellIs" dxfId="257" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ55">
+  <conditionalFormatting sqref="AJ19">
     <cfRule type="cellIs" dxfId="256" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI19">
+  <conditionalFormatting sqref="AI18">
     <cfRule type="cellIs" dxfId="255" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19">
+  <conditionalFormatting sqref="AJ18">
     <cfRule type="cellIs" dxfId="254" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI18">
+  <conditionalFormatting sqref="AI17">
     <cfRule type="cellIs" dxfId="253" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ18">
+  <conditionalFormatting sqref="AJ17">
     <cfRule type="cellIs" dxfId="252" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI17">
+  <conditionalFormatting sqref="AI86">
     <cfRule type="cellIs" dxfId="251" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ17">
+  <conditionalFormatting sqref="AI40">
     <cfRule type="cellIs" dxfId="250" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI86">
+  <conditionalFormatting sqref="AJ20">
     <cfRule type="cellIs" dxfId="249" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI40">
+  <conditionalFormatting sqref="AJ62">
     <cfRule type="cellIs" dxfId="248" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="247" priority="140" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="246" priority="139" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="245" priority="137" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
+    <cfRule type="cellIs" dxfId="246" priority="137" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI21">
+    <cfRule type="cellIs" dxfId="245" priority="136" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI64">
     <cfRule type="cellIs" dxfId="244" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI21">
+  <conditionalFormatting sqref="AI23">
     <cfRule type="cellIs" dxfId="243" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI64">
+  <conditionalFormatting sqref="AJ24">
     <cfRule type="cellIs" dxfId="242" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI23">
+  <conditionalFormatting sqref="AI25">
     <cfRule type="cellIs" dxfId="241" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ24">
+  <conditionalFormatting sqref="AJ25">
     <cfRule type="cellIs" dxfId="240" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI25">
+  <conditionalFormatting sqref="AJ67">
     <cfRule type="cellIs" dxfId="239" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ25">
+  <conditionalFormatting sqref="AI26">
     <cfRule type="cellIs" dxfId="238" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ67">
+  <conditionalFormatting sqref="AJ26:AJ27">
     <cfRule type="cellIs" dxfId="237" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI26">
+  <conditionalFormatting sqref="AI28:AI30">
     <cfRule type="cellIs" dxfId="236" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ26:AJ27">
+  <conditionalFormatting sqref="AJ28:AJ31">
     <cfRule type="cellIs" dxfId="235" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI28:AI30">
+  <conditionalFormatting sqref="AI72">
     <cfRule type="cellIs" dxfId="234" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ28:AJ31">
+  <conditionalFormatting sqref="AJ72">
     <cfRule type="cellIs" dxfId="233" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI72">
+  <conditionalFormatting sqref="AI73">
     <cfRule type="cellIs" dxfId="232" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ72">
+  <conditionalFormatting sqref="AJ73">
     <cfRule type="cellIs" dxfId="231" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI73">
+  <conditionalFormatting sqref="AI32">
     <cfRule type="cellIs" dxfId="230" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ73">
+  <conditionalFormatting sqref="AJ32">
     <cfRule type="cellIs" dxfId="229" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI32">
+  <conditionalFormatting sqref="AI33">
     <cfRule type="cellIs" dxfId="228" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ32">
+  <conditionalFormatting sqref="AJ33">
     <cfRule type="cellIs" dxfId="227" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI33">
+  <conditionalFormatting sqref="AI34:AI35">
     <cfRule type="cellIs" dxfId="226" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ33">
+  <conditionalFormatting sqref="AJ34:AJ36">
     <cfRule type="cellIs" dxfId="225" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI34:AI35">
+  <conditionalFormatting sqref="AI61">
     <cfRule type="cellIs" dxfId="224" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ34:AJ36">
+  <conditionalFormatting sqref="AI63">
     <cfRule type="cellIs" dxfId="223" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI61">
+  <conditionalFormatting sqref="AJ70">
     <cfRule type="cellIs" dxfId="222" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI63">
+  <conditionalFormatting sqref="AI70">
     <cfRule type="cellIs" dxfId="221" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ70">
+  <conditionalFormatting sqref="AI68">
     <cfRule type="cellIs" dxfId="220" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI70">
+  <conditionalFormatting sqref="AJ76">
     <cfRule type="cellIs" dxfId="219" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI68">
+  <conditionalFormatting sqref="AI76">
     <cfRule type="cellIs" dxfId="218" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ76">
+  <conditionalFormatting sqref="AJ78">
     <cfRule type="cellIs" dxfId="217" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI76">
+  <conditionalFormatting sqref="AI78">
     <cfRule type="cellIs" dxfId="216" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ78">
+  <conditionalFormatting sqref="AJ38">
     <cfRule type="cellIs" dxfId="215" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI78">
+  <conditionalFormatting sqref="AI38">
     <cfRule type="cellIs" dxfId="214" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ38">
+  <conditionalFormatting sqref="AJ77">
     <cfRule type="cellIs" dxfId="213" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI38">
+  <conditionalFormatting sqref="AI77">
     <cfRule type="cellIs" dxfId="212" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ77">
+  <conditionalFormatting sqref="AJ79">
     <cfRule type="cellIs" dxfId="211" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI77">
+  <conditionalFormatting sqref="AI79">
     <cfRule type="cellIs" dxfId="210" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ79">
+  <conditionalFormatting sqref="AJ80">
     <cfRule type="cellIs" dxfId="209" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI79">
+  <conditionalFormatting sqref="AI80">
     <cfRule type="cellIs" dxfId="208" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ80">
+  <conditionalFormatting sqref="AJ81">
     <cfRule type="cellIs" dxfId="207" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI80">
+  <conditionalFormatting sqref="AI81">
     <cfRule type="cellIs" dxfId="206" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ81">
+  <conditionalFormatting sqref="AJ82">
     <cfRule type="cellIs" dxfId="205" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI81">
+  <conditionalFormatting sqref="AI82">
     <cfRule type="cellIs" dxfId="204" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ82">
+  <conditionalFormatting sqref="AI83">
     <cfRule type="cellIs" dxfId="203" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI82">
+  <conditionalFormatting sqref="AI84:AI85">
     <cfRule type="cellIs" dxfId="202" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI83">
+  <conditionalFormatting sqref="AI39">
     <cfRule type="cellIs" dxfId="201" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI84:AI85">
+  <conditionalFormatting sqref="J31">
     <cfRule type="cellIs" dxfId="200" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI39">
+  <conditionalFormatting sqref="O61">
     <cfRule type="cellIs" dxfId="199" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
+  <conditionalFormatting sqref="O54">
     <cfRule type="cellIs" dxfId="198" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O61">
+  <conditionalFormatting sqref="O57">
     <cfRule type="cellIs" dxfId="197" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O54">
+  <conditionalFormatting sqref="O58">
     <cfRule type="cellIs" dxfId="196" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O57">
+  <conditionalFormatting sqref="O67">
     <cfRule type="cellIs" dxfId="195" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O58">
+  <conditionalFormatting sqref="O71">
     <cfRule type="cellIs" dxfId="194" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O67">
+  <conditionalFormatting sqref="O72">
     <cfRule type="cellIs" dxfId="193" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O71">
+  <conditionalFormatting sqref="O80">
     <cfRule type="cellIs" dxfId="192" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O72">
+  <conditionalFormatting sqref="O82">
     <cfRule type="cellIs" dxfId="191" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80">
+  <conditionalFormatting sqref="K62">
     <cfRule type="cellIs" dxfId="190" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82">
+  <conditionalFormatting sqref="L62">
     <cfRule type="cellIs" dxfId="189" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="cellIs" dxfId="188" priority="79" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L75">
+    <cfRule type="cellIs" dxfId="188" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="187" priority="78" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI12">
+    <cfRule type="cellIs" dxfId="187" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L75">
+  <conditionalFormatting sqref="X2">
     <cfRule type="cellIs" dxfId="186" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI12">
+  <conditionalFormatting sqref="W4:W5 W7:W13 W15:W19 W62:W86 W21:W59">
     <cfRule type="cellIs" dxfId="185" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
+  <conditionalFormatting sqref="AB2">
     <cfRule type="cellIs" dxfId="184" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W4:W5 W7:W13 W15:W86">
+  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
     <cfRule type="cellIs" dxfId="183" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2">
+  <conditionalFormatting sqref="Z2">
     <cfRule type="cellIs" dxfId="182" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
+  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y86 Y33:Y59">
     <cfRule type="cellIs" dxfId="181" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2">
+  <conditionalFormatting sqref="AD2">
     <cfRule type="cellIs" dxfId="180" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y13 Y15:Y86">
+  <conditionalFormatting sqref="AC2:AC86">
     <cfRule type="cellIs" dxfId="179" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2">
+  <conditionalFormatting sqref="V2">
     <cfRule type="cellIs" dxfId="178" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC86">
+  <conditionalFormatting sqref="U2:U86">
     <cfRule type="cellIs" dxfId="177" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2">
+  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
     <cfRule type="cellIs" dxfId="176" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U86">
+  <conditionalFormatting sqref="AA48">
     <cfRule type="cellIs" dxfId="175" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
+  <conditionalFormatting sqref="AA11">
     <cfRule type="cellIs" dxfId="174" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA48">
+  <conditionalFormatting sqref="AA51">
     <cfRule type="cellIs" dxfId="173" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA11">
+  <conditionalFormatting sqref="AA52">
     <cfRule type="cellIs" dxfId="172" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA51">
+  <conditionalFormatting sqref="AA53">
     <cfRule type="cellIs" dxfId="171" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA52">
+  <conditionalFormatting sqref="AA57 AA54:AA55">
     <cfRule type="cellIs" dxfId="170" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA53">
+  <conditionalFormatting sqref="AA20">
     <cfRule type="cellIs" dxfId="169" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA57 AA54:AA55">
+  <conditionalFormatting sqref="AA21">
     <cfRule type="cellIs" dxfId="168" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA20">
+  <conditionalFormatting sqref="AA66">
     <cfRule type="cellIs" dxfId="167" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA21">
+  <conditionalFormatting sqref="AA25">
     <cfRule type="cellIs" dxfId="166" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA66">
+  <conditionalFormatting sqref="AA26">
     <cfRule type="cellIs" dxfId="165" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA25">
+  <conditionalFormatting sqref="AA28">
     <cfRule type="cellIs" dxfId="164" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA26">
+  <conditionalFormatting sqref="AA32">
     <cfRule type="cellIs" dxfId="163" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA28">
+  <conditionalFormatting sqref="AA34">
     <cfRule type="cellIs" dxfId="162" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA32">
+  <conditionalFormatting sqref="AA27">
     <cfRule type="cellIs" dxfId="161" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA34">
+  <conditionalFormatting sqref="AA33 AA31">
     <cfRule type="cellIs" dxfId="160" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA27">
+  <conditionalFormatting sqref="AA61 M61">
     <cfRule type="cellIs" dxfId="159" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA33 AA31">
+  <conditionalFormatting sqref="AA62">
     <cfRule type="cellIs" dxfId="158" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA61 M61">
+  <conditionalFormatting sqref="AA63 M63">
     <cfRule type="cellIs" dxfId="157" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA62">
+  <conditionalFormatting sqref="AA65">
     <cfRule type="cellIs" dxfId="156" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA63 M63">
+  <conditionalFormatting sqref="AA67">
     <cfRule type="cellIs" dxfId="155" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA65">
+  <conditionalFormatting sqref="AA68">
     <cfRule type="cellIs" dxfId="154" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA67">
+  <conditionalFormatting sqref="AA70:AA73">
     <cfRule type="cellIs" dxfId="153" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA68">
+  <conditionalFormatting sqref="AA77">
     <cfRule type="cellIs" dxfId="152" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA70:AA73">
+  <conditionalFormatting sqref="AA74 AA38">
     <cfRule type="cellIs" dxfId="151" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA77">
+  <conditionalFormatting sqref="AA37">
     <cfRule type="cellIs" dxfId="150" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA74 AA38">
+  <conditionalFormatting sqref="S9">
     <cfRule type="cellIs" dxfId="149" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA37">
+  <conditionalFormatting sqref="S46">
     <cfRule type="cellIs" dxfId="148" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
+  <conditionalFormatting sqref="S48">
     <cfRule type="cellIs" dxfId="147" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S46">
+  <conditionalFormatting sqref="S18">
     <cfRule type="cellIs" dxfId="146" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48">
+  <conditionalFormatting sqref="S54">
     <cfRule type="cellIs" dxfId="145" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
+  <conditionalFormatting sqref="S55">
     <cfRule type="cellIs" dxfId="144" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S54">
+  <conditionalFormatting sqref="S57">
     <cfRule type="cellIs" dxfId="143" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S55">
+  <conditionalFormatting sqref="S76">
     <cfRule type="cellIs" dxfId="142" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S57">
+  <conditionalFormatting sqref="S78">
     <cfRule type="cellIs" dxfId="141" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S76">
+  <conditionalFormatting sqref="S81">
     <cfRule type="cellIs" dxfId="140" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S78">
+  <conditionalFormatting sqref="S82">
     <cfRule type="cellIs" dxfId="139" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S81">
+  <conditionalFormatting sqref="J32">
     <cfRule type="cellIs" dxfId="138" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S82">
+  <conditionalFormatting sqref="K66">
     <cfRule type="cellIs" dxfId="137" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
+  <conditionalFormatting sqref="L67">
     <cfRule type="cellIs" dxfId="136" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="135" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L67">
+  <conditionalFormatting sqref="L27">
     <cfRule type="cellIs" dxfId="134" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="G7">
     <cfRule type="cellIs" dxfId="133" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="132" priority="22" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G20">
+    <cfRule type="cellIs" dxfId="132" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="131" priority="21" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="131" priority="20" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
+  <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" dxfId="130" priority="19" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
+  <conditionalFormatting sqref="X3">
     <cfRule type="cellIs" dxfId="129" priority="18" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="128" priority="17" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L13">
+    <cfRule type="cellIs" dxfId="128" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3">
-    <cfRule type="cellIs" dxfId="127" priority="16" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L55">
+    <cfRule type="cellIs" dxfId="127" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
+  <conditionalFormatting sqref="L56">
     <cfRule type="cellIs" dxfId="126" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L55">
+  <conditionalFormatting sqref="L14">
     <cfRule type="cellIs" dxfId="125" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
+  <conditionalFormatting sqref="L60">
     <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
+  <conditionalFormatting sqref="K76">
     <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L60">
+  <conditionalFormatting sqref="L76">
     <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
+  <conditionalFormatting sqref="L6">
     <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76">
+  <conditionalFormatting sqref="L7">
     <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
+  <conditionalFormatting sqref="L8">
     <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
+  <conditionalFormatting sqref="L9">
     <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
+  <conditionalFormatting sqref="Y14">
     <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9">
+  <conditionalFormatting sqref="J4">
     <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y14">
+  <conditionalFormatting sqref="AK14">
     <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="X61">
+    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -46912,448 +46985,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="114" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="113" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="112" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="111" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="110" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="109" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="108" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="107" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="106" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="105" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="104" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="103" priority="93">
+    <cfRule type="containsBlanks" dxfId="102" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="102" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="101" priority="91">
+    <cfRule type="containsBlanks" dxfId="100" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="100" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="99" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="98" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="97" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="96" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="95" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="94" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="93" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="92" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="91" priority="69">
+    <cfRule type="containsBlanks" dxfId="90" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="89" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="88" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="87" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="86" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="85" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="84" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="83" priority="63">
+    <cfRule type="containsBlanks" dxfId="82" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="82" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="81" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="80" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="79" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="78" priority="59">
+    <cfRule type="containsBlanks" dxfId="77" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="77" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="76" priority="56">
+    <cfRule type="containsBlanks" dxfId="75" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="75" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="74" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="73" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="72" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="71" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="70" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="69" priority="50">
+    <cfRule type="containsBlanks" dxfId="68" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="68" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="67" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="66" priority="47">
+    <cfRule type="containsBlanks" dxfId="65" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="65" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="64" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="63" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="62" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="61" priority="42">
+    <cfRule type="containsBlanks" dxfId="60" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="60" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="59" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="58" priority="39">
+    <cfRule type="containsBlanks" dxfId="57" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="57" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="56" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="55" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="53" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="52" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="51" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="50" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="49" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="47" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="46" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="44" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="43" priority="23">
+    <cfRule type="containsBlanks" dxfId="42" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="41" priority="19">
+    <cfRule type="containsBlanks" dxfId="40" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="38" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="37" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="34" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="32" priority="22">
+    <cfRule type="containsBlanks" dxfId="31" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="31" priority="11">
+    <cfRule type="containsBlanks" dxfId="30" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -62248,111 +62321,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="20" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="18" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="17" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="15" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="14" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="13" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="12" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="10" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -63676,7 +63749,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43543</v>
+        <v>43550</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -64025,7 +64098,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43543</v>
+        <v>43550</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -68032,7 +68105,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated record drawing status info
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4179CE-BB0C-4EFA-8A9E-2292E4BD023E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C20B89E-7A40-43AE-8881-A8D77918D35C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8989" uniqueCount="1377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8993" uniqueCount="1382">
   <si>
     <t>#</t>
   </si>
@@ -4176,6 +4176,21 @@
   </si>
   <si>
     <t>combined-warranty-file-in-SP</t>
+  </si>
+  <si>
+    <t>OM's Vols1-4 digitally in SP</t>
+  </si>
+  <si>
+    <t>04-111476</t>
+  </si>
+  <si>
+    <t>digitally in SP 4/24/19</t>
+  </si>
+  <si>
+    <t>see #11220; S</t>
+  </si>
+  <si>
+    <t>Yes, on SP, but not divided (5/10/19)</t>
   </si>
 </sst>
 </file>
@@ -5265,7 +5280,21 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="346">
+  <dxfs count="350">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7688,6 +7717,20 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7934,7 +7977,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4/9/2019</c:v>
+                  <c:v>5/10/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9691,10 +9734,10 @@
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1605" activePane="bottomLeft"/>
-      <selection activeCell="Y1" sqref="Y1"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection activeCell="G1" sqref="G1:CE1048576"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -12765,10 +12808,12 @@
       <c r="J18" s="118" t="s">
         <v>1134</v>
       </c>
-      <c r="K18" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="L18" s="13"/>
+      <c r="K18" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>1381</v>
+      </c>
       <c r="M18" s="48" t="s">
         <v>170</v>
       </c>
@@ -13274,8 +13319,8 @@
       <c r="J21" s="118" t="s">
         <v>419</v>
       </c>
-      <c r="K21" s="146" t="s">
-        <v>1112</v>
+      <c r="K21" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L21" s="13" t="s">
         <v>1140</v>
@@ -13449,12 +13494,10 @@
       <c r="J22" s="118" t="s">
         <v>1134</v>
       </c>
-      <c r="K22" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L22" s="146" t="s">
-        <v>1345</v>
-      </c>
+      <c r="K22" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="L22" s="146"/>
       <c r="M22" s="52" t="s">
         <v>166</v>
       </c>
@@ -14288,8 +14331,8 @@
       <c r="J27" s="118" t="s">
         <v>418</v>
       </c>
-      <c r="K27" s="146" t="s">
-        <v>1112</v>
+      <c r="K27" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L27" s="13" t="s">
         <v>1140</v>
@@ -14459,8 +14502,8 @@
       <c r="J28" s="118" t="s">
         <v>418</v>
       </c>
-      <c r="K28" s="118" t="s">
-        <v>567</v>
+      <c r="K28" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L28" s="13"/>
       <c r="M28" s="52" t="s">
@@ -15469,8 +15512,8 @@
       <c r="J34" s="118" t="s">
         <v>418</v>
       </c>
-      <c r="K34" s="118" t="s">
-        <v>567</v>
+      <c r="K34" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L34" s="13"/>
       <c r="M34" s="48" t="s">
@@ -15672,11 +15715,11 @@
       <c r="V35" s="118">
         <v>1</v>
       </c>
-      <c r="W35" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X35" s="118">
-        <v>1</v>
+      <c r="W35" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="X35" s="118" t="s">
+        <v>1377</v>
       </c>
       <c r="Y35" s="118" t="s">
         <v>567</v>
@@ -17010,10 +17053,12 @@
       <c r="J43" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="K43" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="L43" s="19"/>
+      <c r="K43" s="145" t="s">
+        <v>1116</v>
+      </c>
+      <c r="L43" s="19" t="s">
+        <v>1380</v>
+      </c>
       <c r="M43" s="145" t="s">
         <v>1116</v>
       </c>
@@ -17551,8 +17596,8 @@
       <c r="J46" s="118" t="s">
         <v>1223</v>
       </c>
-      <c r="K46" s="146" t="s">
-        <v>1112</v>
+      <c r="K46" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L46" s="13" t="s">
         <v>1138</v>
@@ -17889,8 +17934,8 @@
       <c r="J48" s="118" t="s">
         <v>419</v>
       </c>
-      <c r="K48" s="146" t="s">
-        <v>1112</v>
+      <c r="K48" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L48" s="13" t="s">
         <v>1138</v>
@@ -18227,8 +18272,8 @@
       <c r="J50" s="118" t="s">
         <v>419</v>
       </c>
-      <c r="K50" s="146" t="s">
-        <v>1112</v>
+      <c r="K50" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L50" s="13" t="s">
         <v>1140</v>
@@ -18430,8 +18475,8 @@
       <c r="J51" s="118" t="s">
         <v>418</v>
       </c>
-      <c r="K51" s="146" t="s">
-        <v>1112</v>
+      <c r="K51" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L51" s="13" t="s">
         <v>1140</v>
@@ -18937,8 +18982,8 @@
       <c r="J54" s="118" t="s">
         <v>1223</v>
       </c>
-      <c r="K54" s="48" t="s">
-        <v>170</v>
+      <c r="K54" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L54" s="13"/>
       <c r="M54" s="118" t="s">
@@ -20315,8 +20360,8 @@
       <c r="J62" s="118" t="s">
         <v>419</v>
       </c>
-      <c r="K62" s="146" t="s">
-        <v>1112</v>
+      <c r="K62" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L62" s="13" t="s">
         <v>1138</v>
@@ -22508,11 +22553,11 @@
       <c r="F75" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="145" t="s">
-        <v>1116</v>
+      <c r="G75" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H75" s="118" t="s">
-        <v>17</v>
+        <v>1378</v>
       </c>
       <c r="I75" s="52" t="s">
         <v>166</v>
@@ -22552,17 +22597,17 @@
       <c r="V75" s="118">
         <v>1</v>
       </c>
-      <c r="W75" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X75" s="118">
-        <v>1</v>
-      </c>
-      <c r="Y75" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z75" s="118">
-        <v>1</v>
+      <c r="W75" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="X75" s="118" t="s">
+        <v>1379</v>
+      </c>
+      <c r="Y75" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z75" s="118" t="s">
+        <v>1379</v>
       </c>
       <c r="AA75" s="145" t="s">
         <v>1116</v>
@@ -22721,8 +22766,8 @@
       <c r="J76" s="118" t="s">
         <v>444</v>
       </c>
-      <c r="K76" s="146" t="s">
-        <v>1112</v>
+      <c r="K76" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="L76" s="146" t="s">
         <v>1345</v>
@@ -24737,1393 +24782,1405 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
-    <cfRule type="cellIs" dxfId="345" priority="284" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="349" priority="288" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI9:BJ9">
-    <cfRule type="cellIs" dxfId="344" priority="283" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="348" priority="287" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="343" priority="282" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="347" priority="286" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="342" priority="281" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="346" priority="285" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
-    <cfRule type="cellIs" dxfId="341" priority="279" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="345" priority="283" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="340" priority="278" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="344" priority="282" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="339" priority="277" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="343" priority="281" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="338" priority="273" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="342" priority="277" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="337" priority="263" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="341" priority="267" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I3 I44 I14 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="336" priority="250" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="340" priority="254" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="335" priority="239" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="339" priority="243" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
+    <cfRule type="cellIs" dxfId="338" priority="240" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CD2">
+    <cfRule type="cellIs" dxfId="337" priority="239" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K41:K42 K63 K77:K82 K68:K74 K29 K47 K10 K33 K12 K53 K15:K17 K57 K31 K44 K49 K35:K38">
+    <cfRule type="cellIs" dxfId="336" priority="238" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
+    <cfRule type="cellIs" dxfId="335" priority="237" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L85 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5">
     <cfRule type="cellIs" dxfId="334" priority="236" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CD2">
+  <conditionalFormatting sqref="I35">
     <cfRule type="cellIs" dxfId="333" priority="235" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K44 K63 K77:K82 K68:K74 K28:K29 K46:K51 K10 K33:K38 K12 K53:K54 K15:K18 K57 K31">
-    <cfRule type="cellIs" dxfId="332" priority="234" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
-    <cfRule type="cellIs" dxfId="331" priority="233" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L85 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5">
-    <cfRule type="cellIs" dxfId="330" priority="232" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="329" priority="231" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="328" priority="228" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="332" priority="232" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="327" priority="227" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="331" priority="231" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="326" priority="225" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="330" priority="229" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="325" priority="223" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="329" priority="227" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
+    <cfRule type="cellIs" dxfId="328" priority="225" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+    <cfRule type="cellIs" dxfId="327" priority="224" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q86">
+    <cfRule type="cellIs" dxfId="326" priority="223" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
+    <cfRule type="cellIs" dxfId="325" priority="222" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2:AE86">
     <cfRule type="cellIs" dxfId="324" priority="221" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
     <cfRule type="cellIs" dxfId="323" priority="220" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q86">
+  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
     <cfRule type="cellIs" dxfId="322" priority="219" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
+  <conditionalFormatting sqref="AK2:AK13 AK15:AK86">
     <cfRule type="cellIs" dxfId="321" priority="218" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE86">
+  <conditionalFormatting sqref="AM2:AM86">
     <cfRule type="cellIs" dxfId="320" priority="217" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
+  <conditionalFormatting sqref="N46">
     <cfRule type="cellIs" dxfId="319" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
+  <conditionalFormatting sqref="N9">
     <cfRule type="cellIs" dxfId="318" priority="215" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK13 AK15:AK86">
+  <conditionalFormatting sqref="N6">
     <cfRule type="cellIs" dxfId="317" priority="214" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AM86">
+  <conditionalFormatting sqref="N48">
     <cfRule type="cellIs" dxfId="316" priority="213" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46">
+  <conditionalFormatting sqref="N45">
     <cfRule type="cellIs" dxfId="315" priority="212" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9">
+  <conditionalFormatting sqref="N50">
     <cfRule type="cellIs" dxfId="314" priority="211" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6">
+  <conditionalFormatting sqref="N5">
     <cfRule type="cellIs" dxfId="313" priority="210" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N48">
+  <conditionalFormatting sqref="N2">
     <cfRule type="cellIs" dxfId="312" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N45">
+  <conditionalFormatting sqref="N3">
     <cfRule type="cellIs" dxfId="311" priority="208" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N10">
     <cfRule type="cellIs" dxfId="310" priority="207" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="309" priority="206" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N52">
+    <cfRule type="cellIs" dxfId="309" priority="203" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="308" priority="205" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N16">
+    <cfRule type="cellIs" dxfId="308" priority="202" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="307" priority="204" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N60">
+    <cfRule type="cellIs" dxfId="307" priority="201" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="306" priority="203" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="M14:N14">
+    <cfRule type="cellIs" dxfId="306" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
+  <conditionalFormatting sqref="M34">
     <cfRule type="cellIs" dxfId="305" priority="199" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
+  <conditionalFormatting sqref="N26">
     <cfRule type="cellIs" dxfId="304" priority="198" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N60">
+  <conditionalFormatting sqref="M26">
     <cfRule type="cellIs" dxfId="303" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:N14">
+  <conditionalFormatting sqref="N28">
     <cfRule type="cellIs" dxfId="302" priority="196" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M34">
+  <conditionalFormatting sqref="M68">
     <cfRule type="cellIs" dxfId="301" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
+  <conditionalFormatting sqref="AJ43">
     <cfRule type="cellIs" dxfId="300" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
+  <conditionalFormatting sqref="AI43">
     <cfRule type="cellIs" dxfId="299" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
+  <conditionalFormatting sqref="AJ3">
     <cfRule type="cellIs" dxfId="298" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M68">
+  <conditionalFormatting sqref="AI3">
     <cfRule type="cellIs" dxfId="297" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ43">
+  <conditionalFormatting sqref="AJ4">
     <cfRule type="cellIs" dxfId="296" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI43">
+  <conditionalFormatting sqref="AI4">
     <cfRule type="cellIs" dxfId="295" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ3">
+  <conditionalFormatting sqref="AJ5">
     <cfRule type="cellIs" dxfId="294" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI3">
+  <conditionalFormatting sqref="AI5">
     <cfRule type="cellIs" dxfId="293" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ4">
+  <conditionalFormatting sqref="AJ6">
     <cfRule type="cellIs" dxfId="292" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI4">
+  <conditionalFormatting sqref="AI6">
     <cfRule type="cellIs" dxfId="291" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ5">
+  <conditionalFormatting sqref="AJ7">
     <cfRule type="cellIs" dxfId="290" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI5">
+  <conditionalFormatting sqref="AI7">
     <cfRule type="cellIs" dxfId="289" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ6">
+  <conditionalFormatting sqref="AJ8:AJ9">
     <cfRule type="cellIs" dxfId="288" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI6">
+  <conditionalFormatting sqref="AI8">
     <cfRule type="cellIs" dxfId="287" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ7">
+  <conditionalFormatting sqref="AJ46">
     <cfRule type="cellIs" dxfId="286" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI7">
+  <conditionalFormatting sqref="AI46">
     <cfRule type="cellIs" dxfId="285" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ8:AJ9">
+  <conditionalFormatting sqref="AJ47">
     <cfRule type="cellIs" dxfId="284" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI8">
+  <conditionalFormatting sqref="AI47">
     <cfRule type="cellIs" dxfId="283" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ46">
+  <conditionalFormatting sqref="AJ10">
     <cfRule type="cellIs" dxfId="282" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI46">
+  <conditionalFormatting sqref="AI10">
     <cfRule type="cellIs" dxfId="281" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ47">
+  <conditionalFormatting sqref="AJ48">
     <cfRule type="cellIs" dxfId="280" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI47">
+  <conditionalFormatting sqref="AI48">
     <cfRule type="cellIs" dxfId="279" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ10">
+  <conditionalFormatting sqref="AJ49">
     <cfRule type="cellIs" dxfId="278" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI10">
+  <conditionalFormatting sqref="AI49">
     <cfRule type="cellIs" dxfId="277" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ48">
+  <conditionalFormatting sqref="AJ50">
     <cfRule type="cellIs" dxfId="276" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI48">
-    <cfRule type="cellIs" dxfId="275" priority="169" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI50">
+    <cfRule type="cellIs" dxfId="275" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ49">
-    <cfRule type="cellIs" dxfId="274" priority="168" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ11:AJ13">
+    <cfRule type="cellIs" dxfId="274" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="273" priority="167" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI11">
+    <cfRule type="cellIs" dxfId="273" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="272" priority="166" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ51">
+    <cfRule type="cellIs" dxfId="272" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI50">
+  <conditionalFormatting sqref="AI52">
     <cfRule type="cellIs" dxfId="271" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11:AJ13">
+  <conditionalFormatting sqref="AJ52:AJ54">
     <cfRule type="cellIs" dxfId="270" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI11">
+  <conditionalFormatting sqref="AJ56">
     <cfRule type="cellIs" dxfId="269" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ51">
+  <conditionalFormatting sqref="AI56">
     <cfRule type="cellIs" dxfId="268" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI52">
+  <conditionalFormatting sqref="AJ57:AJ58">
     <cfRule type="cellIs" dxfId="267" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ52:AJ54">
+  <conditionalFormatting sqref="AI57:AI58">
     <cfRule type="cellIs" dxfId="266" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ56">
+  <conditionalFormatting sqref="AJ15:AJ16">
     <cfRule type="cellIs" dxfId="265" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI56">
+  <conditionalFormatting sqref="AI15:AI16">
     <cfRule type="cellIs" dxfId="264" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ57:AJ58">
+  <conditionalFormatting sqref="AJ59:AJ60">
     <cfRule type="cellIs" dxfId="263" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI57:AI58">
+  <conditionalFormatting sqref="AJ55">
     <cfRule type="cellIs" dxfId="262" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15:AJ16">
+  <conditionalFormatting sqref="AI19">
     <cfRule type="cellIs" dxfId="261" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI15:AI16">
+  <conditionalFormatting sqref="AJ19">
     <cfRule type="cellIs" dxfId="260" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ59:AJ60">
+  <conditionalFormatting sqref="AI18">
     <cfRule type="cellIs" dxfId="259" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ55">
+  <conditionalFormatting sqref="AJ18">
     <cfRule type="cellIs" dxfId="258" priority="151" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI19">
+  <conditionalFormatting sqref="AI17">
     <cfRule type="cellIs" dxfId="257" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19">
+  <conditionalFormatting sqref="AJ17">
     <cfRule type="cellIs" dxfId="256" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI18">
+  <conditionalFormatting sqref="AI86">
     <cfRule type="cellIs" dxfId="255" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ18">
+  <conditionalFormatting sqref="AI40">
     <cfRule type="cellIs" dxfId="254" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI17">
+  <conditionalFormatting sqref="AJ20">
     <cfRule type="cellIs" dxfId="253" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ17">
+  <conditionalFormatting sqref="AJ62">
     <cfRule type="cellIs" dxfId="252" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI86">
-    <cfRule type="cellIs" dxfId="251" priority="144" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI40">
-    <cfRule type="cellIs" dxfId="250" priority="143" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="249" priority="142" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="248" priority="141" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="247" priority="139" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
+    <cfRule type="cellIs" dxfId="250" priority="141" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI21">
+    <cfRule type="cellIs" dxfId="249" priority="140" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI64">
+    <cfRule type="cellIs" dxfId="248" priority="139" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI23">
+    <cfRule type="cellIs" dxfId="247" priority="138" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ24">
     <cfRule type="cellIs" dxfId="246" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI21">
+  <conditionalFormatting sqref="AI25">
     <cfRule type="cellIs" dxfId="245" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI64">
+  <conditionalFormatting sqref="AJ25">
     <cfRule type="cellIs" dxfId="244" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI23">
+  <conditionalFormatting sqref="AJ67">
     <cfRule type="cellIs" dxfId="243" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ24">
+  <conditionalFormatting sqref="AI26">
     <cfRule type="cellIs" dxfId="242" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI25">
+  <conditionalFormatting sqref="AJ26:AJ27">
     <cfRule type="cellIs" dxfId="241" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ25">
+  <conditionalFormatting sqref="AI28:AI30">
     <cfRule type="cellIs" dxfId="240" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ67">
+  <conditionalFormatting sqref="AJ28:AJ31">
     <cfRule type="cellIs" dxfId="239" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI26">
+  <conditionalFormatting sqref="AI72">
     <cfRule type="cellIs" dxfId="238" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ26:AJ27">
+  <conditionalFormatting sqref="AJ72">
     <cfRule type="cellIs" dxfId="237" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI28:AI30">
+  <conditionalFormatting sqref="AI73">
     <cfRule type="cellIs" dxfId="236" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ28:AJ31">
+  <conditionalFormatting sqref="AJ73">
     <cfRule type="cellIs" dxfId="235" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI72">
+  <conditionalFormatting sqref="AI32">
     <cfRule type="cellIs" dxfId="234" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ72">
+  <conditionalFormatting sqref="AJ32">
     <cfRule type="cellIs" dxfId="233" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI73">
+  <conditionalFormatting sqref="AI33">
     <cfRule type="cellIs" dxfId="232" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ73">
+  <conditionalFormatting sqref="AJ33">
     <cfRule type="cellIs" dxfId="231" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI32">
+  <conditionalFormatting sqref="AI34:AI35">
     <cfRule type="cellIs" dxfId="230" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ32">
+  <conditionalFormatting sqref="AJ34:AJ36">
     <cfRule type="cellIs" dxfId="229" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI33">
+  <conditionalFormatting sqref="AI61">
     <cfRule type="cellIs" dxfId="228" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ33">
+  <conditionalFormatting sqref="AI63">
     <cfRule type="cellIs" dxfId="227" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI34:AI35">
+  <conditionalFormatting sqref="AJ70">
     <cfRule type="cellIs" dxfId="226" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ34:AJ36">
+  <conditionalFormatting sqref="AI70">
     <cfRule type="cellIs" dxfId="225" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI61">
+  <conditionalFormatting sqref="AI68">
     <cfRule type="cellIs" dxfId="224" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI63">
+  <conditionalFormatting sqref="AJ76">
     <cfRule type="cellIs" dxfId="223" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ70">
+  <conditionalFormatting sqref="AI76">
     <cfRule type="cellIs" dxfId="222" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI70">
+  <conditionalFormatting sqref="AJ78">
     <cfRule type="cellIs" dxfId="221" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI68">
+  <conditionalFormatting sqref="AI78">
     <cfRule type="cellIs" dxfId="220" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ76">
+  <conditionalFormatting sqref="AJ38">
     <cfRule type="cellIs" dxfId="219" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI76">
+  <conditionalFormatting sqref="AI38">
     <cfRule type="cellIs" dxfId="218" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ78">
+  <conditionalFormatting sqref="AJ77">
     <cfRule type="cellIs" dxfId="217" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI78">
+  <conditionalFormatting sqref="AI77">
     <cfRule type="cellIs" dxfId="216" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ38">
+  <conditionalFormatting sqref="AJ79">
     <cfRule type="cellIs" dxfId="215" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI38">
+  <conditionalFormatting sqref="AI79">
     <cfRule type="cellIs" dxfId="214" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ77">
+  <conditionalFormatting sqref="AJ80">
     <cfRule type="cellIs" dxfId="213" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI77">
+  <conditionalFormatting sqref="AI80">
     <cfRule type="cellIs" dxfId="212" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ79">
+  <conditionalFormatting sqref="AJ81">
     <cfRule type="cellIs" dxfId="211" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI79">
+  <conditionalFormatting sqref="AI81">
     <cfRule type="cellIs" dxfId="210" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ80">
+  <conditionalFormatting sqref="AJ82">
     <cfRule type="cellIs" dxfId="209" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI80">
+  <conditionalFormatting sqref="AI82">
     <cfRule type="cellIs" dxfId="208" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ81">
+  <conditionalFormatting sqref="AI83">
     <cfRule type="cellIs" dxfId="207" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI81">
+  <conditionalFormatting sqref="AI84:AI85">
     <cfRule type="cellIs" dxfId="206" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ82">
+  <conditionalFormatting sqref="AI39">
     <cfRule type="cellIs" dxfId="205" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI82">
+  <conditionalFormatting sqref="J31">
     <cfRule type="cellIs" dxfId="204" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI83">
+  <conditionalFormatting sqref="O61">
     <cfRule type="cellIs" dxfId="203" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI84:AI85">
+  <conditionalFormatting sqref="O54">
     <cfRule type="cellIs" dxfId="202" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI39">
+  <conditionalFormatting sqref="O57">
     <cfRule type="cellIs" dxfId="201" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
+  <conditionalFormatting sqref="O58">
     <cfRule type="cellIs" dxfId="200" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O61">
+  <conditionalFormatting sqref="O67">
     <cfRule type="cellIs" dxfId="199" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O54">
+  <conditionalFormatting sqref="O71">
     <cfRule type="cellIs" dxfId="198" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O57">
+  <conditionalFormatting sqref="O72">
     <cfRule type="cellIs" dxfId="197" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O58">
+  <conditionalFormatting sqref="O80">
     <cfRule type="cellIs" dxfId="196" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O67">
+  <conditionalFormatting sqref="O82">
     <cfRule type="cellIs" dxfId="195" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O71">
-    <cfRule type="cellIs" dxfId="194" priority="85" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O72">
+  <conditionalFormatting sqref="L62">
     <cfRule type="cellIs" dxfId="193" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="192" priority="83" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L75">
+    <cfRule type="cellIs" dxfId="192" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="191" priority="82" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI12">
+    <cfRule type="cellIs" dxfId="191" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="cellIs" dxfId="190" priority="81" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="X2">
+    <cfRule type="cellIs" dxfId="190" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="189" priority="80" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="W4:W5 W7:W13 W15:W19 W62:W74 W21:W34 W36:W59 W76:W86">
+    <cfRule type="cellIs" dxfId="189" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L75">
+  <conditionalFormatting sqref="AB2">
     <cfRule type="cellIs" dxfId="188" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI12">
+  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
     <cfRule type="cellIs" dxfId="187" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
+  <conditionalFormatting sqref="Z2">
     <cfRule type="cellIs" dxfId="186" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W4:W5 W7:W13 W15:W19 W62:W86 W21:W59">
+  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y74 Y33:Y59 Y76:Y86">
     <cfRule type="cellIs" dxfId="185" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2">
+  <conditionalFormatting sqref="AD2">
     <cfRule type="cellIs" dxfId="184" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
+  <conditionalFormatting sqref="AC2:AC86">
     <cfRule type="cellIs" dxfId="183" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2">
+  <conditionalFormatting sqref="V2">
     <cfRule type="cellIs" dxfId="182" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y86 Y33:Y59">
+  <conditionalFormatting sqref="U2:U86">
     <cfRule type="cellIs" dxfId="181" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2">
+  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
     <cfRule type="cellIs" dxfId="180" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC86">
+  <conditionalFormatting sqref="AA48">
     <cfRule type="cellIs" dxfId="179" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2">
+  <conditionalFormatting sqref="AA11">
     <cfRule type="cellIs" dxfId="178" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U86">
+  <conditionalFormatting sqref="AA51">
     <cfRule type="cellIs" dxfId="177" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
+  <conditionalFormatting sqref="AA52">
     <cfRule type="cellIs" dxfId="176" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA48">
+  <conditionalFormatting sqref="AA53">
     <cfRule type="cellIs" dxfId="175" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA11">
+  <conditionalFormatting sqref="AA57 AA54:AA55">
     <cfRule type="cellIs" dxfId="174" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA51">
+  <conditionalFormatting sqref="AA20">
     <cfRule type="cellIs" dxfId="173" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA52">
+  <conditionalFormatting sqref="AA21">
     <cfRule type="cellIs" dxfId="172" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA53">
+  <conditionalFormatting sqref="AA66">
     <cfRule type="cellIs" dxfId="171" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA57 AA54:AA55">
+  <conditionalFormatting sqref="AA25">
     <cfRule type="cellIs" dxfId="170" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA20">
+  <conditionalFormatting sqref="AA26">
     <cfRule type="cellIs" dxfId="169" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA21">
+  <conditionalFormatting sqref="AA28">
     <cfRule type="cellIs" dxfId="168" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA66">
+  <conditionalFormatting sqref="AA32">
     <cfRule type="cellIs" dxfId="167" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA25">
+  <conditionalFormatting sqref="AA34">
     <cfRule type="cellIs" dxfId="166" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA26">
+  <conditionalFormatting sqref="AA27">
     <cfRule type="cellIs" dxfId="165" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA28">
+  <conditionalFormatting sqref="AA33 AA31">
     <cfRule type="cellIs" dxfId="164" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA32">
+  <conditionalFormatting sqref="AA61 M61">
     <cfRule type="cellIs" dxfId="163" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA34">
+  <conditionalFormatting sqref="AA62">
     <cfRule type="cellIs" dxfId="162" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA27">
+  <conditionalFormatting sqref="AA63 M63">
     <cfRule type="cellIs" dxfId="161" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA33 AA31">
+  <conditionalFormatting sqref="AA65">
     <cfRule type="cellIs" dxfId="160" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA61 M61">
+  <conditionalFormatting sqref="AA67">
     <cfRule type="cellIs" dxfId="159" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA62">
+  <conditionalFormatting sqref="AA68">
     <cfRule type="cellIs" dxfId="158" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA63 M63">
+  <conditionalFormatting sqref="AA70:AA73">
     <cfRule type="cellIs" dxfId="157" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA65">
+  <conditionalFormatting sqref="AA77">
     <cfRule type="cellIs" dxfId="156" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA67">
+  <conditionalFormatting sqref="AA74 AA38">
     <cfRule type="cellIs" dxfId="155" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA68">
+  <conditionalFormatting sqref="AA37">
     <cfRule type="cellIs" dxfId="154" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA70:AA73">
+  <conditionalFormatting sqref="S9">
     <cfRule type="cellIs" dxfId="153" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA77">
+  <conditionalFormatting sqref="S46">
     <cfRule type="cellIs" dxfId="152" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA74 AA38">
+  <conditionalFormatting sqref="S48">
     <cfRule type="cellIs" dxfId="151" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA37">
+  <conditionalFormatting sqref="S18">
     <cfRule type="cellIs" dxfId="150" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
+  <conditionalFormatting sqref="S54">
     <cfRule type="cellIs" dxfId="149" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S46">
+  <conditionalFormatting sqref="S55">
     <cfRule type="cellIs" dxfId="148" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48">
+  <conditionalFormatting sqref="S57">
     <cfRule type="cellIs" dxfId="147" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
+  <conditionalFormatting sqref="S76">
     <cfRule type="cellIs" dxfId="146" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S54">
+  <conditionalFormatting sqref="S78">
     <cfRule type="cellIs" dxfId="145" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S55">
+  <conditionalFormatting sqref="S81">
     <cfRule type="cellIs" dxfId="144" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S57">
+  <conditionalFormatting sqref="S82">
     <cfRule type="cellIs" dxfId="143" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S76">
+  <conditionalFormatting sqref="J32">
     <cfRule type="cellIs" dxfId="142" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S78">
+  <conditionalFormatting sqref="K66">
     <cfRule type="cellIs" dxfId="141" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S81">
+  <conditionalFormatting sqref="L67">
     <cfRule type="cellIs" dxfId="140" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S82">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="139" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
+  <conditionalFormatting sqref="L27">
     <cfRule type="cellIs" dxfId="138" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
+  <conditionalFormatting sqref="G7">
     <cfRule type="cellIs" dxfId="137" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L67">
-    <cfRule type="cellIs" dxfId="136" priority="26" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="135" priority="25" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="134" priority="24" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="133" priority="23" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="132" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="136" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="131" priority="20" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="130" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="134" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="cellIs" dxfId="129" priority="18" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="133" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
+    <cfRule type="cellIs" dxfId="132" priority="19" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L55">
+    <cfRule type="cellIs" dxfId="131" priority="18" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L56">
+    <cfRule type="cellIs" dxfId="130" priority="17" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="cellIs" dxfId="129" priority="16" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L60">
     <cfRule type="cellIs" dxfId="128" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L55">
-    <cfRule type="cellIs" dxfId="127" priority="14" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
+  <conditionalFormatting sqref="L76">
     <cfRule type="cellIs" dxfId="126" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
+  <conditionalFormatting sqref="L6">
     <cfRule type="cellIs" dxfId="125" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L60">
+  <conditionalFormatting sqref="L7">
     <cfRule type="cellIs" dxfId="124" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
+  <conditionalFormatting sqref="L8">
     <cfRule type="cellIs" dxfId="123" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76">
+  <conditionalFormatting sqref="L9">
     <cfRule type="cellIs" dxfId="122" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
+  <conditionalFormatting sqref="Y14">
     <cfRule type="cellIs" dxfId="121" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
+  <conditionalFormatting sqref="J4">
     <cfRule type="cellIs" dxfId="120" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
+  <conditionalFormatting sqref="AK14">
     <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9">
+  <conditionalFormatting sqref="X61">
     <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y14">
+  <conditionalFormatting sqref="W75">
     <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
+  <conditionalFormatting sqref="Y75">
     <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK14">
-    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K76">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X61">
-    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K22">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -46985,448 +47042,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="115" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="114" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="102" priority="93">
+    <cfRule type="containsBlanks" dxfId="104" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="100" priority="91">
+    <cfRule type="containsBlanks" dxfId="102" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="101" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="100" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="90" priority="69">
+    <cfRule type="containsBlanks" dxfId="92" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="91" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="90" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="88" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="82" priority="63">
+    <cfRule type="containsBlanks" dxfId="84" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="83" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="82" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="77" priority="59">
+    <cfRule type="containsBlanks" dxfId="79" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="78" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="75" priority="56">
+    <cfRule type="containsBlanks" dxfId="77" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="76" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="75" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="68" priority="50">
+    <cfRule type="containsBlanks" dxfId="70" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="69" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="68" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="65" priority="47">
+    <cfRule type="containsBlanks" dxfId="67" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="66" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="65" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="60" priority="42">
+    <cfRule type="containsBlanks" dxfId="62" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="61" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="60" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="57" priority="39">
+    <cfRule type="containsBlanks" dxfId="59" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="58" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="57" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="42" priority="23">
+    <cfRule type="containsBlanks" dxfId="44" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="40" priority="19">
+    <cfRule type="containsBlanks" dxfId="42" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="40" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="31" priority="22">
+    <cfRule type="containsBlanks" dxfId="33" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="30" priority="11">
+    <cfRule type="containsBlanks" dxfId="32" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="31" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -62321,111 +62378,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -63749,7 +63806,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43564</v>
+        <v>43595</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -64059,7 +64116,7 @@
   <dimension ref="B1:Y87"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="8055" activePane="bottomLeft"/>
+      <pane ySplit="8063" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -64098,7 +64155,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43564</v>
+        <v>43595</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -68105,13 +68162,13 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.01" right="0.01" top="0.01" bottom="0.01" header="0.01" footer="0.01"/>
-  <pageSetup paperSize="3" scale="92" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="3" scale="94" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;C&amp;R</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
update data loaded to SP
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3563871E-2056-4BBB-9419-8BC93BF3E82E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C629CDEE-3000-4C5F-ACEE-1E561F5623C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58050" yWindow="5595" windowWidth="11610" windowHeight="4755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1433" yWindow="7710" windowWidth="18180" windowHeight="4890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9027" uniqueCount="1404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9029" uniqueCount="1408">
   <si>
     <t>#</t>
   </si>
@@ -4067,9 +4067,6 @@
     <t>04-111330 (main bldg certified; 04-115098 (ceiling work - not certified)</t>
   </si>
   <si>
-    <t>04-107524; 04-113290 ("Accepted", although DSA tracker shows a sstill open 2/8/19)</t>
-  </si>
-  <si>
     <t>Certfied (04-110878; 04-111010; 04-111216); Not Certified: 04-115435 (Alts to CP)</t>
   </si>
   <si>
@@ -4220,15 +4217,6 @@
     <t>&lt;CAD files only appear to be on R drive&gt;&gt;</t>
   </si>
   <si>
-    <t>R drive has bid set</t>
-  </si>
-  <si>
-    <t>files appear to be on R drive&gt;&gt; CE-008</t>
-  </si>
-  <si>
-    <t>files appear to be on R drive</t>
-  </si>
-  <si>
     <t>divided in  SP</t>
   </si>
   <si>
@@ -4257,6 +4245,30 @@
   </si>
   <si>
     <t xml:space="preserve">CE-012; 014-015 </t>
+  </si>
+  <si>
+    <t>in SP as single file</t>
+  </si>
+  <si>
+    <t>do have Testing and Balance report in SP</t>
+  </si>
+  <si>
+    <t>Record dwgs in SP combined with bid set</t>
+  </si>
+  <si>
+    <t>put in SP 6/10/2019</t>
+  </si>
+  <si>
+    <t>04-107524; 04-113290 ("Accepted", although DSA tracker shows a still open 2/8/19)</t>
+  </si>
+  <si>
+    <t>Some in SP -- but no Arch etc - CE-012; 014-016; 018-020</t>
+  </si>
+  <si>
+    <t>in SP ; also  CE-008</t>
+  </si>
+  <si>
+    <t>missing some structural</t>
   </si>
 </sst>
 </file>
@@ -5281,6 +5293,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5337,10 +5353,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -8418,7 +8430,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5/21/2019</c:v>
+                  <c:v>6/12/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10175,10 +10187,10 @@
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1020" topLeftCell="A38" activePane="bottomLeft"/>
-      <selection activeCell="H1" sqref="F1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="1110" activePane="bottomLeft"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -10191,8 +10203,8 @@
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="7.1328125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.73046875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.59765625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1328125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.59765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1328125" style="1" customWidth="1"/>
     <col min="11" max="11" width="6.59765625" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.3984375" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
@@ -10501,7 +10513,7 @@
         <v>170</v>
       </c>
       <c r="J2" s="119" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="K2" s="52" t="s">
         <v>166</v>
@@ -10541,7 +10553,7 @@
         <v>166</v>
       </c>
       <c r="X2" s="118" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="Y2" s="118" t="s">
         <v>567</v>
@@ -10672,7 +10684,7 @@
         <v>170</v>
       </c>
       <c r="J3" s="119" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="K3" s="52" t="s">
         <v>166</v>
@@ -10714,7 +10726,7 @@
         <v>166</v>
       </c>
       <c r="X3" s="118" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="Y3" s="118" t="s">
         <v>567</v>
@@ -10843,13 +10855,13 @@
         <v>166</v>
       </c>
       <c r="J4" s="118" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="K4" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="M4" s="13" t="s">
         <v>567</v>
@@ -10885,7 +10897,7 @@
         <v>170</v>
       </c>
       <c r="X4" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y4" s="118" t="s">
         <v>567</v>
@@ -11010,7 +11022,7 @@
         <v>170</v>
       </c>
       <c r="H5" s="118" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="I5" s="52" t="s">
         <v>166</v>
@@ -11056,7 +11068,7 @@
         <v>170</v>
       </c>
       <c r="X5" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y5" s="118" t="s">
         <v>567</v>
@@ -11229,13 +11241,13 @@
         <v>166</v>
       </c>
       <c r="X6" s="118" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="Y6" s="118" t="s">
         <v>567</v>
       </c>
       <c r="Z6" s="118" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="AA6" s="52" t="s">
         <v>166</v>
@@ -11257,7 +11269,7 @@
         <v>166</v>
       </c>
       <c r="AH6" s="118" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="AI6" s="48" t="s">
         <v>170</v>
@@ -11370,7 +11382,7 @@
         <v>1112</v>
       </c>
       <c r="H7" s="118" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="I7" s="145" t="s">
         <v>1116</v>
@@ -11380,7 +11392,7 @@
         <v>166</v>
       </c>
       <c r="L7" s="52" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="M7" s="13" t="s">
         <v>567</v>
@@ -11416,7 +11428,7 @@
         <v>170</v>
       </c>
       <c r="X7" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y7" s="118" t="s">
         <v>567</v>
@@ -11549,13 +11561,13 @@
         <v>166</v>
       </c>
       <c r="J8" s="118" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="K8" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L8" s="52" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="M8" s="13" t="s">
         <v>567</v>
@@ -11591,7 +11603,7 @@
         <v>170</v>
       </c>
       <c r="X8" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y8" s="118" t="s">
         <v>567</v>
@@ -11762,7 +11774,7 @@
         <v>170</v>
       </c>
       <c r="X9" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y9" s="118" t="s">
         <v>567</v>
@@ -11788,7 +11800,7 @@
         <v>166</v>
       </c>
       <c r="AH9" s="118" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="AI9" s="118" t="s">
         <v>567</v>
@@ -11885,7 +11897,7 @@
         <v>170</v>
       </c>
       <c r="H10" s="118" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="I10" s="145" t="s">
         <v>1116</v>
@@ -11931,7 +11943,7 @@
         <v>170</v>
       </c>
       <c r="X10" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y10" s="118" t="s">
         <v>567</v>
@@ -12100,7 +12112,7 @@
         <v>170</v>
       </c>
       <c r="X11" s="118" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="Y11" s="118" t="s">
         <v>567</v>
@@ -12235,7 +12247,7 @@
         <v>170</v>
       </c>
       <c r="J12" s="118" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="K12" s="118" t="s">
         <v>567</v>
@@ -12273,7 +12285,7 @@
         <v>170</v>
       </c>
       <c r="X12" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y12" s="118" t="s">
         <v>567</v>
@@ -12442,7 +12454,7 @@
         <v>1112</v>
       </c>
       <c r="X13" s="118" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="Y13" s="118" t="s">
         <v>567</v>
@@ -12571,13 +12583,13 @@
         <v>170</v>
       </c>
       <c r="J14" s="118" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="K14" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="M14" s="48" t="s">
         <v>170</v>
@@ -12611,19 +12623,19 @@
         <v>166</v>
       </c>
       <c r="X14" s="118" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="Y14" s="146" t="s">
         <v>1112</v>
       </c>
       <c r="Z14" s="118" t="s">
+        <v>1359</v>
+      </c>
+      <c r="AA14" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB14" s="118" t="s">
         <v>1360</v>
-      </c>
-      <c r="AA14" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="AB14" s="118" t="s">
-        <v>1361</v>
       </c>
       <c r="AC14" s="118" t="s">
         <v>567</v>
@@ -12649,7 +12661,7 @@
         <v>166</v>
       </c>
       <c r="AL14" s="118" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="AM14" s="118" t="s">
         <v>567</v>
@@ -12740,7 +12752,7 @@
         <v>170</v>
       </c>
       <c r="J15" s="118" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="K15" s="118" t="s">
         <v>567</v>
@@ -12780,7 +12792,7 @@
         <v>170</v>
       </c>
       <c r="X15" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y15" s="118" t="s">
         <v>567</v>
@@ -12947,7 +12959,7 @@
         <v>170</v>
       </c>
       <c r="X16" s="118" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="Y16" s="118" t="s">
         <v>567</v>
@@ -13251,7 +13263,7 @@
         <v>170</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="M18" s="48" t="s">
         <v>170</v>
@@ -13625,13 +13637,13 @@
         <v>1112</v>
       </c>
       <c r="Z20" s="118" t="s">
+        <v>1364</v>
+      </c>
+      <c r="AA20" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB20" s="118" t="s">
         <v>1365</v>
-      </c>
-      <c r="AA20" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="AB20" s="118" t="s">
-        <v>1366</v>
       </c>
       <c r="AC20" s="118" t="s">
         <v>567</v>
@@ -14285,7 +14297,7 @@
         <v>170</v>
       </c>
       <c r="X24" s="118" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="Y24" s="118" t="s">
         <v>567</v>
@@ -14416,13 +14428,13 @@
         <v>170</v>
       </c>
       <c r="J25" s="118" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="K25" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="M25" s="52" t="s">
         <v>166</v>
@@ -15096,7 +15108,7 @@
         <v>1112</v>
       </c>
       <c r="L29" s="52" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
       <c r="M29" s="52" t="s">
         <v>166</v>
@@ -15253,7 +15265,7 @@
         <v>166</v>
       </c>
       <c r="H30" s="118" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="I30" s="52" t="s">
         <v>166</v>
@@ -15265,7 +15277,7 @@
         <v>166</v>
       </c>
       <c r="L30" s="52" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="M30" s="52" t="s">
         <v>166</v>
@@ -15299,7 +15311,7 @@
         <v>170</v>
       </c>
       <c r="X30" s="118" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="Y30" s="118" t="s">
         <v>567</v>
@@ -15591,13 +15603,13 @@
         <v>170</v>
       </c>
       <c r="J32" s="118" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="K32" s="52" t="s">
         <v>166</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="M32" s="52" t="s">
         <v>166</v>
@@ -15631,13 +15643,13 @@
         <v>1112</v>
       </c>
       <c r="X32" s="118" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="Y32" s="52" t="s">
         <v>166</v>
       </c>
       <c r="Z32" s="118" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="AA32" s="48" t="s">
         <v>170</v>
@@ -15768,7 +15780,7 @@
         <v>1112</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="M33" s="118" t="s">
         <v>567</v>
@@ -15800,7 +15812,7 @@
         <v>166</v>
       </c>
       <c r="X33" s="118" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="Y33" s="118" t="s">
         <v>567</v>
@@ -16096,7 +16108,7 @@
         <v>170</v>
       </c>
       <c r="J35" s="119" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="K35" s="118" t="s">
         <v>567</v>
@@ -16134,7 +16146,7 @@
         <v>166</v>
       </c>
       <c r="X35" s="118" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="Y35" s="118" t="s">
         <v>567</v>
@@ -16261,13 +16273,13 @@
         <v>170</v>
       </c>
       <c r="J36" s="118" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="K36" s="150" t="s">
         <v>166</v>
       </c>
       <c r="L36" s="52" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="M36" s="118" t="s">
         <v>567</v>
@@ -16422,7 +16434,7 @@
         <v>166</v>
       </c>
       <c r="H37" s="118" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="I37" s="52" t="s">
         <v>166</v>
@@ -16474,7 +16486,7 @@
         <v>1112</v>
       </c>
       <c r="AB37" s="118" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="AC37" s="118" t="s">
         <v>567</v>
@@ -16565,7 +16577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38" s="13" t="s">
         <v>86</v>
       </c>
@@ -16595,7 +16607,7 @@
         <v>166</v>
       </c>
       <c r="L38" s="52" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
       <c r="M38" s="48" t="s">
         <v>170</v>
@@ -16626,14 +16638,14 @@
       <c r="W38" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="X38" s="172" t="s">
-        <v>1398</v>
-      </c>
-      <c r="Y38" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z38" s="118">
-        <v>1</v>
+      <c r="X38" s="153" t="s">
+        <v>1394</v>
+      </c>
+      <c r="Y38" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z38" s="118" t="s">
+        <v>1400</v>
       </c>
       <c r="AA38" s="48" t="s">
         <v>170</v>
@@ -16649,10 +16661,12 @@
         <v>567</v>
       </c>
       <c r="AF38" s="118"/>
-      <c r="AG38" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="AH38" s="118"/>
+      <c r="AG38" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AH38" s="118" t="s">
+        <v>1401</v>
+      </c>
       <c r="AI38" s="150" t="s">
         <v>166</v>
       </c>
@@ -17130,7 +17144,7 @@
         <v>170</v>
       </c>
       <c r="H41" s="118" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="I41" s="118" t="s">
         <v>567</v>
@@ -17466,7 +17480,7 @@
         <v>1116</v>
       </c>
       <c r="L43" s="19" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="M43" s="145" t="s">
         <v>1116</v>
@@ -17685,7 +17699,7 @@
         <v>166</v>
       </c>
       <c r="T44" s="118" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="U44" s="118" t="s">
         <v>567</v>
@@ -18041,7 +18055,7 @@
         <v>170</v>
       </c>
       <c r="X46" s="118" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="Y46" s="118" t="s">
         <v>567</v>
@@ -18176,7 +18190,7 @@
         <v>1112</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="M47" s="52" t="s">
         <v>166</v>
@@ -18210,7 +18224,7 @@
         <v>170</v>
       </c>
       <c r="X47" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y47" s="118" t="s">
         <v>567</v>
@@ -18381,7 +18395,7 @@
         <v>170</v>
       </c>
       <c r="X48" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y48" s="118" t="s">
         <v>567</v>
@@ -18717,7 +18731,7 @@
         <v>170</v>
       </c>
       <c r="X50" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y50" s="118" t="s">
         <v>567</v>
@@ -18920,7 +18934,7 @@
         <v>170</v>
       </c>
       <c r="X51" s="118" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="Y51" s="118" t="s">
         <v>567</v>
@@ -19043,7 +19057,7 @@
         <v>166</v>
       </c>
       <c r="H52" s="118" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="I52" s="52" t="s">
         <v>166</v>
@@ -19089,7 +19103,7 @@
         <v>170</v>
       </c>
       <c r="X52" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y52" s="118" t="s">
         <v>567</v>
@@ -19260,7 +19274,7 @@
         <v>170</v>
       </c>
       <c r="X53" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y53" s="118" t="s">
         <v>567</v>
@@ -19425,7 +19439,7 @@
         <v>170</v>
       </c>
       <c r="X54" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y54" s="118" t="s">
         <v>567</v>
@@ -19602,7 +19616,7 @@
         <v>170</v>
       </c>
       <c r="X55" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y55" s="118" t="s">
         <v>567</v>
@@ -19934,7 +19948,7 @@
         <v>170</v>
       </c>
       <c r="X57" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y57" s="118" t="s">
         <v>567</v>
@@ -20099,7 +20113,7 @@
         <v>170</v>
       </c>
       <c r="X58" s="118" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="Y58" s="118" t="s">
         <v>567</v>
@@ -20302,7 +20316,7 @@
         <v>166</v>
       </c>
       <c r="X59" s="118" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="Y59" s="118" t="s">
         <v>567</v>
@@ -20439,7 +20453,7 @@
         <v>166</v>
       </c>
       <c r="L60" s="13" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="M60" s="52" t="s">
         <v>166</v>
@@ -20477,7 +20491,7 @@
         <v>166</v>
       </c>
       <c r="Z60" s="118" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="AA60" s="52" t="s">
         <v>166</v>
@@ -22103,7 +22117,7 @@
         <v>1112</v>
       </c>
       <c r="L70" s="13" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="M70" s="118" t="s">
         <v>567</v>
@@ -22761,7 +22775,7 @@
         <v>170</v>
       </c>
       <c r="L74" s="146" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
       <c r="M74" s="48" t="s">
         <v>170</v>
@@ -22948,7 +22962,7 @@
         <v>166</v>
       </c>
       <c r="H75" s="118" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="I75" s="52" t="s">
         <v>166</v>
@@ -22992,13 +23006,13 @@
         <v>166</v>
       </c>
       <c r="X75" s="118" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="Y75" s="52" t="s">
         <v>166</v>
       </c>
       <c r="Z75" s="118" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="AA75" s="145" t="s">
         <v>1116</v>
@@ -23161,7 +23175,7 @@
         <v>170</v>
       </c>
       <c r="L76" s="146" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="M76" s="48" t="s">
         <v>170</v>
@@ -23193,7 +23207,7 @@
         <v>166</v>
       </c>
       <c r="X76" s="118" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="Y76" s="118" t="s">
         <v>567</v>
@@ -23324,7 +23338,7 @@
         <v>1112</v>
       </c>
       <c r="H77" s="118" t="s">
-        <v>1340</v>
+        <v>1404</v>
       </c>
       <c r="I77" s="52" t="s">
         <v>166</v>
@@ -23332,11 +23346,11 @@
       <c r="J77" s="118" t="s">
         <v>418</v>
       </c>
-      <c r="K77" s="48" t="s">
-        <v>170</v>
+      <c r="K77" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="L77" s="13" t="s">
-        <v>1391</v>
+        <v>1402</v>
       </c>
       <c r="M77" s="48" t="s">
         <v>170</v>
@@ -23357,7 +23371,9 @@
       <c r="S77" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="T77" s="118"/>
+      <c r="T77" s="118" t="s">
+        <v>1403</v>
+      </c>
       <c r="U77" s="118" t="s">
         <v>567</v>
       </c>
@@ -23368,7 +23384,7 @@
         <v>170</v>
       </c>
       <c r="X77" s="118" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="Y77" s="118" t="s">
         <v>567</v>
@@ -23503,11 +23519,11 @@
       <c r="J78" s="118" t="s">
         <v>419</v>
       </c>
-      <c r="K78" s="118" t="s">
-        <v>567</v>
+      <c r="K78" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="L78" s="52" t="s">
-        <v>489</v>
+        <v>1405</v>
       </c>
       <c r="M78" s="48" t="s">
         <v>170</v>
@@ -23535,16 +23551,14 @@
       <c r="V78" s="118">
         <v>1</v>
       </c>
-      <c r="W78" s="48" t="s">
-        <v>170</v>
+      <c r="W78" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="X78" s="118"/>
-      <c r="Y78" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z78" s="118">
-        <v>1</v>
-      </c>
+      <c r="Y78" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z78" s="118"/>
       <c r="AA78" s="52" t="s">
         <v>166</v>
       </c>
@@ -23666,11 +23680,11 @@
       <c r="J79" s="118" t="s">
         <v>444</v>
       </c>
-      <c r="K79" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="L79" s="146" t="s">
-        <v>1392</v>
+      <c r="K79" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="L79" s="153" t="s">
+        <v>1406</v>
       </c>
       <c r="M79" s="48" t="s">
         <v>170</v>
@@ -23700,18 +23714,14 @@
       <c r="V79" s="118">
         <v>1</v>
       </c>
-      <c r="W79" s="146" t="s">
-        <v>1112</v>
-      </c>
-      <c r="X79" s="146" t="s">
-        <v>1393</v>
-      </c>
-      <c r="Y79" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="Z79" s="118">
-        <v>1</v>
-      </c>
+      <c r="W79" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="X79" s="118"/>
+      <c r="Y79" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z79" s="118"/>
       <c r="AA79" s="52" t="s">
         <v>166</v>
       </c>
@@ -23823,7 +23833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B80" s="13" t="s">
         <v>4</v>
       </c>
@@ -23849,11 +23859,11 @@
       <c r="J80" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="K80" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="L80" s="146" t="s">
-        <v>1393</v>
+      <c r="K80" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="L80" s="153" t="s">
+        <v>1407</v>
       </c>
       <c r="M80" s="48" t="s">
         <v>170</v>
@@ -25159,7 +25169,7 @@
   <autoFilter ref="B1:BZ86" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="14220"/>
+        <filter val="14520"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -25169,1734 +25179,1722 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
-    <cfRule type="cellIs" dxfId="402" priority="352" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="402" priority="354" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI9:BJ9">
-    <cfRule type="cellIs" dxfId="401" priority="351" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="401" priority="353" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="400" priority="350" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="400" priority="352" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="399" priority="349" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="399" priority="351" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
-    <cfRule type="cellIs" dxfId="398" priority="347" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="398" priority="349" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="397" priority="346" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="397" priority="348" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="396" priority="345" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="396" priority="347" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="395" priority="341" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="395" priority="343" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="394" priority="331" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="394" priority="333" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I3 I44 I14 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="393" priority="318" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="393" priority="320" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="392" priority="307" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="392" priority="309" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
-    <cfRule type="cellIs" dxfId="391" priority="304" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="391" priority="306" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD2">
-    <cfRule type="cellIs" dxfId="390" priority="303" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="390" priority="305" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K42 K63 K10 K12 K53 K15:K17 K57 K31 K44 K49 K68:K73 K35 K37:K38 K78:K79 K81:K82">
-    <cfRule type="cellIs" dxfId="389" priority="302" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K41:K42 K63 K10 K12 K53 K15:K17 K57 K31 K44 K49 K68:K73 K35 K37:K38 K81:K82">
+    <cfRule type="cellIs" dxfId="389" priority="304" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
-    <cfRule type="cellIs" dxfId="388" priority="301" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="388" priority="303" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L79 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5 L81:L85">
-    <cfRule type="cellIs" dxfId="387" priority="300" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="387" priority="302" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="386" priority="299" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="386" priority="301" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="385" priority="296" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="385" priority="298" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="384" priority="295" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="384" priority="297" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="383" priority="293" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="383" priority="295" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="382" priority="291" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="382" priority="293" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
-    <cfRule type="cellIs" dxfId="381" priority="289" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="381" priority="291" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
-    <cfRule type="cellIs" dxfId="380" priority="288" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="380" priority="290" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q86">
-    <cfRule type="cellIs" dxfId="379" priority="287" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="379" priority="289" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
-    <cfRule type="cellIs" dxfId="378" priority="286" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="378" priority="288" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AE86">
-    <cfRule type="cellIs" dxfId="377" priority="285" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="377" priority="287" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
-    <cfRule type="cellIs" dxfId="376" priority="284" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="376" priority="286" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
-    <cfRule type="cellIs" dxfId="375" priority="283" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="375" priority="285" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK2:AK13 AK15:AK86">
-    <cfRule type="cellIs" dxfId="374" priority="282" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="374" priority="284" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM2:AM86">
-    <cfRule type="cellIs" dxfId="373" priority="281" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="373" priority="283" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="cellIs" dxfId="372" priority="280" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="372" priority="282" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="371" priority="279" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="371" priority="281" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="370" priority="278" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="370" priority="280" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="369" priority="277" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="369" priority="279" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="cellIs" dxfId="368" priority="276" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="368" priority="278" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
-    <cfRule type="cellIs" dxfId="367" priority="275" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="367" priority="277" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="366" priority="274" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="366" priority="276" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="365" priority="273" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="365" priority="275" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="364" priority="272" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="364" priority="274" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="363" priority="271" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="363" priority="273" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="362" priority="267" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="362" priority="269" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="361" priority="266" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="361" priority="268" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60">
-    <cfRule type="cellIs" dxfId="360" priority="265" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="360" priority="267" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:N14">
-    <cfRule type="cellIs" dxfId="359" priority="264" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="359" priority="266" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="358" priority="263" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="358" priority="265" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="357" priority="262" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="357" priority="264" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
-    <cfRule type="cellIs" dxfId="356" priority="261" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="356" priority="263" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="cellIs" dxfId="355" priority="260" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="355" priority="262" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="cellIs" dxfId="354" priority="259" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="354" priority="261" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ43">
-    <cfRule type="cellIs" dxfId="353" priority="258" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="353" priority="260" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI43">
-    <cfRule type="cellIs" dxfId="352" priority="257" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="352" priority="259" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3">
-    <cfRule type="cellIs" dxfId="351" priority="256" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="351" priority="258" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="cellIs" dxfId="350" priority="255" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="350" priority="257" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ4">
-    <cfRule type="cellIs" dxfId="349" priority="254" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="349" priority="256" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI4">
-    <cfRule type="cellIs" dxfId="348" priority="253" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="348" priority="255" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ5">
-    <cfRule type="cellIs" dxfId="347" priority="252" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="347" priority="254" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI5">
-    <cfRule type="cellIs" dxfId="346" priority="251" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="346" priority="253" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ6">
-    <cfRule type="cellIs" dxfId="345" priority="250" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="345" priority="252" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6">
-    <cfRule type="cellIs" dxfId="344" priority="249" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="344" priority="251" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ7">
-    <cfRule type="cellIs" dxfId="343" priority="248" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="343" priority="250" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI7">
-    <cfRule type="cellIs" dxfId="342" priority="247" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="342" priority="249" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:AJ9">
-    <cfRule type="cellIs" dxfId="341" priority="246" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="341" priority="248" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI8">
-    <cfRule type="cellIs" dxfId="340" priority="245" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="340" priority="247" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ46">
-    <cfRule type="cellIs" dxfId="339" priority="244" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="339" priority="246" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI46">
-    <cfRule type="cellIs" dxfId="338" priority="243" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="338" priority="245" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ47">
-    <cfRule type="cellIs" dxfId="337" priority="242" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="337" priority="244" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI47">
-    <cfRule type="cellIs" dxfId="336" priority="241" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="336" priority="243" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10">
-    <cfRule type="cellIs" dxfId="335" priority="240" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="335" priority="242" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI10">
-    <cfRule type="cellIs" dxfId="334" priority="239" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="334" priority="241" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ48">
-    <cfRule type="cellIs" dxfId="333" priority="238" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="333" priority="240" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI48">
-    <cfRule type="cellIs" dxfId="332" priority="237" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="332" priority="239" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ49">
-    <cfRule type="cellIs" dxfId="331" priority="236" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="331" priority="238" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="330" priority="235" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="330" priority="237" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="329" priority="234" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="329" priority="236" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI50">
-    <cfRule type="cellIs" dxfId="328" priority="232" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="328" priority="234" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11:AJ13">
-    <cfRule type="cellIs" dxfId="327" priority="231" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="327" priority="233" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI11">
-    <cfRule type="cellIs" dxfId="326" priority="230" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="326" priority="232" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ51">
-    <cfRule type="cellIs" dxfId="325" priority="229" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="325" priority="231" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI52">
-    <cfRule type="cellIs" dxfId="324" priority="228" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="324" priority="230" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ52:AJ54">
-    <cfRule type="cellIs" dxfId="323" priority="227" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="323" priority="229" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ56">
-    <cfRule type="cellIs" dxfId="322" priority="226" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="322" priority="228" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI56">
-    <cfRule type="cellIs" dxfId="321" priority="225" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="321" priority="227" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ57:AJ58">
-    <cfRule type="cellIs" dxfId="320" priority="224" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="320" priority="226" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI57:AI58">
-    <cfRule type="cellIs" dxfId="319" priority="223" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="319" priority="225" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ15:AJ16">
-    <cfRule type="cellIs" dxfId="318" priority="222" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="318" priority="224" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI15:AI16">
-    <cfRule type="cellIs" dxfId="317" priority="221" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="317" priority="223" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ59:AJ60">
-    <cfRule type="cellIs" dxfId="316" priority="220" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="316" priority="222" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ55">
-    <cfRule type="cellIs" dxfId="315" priority="219" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="315" priority="221" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="cellIs" dxfId="314" priority="218" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="314" priority="220" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="cellIs" dxfId="313" priority="217" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="313" priority="219" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI18">
-    <cfRule type="cellIs" dxfId="312" priority="216" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="312" priority="218" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="311" priority="215" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="311" priority="217" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI17">
-    <cfRule type="cellIs" dxfId="310" priority="214" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="310" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ17">
-    <cfRule type="cellIs" dxfId="309" priority="213" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="309" priority="215" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI86">
-    <cfRule type="cellIs" dxfId="308" priority="212" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="308" priority="214" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI40">
-    <cfRule type="cellIs" dxfId="307" priority="211" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="307" priority="213" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="306" priority="210" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="306" priority="212" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="305" priority="209" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="305" priority="211" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="304" priority="207" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="304" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
-    <cfRule type="cellIs" dxfId="303" priority="205" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="303" priority="207" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21">
-    <cfRule type="cellIs" dxfId="302" priority="204" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="302" priority="206" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI64">
-    <cfRule type="cellIs" dxfId="301" priority="203" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="301" priority="205" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI23">
-    <cfRule type="cellIs" dxfId="300" priority="202" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="300" priority="204" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ24">
-    <cfRule type="cellIs" dxfId="299" priority="201" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="299" priority="203" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI25">
-    <cfRule type="cellIs" dxfId="298" priority="200" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="298" priority="202" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ25">
-    <cfRule type="cellIs" dxfId="297" priority="199" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="297" priority="201" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ67">
-    <cfRule type="cellIs" dxfId="296" priority="198" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="296" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI26">
-    <cfRule type="cellIs" dxfId="295" priority="197" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="295" priority="199" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ26:AJ27">
-    <cfRule type="cellIs" dxfId="294" priority="196" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="294" priority="198" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI28:AI30">
-    <cfRule type="cellIs" dxfId="293" priority="195" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="293" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28:AJ31">
-    <cfRule type="cellIs" dxfId="292" priority="194" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="292" priority="196" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI72">
-    <cfRule type="cellIs" dxfId="291" priority="193" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="291" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ72">
-    <cfRule type="cellIs" dxfId="290" priority="192" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="290" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI73">
-    <cfRule type="cellIs" dxfId="289" priority="191" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="289" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ73">
-    <cfRule type="cellIs" dxfId="288" priority="190" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="288" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI32">
-    <cfRule type="cellIs" dxfId="287" priority="189" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="287" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="cellIs" dxfId="286" priority="188" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="286" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI33">
-    <cfRule type="cellIs" dxfId="285" priority="187" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="285" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ33">
-    <cfRule type="cellIs" dxfId="284" priority="186" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="284" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI34:AI35">
-    <cfRule type="cellIs" dxfId="283" priority="185" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="283" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ34:AJ36">
-    <cfRule type="cellIs" dxfId="282" priority="184" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="282" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI61">
-    <cfRule type="cellIs" dxfId="281" priority="183" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="281" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI63">
-    <cfRule type="cellIs" dxfId="280" priority="182" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="280" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ70">
-    <cfRule type="cellIs" dxfId="279" priority="181" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="279" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI70">
-    <cfRule type="cellIs" dxfId="278" priority="180" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="278" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI68">
-    <cfRule type="cellIs" dxfId="277" priority="179" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="277" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ76">
-    <cfRule type="cellIs" dxfId="276" priority="178" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="276" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI76">
-    <cfRule type="cellIs" dxfId="275" priority="177" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="275" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ78">
-    <cfRule type="cellIs" dxfId="274" priority="176" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="274" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI78">
-    <cfRule type="cellIs" dxfId="273" priority="175" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="273" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38">
-    <cfRule type="cellIs" dxfId="272" priority="174" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="272" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38">
-    <cfRule type="cellIs" dxfId="271" priority="173" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="271" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ77">
-    <cfRule type="cellIs" dxfId="270" priority="172" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="270" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI77">
-    <cfRule type="cellIs" dxfId="269" priority="171" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="269" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ79">
-    <cfRule type="cellIs" dxfId="268" priority="170" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="268" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI79">
-    <cfRule type="cellIs" dxfId="267" priority="169" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="267" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ80">
-    <cfRule type="cellIs" dxfId="266" priority="168" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="266" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80">
-    <cfRule type="cellIs" dxfId="265" priority="167" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="265" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ81">
-    <cfRule type="cellIs" dxfId="264" priority="166" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="264" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI81">
-    <cfRule type="cellIs" dxfId="263" priority="165" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="263" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ82">
-    <cfRule type="cellIs" dxfId="262" priority="164" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="262" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI82">
-    <cfRule type="cellIs" dxfId="261" priority="163" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="261" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI83">
-    <cfRule type="cellIs" dxfId="260" priority="162" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="260" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI84:AI85">
-    <cfRule type="cellIs" dxfId="259" priority="161" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="259" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI39">
-    <cfRule type="cellIs" dxfId="258" priority="160" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="258" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="cellIs" dxfId="257" priority="159" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="257" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O61">
-    <cfRule type="cellIs" dxfId="256" priority="158" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="256" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54">
-    <cfRule type="cellIs" dxfId="255" priority="157" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="255" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O57">
-    <cfRule type="cellIs" dxfId="254" priority="156" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="254" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O58">
-    <cfRule type="cellIs" dxfId="253" priority="155" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="253" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O67">
-    <cfRule type="cellIs" dxfId="252" priority="154" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="252" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71">
-    <cfRule type="cellIs" dxfId="251" priority="153" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72">
-    <cfRule type="cellIs" dxfId="250" priority="152" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="250" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="249" priority="151" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="249" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="248" priority="150" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="248" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="247" priority="148" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L75">
-    <cfRule type="cellIs" dxfId="246" priority="146" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="246" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI12">
-    <cfRule type="cellIs" dxfId="245" priority="145" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2">
-    <cfRule type="cellIs" dxfId="244" priority="144" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="244" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10 W65:W67 W86 W40:W42 W44 W32 W69:W71">
-    <cfRule type="cellIs" dxfId="243" priority="143" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="243" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="cellIs" dxfId="242" priority="142" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="242" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
-    <cfRule type="cellIs" dxfId="241" priority="141" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="241" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2">
-    <cfRule type="cellIs" dxfId="240" priority="140" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="240" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y74 Y33:Y59 Y76:Y86">
-    <cfRule type="cellIs" dxfId="239" priority="139" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y74 Y33:Y37 Y76:Y77 Y39:Y59 Y80:Y86">
+    <cfRule type="cellIs" dxfId="239" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2">
-    <cfRule type="cellIs" dxfId="238" priority="138" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="238" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="237" priority="137" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="237" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="cellIs" dxfId="236" priority="136" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="236" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="235" priority="135" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="235" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
-    <cfRule type="cellIs" dxfId="234" priority="134" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="234" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA48">
-    <cfRule type="cellIs" dxfId="233" priority="133" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="233" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA11">
-    <cfRule type="cellIs" dxfId="232" priority="132" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="232" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA51">
-    <cfRule type="cellIs" dxfId="231" priority="131" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="231" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA52">
-    <cfRule type="cellIs" dxfId="230" priority="130" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="230" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA53">
-    <cfRule type="cellIs" dxfId="229" priority="129" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="229" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57 AA54:AA55">
-    <cfRule type="cellIs" dxfId="228" priority="128" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="228" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA20">
-    <cfRule type="cellIs" dxfId="227" priority="127" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="227" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA21">
-    <cfRule type="cellIs" dxfId="226" priority="126" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="226" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA66">
-    <cfRule type="cellIs" dxfId="225" priority="125" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="225" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA25">
-    <cfRule type="cellIs" dxfId="224" priority="124" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="224" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA26">
-    <cfRule type="cellIs" dxfId="223" priority="123" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="223" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA28">
-    <cfRule type="cellIs" dxfId="222" priority="122" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="222" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA32">
-    <cfRule type="cellIs" dxfId="221" priority="121" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="221" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA34">
-    <cfRule type="cellIs" dxfId="220" priority="120" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="220" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27">
-    <cfRule type="cellIs" dxfId="219" priority="119" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="219" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA33 AA31">
-    <cfRule type="cellIs" dxfId="218" priority="118" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="218" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA61 M61">
-    <cfRule type="cellIs" dxfId="217" priority="117" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="217" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA62">
-    <cfRule type="cellIs" dxfId="216" priority="116" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="216" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA63 M63">
-    <cfRule type="cellIs" dxfId="215" priority="115" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="215" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA65">
-    <cfRule type="cellIs" dxfId="214" priority="114" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="214" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA67">
-    <cfRule type="cellIs" dxfId="213" priority="113" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="213" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA68">
-    <cfRule type="cellIs" dxfId="212" priority="112" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="212" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA70:AA73">
-    <cfRule type="cellIs" dxfId="211" priority="111" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="211" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA77">
-    <cfRule type="cellIs" dxfId="210" priority="110" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="210" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA74 AA38">
-    <cfRule type="cellIs" dxfId="209" priority="109" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="209" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37">
-    <cfRule type="cellIs" dxfId="208" priority="108" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="208" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="207" priority="107" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="207" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S46">
-    <cfRule type="cellIs" dxfId="206" priority="106" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="206" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S48">
-    <cfRule type="cellIs" dxfId="205" priority="105" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="205" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S18">
-    <cfRule type="cellIs" dxfId="204" priority="104" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="204" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54">
-    <cfRule type="cellIs" dxfId="203" priority="103" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="203" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S55">
-    <cfRule type="cellIs" dxfId="202" priority="102" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="202" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S57">
-    <cfRule type="cellIs" dxfId="201" priority="101" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="201" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S76">
-    <cfRule type="cellIs" dxfId="200" priority="100" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="200" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S78">
-    <cfRule type="cellIs" dxfId="199" priority="99" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="199" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S81">
-    <cfRule type="cellIs" dxfId="198" priority="98" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="198" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S82">
-    <cfRule type="cellIs" dxfId="197" priority="97" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="197" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="196" priority="96" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="196" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="cellIs" dxfId="195" priority="95" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="195" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L67">
-    <cfRule type="cellIs" dxfId="194" priority="94" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="194" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="193" priority="93" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="193" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="192" priority="92" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="192" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="191" priority="91" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="191" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="190" priority="89" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="190" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="189" priority="88" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="189" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="188" priority="87" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="188" priority="89" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="cellIs" dxfId="187" priority="86" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="187" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="186" priority="83" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="186" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55">
-    <cfRule type="cellIs" dxfId="185" priority="82" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="185" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="184" priority="81" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="184" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="183" priority="80" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="183" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60">
-    <cfRule type="cellIs" dxfId="182" priority="79" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="182" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L76">
-    <cfRule type="cellIs" dxfId="181" priority="77" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="181" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="cellIs" dxfId="180" priority="76" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="180" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="cellIs" dxfId="179" priority="75" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="179" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="cellIs" dxfId="178" priority="74" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="178" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="177" priority="73" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="177" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y14">
-    <cfRule type="cellIs" dxfId="176" priority="72" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="176" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="175" priority="71" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="175" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK14">
-    <cfRule type="cellIs" dxfId="174" priority="70" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="174" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X61">
-    <cfRule type="cellIs" dxfId="173" priority="69" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="173" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W75">
-    <cfRule type="cellIs" dxfId="172" priority="68" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="172" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y75">
-    <cfRule type="cellIs" dxfId="171" priority="67" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="171" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76">
-    <cfRule type="cellIs" dxfId="170" priority="66" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="170" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="169" priority="65" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="169" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="168" priority="64" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="168" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W76">
-    <cfRule type="cellIs" dxfId="167" priority="63" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="167" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W77">
-    <cfRule type="cellIs" dxfId="166" priority="62" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W78">
-    <cfRule type="cellIs" dxfId="165" priority="61" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="166" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W80">
-    <cfRule type="cellIs" dxfId="164" priority="60" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="165" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W37">
+    <cfRule type="cellIs" dxfId="164" priority="61" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W74">
     <cfRule type="cellIs" dxfId="163" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W74">
-    <cfRule type="cellIs" dxfId="162" priority="57" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="W45">
-    <cfRule type="cellIs" dxfId="161" priority="56" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="162" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W46">
-    <cfRule type="cellIs" dxfId="160" priority="55" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="161" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W47">
-    <cfRule type="cellIs" dxfId="159" priority="54" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="160" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4">
-    <cfRule type="cellIs" dxfId="158" priority="53" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="159" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W5">
-    <cfRule type="cellIs" dxfId="157" priority="52" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="158" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="156" priority="51" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="157" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8">
-    <cfRule type="cellIs" dxfId="155" priority="50" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="156" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W9">
-    <cfRule type="cellIs" dxfId="154" priority="49" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="155" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W48">
-    <cfRule type="cellIs" dxfId="153" priority="48" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="154" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W50">
-    <cfRule type="cellIs" dxfId="152" priority="47" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="153" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W11">
-    <cfRule type="cellIs" dxfId="151" priority="46" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="152" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W12">
-    <cfRule type="cellIs" dxfId="150" priority="45" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="151" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W13">
-    <cfRule type="cellIs" dxfId="149" priority="44" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="150" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W15">
-    <cfRule type="cellIs" dxfId="148" priority="43" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="149" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W16">
-    <cfRule type="cellIs" dxfId="147" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="148" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W51">
-    <cfRule type="cellIs" dxfId="146" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="147" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W52">
-    <cfRule type="cellIs" dxfId="145" priority="40" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="146" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W53">
-    <cfRule type="cellIs" dxfId="144" priority="39" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="145" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W54">
-    <cfRule type="cellIs" dxfId="143" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="144" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W55">
-    <cfRule type="cellIs" dxfId="142" priority="37" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="143" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W57">
-    <cfRule type="cellIs" dxfId="141" priority="36" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="142" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W58">
+    <cfRule type="cellIs" dxfId="141" priority="37" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W62">
     <cfRule type="cellIs" dxfId="140" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W62">
-    <cfRule type="cellIs" dxfId="139" priority="33" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="W63">
-    <cfRule type="cellIs" dxfId="138" priority="32" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="139" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W21">
-    <cfRule type="cellIs" dxfId="137" priority="31" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="138" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W22">
-    <cfRule type="cellIs" dxfId="136" priority="30" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="137" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W24">
-    <cfRule type="cellIs" dxfId="135" priority="29" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="136" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W25">
-    <cfRule type="cellIs" dxfId="134" priority="28" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W27">
-    <cfRule type="cellIs" dxfId="133" priority="27" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="134" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W28">
-    <cfRule type="cellIs" dxfId="132" priority="26" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="133" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W29">
-    <cfRule type="cellIs" dxfId="131" priority="25" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="132" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W30">
-    <cfRule type="cellIs" dxfId="130" priority="24" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="131" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W31">
-    <cfRule type="cellIs" dxfId="129" priority="23" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="130" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W72">
-    <cfRule type="cellIs" dxfId="128" priority="22" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="129" priority="24" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W73">
-    <cfRule type="cellIs" dxfId="127" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="128" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W68">
-    <cfRule type="cellIs" dxfId="126" priority="18" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="127" priority="20" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W38">
-    <cfRule type="cellIs" dxfId="125" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="126" priority="19" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X38">
-    <cfRule type="cellIs" dxfId="124" priority="16" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K77">
-    <cfRule type="cellIs" dxfId="123" priority="14" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W79">
-    <cfRule type="cellIs" dxfId="122" priority="13" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X79">
-    <cfRule type="cellIs" dxfId="121" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="125" priority="18" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L80">
-    <cfRule type="cellIs" dxfId="120" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="122" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K80">
+    <cfRule type="cellIs" dxfId="121" priority="10" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="cellIs" dxfId="120" priority="9" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="119" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K36">
     <cfRule type="cellIs" dxfId="118" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K74">
     <cfRule type="cellIs" dxfId="117" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
-    <cfRule type="cellIs" dxfId="116" priority="5" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G37">
+    <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="cellIs" dxfId="115" priority="4" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="Y38">
+    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
+  <conditionalFormatting sqref="K78">
     <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -48330,34 +48328,34 @@
       <c r="D19" s="112"/>
       <c r="E19" s="112"/>
       <c r="F19" s="112"/>
-      <c r="G19" s="153" t="s">
+      <c r="G19" s="154" t="s">
         <v>717</v>
       </c>
-      <c r="H19" s="154"/>
-      <c r="I19" s="154"/>
-      <c r="J19" s="154"/>
-      <c r="K19" s="155"/>
-      <c r="M19" s="153" t="s">
+      <c r="H19" s="155"/>
+      <c r="I19" s="155"/>
+      <c r="J19" s="155"/>
+      <c r="K19" s="156"/>
+      <c r="M19" s="154" t="s">
         <v>718</v>
       </c>
-      <c r="N19" s="154"/>
-      <c r="O19" s="154"/>
-      <c r="P19" s="154"/>
-      <c r="Q19" s="155"/>
-      <c r="S19" s="153" t="s">
+      <c r="N19" s="155"/>
+      <c r="O19" s="155"/>
+      <c r="P19" s="155"/>
+      <c r="Q19" s="156"/>
+      <c r="S19" s="154" t="s">
         <v>716</v>
       </c>
-      <c r="T19" s="154"/>
-      <c r="U19" s="154"/>
-      <c r="V19" s="154"/>
-      <c r="W19" s="155"/>
-      <c r="Y19" s="153" t="s">
+      <c r="T19" s="155"/>
+      <c r="U19" s="155"/>
+      <c r="V19" s="155"/>
+      <c r="W19" s="156"/>
+      <c r="Y19" s="154" t="s">
         <v>724</v>
       </c>
-      <c r="Z19" s="154"/>
-      <c r="AA19" s="154"/>
-      <c r="AB19" s="154"/>
-      <c r="AC19" s="155"/>
+      <c r="Z19" s="155"/>
+      <c r="AA19" s="155"/>
+      <c r="AB19" s="155"/>
+      <c r="AC19" s="156"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A20" s="113"/>
@@ -48366,26 +48364,26 @@
       <c r="D20" s="112"/>
       <c r="E20" s="112"/>
       <c r="F20" s="112"/>
-      <c r="G20" s="156"/>
-      <c r="H20" s="157"/>
-      <c r="I20" s="157"/>
-      <c r="J20" s="157"/>
-      <c r="K20" s="158"/>
-      <c r="M20" s="156"/>
-      <c r="N20" s="157"/>
-      <c r="O20" s="157"/>
-      <c r="P20" s="157"/>
-      <c r="Q20" s="158"/>
-      <c r="S20" s="156"/>
-      <c r="T20" s="157"/>
-      <c r="U20" s="157"/>
-      <c r="V20" s="157"/>
-      <c r="W20" s="158"/>
-      <c r="Y20" s="156"/>
-      <c r="Z20" s="157"/>
-      <c r="AA20" s="157"/>
-      <c r="AB20" s="157"/>
-      <c r="AC20" s="158"/>
+      <c r="G20" s="157"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="158"/>
+      <c r="J20" s="158"/>
+      <c r="K20" s="159"/>
+      <c r="M20" s="157"/>
+      <c r="N20" s="158"/>
+      <c r="O20" s="158"/>
+      <c r="P20" s="158"/>
+      <c r="Q20" s="159"/>
+      <c r="S20" s="157"/>
+      <c r="T20" s="158"/>
+      <c r="U20" s="158"/>
+      <c r="V20" s="158"/>
+      <c r="W20" s="159"/>
+      <c r="Y20" s="157"/>
+      <c r="Z20" s="158"/>
+      <c r="AA20" s="158"/>
+      <c r="AB20" s="158"/>
+      <c r="AC20" s="159"/>
     </row>
     <row r="21" spans="1:29" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="113"/>
@@ -48394,26 +48392,26 @@
       <c r="D21" s="112"/>
       <c r="E21" s="112"/>
       <c r="F21" s="112"/>
-      <c r="G21" s="159"/>
-      <c r="H21" s="160"/>
-      <c r="I21" s="160"/>
-      <c r="J21" s="160"/>
-      <c r="K21" s="161"/>
-      <c r="M21" s="159"/>
-      <c r="N21" s="160"/>
-      <c r="O21" s="160"/>
-      <c r="P21" s="160"/>
-      <c r="Q21" s="161"/>
-      <c r="S21" s="159"/>
-      <c r="T21" s="160"/>
-      <c r="U21" s="160"/>
-      <c r="V21" s="160"/>
-      <c r="W21" s="161"/>
-      <c r="Y21" s="159"/>
-      <c r="Z21" s="160"/>
-      <c r="AA21" s="160"/>
-      <c r="AB21" s="160"/>
-      <c r="AC21" s="161"/>
+      <c r="G21" s="160"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161"/>
+      <c r="J21" s="161"/>
+      <c r="K21" s="162"/>
+      <c r="M21" s="160"/>
+      <c r="N21" s="161"/>
+      <c r="O21" s="161"/>
+      <c r="P21" s="161"/>
+      <c r="Q21" s="162"/>
+      <c r="S21" s="160"/>
+      <c r="T21" s="161"/>
+      <c r="U21" s="161"/>
+      <c r="V21" s="161"/>
+      <c r="W21" s="162"/>
+      <c r="Y21" s="160"/>
+      <c r="Z21" s="161"/>
+      <c r="AA21" s="161"/>
+      <c r="AB21" s="161"/>
+      <c r="AC21" s="162"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B24" s="12" t="s">
@@ -48436,95 +48434,95 @@
     </row>
     <row r="40" spans="1:29" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="41" spans="1:29" ht="12.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="153" t="s">
+      <c r="A41" s="154" t="s">
         <v>719</v>
       </c>
-      <c r="B41" s="154"/>
-      <c r="C41" s="154"/>
-      <c r="D41" s="154"/>
-      <c r="E41" s="155"/>
-      <c r="G41" s="153" t="s">
+      <c r="B41" s="155"/>
+      <c r="C41" s="155"/>
+      <c r="D41" s="155"/>
+      <c r="E41" s="156"/>
+      <c r="G41" s="154" t="s">
         <v>722</v>
       </c>
-      <c r="H41" s="154"/>
-      <c r="I41" s="154"/>
-      <c r="J41" s="154"/>
-      <c r="K41" s="155"/>
-      <c r="M41" s="153" t="s">
+      <c r="H41" s="155"/>
+      <c r="I41" s="155"/>
+      <c r="J41" s="155"/>
+      <c r="K41" s="156"/>
+      <c r="M41" s="154" t="s">
         <v>723</v>
       </c>
-      <c r="N41" s="154"/>
-      <c r="O41" s="154"/>
-      <c r="P41" s="154"/>
-      <c r="Q41" s="155"/>
-      <c r="S41" s="153" t="s">
+      <c r="N41" s="155"/>
+      <c r="O41" s="155"/>
+      <c r="P41" s="155"/>
+      <c r="Q41" s="156"/>
+      <c r="S41" s="154" t="s">
         <v>729</v>
       </c>
-      <c r="T41" s="154"/>
-      <c r="U41" s="154"/>
-      <c r="V41" s="154"/>
-      <c r="W41" s="155"/>
-      <c r="Y41" s="153" t="s">
+      <c r="T41" s="155"/>
+      <c r="U41" s="155"/>
+      <c r="V41" s="155"/>
+      <c r="W41" s="156"/>
+      <c r="Y41" s="154" t="s">
         <v>731</v>
       </c>
-      <c r="Z41" s="154"/>
-      <c r="AA41" s="154"/>
-      <c r="AB41" s="154"/>
-      <c r="AC41" s="155"/>
+      <c r="Z41" s="155"/>
+      <c r="AA41" s="155"/>
+      <c r="AB41" s="155"/>
+      <c r="AC41" s="156"/>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A42" s="156"/>
-      <c r="B42" s="157"/>
-      <c r="C42" s="157"/>
-      <c r="D42" s="157"/>
-      <c r="E42" s="158"/>
-      <c r="G42" s="156"/>
-      <c r="H42" s="157"/>
-      <c r="I42" s="157"/>
-      <c r="J42" s="157"/>
-      <c r="K42" s="158"/>
-      <c r="M42" s="156"/>
-      <c r="N42" s="157"/>
-      <c r="O42" s="157"/>
-      <c r="P42" s="157"/>
-      <c r="Q42" s="158"/>
-      <c r="S42" s="156"/>
-      <c r="T42" s="157"/>
-      <c r="U42" s="157"/>
-      <c r="V42" s="157"/>
-      <c r="W42" s="158"/>
-      <c r="Y42" s="156"/>
-      <c r="Z42" s="157"/>
-      <c r="AA42" s="157"/>
-      <c r="AB42" s="157"/>
-      <c r="AC42" s="158"/>
+      <c r="A42" s="157"/>
+      <c r="B42" s="158"/>
+      <c r="C42" s="158"/>
+      <c r="D42" s="158"/>
+      <c r="E42" s="159"/>
+      <c r="G42" s="157"/>
+      <c r="H42" s="158"/>
+      <c r="I42" s="158"/>
+      <c r="J42" s="158"/>
+      <c r="K42" s="159"/>
+      <c r="M42" s="157"/>
+      <c r="N42" s="158"/>
+      <c r="O42" s="158"/>
+      <c r="P42" s="158"/>
+      <c r="Q42" s="159"/>
+      <c r="S42" s="157"/>
+      <c r="T42" s="158"/>
+      <c r="U42" s="158"/>
+      <c r="V42" s="158"/>
+      <c r="W42" s="159"/>
+      <c r="Y42" s="157"/>
+      <c r="Z42" s="158"/>
+      <c r="AA42" s="158"/>
+      <c r="AB42" s="158"/>
+      <c r="AC42" s="159"/>
     </row>
     <row r="43" spans="1:29" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="159"/>
-      <c r="B43" s="160"/>
-      <c r="C43" s="160"/>
-      <c r="D43" s="160"/>
-      <c r="E43" s="161"/>
-      <c r="G43" s="159"/>
-      <c r="H43" s="160"/>
-      <c r="I43" s="160"/>
-      <c r="J43" s="160"/>
-      <c r="K43" s="161"/>
-      <c r="M43" s="159"/>
-      <c r="N43" s="160"/>
-      <c r="O43" s="160"/>
-      <c r="P43" s="160"/>
-      <c r="Q43" s="161"/>
-      <c r="S43" s="159"/>
-      <c r="T43" s="160"/>
-      <c r="U43" s="160"/>
-      <c r="V43" s="160"/>
-      <c r="W43" s="161"/>
-      <c r="Y43" s="159"/>
-      <c r="Z43" s="160"/>
-      <c r="AA43" s="160"/>
-      <c r="AB43" s="160"/>
-      <c r="AC43" s="161"/>
+      <c r="A43" s="160"/>
+      <c r="B43" s="161"/>
+      <c r="C43" s="161"/>
+      <c r="D43" s="161"/>
+      <c r="E43" s="162"/>
+      <c r="G43" s="160"/>
+      <c r="H43" s="161"/>
+      <c r="I43" s="161"/>
+      <c r="J43" s="161"/>
+      <c r="K43" s="162"/>
+      <c r="M43" s="160"/>
+      <c r="N43" s="161"/>
+      <c r="O43" s="161"/>
+      <c r="P43" s="161"/>
+      <c r="Q43" s="162"/>
+      <c r="S43" s="160"/>
+      <c r="T43" s="161"/>
+      <c r="U43" s="161"/>
+      <c r="V43" s="161"/>
+      <c r="W43" s="162"/>
+      <c r="Y43" s="160"/>
+      <c r="Z43" s="161"/>
+      <c r="AA43" s="161"/>
+      <c r="AB43" s="161"/>
+      <c r="AC43" s="162"/>
     </row>
     <row r="45" spans="1:29" s="112" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45"/>
@@ -48609,98 +48607,98 @@
       <c r="L63" s="112"/>
     </row>
     <row r="64" spans="1:29" ht="12.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="153" t="s">
+      <c r="A64" s="154" t="s">
         <v>734</v>
       </c>
-      <c r="B64" s="154"/>
-      <c r="C64" s="154"/>
-      <c r="D64" s="154"/>
-      <c r="E64" s="155"/>
-      <c r="G64" s="153" t="s">
+      <c r="B64" s="155"/>
+      <c r="C64" s="155"/>
+      <c r="D64" s="155"/>
+      <c r="E64" s="156"/>
+      <c r="G64" s="154" t="s">
         <v>735</v>
       </c>
-      <c r="H64" s="154"/>
-      <c r="I64" s="154"/>
-      <c r="J64" s="154"/>
-      <c r="K64" s="155"/>
+      <c r="H64" s="155"/>
+      <c r="I64" s="155"/>
+      <c r="J64" s="155"/>
+      <c r="K64" s="156"/>
       <c r="L64" s="112"/>
-      <c r="M64" s="162" t="s">
+      <c r="M64" s="163" t="s">
         <v>739</v>
       </c>
-      <c r="N64" s="163"/>
-      <c r="O64" s="163"/>
-      <c r="P64" s="163"/>
-      <c r="Q64" s="164"/>
-      <c r="S64" s="162" t="s">
+      <c r="N64" s="164"/>
+      <c r="O64" s="164"/>
+      <c r="P64" s="164"/>
+      <c r="Q64" s="165"/>
+      <c r="S64" s="163" t="s">
         <v>740</v>
       </c>
-      <c r="T64" s="163"/>
-      <c r="U64" s="163"/>
-      <c r="V64" s="163"/>
-      <c r="W64" s="164"/>
-      <c r="Y64" s="162" t="s">
+      <c r="T64" s="164"/>
+      <c r="U64" s="164"/>
+      <c r="V64" s="164"/>
+      <c r="W64" s="165"/>
+      <c r="Y64" s="163" t="s">
         <v>741</v>
       </c>
-      <c r="Z64" s="163"/>
-      <c r="AA64" s="163"/>
-      <c r="AB64" s="163"/>
-      <c r="AC64" s="164"/>
+      <c r="Z64" s="164"/>
+      <c r="AA64" s="164"/>
+      <c r="AB64" s="164"/>
+      <c r="AC64" s="165"/>
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A65" s="156"/>
-      <c r="B65" s="157"/>
-      <c r="C65" s="157"/>
-      <c r="D65" s="157"/>
-      <c r="E65" s="158"/>
-      <c r="G65" s="156"/>
-      <c r="H65" s="157"/>
-      <c r="I65" s="157"/>
-      <c r="J65" s="157"/>
-      <c r="K65" s="158"/>
+      <c r="A65" s="157"/>
+      <c r="B65" s="158"/>
+      <c r="C65" s="158"/>
+      <c r="D65" s="158"/>
+      <c r="E65" s="159"/>
+      <c r="G65" s="157"/>
+      <c r="H65" s="158"/>
+      <c r="I65" s="158"/>
+      <c r="J65" s="158"/>
+      <c r="K65" s="159"/>
       <c r="L65" s="112"/>
-      <c r="M65" s="165"/>
-      <c r="N65" s="166"/>
-      <c r="O65" s="166"/>
-      <c r="P65" s="166"/>
-      <c r="Q65" s="167"/>
-      <c r="S65" s="165"/>
-      <c r="T65" s="166"/>
-      <c r="U65" s="166"/>
-      <c r="V65" s="166"/>
-      <c r="W65" s="167"/>
-      <c r="Y65" s="165"/>
-      <c r="Z65" s="166"/>
-      <c r="AA65" s="166"/>
-      <c r="AB65" s="166"/>
-      <c r="AC65" s="167"/>
+      <c r="M65" s="166"/>
+      <c r="N65" s="167"/>
+      <c r="O65" s="167"/>
+      <c r="P65" s="167"/>
+      <c r="Q65" s="168"/>
+      <c r="S65" s="166"/>
+      <c r="T65" s="167"/>
+      <c r="U65" s="167"/>
+      <c r="V65" s="167"/>
+      <c r="W65" s="168"/>
+      <c r="Y65" s="166"/>
+      <c r="Z65" s="167"/>
+      <c r="AA65" s="167"/>
+      <c r="AB65" s="167"/>
+      <c r="AC65" s="168"/>
     </row>
     <row r="66" spans="1:29" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="159"/>
-      <c r="B66" s="160"/>
-      <c r="C66" s="160"/>
-      <c r="D66" s="160"/>
-      <c r="E66" s="161"/>
-      <c r="G66" s="159"/>
-      <c r="H66" s="160"/>
-      <c r="I66" s="160"/>
-      <c r="J66" s="160"/>
-      <c r="K66" s="161"/>
+      <c r="A66" s="160"/>
+      <c r="B66" s="161"/>
+      <c r="C66" s="161"/>
+      <c r="D66" s="161"/>
+      <c r="E66" s="162"/>
+      <c r="G66" s="160"/>
+      <c r="H66" s="161"/>
+      <c r="I66" s="161"/>
+      <c r="J66" s="161"/>
+      <c r="K66" s="162"/>
       <c r="L66" s="112"/>
-      <c r="M66" s="168"/>
-      <c r="N66" s="169"/>
-      <c r="O66" s="169"/>
-      <c r="P66" s="169"/>
-      <c r="Q66" s="170"/>
-      <c r="S66" s="168"/>
-      <c r="T66" s="169"/>
-      <c r="U66" s="169"/>
-      <c r="V66" s="169"/>
-      <c r="W66" s="170"/>
-      <c r="Y66" s="168"/>
-      <c r="Z66" s="169"/>
-      <c r="AA66" s="169"/>
-      <c r="AB66" s="169"/>
-      <c r="AC66" s="170"/>
+      <c r="M66" s="169"/>
+      <c r="N66" s="170"/>
+      <c r="O66" s="170"/>
+      <c r="P66" s="170"/>
+      <c r="Q66" s="171"/>
+      <c r="S66" s="169"/>
+      <c r="T66" s="170"/>
+      <c r="U66" s="170"/>
+      <c r="V66" s="170"/>
+      <c r="W66" s="171"/>
+      <c r="Y66" s="169"/>
+      <c r="Z66" s="170"/>
+      <c r="AA66" s="170"/>
+      <c r="AB66" s="170"/>
+      <c r="AC66" s="171"/>
     </row>
     <row r="69" spans="1:29" ht="23.65" x14ac:dyDescent="0.4">
       <c r="D69" s="116" t="s">
@@ -64492,13 +64490,13 @@
       <c r="C1" s="66" t="s">
         <v>477</v>
       </c>
-      <c r="F1" s="171" t="s">
+      <c r="F1" s="172" t="s">
         <v>476</v>
       </c>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="171"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="172"/>
+      <c r="J1" s="172"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D2" s="61" t="s">
@@ -64523,7 +64521,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43606</v>
+        <v>43628</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -64833,7 +64831,7 @@
   <dimension ref="B1:Y87"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="7545" activePane="bottomLeft"/>
+      <pane ySplit="7080" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -64872,7 +64870,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43606</v>
+        <v>43628</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
update record drawings status
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C629CDEE-3000-4C5F-ACEE-1E561F5623C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90B708C-EA92-4319-B06D-635C6F00CC5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1433" yWindow="7710" windowWidth="18180" windowHeight="4890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -5363,6 +5363,20 @@
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="403">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -8170,20 +8184,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -8430,7 +8430,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6/12/2019</c:v>
+                  <c:v>6/19/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10182,15 +10182,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1110" activePane="bottomLeft"/>
+      <pane ySplit="1095" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="K89" sqref="K89"/>
+      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -10489,7 +10489,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="2" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>86</v>
       </c>
@@ -10660,7 +10660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>86</v>
       </c>
@@ -10831,7 +10831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>86</v>
       </c>
@@ -11004,7 +11004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="13" t="s">
         <v>86</v>
       </c>
@@ -11175,7 +11175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>86</v>
       </c>
@@ -11364,7 +11364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:82" s="18" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:82" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="13" t="s">
         <v>86</v>
       </c>
@@ -11537,7 +11537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:82" s="18" customFormat="1" ht="34.35" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:82" s="18" customFormat="1" ht="34.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>86</v>
       </c>
@@ -11708,7 +11708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>86</v>
       </c>
@@ -11879,7 +11879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:82" s="18" customFormat="1" ht="26.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:82" s="18" customFormat="1" ht="26.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13" t="s">
         <v>86</v>
       </c>
@@ -12050,7 +12050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13" t="s">
         <v>86</v>
       </c>
@@ -12223,7 +12223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>86</v>
       </c>
@@ -12249,8 +12249,8 @@
       <c r="J12" s="118" t="s">
         <v>1354</v>
       </c>
-      <c r="K12" s="118" t="s">
-        <v>567</v>
+      <c r="K12" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="L12" s="13"/>
       <c r="M12" s="48" t="s">
@@ -12388,7 +12388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="13" t="s">
         <v>86</v>
       </c>
@@ -12559,7 +12559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="13" t="s">
         <v>86</v>
       </c>
@@ -12728,7 +12728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="13" t="s">
         <v>86</v>
       </c>
@@ -12754,8 +12754,8 @@
       <c r="J15" s="118" t="s">
         <v>1354</v>
       </c>
-      <c r="K15" s="118" t="s">
-        <v>567</v>
+      <c r="K15" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="L15" s="13"/>
       <c r="M15" s="48" t="s">
@@ -12895,7 +12895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:82" s="18" customFormat="1" ht="26.1" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:82" s="18" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="13" t="s">
         <v>86</v>
       </c>
@@ -13068,7 +13068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
         <v>86</v>
       </c>
@@ -13233,7 +13233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B18" s="13" t="s">
         <v>86</v>
       </c>
@@ -13404,7 +13404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B19" s="13" t="s">
         <v>86</v>
       </c>
@@ -13567,7 +13567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B20" s="13" t="s">
         <v>86</v>
       </c>
@@ -13738,7 +13738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B21" s="13" t="s">
         <v>86</v>
       </c>
@@ -13911,7 +13911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B22" s="13" t="s">
         <v>86</v>
       </c>
@@ -14074,7 +14074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B23" s="13" t="s">
         <v>86</v>
       </c>
@@ -14233,7 +14233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B24" s="13" t="s">
         <v>86</v>
       </c>
@@ -14404,7 +14404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B25" s="13" t="s">
         <v>86</v>
       </c>
@@ -14573,7 +14573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B26" s="13" t="s">
         <v>86</v>
       </c>
@@ -14740,7 +14740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B27" s="13" t="s">
         <v>86</v>
       </c>
@@ -14909,7 +14909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B28" s="13" t="s">
         <v>86</v>
       </c>
@@ -15078,7 +15078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B29" s="13" t="s">
         <v>86</v>
       </c>
@@ -15247,7 +15247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B30" s="13" t="s">
         <v>86</v>
       </c>
@@ -15418,7 +15418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B31" s="13" t="s">
         <v>86</v>
       </c>
@@ -15444,8 +15444,8 @@
       <c r="J31" s="118" t="s">
         <v>1223</v>
       </c>
-      <c r="K31" s="118" t="s">
-        <v>567</v>
+      <c r="K31" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="L31" s="13"/>
       <c r="M31" s="118" t="s">
@@ -15579,7 +15579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:82" s="18" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:82" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="B32" s="13" t="s">
         <v>86</v>
       </c>
@@ -15750,7 +15750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B33" s="13" t="s">
         <v>86</v>
       </c>
@@ -15915,7 +15915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B34" s="13" t="s">
         <v>86</v>
       </c>
@@ -16084,7 +16084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B35" s="13" t="s">
         <v>86</v>
       </c>
@@ -16110,8 +16110,8 @@
       <c r="J35" s="119" t="s">
         <v>1353</v>
       </c>
-      <c r="K35" s="118" t="s">
-        <v>567</v>
+      <c r="K35" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="L35" s="13"/>
       <c r="M35" s="52" t="s">
@@ -16249,7 +16249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:82" s="18" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:82" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="B36" s="13" t="s">
         <v>86</v>
       </c>
@@ -16416,7 +16416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B37" s="13" t="s">
         <v>86</v>
       </c>
@@ -16577,7 +16577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B38" s="13" t="s">
         <v>86</v>
       </c>
@@ -16748,7 +16748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
         <v>86</v>
       </c>
@@ -16937,7 +16937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B40" s="13" t="s">
         <v>86</v>
       </c>
@@ -17126,7 +17126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:82" s="18" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:82" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="B41" s="13" t="s">
         <v>86</v>
       </c>
@@ -17289,7 +17289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:82" s="18" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:82" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="B42" s="13" t="s">
         <v>86</v>
       </c>
@@ -17450,7 +17450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B43" s="13" t="s">
         <v>4</v>
       </c>
@@ -17651,7 +17651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B44" s="13" t="s">
         <v>4</v>
       </c>
@@ -17812,7 +17812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B45" s="13" t="s">
         <v>4</v>
       </c>
@@ -17989,7 +17989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B46" s="13" t="s">
         <v>4</v>
       </c>
@@ -18160,7 +18160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B47" s="13" t="s">
         <v>4</v>
       </c>
@@ -18329,7 +18329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B48" s="13" t="s">
         <v>4</v>
       </c>
@@ -18502,7 +18502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B49" s="13" t="s">
         <v>4</v>
       </c>
@@ -18667,7 +18667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B50" s="13" t="s">
         <v>4</v>
       </c>
@@ -18870,7 +18870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B51" s="13" t="s">
         <v>4</v>
       </c>
@@ -19039,7 +19039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B52" s="13" t="s">
         <v>4</v>
       </c>
@@ -19212,7 +19212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B53" s="13" t="s">
         <v>4</v>
       </c>
@@ -19377,7 +19377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B54" s="13" t="s">
         <v>4</v>
       </c>
@@ -19556,7 +19556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B55" s="13" t="s">
         <v>4</v>
       </c>
@@ -19721,7 +19721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B56" s="13" t="s">
         <v>4</v>
       </c>
@@ -19888,7 +19888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B57" s="13" t="s">
         <v>4</v>
       </c>
@@ -20053,7 +20053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B58" s="13" t="s">
         <v>4</v>
       </c>
@@ -20252,7 +20252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B59" s="13" t="s">
         <v>4</v>
       </c>
@@ -20423,7 +20423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B60" s="13" t="s">
         <v>4</v>
       </c>
@@ -20586,7 +20586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B61" s="13" t="s">
         <v>4</v>
       </c>
@@ -20751,7 +20751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B62" s="13" t="s">
         <v>4</v>
       </c>
@@ -20918,7 +20918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B63" s="13" t="s">
         <v>4</v>
       </c>
@@ -21073,7 +21073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B64" s="13" t="s">
         <v>4</v>
       </c>
@@ -21242,7 +21242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B65" s="13" t="s">
         <v>4</v>
       </c>
@@ -21413,7 +21413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B66" s="13" t="s">
         <v>4</v>
       </c>
@@ -21584,7 +21584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B67" s="13" t="s">
         <v>4</v>
       </c>
@@ -21751,7 +21751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B68" s="13" t="s">
         <v>4</v>
       </c>
@@ -21777,8 +21777,8 @@
       <c r="J68" s="118" t="s">
         <v>1136</v>
       </c>
-      <c r="K68" s="118" t="s">
-        <v>567</v>
+      <c r="K68" s="145" t="s">
+        <v>1116</v>
       </c>
       <c r="L68" s="13"/>
       <c r="M68" s="145" t="s">
@@ -21922,7 +21922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B69" s="13" t="s">
         <v>4</v>
       </c>
@@ -22087,7 +22087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B70" s="13" t="s">
         <v>4</v>
       </c>
@@ -22254,7 +22254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:82" s="18" customFormat="1" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:82" s="18" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="13" t="s">
         <v>4</v>
       </c>
@@ -22419,7 +22419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:82" s="18" customFormat="1" ht="9.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:82" s="18" customFormat="1" ht="9.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" s="13" t="s">
         <v>4</v>
       </c>
@@ -22582,7 +22582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B73" s="13" t="s">
         <v>4</v>
       </c>
@@ -22608,8 +22608,8 @@
       <c r="J73" s="118" t="s">
         <v>1223</v>
       </c>
-      <c r="K73" s="118" t="s">
-        <v>567</v>
+      <c r="K73" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="L73" s="13"/>
       <c r="M73" s="118" t="s">
@@ -22745,7 +22745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:82" s="18" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:82" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="B74" s="13" t="s">
         <v>4</v>
       </c>
@@ -22944,7 +22944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B75" s="13" t="s">
         <v>4</v>
       </c>
@@ -23145,7 +23145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B76" s="13" t="s">
         <v>4</v>
       </c>
@@ -23320,7 +23320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:82" s="18" customFormat="1" ht="23.65" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B77" s="13" t="s">
         <v>4</v>
       </c>
@@ -23493,7 +23493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B78" s="13" t="s">
         <v>4</v>
       </c>
@@ -23654,7 +23654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B79" s="13" t="s">
         <v>4</v>
       </c>
@@ -24002,7 +24002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B81" s="13" t="s">
         <v>4</v>
       </c>
@@ -24197,7 +24197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:82" s="18" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B82" s="13" t="s">
         <v>4</v>
       </c>
@@ -24392,7 +24392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B83" s="13" t="s">
         <v>4</v>
       </c>
@@ -24581,7 +24581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:82" s="18" customFormat="1" ht="9.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:82" s="18" customFormat="1" ht="9.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="13" t="s">
         <v>4</v>
       </c>
@@ -24772,7 +24772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B85" s="13" t="s">
         <v>4</v>
       </c>
@@ -24963,7 +24963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:82" s="18" customFormat="1" ht="7.9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
       <c r="B86" s="13" t="s">
         <v>4</v>
       </c>
@@ -25166,1736 +25166,1742 @@
       <c r="L101" s="147"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:BZ86" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="14520"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:BZ86" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:CA86">
     <sortCondition ref="B2:B86"/>
     <sortCondition ref="D2:D86"/>
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
-    <cfRule type="cellIs" dxfId="402" priority="354" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="402" priority="356" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI9:BJ9">
-    <cfRule type="cellIs" dxfId="401" priority="353" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="401" priority="355" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="400" priority="352" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="400" priority="354" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="399" priority="351" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="399" priority="353" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
-    <cfRule type="cellIs" dxfId="398" priority="349" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="398" priority="351" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="397" priority="348" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="397" priority="350" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="396" priority="347" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="396" priority="349" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="395" priority="343" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="395" priority="345" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="394" priority="333" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="394" priority="335" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I3 I44 I14 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="393" priority="320" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="393" priority="322" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="392" priority="309" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="392" priority="311" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
-    <cfRule type="cellIs" dxfId="391" priority="306" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="391" priority="308" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD2">
-    <cfRule type="cellIs" dxfId="390" priority="305" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="390" priority="307" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K42 K63 K10 K12 K53 K15:K17 K57 K31 K44 K49 K68:K73 K35 K37:K38 K81:K82">
-    <cfRule type="cellIs" dxfId="389" priority="304" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K41:K42 K63 K10 K53 K16:K17 K57 K31 K44 K49 K37:K38 K81:K82 K69:K73">
+    <cfRule type="cellIs" dxfId="389" priority="306" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
-    <cfRule type="cellIs" dxfId="388" priority="303" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="388" priority="305" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L79 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5 L81:L85">
-    <cfRule type="cellIs" dxfId="387" priority="302" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="387" priority="304" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="386" priority="301" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="386" priority="303" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="385" priority="298" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="385" priority="300" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="384" priority="297" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="384" priority="299" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="383" priority="295" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="383" priority="297" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="382" priority="293" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="382" priority="295" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
-    <cfRule type="cellIs" dxfId="381" priority="291" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="381" priority="293" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
-    <cfRule type="cellIs" dxfId="380" priority="290" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="380" priority="292" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q86">
-    <cfRule type="cellIs" dxfId="379" priority="289" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="379" priority="291" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
-    <cfRule type="cellIs" dxfId="378" priority="288" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="378" priority="290" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AE86">
-    <cfRule type="cellIs" dxfId="377" priority="287" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="377" priority="289" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
-    <cfRule type="cellIs" dxfId="376" priority="286" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="376" priority="288" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
-    <cfRule type="cellIs" dxfId="375" priority="285" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="375" priority="287" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK2:AK13 AK15:AK86">
-    <cfRule type="cellIs" dxfId="374" priority="284" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="374" priority="286" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM2:AM86">
-    <cfRule type="cellIs" dxfId="373" priority="283" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="373" priority="285" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="cellIs" dxfId="372" priority="282" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="372" priority="284" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="371" priority="281" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="371" priority="283" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="370" priority="280" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="370" priority="282" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="369" priority="279" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="369" priority="281" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="cellIs" dxfId="368" priority="278" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="368" priority="280" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
-    <cfRule type="cellIs" dxfId="367" priority="277" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="367" priority="279" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="366" priority="276" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="366" priority="278" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="365" priority="275" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="365" priority="277" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="364" priority="274" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="364" priority="276" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="363" priority="273" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="363" priority="275" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="362" priority="269" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="362" priority="271" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="361" priority="268" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="361" priority="270" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60">
-    <cfRule type="cellIs" dxfId="360" priority="267" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="360" priority="269" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:N14">
-    <cfRule type="cellIs" dxfId="359" priority="266" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="359" priority="268" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="358" priority="265" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="358" priority="267" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="357" priority="264" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="357" priority="266" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
-    <cfRule type="cellIs" dxfId="356" priority="263" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="356" priority="265" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="cellIs" dxfId="355" priority="262" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="355" priority="264" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="cellIs" dxfId="354" priority="261" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="354" priority="263" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ43">
-    <cfRule type="cellIs" dxfId="353" priority="260" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="353" priority="262" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI43">
-    <cfRule type="cellIs" dxfId="352" priority="259" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="352" priority="261" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3">
-    <cfRule type="cellIs" dxfId="351" priority="258" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="351" priority="260" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3">
-    <cfRule type="cellIs" dxfId="350" priority="257" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="350" priority="259" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ4">
-    <cfRule type="cellIs" dxfId="349" priority="256" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="349" priority="258" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI4">
-    <cfRule type="cellIs" dxfId="348" priority="255" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="348" priority="257" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ5">
-    <cfRule type="cellIs" dxfId="347" priority="254" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="347" priority="256" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI5">
-    <cfRule type="cellIs" dxfId="346" priority="253" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="346" priority="255" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ6">
-    <cfRule type="cellIs" dxfId="345" priority="252" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="345" priority="254" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6">
-    <cfRule type="cellIs" dxfId="344" priority="251" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="344" priority="253" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ7">
-    <cfRule type="cellIs" dxfId="343" priority="250" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="343" priority="252" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI7">
-    <cfRule type="cellIs" dxfId="342" priority="249" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="342" priority="251" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:AJ9">
-    <cfRule type="cellIs" dxfId="341" priority="248" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="341" priority="250" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI8">
-    <cfRule type="cellIs" dxfId="340" priority="247" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="340" priority="249" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ46">
-    <cfRule type="cellIs" dxfId="339" priority="246" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="339" priority="248" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI46">
-    <cfRule type="cellIs" dxfId="338" priority="245" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="338" priority="247" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ47">
-    <cfRule type="cellIs" dxfId="337" priority="244" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="337" priority="246" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI47">
-    <cfRule type="cellIs" dxfId="336" priority="243" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="336" priority="245" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10">
-    <cfRule type="cellIs" dxfId="335" priority="242" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="335" priority="244" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI10">
-    <cfRule type="cellIs" dxfId="334" priority="241" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="334" priority="243" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ48">
-    <cfRule type="cellIs" dxfId="333" priority="240" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="333" priority="242" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI48">
-    <cfRule type="cellIs" dxfId="332" priority="239" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="332" priority="241" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ49">
-    <cfRule type="cellIs" dxfId="331" priority="238" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="331" priority="240" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="330" priority="237" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="330" priority="239" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="329" priority="236" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="329" priority="238" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI50">
-    <cfRule type="cellIs" dxfId="328" priority="234" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="328" priority="236" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11:AJ13">
-    <cfRule type="cellIs" dxfId="327" priority="233" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="327" priority="235" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI11">
-    <cfRule type="cellIs" dxfId="326" priority="232" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="326" priority="234" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ51">
-    <cfRule type="cellIs" dxfId="325" priority="231" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="325" priority="233" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI52">
-    <cfRule type="cellIs" dxfId="324" priority="230" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="324" priority="232" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ52:AJ54">
-    <cfRule type="cellIs" dxfId="323" priority="229" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="323" priority="231" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ56">
-    <cfRule type="cellIs" dxfId="322" priority="228" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="322" priority="230" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI56">
-    <cfRule type="cellIs" dxfId="321" priority="227" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="321" priority="229" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ57:AJ58">
-    <cfRule type="cellIs" dxfId="320" priority="226" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="320" priority="228" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI57:AI58">
-    <cfRule type="cellIs" dxfId="319" priority="225" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="319" priority="227" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ15:AJ16">
-    <cfRule type="cellIs" dxfId="318" priority="224" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="318" priority="226" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI15:AI16">
-    <cfRule type="cellIs" dxfId="317" priority="223" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="317" priority="225" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ59:AJ60">
-    <cfRule type="cellIs" dxfId="316" priority="222" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="316" priority="224" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ55">
-    <cfRule type="cellIs" dxfId="315" priority="221" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="315" priority="223" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="cellIs" dxfId="314" priority="220" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="314" priority="222" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="cellIs" dxfId="313" priority="219" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="313" priority="221" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI18">
-    <cfRule type="cellIs" dxfId="312" priority="218" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="312" priority="220" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="311" priority="217" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="311" priority="219" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI17">
-    <cfRule type="cellIs" dxfId="310" priority="216" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="310" priority="218" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ17">
-    <cfRule type="cellIs" dxfId="309" priority="215" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="309" priority="217" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI86">
-    <cfRule type="cellIs" dxfId="308" priority="214" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="308" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI40">
-    <cfRule type="cellIs" dxfId="307" priority="213" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="307" priority="215" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="306" priority="212" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="306" priority="214" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="305" priority="211" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="305" priority="213" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="304" priority="209" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="304" priority="211" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
-    <cfRule type="cellIs" dxfId="303" priority="207" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="303" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21">
-    <cfRule type="cellIs" dxfId="302" priority="206" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="302" priority="208" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI64">
-    <cfRule type="cellIs" dxfId="301" priority="205" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="301" priority="207" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI23">
-    <cfRule type="cellIs" dxfId="300" priority="204" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="300" priority="206" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ24">
-    <cfRule type="cellIs" dxfId="299" priority="203" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="299" priority="205" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI25">
-    <cfRule type="cellIs" dxfId="298" priority="202" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="298" priority="204" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ25">
-    <cfRule type="cellIs" dxfId="297" priority="201" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="297" priority="203" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ67">
-    <cfRule type="cellIs" dxfId="296" priority="200" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="296" priority="202" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI26">
-    <cfRule type="cellIs" dxfId="295" priority="199" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="295" priority="201" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ26:AJ27">
-    <cfRule type="cellIs" dxfId="294" priority="198" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="294" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI28:AI30">
-    <cfRule type="cellIs" dxfId="293" priority="197" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="293" priority="199" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ28:AJ31">
-    <cfRule type="cellIs" dxfId="292" priority="196" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="292" priority="198" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI72">
-    <cfRule type="cellIs" dxfId="291" priority="195" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="291" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ72">
-    <cfRule type="cellIs" dxfId="290" priority="194" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="290" priority="196" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI73">
-    <cfRule type="cellIs" dxfId="289" priority="193" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="289" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ73">
-    <cfRule type="cellIs" dxfId="288" priority="192" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="288" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI32">
-    <cfRule type="cellIs" dxfId="287" priority="191" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="287" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="cellIs" dxfId="286" priority="190" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="286" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI33">
-    <cfRule type="cellIs" dxfId="285" priority="189" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="285" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ33">
-    <cfRule type="cellIs" dxfId="284" priority="188" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="284" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI34:AI35">
-    <cfRule type="cellIs" dxfId="283" priority="187" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="283" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ34:AJ36">
-    <cfRule type="cellIs" dxfId="282" priority="186" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="282" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI61">
-    <cfRule type="cellIs" dxfId="281" priority="185" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="281" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI63">
-    <cfRule type="cellIs" dxfId="280" priority="184" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="280" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ70">
-    <cfRule type="cellIs" dxfId="279" priority="183" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="279" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI70">
-    <cfRule type="cellIs" dxfId="278" priority="182" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="278" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI68">
-    <cfRule type="cellIs" dxfId="277" priority="181" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="277" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ76">
-    <cfRule type="cellIs" dxfId="276" priority="180" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="276" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI76">
-    <cfRule type="cellIs" dxfId="275" priority="179" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="275" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ78">
-    <cfRule type="cellIs" dxfId="274" priority="178" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="274" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI78">
-    <cfRule type="cellIs" dxfId="273" priority="177" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="273" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38">
-    <cfRule type="cellIs" dxfId="272" priority="176" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="272" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38">
-    <cfRule type="cellIs" dxfId="271" priority="175" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="271" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ77">
-    <cfRule type="cellIs" dxfId="270" priority="174" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="270" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI77">
-    <cfRule type="cellIs" dxfId="269" priority="173" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="269" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ79">
-    <cfRule type="cellIs" dxfId="268" priority="172" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="268" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI79">
-    <cfRule type="cellIs" dxfId="267" priority="171" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="267" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ80">
-    <cfRule type="cellIs" dxfId="266" priority="170" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="266" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80">
-    <cfRule type="cellIs" dxfId="265" priority="169" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="265" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ81">
-    <cfRule type="cellIs" dxfId="264" priority="168" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="264" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI81">
-    <cfRule type="cellIs" dxfId="263" priority="167" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="263" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ82">
-    <cfRule type="cellIs" dxfId="262" priority="166" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="262" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI82">
-    <cfRule type="cellIs" dxfId="261" priority="165" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="261" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI83">
-    <cfRule type="cellIs" dxfId="260" priority="164" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="260" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI84:AI85">
-    <cfRule type="cellIs" dxfId="259" priority="163" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="259" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI39">
-    <cfRule type="cellIs" dxfId="258" priority="162" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="258" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="cellIs" dxfId="257" priority="161" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="257" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O61">
-    <cfRule type="cellIs" dxfId="256" priority="160" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="256" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54">
-    <cfRule type="cellIs" dxfId="255" priority="159" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="255" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O57">
-    <cfRule type="cellIs" dxfId="254" priority="158" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="254" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O58">
-    <cfRule type="cellIs" dxfId="253" priority="157" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="253" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O67">
-    <cfRule type="cellIs" dxfId="252" priority="156" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="252" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71">
-    <cfRule type="cellIs" dxfId="251" priority="155" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="251" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72">
-    <cfRule type="cellIs" dxfId="250" priority="154" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="250" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="249" priority="153" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="249" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="248" priority="152" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="248" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="247" priority="150" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="247" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L75">
-    <cfRule type="cellIs" dxfId="246" priority="148" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="246" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI12">
-    <cfRule type="cellIs" dxfId="245" priority="147" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="245" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2">
-    <cfRule type="cellIs" dxfId="244" priority="146" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="244" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10 W65:W67 W86 W40:W42 W44 W32 W69:W71">
-    <cfRule type="cellIs" dxfId="243" priority="145" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="243" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="cellIs" dxfId="242" priority="144" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="242" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
-    <cfRule type="cellIs" dxfId="241" priority="143" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="241" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2">
-    <cfRule type="cellIs" dxfId="240" priority="142" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="240" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y74 Y33:Y37 Y76:Y77 Y39:Y59 Y80:Y86">
-    <cfRule type="cellIs" dxfId="239" priority="141" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="239" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2">
-    <cfRule type="cellIs" dxfId="238" priority="140" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="238" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="237" priority="139" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="237" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="cellIs" dxfId="236" priority="138" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="236" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="235" priority="137" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="235" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
-    <cfRule type="cellIs" dxfId="234" priority="136" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="234" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA48">
-    <cfRule type="cellIs" dxfId="233" priority="135" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="233" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA11">
-    <cfRule type="cellIs" dxfId="232" priority="134" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="232" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA51">
-    <cfRule type="cellIs" dxfId="231" priority="133" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="231" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA52">
-    <cfRule type="cellIs" dxfId="230" priority="132" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="230" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA53">
-    <cfRule type="cellIs" dxfId="229" priority="131" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="229" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57 AA54:AA55">
-    <cfRule type="cellIs" dxfId="228" priority="130" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="228" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA20">
-    <cfRule type="cellIs" dxfId="227" priority="129" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="227" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA21">
-    <cfRule type="cellIs" dxfId="226" priority="128" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="226" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA66">
-    <cfRule type="cellIs" dxfId="225" priority="127" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="225" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA25">
-    <cfRule type="cellIs" dxfId="224" priority="126" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="224" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA26">
-    <cfRule type="cellIs" dxfId="223" priority="125" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="223" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA28">
-    <cfRule type="cellIs" dxfId="222" priority="124" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="222" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA32">
-    <cfRule type="cellIs" dxfId="221" priority="123" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="221" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA34">
-    <cfRule type="cellIs" dxfId="220" priority="122" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="220" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27">
-    <cfRule type="cellIs" dxfId="219" priority="121" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="219" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA33 AA31">
-    <cfRule type="cellIs" dxfId="218" priority="120" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="218" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA61 M61">
-    <cfRule type="cellIs" dxfId="217" priority="119" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="217" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA62">
-    <cfRule type="cellIs" dxfId="216" priority="118" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="216" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA63 M63">
-    <cfRule type="cellIs" dxfId="215" priority="117" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="215" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA65">
-    <cfRule type="cellIs" dxfId="214" priority="116" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="214" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA67">
-    <cfRule type="cellIs" dxfId="213" priority="115" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="213" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA68">
-    <cfRule type="cellIs" dxfId="212" priority="114" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="212" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA70:AA73">
-    <cfRule type="cellIs" dxfId="211" priority="113" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="211" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA77">
-    <cfRule type="cellIs" dxfId="210" priority="112" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="210" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA74 AA38">
-    <cfRule type="cellIs" dxfId="209" priority="111" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="209" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA37">
-    <cfRule type="cellIs" dxfId="208" priority="110" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="208" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="207" priority="109" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="207" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S46">
-    <cfRule type="cellIs" dxfId="206" priority="108" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="206" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S48">
-    <cfRule type="cellIs" dxfId="205" priority="107" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="205" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S18">
-    <cfRule type="cellIs" dxfId="204" priority="106" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="204" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54">
-    <cfRule type="cellIs" dxfId="203" priority="105" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="203" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S55">
-    <cfRule type="cellIs" dxfId="202" priority="104" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="202" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S57">
-    <cfRule type="cellIs" dxfId="201" priority="103" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="201" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S76">
-    <cfRule type="cellIs" dxfId="200" priority="102" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="200" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S78">
-    <cfRule type="cellIs" dxfId="199" priority="101" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="199" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S81">
-    <cfRule type="cellIs" dxfId="198" priority="100" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="198" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S82">
-    <cfRule type="cellIs" dxfId="197" priority="99" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="197" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="196" priority="98" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="196" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="cellIs" dxfId="195" priority="97" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="195" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L67">
-    <cfRule type="cellIs" dxfId="194" priority="96" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="194" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="193" priority="95" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="193" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="192" priority="94" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="192" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="191" priority="93" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="191" priority="95" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="190" priority="91" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="190" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="189" priority="90" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="189" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="188" priority="89" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="188" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="cellIs" dxfId="187" priority="88" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="187" priority="90" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="186" priority="85" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="186" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55">
-    <cfRule type="cellIs" dxfId="185" priority="84" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="185" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="184" priority="83" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="184" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="183" priority="82" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="183" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60">
-    <cfRule type="cellIs" dxfId="182" priority="81" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="182" priority="83" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L76">
-    <cfRule type="cellIs" dxfId="181" priority="79" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="181" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="cellIs" dxfId="180" priority="78" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="180" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="cellIs" dxfId="179" priority="77" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="179" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="cellIs" dxfId="178" priority="76" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="178" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="177" priority="75" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="177" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y14">
-    <cfRule type="cellIs" dxfId="176" priority="74" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="176" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="175" priority="73" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="175" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK14">
-    <cfRule type="cellIs" dxfId="174" priority="72" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="174" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X61">
-    <cfRule type="cellIs" dxfId="173" priority="71" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="173" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W75">
-    <cfRule type="cellIs" dxfId="172" priority="70" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="172" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y75">
-    <cfRule type="cellIs" dxfId="171" priority="69" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="171" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76">
-    <cfRule type="cellIs" dxfId="170" priority="68" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="170" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="169" priority="67" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="169" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="168" priority="66" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="168" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W76">
-    <cfRule type="cellIs" dxfId="167" priority="65" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="167" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W77">
-    <cfRule type="cellIs" dxfId="166" priority="64" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="166" priority="66" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W80">
-    <cfRule type="cellIs" dxfId="165" priority="62" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="165" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W37">
-    <cfRule type="cellIs" dxfId="164" priority="61" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="164" priority="63" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W74">
-    <cfRule type="cellIs" dxfId="163" priority="59" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="163" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W45">
-    <cfRule type="cellIs" dxfId="162" priority="58" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="162" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W46">
-    <cfRule type="cellIs" dxfId="161" priority="57" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="161" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W47">
-    <cfRule type="cellIs" dxfId="160" priority="56" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="160" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4">
-    <cfRule type="cellIs" dxfId="159" priority="55" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="159" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W5">
-    <cfRule type="cellIs" dxfId="158" priority="54" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="158" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7">
-    <cfRule type="cellIs" dxfId="157" priority="53" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="157" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8">
-    <cfRule type="cellIs" dxfId="156" priority="52" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="156" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W9">
-    <cfRule type="cellIs" dxfId="155" priority="51" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="155" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W48">
-    <cfRule type="cellIs" dxfId="154" priority="50" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="154" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W50">
-    <cfRule type="cellIs" dxfId="153" priority="49" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="153" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W11">
-    <cfRule type="cellIs" dxfId="152" priority="48" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="152" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W12">
-    <cfRule type="cellIs" dxfId="151" priority="47" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="151" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W13">
-    <cfRule type="cellIs" dxfId="150" priority="46" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="150" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W15">
-    <cfRule type="cellIs" dxfId="149" priority="45" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="149" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W16">
-    <cfRule type="cellIs" dxfId="148" priority="44" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="148" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W51">
-    <cfRule type="cellIs" dxfId="147" priority="43" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="147" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W52">
-    <cfRule type="cellIs" dxfId="146" priority="42" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="146" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W53">
-    <cfRule type="cellIs" dxfId="145" priority="41" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="145" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W54">
-    <cfRule type="cellIs" dxfId="144" priority="40" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="144" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W55">
-    <cfRule type="cellIs" dxfId="143" priority="39" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="143" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W57">
-    <cfRule type="cellIs" dxfId="142" priority="38" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="142" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W58">
-    <cfRule type="cellIs" dxfId="141" priority="37" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="141" priority="39" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W62">
-    <cfRule type="cellIs" dxfId="140" priority="35" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="140" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W63">
-    <cfRule type="cellIs" dxfId="139" priority="34" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="139" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W21">
-    <cfRule type="cellIs" dxfId="138" priority="33" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="138" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W22">
-    <cfRule type="cellIs" dxfId="137" priority="32" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="137" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W24">
-    <cfRule type="cellIs" dxfId="136" priority="31" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="136" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W25">
-    <cfRule type="cellIs" dxfId="135" priority="30" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W27">
-    <cfRule type="cellIs" dxfId="134" priority="29" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="134" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W28">
-    <cfRule type="cellIs" dxfId="133" priority="28" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="133" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W29">
-    <cfRule type="cellIs" dxfId="132" priority="27" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="132" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W30">
-    <cfRule type="cellIs" dxfId="131" priority="26" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="131" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W31">
-    <cfRule type="cellIs" dxfId="130" priority="25" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="130" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W72">
-    <cfRule type="cellIs" dxfId="129" priority="24" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="129" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W73">
-    <cfRule type="cellIs" dxfId="128" priority="23" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="128" priority="25" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W68">
-    <cfRule type="cellIs" dxfId="127" priority="20" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="127" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W38">
-    <cfRule type="cellIs" dxfId="126" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="126" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X38">
-    <cfRule type="cellIs" dxfId="125" priority="18" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="125" priority="20" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L80">
-    <cfRule type="cellIs" dxfId="122" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="124" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K80">
+    <cfRule type="cellIs" dxfId="123" priority="12" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="cellIs" dxfId="122" priority="11" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="121" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K36">
     <cfRule type="cellIs" dxfId="120" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K74">
     <cfRule type="cellIs" dxfId="119" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
-    <cfRule type="cellIs" dxfId="118" priority="7" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G37">
+    <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="cellIs" dxfId="117" priority="6" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="Y38">
+    <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
+  <conditionalFormatting sqref="K78">
     <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y38">
-    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K68">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K78">
-    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K35">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -47757,448 +47763,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="115" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="114" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="102" priority="93">
+    <cfRule type="containsBlanks" dxfId="104" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="100" priority="91">
+    <cfRule type="containsBlanks" dxfId="102" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="101" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="100" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="90" priority="69">
+    <cfRule type="containsBlanks" dxfId="92" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="91" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="90" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="88" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="82" priority="63">
+    <cfRule type="containsBlanks" dxfId="84" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="83" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="82" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="77" priority="59">
+    <cfRule type="containsBlanks" dxfId="79" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="78" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="75" priority="56">
+    <cfRule type="containsBlanks" dxfId="77" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="76" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="75" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="68" priority="50">
+    <cfRule type="containsBlanks" dxfId="70" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="69" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="68" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="65" priority="47">
+    <cfRule type="containsBlanks" dxfId="67" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="66" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="65" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="60" priority="42">
+    <cfRule type="containsBlanks" dxfId="62" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="61" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="60" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="57" priority="39">
+    <cfRule type="containsBlanks" dxfId="59" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="58" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="57" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="42" priority="23">
+    <cfRule type="containsBlanks" dxfId="44" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="40" priority="19">
+    <cfRule type="containsBlanks" dxfId="42" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="40" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="31" priority="22">
+    <cfRule type="containsBlanks" dxfId="33" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="30" priority="11">
+    <cfRule type="containsBlanks" dxfId="32" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="31" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -63093,111 +63099,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -64521,7 +64527,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43628</v>
+        <v>43635</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -64831,7 +64837,7 @@
   <dimension ref="B1:Y87"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="7080" activePane="bottomLeft"/>
+      <pane ySplit="6930" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
@@ -64870,7 +64876,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43628</v>
+        <v>43635</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -68877,7 +68883,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated 04-115516 dsa cert mesa fine arts
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90B708C-EA92-4319-B06D-635C6F00CC5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDB7F11-A1C8-4397-8F46-D778926E78B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9029" uniqueCount="1408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9030" uniqueCount="1409">
   <si>
     <t>#</t>
   </si>
@@ -4269,6 +4269,9 @@
   </si>
   <si>
     <t>missing some structural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-07-01 (Dow) CM13 and SP minutes in combined pdf </t>
   </si>
 </sst>
 </file>
@@ -5362,21 +5365,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="403">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="404">
     <dxf>
       <fill>
         <patternFill>
@@ -8184,6 +8173,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -8430,7 +8440,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6/19/2019</c:v>
+                  <c:v>8/14/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10190,7 +10200,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1095" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -10533,11 +10543,11 @@
       <c r="P2" s="13" t="s">
         <v>1224</v>
       </c>
-      <c r="Q2" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R2" s="118">
-        <v>1</v>
+      <c r="Q2" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="R2" s="118" t="s">
+        <v>1408</v>
       </c>
       <c r="S2" s="52" t="s">
         <v>166</v>
@@ -11004,7 +11014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:82" s="18" customFormat="1" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="13" t="s">
         <v>86</v>
       </c>
@@ -12309,8 +12319,8 @@
         <v>567</v>
       </c>
       <c r="AF12" s="118"/>
-      <c r="AG12" s="118" t="s">
-        <v>567</v>
+      <c r="AG12" s="150" t="s">
+        <v>166</v>
       </c>
       <c r="AH12" s="118"/>
       <c r="AI12" s="150" t="s">
@@ -12742,8 +12752,8 @@
       <c r="F15" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G15" s="48" t="s">
-        <v>170</v>
+      <c r="G15" s="52" t="s">
+        <v>166</v>
       </c>
       <c r="H15" s="118" t="s">
         <v>1335</v>
@@ -25173,1735 +25183,1741 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
+    <cfRule type="cellIs" dxfId="403" priority="357" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BI9:BJ9">
     <cfRule type="cellIs" dxfId="402" priority="356" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BI9:BJ9">
+  <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
     <cfRule type="cellIs" dxfId="401" priority="355" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
+  <conditionalFormatting sqref="AV39 AV56">
     <cfRule type="cellIs" dxfId="400" priority="354" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="399" priority="353" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
+    <cfRule type="cellIs" dxfId="399" priority="352" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
+  <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
     <cfRule type="cellIs" dxfId="398" priority="351" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
+  <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
     <cfRule type="cellIs" dxfId="397" priority="350" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="396" priority="349" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="395" priority="345" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="396" priority="346" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="394" priority="335" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="395" priority="336" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I3 I44 I14 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="393" priority="322" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="394" priority="323" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="392" priority="311" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="393" priority="312" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
+    <cfRule type="cellIs" dxfId="392" priority="309" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CD2">
     <cfRule type="cellIs" dxfId="391" priority="308" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CD2">
+  <conditionalFormatting sqref="K41:K42 K63 K10 K53 K16:K17 K57 K31 K44 K49 K37:K38 K81:K82 K69:K73">
     <cfRule type="cellIs" dxfId="390" priority="307" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:K42 K63 K10 K53 K16:K17 K57 K31 K44 K49 K37:K38 K81:K82 K69:K73">
+  <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
     <cfRule type="cellIs" dxfId="389" priority="306" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
+  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L79 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5 L81:L85">
     <cfRule type="cellIs" dxfId="388" priority="305" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L79 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5 L81:L85">
+  <conditionalFormatting sqref="I35">
     <cfRule type="cellIs" dxfId="387" priority="304" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="386" priority="303" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="T2">
+    <cfRule type="cellIs" dxfId="386" priority="301" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2">
+  <conditionalFormatting sqref="AH2:AH86">
     <cfRule type="cellIs" dxfId="385" priority="300" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="384" priority="299" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="383" priority="297" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="384" priority="298" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="382" priority="295" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="383" priority="296" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
+    <cfRule type="cellIs" dxfId="382" priority="294" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
     <cfRule type="cellIs" dxfId="381" priority="293" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
+  <conditionalFormatting sqref="Q3:Q86">
     <cfRule type="cellIs" dxfId="380" priority="292" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q86">
+  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
     <cfRule type="cellIs" dxfId="379" priority="291" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
+  <conditionalFormatting sqref="AE2:AE86">
     <cfRule type="cellIs" dxfId="378" priority="290" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE86">
+  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG11 AG13:AG86">
     <cfRule type="cellIs" dxfId="377" priority="289" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG86">
+  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
     <cfRule type="cellIs" dxfId="376" priority="288" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
+  <conditionalFormatting sqref="AK2:AK13 AK15:AK86">
     <cfRule type="cellIs" dxfId="375" priority="287" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK13 AK15:AK86">
+  <conditionalFormatting sqref="AM2:AM86">
     <cfRule type="cellIs" dxfId="374" priority="286" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AM86">
+  <conditionalFormatting sqref="N46">
     <cfRule type="cellIs" dxfId="373" priority="285" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46">
+  <conditionalFormatting sqref="N9">
     <cfRule type="cellIs" dxfId="372" priority="284" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9">
+  <conditionalFormatting sqref="N6">
     <cfRule type="cellIs" dxfId="371" priority="283" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6">
+  <conditionalFormatting sqref="N48">
     <cfRule type="cellIs" dxfId="370" priority="282" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N48">
+  <conditionalFormatting sqref="N45">
     <cfRule type="cellIs" dxfId="369" priority="281" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N45">
+  <conditionalFormatting sqref="N50">
     <cfRule type="cellIs" dxfId="368" priority="280" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N5">
     <cfRule type="cellIs" dxfId="367" priority="279" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
+  <conditionalFormatting sqref="N2">
     <cfRule type="cellIs" dxfId="366" priority="278" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
+  <conditionalFormatting sqref="N3">
     <cfRule type="cellIs" dxfId="365" priority="277" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
+  <conditionalFormatting sqref="N10">
     <cfRule type="cellIs" dxfId="364" priority="276" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="363" priority="275" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="N52">
+    <cfRule type="cellIs" dxfId="363" priority="272" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
+  <conditionalFormatting sqref="N16">
     <cfRule type="cellIs" dxfId="362" priority="271" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
+  <conditionalFormatting sqref="N60">
     <cfRule type="cellIs" dxfId="361" priority="270" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N60">
+  <conditionalFormatting sqref="M14:N14">
     <cfRule type="cellIs" dxfId="360" priority="269" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:N14">
+  <conditionalFormatting sqref="M34">
     <cfRule type="cellIs" dxfId="359" priority="268" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M34">
+  <conditionalFormatting sqref="N26">
     <cfRule type="cellIs" dxfId="358" priority="267" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
+  <conditionalFormatting sqref="M26">
     <cfRule type="cellIs" dxfId="357" priority="266" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26">
+  <conditionalFormatting sqref="N28">
     <cfRule type="cellIs" dxfId="356" priority="265" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
+  <conditionalFormatting sqref="M68">
     <cfRule type="cellIs" dxfId="355" priority="264" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M68">
+  <conditionalFormatting sqref="AJ43">
     <cfRule type="cellIs" dxfId="354" priority="263" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ43">
+  <conditionalFormatting sqref="AI43">
     <cfRule type="cellIs" dxfId="353" priority="262" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI43">
+  <conditionalFormatting sqref="AJ3">
     <cfRule type="cellIs" dxfId="352" priority="261" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ3">
+  <conditionalFormatting sqref="AI3">
     <cfRule type="cellIs" dxfId="351" priority="260" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI3">
+  <conditionalFormatting sqref="AJ4">
     <cfRule type="cellIs" dxfId="350" priority="259" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ4">
+  <conditionalFormatting sqref="AI4">
     <cfRule type="cellIs" dxfId="349" priority="258" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI4">
+  <conditionalFormatting sqref="AJ5">
     <cfRule type="cellIs" dxfId="348" priority="257" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ5">
+  <conditionalFormatting sqref="AI5">
     <cfRule type="cellIs" dxfId="347" priority="256" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI5">
+  <conditionalFormatting sqref="AJ6">
     <cfRule type="cellIs" dxfId="346" priority="255" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ6">
+  <conditionalFormatting sqref="AI6">
     <cfRule type="cellIs" dxfId="345" priority="254" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI6">
+  <conditionalFormatting sqref="AJ7">
     <cfRule type="cellIs" dxfId="344" priority="253" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ7">
+  <conditionalFormatting sqref="AI7">
     <cfRule type="cellIs" dxfId="343" priority="252" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI7">
+  <conditionalFormatting sqref="AJ8:AJ9">
     <cfRule type="cellIs" dxfId="342" priority="251" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ8:AJ9">
+  <conditionalFormatting sqref="AI8">
     <cfRule type="cellIs" dxfId="341" priority="250" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI8">
+  <conditionalFormatting sqref="AJ46">
     <cfRule type="cellIs" dxfId="340" priority="249" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ46">
+  <conditionalFormatting sqref="AI46">
     <cfRule type="cellIs" dxfId="339" priority="248" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI46">
+  <conditionalFormatting sqref="AJ47">
     <cfRule type="cellIs" dxfId="338" priority="247" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ47">
+  <conditionalFormatting sqref="AI47">
     <cfRule type="cellIs" dxfId="337" priority="246" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI47">
+  <conditionalFormatting sqref="AJ10">
     <cfRule type="cellIs" dxfId="336" priority="245" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ10">
+  <conditionalFormatting sqref="AI10">
     <cfRule type="cellIs" dxfId="335" priority="244" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI10">
+  <conditionalFormatting sqref="AJ48">
     <cfRule type="cellIs" dxfId="334" priority="243" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ48">
+  <conditionalFormatting sqref="AI48">
     <cfRule type="cellIs" dxfId="333" priority="242" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI48">
+  <conditionalFormatting sqref="AJ49">
     <cfRule type="cellIs" dxfId="332" priority="241" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ49">
+  <conditionalFormatting sqref="AI49">
     <cfRule type="cellIs" dxfId="331" priority="240" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI49">
+  <conditionalFormatting sqref="AJ50">
     <cfRule type="cellIs" dxfId="330" priority="239" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="329" priority="238" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI50">
+    <cfRule type="cellIs" dxfId="329" priority="237" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI50">
+  <conditionalFormatting sqref="AJ11:AJ13">
     <cfRule type="cellIs" dxfId="328" priority="236" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11:AJ13">
+  <conditionalFormatting sqref="AI11">
     <cfRule type="cellIs" dxfId="327" priority="235" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI11">
+  <conditionalFormatting sqref="AJ51">
     <cfRule type="cellIs" dxfId="326" priority="234" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ51">
+  <conditionalFormatting sqref="AI52">
     <cfRule type="cellIs" dxfId="325" priority="233" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI52">
+  <conditionalFormatting sqref="AJ52:AJ54">
     <cfRule type="cellIs" dxfId="324" priority="232" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ52:AJ54">
+  <conditionalFormatting sqref="AJ56">
     <cfRule type="cellIs" dxfId="323" priority="231" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ56">
+  <conditionalFormatting sqref="AI56">
     <cfRule type="cellIs" dxfId="322" priority="230" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI56">
+  <conditionalFormatting sqref="AJ57:AJ58">
     <cfRule type="cellIs" dxfId="321" priority="229" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ57:AJ58">
+  <conditionalFormatting sqref="AI57:AI58">
     <cfRule type="cellIs" dxfId="320" priority="228" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI57:AI58">
+  <conditionalFormatting sqref="AJ15:AJ16">
     <cfRule type="cellIs" dxfId="319" priority="227" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15:AJ16">
+  <conditionalFormatting sqref="AI15:AI16">
     <cfRule type="cellIs" dxfId="318" priority="226" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI15:AI16">
+  <conditionalFormatting sqref="AJ59:AJ60">
     <cfRule type="cellIs" dxfId="317" priority="225" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ59:AJ60">
+  <conditionalFormatting sqref="AJ55">
     <cfRule type="cellIs" dxfId="316" priority="224" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ55">
+  <conditionalFormatting sqref="AI19">
     <cfRule type="cellIs" dxfId="315" priority="223" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI19">
+  <conditionalFormatting sqref="AJ19">
     <cfRule type="cellIs" dxfId="314" priority="222" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19">
+  <conditionalFormatting sqref="AI18">
     <cfRule type="cellIs" dxfId="313" priority="221" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI18">
+  <conditionalFormatting sqref="AJ18">
     <cfRule type="cellIs" dxfId="312" priority="220" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ18">
+  <conditionalFormatting sqref="AI17">
     <cfRule type="cellIs" dxfId="311" priority="219" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI17">
+  <conditionalFormatting sqref="AJ17">
     <cfRule type="cellIs" dxfId="310" priority="218" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ17">
+  <conditionalFormatting sqref="AI86">
     <cfRule type="cellIs" dxfId="309" priority="217" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI86">
+  <conditionalFormatting sqref="AI40">
     <cfRule type="cellIs" dxfId="308" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI40">
+  <conditionalFormatting sqref="AJ20">
     <cfRule type="cellIs" dxfId="307" priority="215" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ20">
+  <conditionalFormatting sqref="AJ62">
     <cfRule type="cellIs" dxfId="306" priority="214" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="305" priority="213" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AJ21">
-    <cfRule type="cellIs" dxfId="304" priority="211" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="305" priority="212" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ64:AJ65">
+    <cfRule type="cellIs" dxfId="304" priority="210" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI21">
     <cfRule type="cellIs" dxfId="303" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI21">
+  <conditionalFormatting sqref="AI64">
     <cfRule type="cellIs" dxfId="302" priority="208" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI64">
+  <conditionalFormatting sqref="AI23">
     <cfRule type="cellIs" dxfId="301" priority="207" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI23">
+  <conditionalFormatting sqref="AJ24">
     <cfRule type="cellIs" dxfId="300" priority="206" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ24">
+  <conditionalFormatting sqref="AI25">
     <cfRule type="cellIs" dxfId="299" priority="205" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI25">
+  <conditionalFormatting sqref="AJ25">
     <cfRule type="cellIs" dxfId="298" priority="204" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ25">
+  <conditionalFormatting sqref="AJ67">
     <cfRule type="cellIs" dxfId="297" priority="203" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ67">
+  <conditionalFormatting sqref="AI26">
     <cfRule type="cellIs" dxfId="296" priority="202" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI26">
+  <conditionalFormatting sqref="AJ26:AJ27">
     <cfRule type="cellIs" dxfId="295" priority="201" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ26:AJ27">
+  <conditionalFormatting sqref="AI28:AI30">
     <cfRule type="cellIs" dxfId="294" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI28:AI30">
+  <conditionalFormatting sqref="AJ28:AJ31">
     <cfRule type="cellIs" dxfId="293" priority="199" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ28:AJ31">
+  <conditionalFormatting sqref="AI72">
     <cfRule type="cellIs" dxfId="292" priority="198" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI72">
+  <conditionalFormatting sqref="AJ72">
     <cfRule type="cellIs" dxfId="291" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ72">
+  <conditionalFormatting sqref="AI73">
     <cfRule type="cellIs" dxfId="290" priority="196" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI73">
+  <conditionalFormatting sqref="AJ73">
     <cfRule type="cellIs" dxfId="289" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ73">
+  <conditionalFormatting sqref="AI32">
     <cfRule type="cellIs" dxfId="288" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI32">
+  <conditionalFormatting sqref="AJ32">
     <cfRule type="cellIs" dxfId="287" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ32">
+  <conditionalFormatting sqref="AI33">
     <cfRule type="cellIs" dxfId="286" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI33">
+  <conditionalFormatting sqref="AJ33">
     <cfRule type="cellIs" dxfId="285" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ33">
+  <conditionalFormatting sqref="AI34:AI35">
     <cfRule type="cellIs" dxfId="284" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI34:AI35">
+  <conditionalFormatting sqref="AJ34:AJ36">
     <cfRule type="cellIs" dxfId="283" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ34:AJ36">
+  <conditionalFormatting sqref="AI61">
     <cfRule type="cellIs" dxfId="282" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI61">
+  <conditionalFormatting sqref="AI63">
     <cfRule type="cellIs" dxfId="281" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI63">
+  <conditionalFormatting sqref="AJ70">
     <cfRule type="cellIs" dxfId="280" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ70">
+  <conditionalFormatting sqref="AI70">
     <cfRule type="cellIs" dxfId="279" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI70">
+  <conditionalFormatting sqref="AI68">
     <cfRule type="cellIs" dxfId="278" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI68">
+  <conditionalFormatting sqref="AJ76">
     <cfRule type="cellIs" dxfId="277" priority="183" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ76">
+  <conditionalFormatting sqref="AI76">
     <cfRule type="cellIs" dxfId="276" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI76">
+  <conditionalFormatting sqref="AJ78">
     <cfRule type="cellIs" dxfId="275" priority="181" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ78">
+  <conditionalFormatting sqref="AI78">
     <cfRule type="cellIs" dxfId="274" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI78">
+  <conditionalFormatting sqref="AJ38">
     <cfRule type="cellIs" dxfId="273" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ38">
+  <conditionalFormatting sqref="AI38">
     <cfRule type="cellIs" dxfId="272" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI38">
+  <conditionalFormatting sqref="AJ77">
     <cfRule type="cellIs" dxfId="271" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ77">
+  <conditionalFormatting sqref="AI77">
     <cfRule type="cellIs" dxfId="270" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI77">
+  <conditionalFormatting sqref="AJ79">
     <cfRule type="cellIs" dxfId="269" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ79">
+  <conditionalFormatting sqref="AI79">
     <cfRule type="cellIs" dxfId="268" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI79">
+  <conditionalFormatting sqref="AJ80">
     <cfRule type="cellIs" dxfId="267" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ80">
+  <conditionalFormatting sqref="AI80">
     <cfRule type="cellIs" dxfId="266" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI80">
+  <conditionalFormatting sqref="AJ81">
     <cfRule type="cellIs" dxfId="265" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ81">
+  <conditionalFormatting sqref="AI81">
     <cfRule type="cellIs" dxfId="264" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI81">
+  <conditionalFormatting sqref="AJ82">
     <cfRule type="cellIs" dxfId="263" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ82">
+  <conditionalFormatting sqref="AI82">
     <cfRule type="cellIs" dxfId="262" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI82">
+  <conditionalFormatting sqref="AI83">
     <cfRule type="cellIs" dxfId="261" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI83">
+  <conditionalFormatting sqref="AI84:AI85">
     <cfRule type="cellIs" dxfId="260" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI84:AI85">
+  <conditionalFormatting sqref="AI39">
     <cfRule type="cellIs" dxfId="259" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI39">
+  <conditionalFormatting sqref="J31">
     <cfRule type="cellIs" dxfId="258" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
+  <conditionalFormatting sqref="O61">
     <cfRule type="cellIs" dxfId="257" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O61">
+  <conditionalFormatting sqref="O54">
     <cfRule type="cellIs" dxfId="256" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O54">
+  <conditionalFormatting sqref="O57">
     <cfRule type="cellIs" dxfId="255" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O57">
+  <conditionalFormatting sqref="O58">
     <cfRule type="cellIs" dxfId="254" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O58">
+  <conditionalFormatting sqref="O67">
     <cfRule type="cellIs" dxfId="253" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O67">
+  <conditionalFormatting sqref="O71">
     <cfRule type="cellIs" dxfId="252" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O71">
+  <conditionalFormatting sqref="O72">
     <cfRule type="cellIs" dxfId="251" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O72">
+  <conditionalFormatting sqref="O80">
     <cfRule type="cellIs" dxfId="250" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80">
+  <conditionalFormatting sqref="O82">
     <cfRule type="cellIs" dxfId="249" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="248" priority="154" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="247" priority="152" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="248" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L75">
+    <cfRule type="cellIs" dxfId="247" priority="151" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI12">
     <cfRule type="cellIs" dxfId="246" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI12">
+  <conditionalFormatting sqref="X2">
     <cfRule type="cellIs" dxfId="245" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
+  <conditionalFormatting sqref="W10 W65:W67 W86 W40:W42 W44 W32 W69:W71">
     <cfRule type="cellIs" dxfId="244" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W10 W65:W67 W86 W40:W42 W44 W32 W69:W71">
+  <conditionalFormatting sqref="AB2">
     <cfRule type="cellIs" dxfId="243" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2">
+  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
     <cfRule type="cellIs" dxfId="242" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
+  <conditionalFormatting sqref="Z2">
     <cfRule type="cellIs" dxfId="241" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2">
+  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y74 Y33:Y37 Y76:Y77 Y39:Y59 Y80:Y86">
     <cfRule type="cellIs" dxfId="240" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y74 Y33:Y37 Y76:Y77 Y39:Y59 Y80:Y86">
+  <conditionalFormatting sqref="AD2">
     <cfRule type="cellIs" dxfId="239" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2">
+  <conditionalFormatting sqref="AC2:AC86">
     <cfRule type="cellIs" dxfId="238" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC86">
+  <conditionalFormatting sqref="V2">
     <cfRule type="cellIs" dxfId="237" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2">
+  <conditionalFormatting sqref="U2:U86">
     <cfRule type="cellIs" dxfId="236" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U86">
+  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
     <cfRule type="cellIs" dxfId="235" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
+  <conditionalFormatting sqref="AA48">
     <cfRule type="cellIs" dxfId="234" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA48">
+  <conditionalFormatting sqref="AA11">
     <cfRule type="cellIs" dxfId="233" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA11">
+  <conditionalFormatting sqref="AA51">
     <cfRule type="cellIs" dxfId="232" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA51">
+  <conditionalFormatting sqref="AA52">
     <cfRule type="cellIs" dxfId="231" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA52">
+  <conditionalFormatting sqref="AA53">
     <cfRule type="cellIs" dxfId="230" priority="134" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA53">
+  <conditionalFormatting sqref="AA57 AA54:AA55">
     <cfRule type="cellIs" dxfId="229" priority="133" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA57 AA54:AA55">
+  <conditionalFormatting sqref="AA20">
     <cfRule type="cellIs" dxfId="228" priority="132" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA20">
+  <conditionalFormatting sqref="AA21">
     <cfRule type="cellIs" dxfId="227" priority="131" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA21">
+  <conditionalFormatting sqref="AA66">
     <cfRule type="cellIs" dxfId="226" priority="130" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA66">
+  <conditionalFormatting sqref="AA25">
     <cfRule type="cellIs" dxfId="225" priority="129" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA25">
+  <conditionalFormatting sqref="AA26">
     <cfRule type="cellIs" dxfId="224" priority="128" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA26">
+  <conditionalFormatting sqref="AA28">
     <cfRule type="cellIs" dxfId="223" priority="127" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA28">
+  <conditionalFormatting sqref="AA32">
     <cfRule type="cellIs" dxfId="222" priority="126" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA32">
+  <conditionalFormatting sqref="AA34">
     <cfRule type="cellIs" dxfId="221" priority="125" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA34">
+  <conditionalFormatting sqref="AA27">
     <cfRule type="cellIs" dxfId="220" priority="124" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA27">
+  <conditionalFormatting sqref="AA33 AA31">
     <cfRule type="cellIs" dxfId="219" priority="123" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA33 AA31">
+  <conditionalFormatting sqref="AA61 M61">
     <cfRule type="cellIs" dxfId="218" priority="122" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA61 M61">
+  <conditionalFormatting sqref="AA62">
     <cfRule type="cellIs" dxfId="217" priority="121" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA62">
+  <conditionalFormatting sqref="AA63 M63">
     <cfRule type="cellIs" dxfId="216" priority="120" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA63 M63">
+  <conditionalFormatting sqref="AA65">
     <cfRule type="cellIs" dxfId="215" priority="119" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA65">
+  <conditionalFormatting sqref="AA67">
     <cfRule type="cellIs" dxfId="214" priority="118" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA67">
+  <conditionalFormatting sqref="AA68">
     <cfRule type="cellIs" dxfId="213" priority="117" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA68">
+  <conditionalFormatting sqref="AA70:AA73">
     <cfRule type="cellIs" dxfId="212" priority="116" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA70:AA73">
+  <conditionalFormatting sqref="AA77">
     <cfRule type="cellIs" dxfId="211" priority="115" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA77">
+  <conditionalFormatting sqref="AA74 AA38">
     <cfRule type="cellIs" dxfId="210" priority="114" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA74 AA38">
+  <conditionalFormatting sqref="AA37">
     <cfRule type="cellIs" dxfId="209" priority="113" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA37">
+  <conditionalFormatting sqref="S9">
     <cfRule type="cellIs" dxfId="208" priority="112" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
+  <conditionalFormatting sqref="S46">
     <cfRule type="cellIs" dxfId="207" priority="111" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S46">
+  <conditionalFormatting sqref="S48">
     <cfRule type="cellIs" dxfId="206" priority="110" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S48">
+  <conditionalFormatting sqref="S18">
     <cfRule type="cellIs" dxfId="205" priority="109" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
+  <conditionalFormatting sqref="S54">
     <cfRule type="cellIs" dxfId="204" priority="108" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S54">
+  <conditionalFormatting sqref="S55">
     <cfRule type="cellIs" dxfId="203" priority="107" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S55">
+  <conditionalFormatting sqref="S57">
     <cfRule type="cellIs" dxfId="202" priority="106" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S57">
+  <conditionalFormatting sqref="S76">
     <cfRule type="cellIs" dxfId="201" priority="105" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S76">
+  <conditionalFormatting sqref="S78">
     <cfRule type="cellIs" dxfId="200" priority="104" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S78">
+  <conditionalFormatting sqref="S81">
     <cfRule type="cellIs" dxfId="199" priority="103" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S81">
+  <conditionalFormatting sqref="S82">
     <cfRule type="cellIs" dxfId="198" priority="102" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S82">
+  <conditionalFormatting sqref="J32">
     <cfRule type="cellIs" dxfId="197" priority="101" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
+  <conditionalFormatting sqref="K66">
     <cfRule type="cellIs" dxfId="196" priority="100" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
+  <conditionalFormatting sqref="L67">
     <cfRule type="cellIs" dxfId="195" priority="99" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L67">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="194" priority="98" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="L27">
     <cfRule type="cellIs" dxfId="193" priority="97" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L27">
+  <conditionalFormatting sqref="G7">
     <cfRule type="cellIs" dxfId="192" priority="96" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="191" priority="95" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G20">
+    <cfRule type="cellIs" dxfId="191" priority="94" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
+  <conditionalFormatting sqref="G10">
     <cfRule type="cellIs" dxfId="190" priority="93" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
+  <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" dxfId="189" priority="92" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
+  <conditionalFormatting sqref="X3">
     <cfRule type="cellIs" dxfId="188" priority="91" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3">
-    <cfRule type="cellIs" dxfId="187" priority="90" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L13">
+    <cfRule type="cellIs" dxfId="187" priority="88" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
+  <conditionalFormatting sqref="L55">
     <cfRule type="cellIs" dxfId="186" priority="87" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L55">
+  <conditionalFormatting sqref="L56">
     <cfRule type="cellIs" dxfId="185" priority="86" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
+  <conditionalFormatting sqref="L14">
     <cfRule type="cellIs" dxfId="184" priority="85" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
+  <conditionalFormatting sqref="L60">
     <cfRule type="cellIs" dxfId="183" priority="84" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L60">
-    <cfRule type="cellIs" dxfId="182" priority="83" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L76">
+    <cfRule type="cellIs" dxfId="182" priority="82" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76">
+  <conditionalFormatting sqref="L6">
     <cfRule type="cellIs" dxfId="181" priority="81" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
+  <conditionalFormatting sqref="L7">
     <cfRule type="cellIs" dxfId="180" priority="80" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
+  <conditionalFormatting sqref="L8">
     <cfRule type="cellIs" dxfId="179" priority="79" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
+  <conditionalFormatting sqref="L9">
     <cfRule type="cellIs" dxfId="178" priority="78" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9">
+  <conditionalFormatting sqref="Y14">
     <cfRule type="cellIs" dxfId="177" priority="77" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y14">
+  <conditionalFormatting sqref="J4">
     <cfRule type="cellIs" dxfId="176" priority="76" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
+  <conditionalFormatting sqref="AK14">
     <cfRule type="cellIs" dxfId="175" priority="75" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK14">
+  <conditionalFormatting sqref="X61">
     <cfRule type="cellIs" dxfId="174" priority="74" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X61">
+  <conditionalFormatting sqref="W75">
     <cfRule type="cellIs" dxfId="173" priority="73" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W75">
+  <conditionalFormatting sqref="Y75">
     <cfRule type="cellIs" dxfId="172" priority="72" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y75">
+  <conditionalFormatting sqref="K76">
     <cfRule type="cellIs" dxfId="171" priority="71" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
+  <conditionalFormatting sqref="K22">
     <cfRule type="cellIs" dxfId="170" priority="70" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
+  <conditionalFormatting sqref="K18">
     <cfRule type="cellIs" dxfId="169" priority="69" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
+  <conditionalFormatting sqref="W76">
     <cfRule type="cellIs" dxfId="168" priority="68" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W76">
+  <conditionalFormatting sqref="W77">
     <cfRule type="cellIs" dxfId="167" priority="67" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W77">
-    <cfRule type="cellIs" dxfId="166" priority="66" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="W80">
+    <cfRule type="cellIs" dxfId="166" priority="65" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W80">
+  <conditionalFormatting sqref="W37">
     <cfRule type="cellIs" dxfId="165" priority="64" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W37">
-    <cfRule type="cellIs" dxfId="164" priority="63" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="W74">
+    <cfRule type="cellIs" dxfId="164" priority="62" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W74">
+  <conditionalFormatting sqref="W45">
     <cfRule type="cellIs" dxfId="163" priority="61" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W45">
+  <conditionalFormatting sqref="W46">
     <cfRule type="cellIs" dxfId="162" priority="60" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W46">
+  <conditionalFormatting sqref="W47">
     <cfRule type="cellIs" dxfId="161" priority="59" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W47">
+  <conditionalFormatting sqref="W4">
     <cfRule type="cellIs" dxfId="160" priority="58" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W4">
+  <conditionalFormatting sqref="W5">
     <cfRule type="cellIs" dxfId="159" priority="57" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W5">
+  <conditionalFormatting sqref="W7">
     <cfRule type="cellIs" dxfId="158" priority="56" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W7">
+  <conditionalFormatting sqref="W8">
     <cfRule type="cellIs" dxfId="157" priority="55" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W8">
+  <conditionalFormatting sqref="W9">
     <cfRule type="cellIs" dxfId="156" priority="54" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W9">
+  <conditionalFormatting sqref="W48">
     <cfRule type="cellIs" dxfId="155" priority="53" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W48">
+  <conditionalFormatting sqref="W50">
     <cfRule type="cellIs" dxfId="154" priority="52" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W50">
+  <conditionalFormatting sqref="W11">
     <cfRule type="cellIs" dxfId="153" priority="51" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W11">
+  <conditionalFormatting sqref="W12">
     <cfRule type="cellIs" dxfId="152" priority="50" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W12">
+  <conditionalFormatting sqref="W13">
     <cfRule type="cellIs" dxfId="151" priority="49" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W13">
+  <conditionalFormatting sqref="W15">
     <cfRule type="cellIs" dxfId="150" priority="48" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W15">
+  <conditionalFormatting sqref="W16">
     <cfRule type="cellIs" dxfId="149" priority="47" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W16">
+  <conditionalFormatting sqref="W51">
     <cfRule type="cellIs" dxfId="148" priority="46" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W51">
+  <conditionalFormatting sqref="W52">
     <cfRule type="cellIs" dxfId="147" priority="45" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W52">
+  <conditionalFormatting sqref="W53">
     <cfRule type="cellIs" dxfId="146" priority="44" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W53">
+  <conditionalFormatting sqref="W54">
     <cfRule type="cellIs" dxfId="145" priority="43" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W54">
+  <conditionalFormatting sqref="W55">
     <cfRule type="cellIs" dxfId="144" priority="42" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W55">
+  <conditionalFormatting sqref="W57">
     <cfRule type="cellIs" dxfId="143" priority="41" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W57">
+  <conditionalFormatting sqref="W58">
     <cfRule type="cellIs" dxfId="142" priority="40" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W58">
-    <cfRule type="cellIs" dxfId="141" priority="39" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="W62">
+    <cfRule type="cellIs" dxfId="141" priority="38" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W62">
+  <conditionalFormatting sqref="W63">
     <cfRule type="cellIs" dxfId="140" priority="37" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W63">
+  <conditionalFormatting sqref="W21">
     <cfRule type="cellIs" dxfId="139" priority="36" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W21">
+  <conditionalFormatting sqref="W22">
     <cfRule type="cellIs" dxfId="138" priority="35" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W22">
+  <conditionalFormatting sqref="W24">
     <cfRule type="cellIs" dxfId="137" priority="34" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W24">
+  <conditionalFormatting sqref="W25">
     <cfRule type="cellIs" dxfId="136" priority="33" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W25">
+  <conditionalFormatting sqref="W27">
     <cfRule type="cellIs" dxfId="135" priority="32" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W27">
+  <conditionalFormatting sqref="W28">
     <cfRule type="cellIs" dxfId="134" priority="31" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W28">
+  <conditionalFormatting sqref="W29">
     <cfRule type="cellIs" dxfId="133" priority="30" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W29">
+  <conditionalFormatting sqref="W30">
     <cfRule type="cellIs" dxfId="132" priority="29" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W30">
+  <conditionalFormatting sqref="W31">
     <cfRule type="cellIs" dxfId="131" priority="28" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W31">
+  <conditionalFormatting sqref="W72">
     <cfRule type="cellIs" dxfId="130" priority="27" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W72">
+  <conditionalFormatting sqref="W73">
     <cfRule type="cellIs" dxfId="129" priority="26" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W73">
-    <cfRule type="cellIs" dxfId="128" priority="25" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="W68">
+    <cfRule type="cellIs" dxfId="128" priority="23" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W68">
+  <conditionalFormatting sqref="W38">
     <cfRule type="cellIs" dxfId="127" priority="22" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W38">
+  <conditionalFormatting sqref="X38">
     <cfRule type="cellIs" dxfId="126" priority="21" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X38">
-    <cfRule type="cellIs" dxfId="125" priority="20" stopIfTrue="1" operator="between">
-      <formula>"""Yes"""</formula>
-      <formula>"""Yes"""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L80">
-    <cfRule type="cellIs" dxfId="124" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="125" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K80">
+    <cfRule type="cellIs" dxfId="124" priority="13" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
     <cfRule type="cellIs" dxfId="123" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="122" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K36">
     <cfRule type="cellIs" dxfId="121" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
+  <conditionalFormatting sqref="K74">
     <cfRule type="cellIs" dxfId="120" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="cellIs" dxfId="119" priority="8" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="G37">
+    <cfRule type="cellIs" dxfId="119" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
+  <conditionalFormatting sqref="Y38">
     <cfRule type="cellIs" dxfId="118" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y38">
+  <conditionalFormatting sqref="K78">
     <cfRule type="cellIs" dxfId="117" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K78">
+  <conditionalFormatting sqref="K68">
     <cfRule type="cellIs" dxfId="116" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="K35">
+    <cfRule type="cellIs" dxfId="115" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AG12">
+    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -47763,448 +47779,448 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="115" priority="85" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD87 AF87">
-    <cfRule type="containsText" dxfId="114" priority="84" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="112" priority="84" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="113" priority="83" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="111" priority="83" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF54 AD52:AD53 AI52:AJ53 AF52:AG53">
-    <cfRule type="containsText" dxfId="112" priority="82" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="111" priority="79" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="109" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD61 AF61:AG61 AI61:AJ61">
-    <cfRule type="containsText" dxfId="110" priority="78" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="108" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="109" priority="77" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="107" priority="77" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD57 AI57:AJ57 AF57:AG57">
-    <cfRule type="containsText" dxfId="108" priority="76" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="106" priority="76" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="107" priority="75" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="105" priority="75" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI66:AJ66 AF66:AG66">
-    <cfRule type="containsText" dxfId="106" priority="74" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="104" priority="74" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD51 AF2:AG51 AI2:AJ51 AD62:AD80 AF67:AG73 AI67:AJ73">
-    <cfRule type="containsText" dxfId="105" priority="90" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="103" priority="90" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="104" priority="93">
+    <cfRule type="containsBlanks" dxfId="102" priority="93">
       <formula>LEN(TRIM(AD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295">
-    <cfRule type="containsText" dxfId="103" priority="89" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="101" priority="89" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD54)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="102" priority="91">
+    <cfRule type="containsBlanks" dxfId="100" priority="91">
       <formula>LEN(TRIM(AD54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG54 AI54:AJ56 AF55:AG56 AD54:AD56 AD58:AD60 AF58:AG60 AI58:AJ60 AI62:AJ65 AF62:AG65 AI79:AJ79 AF79:AG79 AF74:AF78 AD82:AD86 AF83:AF86 AF88 AI89:AJ111 AF89:AG111 AI113:AJ114 AF113:AG114 AD88:AD124 AF116:AG119 AI116:AJ119 AG126 AI126:AJ130 AF127:AG130 AD126:AD139 AG137:AG139 AF142:AG144 AI142:AJ144 AD237:AD250 AF152:AG174 AF175:AF176 AI152:AJ175 AG175 AD195:AD201 AD141:AD193 AF177:AG193 AI177:AJ193 AG195:AG201 AI197:AJ201 AD203:AD235 AF312:AG313 AD312:AD313 AI312:AJ313 AG203:AG218 AF219:AG235 AI212:AJ235 AF237:AG250 AI237:AJ250 AG252 AD252:AD290 AI296:AJ301 AI304:AJ310 AF304:AG310 AF253:AG290 AI252:AJ289 AF292:AG301 AD292:AD310 AI290 AJ290:AJ295 AI292:AI295 AD2:AD51 AF2:AG51 AI2:AJ51 AF67:AG73 AI67:AJ73 AD62:AD80">
-    <cfRule type="containsText" dxfId="101" priority="88" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="99" priority="88" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="100" priority="87" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="87" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD236 AF236:AG236 AI236:AJ236">
-    <cfRule type="containsText" dxfId="99" priority="86" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="86" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="98" priority="81" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="81" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI302:AJ303 AF302:AG303">
-    <cfRule type="containsText" dxfId="97" priority="80" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="95" priority="80" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="96" priority="73" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="73" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG74:AG78 AI74:AJ78">
-    <cfRule type="containsText" dxfId="95" priority="72" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="93" priority="72" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="94" priority="71" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="71" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF80:AF82">
-    <cfRule type="containsText" dxfId="93" priority="70" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="91" priority="70" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsBlanks" dxfId="92" priority="69">
+    <cfRule type="containsBlanks" dxfId="90" priority="69">
       <formula>LEN(TRIM(AG80))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="94" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI80:AJ88 AG80:AG88">
-    <cfRule type="containsText" dxfId="90" priority="68" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="88" priority="68" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="89" priority="67" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD81">
-    <cfRule type="containsText" dxfId="88" priority="66" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="66" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="87" priority="65" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF112">
-    <cfRule type="containsText" dxfId="86" priority="64" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="85" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="83" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG112)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="84" priority="63">
+    <cfRule type="containsBlanks" dxfId="82" priority="63">
       <formula>LEN(TRIM(AG112))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG112 AI112:AJ112">
-    <cfRule type="containsText" dxfId="83" priority="62" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="82" priority="61" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="61" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI115:AJ115 AF115:AG115">
-    <cfRule type="containsText" dxfId="81" priority="60" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="79" priority="60" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="80" priority="58" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="78" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF120)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="79" priority="59">
+    <cfRule type="containsBlanks" dxfId="77" priority="59">
       <formula>LEN(TRIM(AF120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF120:AF124">
-    <cfRule type="containsText" dxfId="78" priority="57" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="76" priority="57" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsBlanks" dxfId="77" priority="56">
+    <cfRule type="containsBlanks" dxfId="75" priority="56">
       <formula>LEN(TRIM(AG120))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG120:AG124 AI120:AJ124">
-    <cfRule type="containsText" dxfId="76" priority="55" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="55" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="75" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF125:AG125 AI125:AJ125 AD125 AF126">
-    <cfRule type="containsText" dxfId="74" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="73" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI131:AJ131 AF131:AG131">
-    <cfRule type="containsText" dxfId="72" priority="51" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="70" priority="51" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="71" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF132)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="70" priority="50">
+    <cfRule type="containsBlanks" dxfId="68" priority="50">
       <formula>LEN(TRIM(AF132))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF132:AG136 AF137:AF139 AI132:AJ139">
-    <cfRule type="containsText" dxfId="69" priority="48" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="67" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="68" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF145)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="67" priority="47">
+    <cfRule type="containsBlanks" dxfId="65" priority="47">
       <formula>LEN(TRIM(AF145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF145:AG151 AI145:AJ151">
-    <cfRule type="containsText" dxfId="66" priority="45" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="45" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="65" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD140">
-    <cfRule type="containsText" dxfId="64" priority="43" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="62" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="63" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF140)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="62" priority="42">
+    <cfRule type="containsBlanks" dxfId="60" priority="42">
       <formula>LEN(TRIM(AF140))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF140:AG140 AI140:AJ140">
-    <cfRule type="containsText" dxfId="61" priority="40" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="60" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AF141)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="59" priority="39">
+    <cfRule type="containsBlanks" dxfId="57" priority="39">
       <formula>LEN(TRIM(AF141))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF141:AG141 AI141:AJ141">
-    <cfRule type="containsText" dxfId="58" priority="37" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AF141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="57" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI176:AJ176 AG176">
-    <cfRule type="containsText" dxfId="56" priority="35" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="54" priority="35" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AG176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="55" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD194 AF194:AG194 AF195:AF201 AI194:AJ196">
-    <cfRule type="containsText" dxfId="54" priority="33" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="53" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF202:AG202 AD202 AF203:AF218 AI202:AJ211">
-    <cfRule type="containsText" dxfId="52" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="31" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="51" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="49" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF311:AG311 AD311 AI311:AJ311">
-    <cfRule type="containsText" dxfId="50" priority="29" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="29" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="49" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD251 AF251:AG251 AI251:AJ251 AF252">
-    <cfRule type="containsText" dxfId="48" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="46" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="47" priority="26" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI291 AF291:AG291 AD291">
-    <cfRule type="containsText" dxfId="46" priority="25" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",AD291)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C307:C310 C313 F237:F250 C54:C56 F54:F56 F58:F60 C58:C60 F82:F86 C82:C86 F88:F124 C88:C159 C237:C250 F195:F201 F126:F193 C161:C201 C203:C235 F203:F235 F312:F313 C252:C290 F252:F290 F294:F310 C292:C305 F2:F51 C2:C51 C62:C80 F62:F80">
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="44" priority="23">
+    <cfRule type="containsBlanks" dxfId="42" priority="23">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F236">
-    <cfRule type="containsText" dxfId="43" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C236">
-    <cfRule type="containsBlanks" dxfId="42" priority="19">
+    <cfRule type="containsBlanks" dxfId="40" priority="19">
       <formula>LEN(TRIM(C236))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="95" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="95" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C306">
-    <cfRule type="containsText" dxfId="40" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87 C87">
-    <cfRule type="containsText" dxfId="39" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C312">
-    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C312)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53 F52:F53">
-    <cfRule type="containsText" dxfId="37" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="36" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61 C61">
-    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="containsText" dxfId="34" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F57)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="33" priority="22">
+    <cfRule type="containsBlanks" dxfId="31" priority="22">
       <formula>LEN(TRIM(F57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="containsBlanks" dxfId="32" priority="11">
+    <cfRule type="containsBlanks" dxfId="30" priority="11">
       <formula>LEN(TRIM(C57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81 C81">
-    <cfRule type="containsText" dxfId="31" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125">
-    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F194">
-    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F194)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202 C202">
-    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F311">
-    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311">
-    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F251 C251">
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292">
-    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291 C291">
-    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C291)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49474,7 +49490,7 @@
       <c r="AN11" s="95"/>
       <c r="AO11" s="94"/>
     </row>
-    <row r="12" spans="2:41" s="99" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:41" s="99" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="94" t="s">
         <v>5</v>
       </c>
@@ -63099,111 +63115,111 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AS2:AS86">
-    <cfRule type="cellIs" dxfId="21" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V39 V46:V74 AC14 AR12:AR85 AR2:AR5 X39 V38:X38 V40:X40 V2:X5 W46:X55 W57:X74 AD4:AD5 AE14:AJ14 AK8:AL8 AK10:AQ12 AE2:AN5 AM8:AN9 AD46:AN74 AK14:AN29 Y46:AC46 Y5:AB5 Y38:AN40 V34:AN36 V43:AN44 Y4:AC4 V8:AJ12 Y48:AC74 Y47:AB47 V76:AN85 W14:AB29 Y2:AD3">
-    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AL9">
-    <cfRule type="cellIs" dxfId="18" priority="16" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ5 AQ8:AQ9 AQ34:AQ36 AQ38:AQ40 AQ43:AQ44 AQ46:AQ74 AQ14:AQ29 AQ76:AQ85">
-    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39 W56">
-    <cfRule type="cellIs" dxfId="16" priority="14" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AO5 AO8:AO9 AO34:AO36 AO38:AO40 AO43:AO44 AO46:AO74 AO14:AO29 AO76:AO85">
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP2:AP5 AP8:AP9 AP34:AP36 AP38:AP40 AP43:AP44 AP46:AP74 AP14:AP29 AP76:AP85">
-    <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14:V29 AC15:AC29 AD14:AD29 AE15:AJ29">
-    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD30">
-    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q12 Q85 T85 T10:T12">
-    <cfRule type="cellIs" dxfId="10" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q5 Q8:Q9 Q34:Q36 Q38:Q40 Q43:Q44 Q14:Q29 Q46:Q74 Q76:Q84 T76:T84 T46:T74 T14:T29 T43:T44 T38:T40 T34:T36 T8:T9 T2:T5">
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 H26:K26 H28:K29 H76:K82 H43:K44 H34:K34 H36:K36 H8:K12 H84:K85 H38:K40 H2:K5 H14:K17 H19:K19 H46:K74">
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83:K83">
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:K33">
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25 H20:K23 H27:K27 H18:K18">
-    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R85:S85 R10:S12">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R76:S84 R46:S74 R14:S29 R43:S44 R38:S40 R34:S36 R8:S9 R2:S5">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
@@ -64527,7 +64543,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43635</v>
+        <v>43691</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -64876,7 +64892,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43635</v>
+        <v>43691</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>
@@ -68883,7 +68899,7 @@
   </sheetData>
   <autoFilter ref="B2:Y87" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <conditionalFormatting sqref="Y3:Y86 J3:X6 J9:X13 J15:X30 J35:X37 J39:X41 J44:X45 J47:X75 J77:X86">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>

</xml_diff>

<commit_message>
added cm13 minutes for some projects
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDB7F11-A1C8-4397-8F46-D778926E78B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD9017B-228F-40FB-9235-EA36CAC7726F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9030" uniqueCount="1409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9033" uniqueCount="1410">
   <si>
     <t>#</t>
   </si>
@@ -4272,6 +4272,9 @@
   </si>
   <si>
     <t xml:space="preserve">2019-07-01 (Dow) CM13 and SP minutes in combined pdf </t>
+  </si>
+  <si>
+    <t>2019-08-22: CM13 minutes combined into single SP file</t>
   </si>
 </sst>
 </file>
@@ -8440,7 +8443,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8/14/2019</c:v>
+                  <c:v>8/22/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10200,7 +10203,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1095" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -22954,7 +22957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B75" s="13" t="s">
         <v>4</v>
       </c>
@@ -22996,11 +22999,11 @@
       <c r="P75" s="118" t="s">
         <v>1269</v>
       </c>
-      <c r="Q75" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R75" s="118">
-        <v>1</v>
+      <c r="Q75" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="R75" s="118" t="s">
+        <v>1409</v>
       </c>
       <c r="S75" s="52" t="s">
         <v>166</v>
@@ -23372,11 +23375,11 @@
       <c r="P77" s="118" t="s">
         <v>1272</v>
       </c>
-      <c r="Q77" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R77" s="118">
-        <v>1</v>
+      <c r="Q77" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="R77" s="118" t="s">
+        <v>1409</v>
       </c>
       <c r="S77" s="52" t="s">
         <v>166</v>
@@ -23503,7 +23506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:82" s="18" customFormat="1" ht="23.65" x14ac:dyDescent="0.35">
       <c r="B78" s="13" t="s">
         <v>4</v>
       </c>
@@ -23545,11 +23548,11 @@
       <c r="P78" s="118" t="s">
         <v>1273</v>
       </c>
-      <c r="Q78" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R78" s="118">
-        <v>1</v>
+      <c r="Q78" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="R78" s="118" t="s">
+        <v>1409</v>
       </c>
       <c r="S78" s="48" t="s">
         <v>170</v>
@@ -25320,7 +25323,7 @@
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q86">
+  <conditionalFormatting sqref="Q3:Q74 Q76 Q79:Q86">
     <cfRule type="cellIs" dxfId="380" priority="292" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -49490,7 +49493,7 @@
       <c r="AN11" s="95"/>
       <c r="AO11" s="94"/>
     </row>
-    <row r="12" spans="2:41" s="99" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:41" s="99" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="B12" s="94" t="s">
         <v>5</v>
       </c>
@@ -64543,7 +64546,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43691</v>
+        <v>43699</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -64892,7 +64895,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43691</v>
+        <v>43699</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
added minutes for 11220
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD9017B-228F-40FB-9235-EA36CAC7726F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076AFDA5-DFCB-47CD-A804-1449367AB1C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9033" uniqueCount="1410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9034" uniqueCount="1411">
   <si>
     <t>#</t>
   </si>
@@ -4275,6 +4275,9 @@
   </si>
   <si>
     <t>2019-08-22: CM13 minutes combined into single SP file</t>
+  </si>
+  <si>
+    <t>CM13 minutes combined and on SP (8/29/19)</t>
   </si>
 </sst>
 </file>
@@ -8443,7 +8446,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8/22/2019</c:v>
+                  <c:v>8/29/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10200,10 +10203,10 @@
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1095" activePane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="1095" topLeftCell="A36" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -17869,11 +17872,11 @@
       <c r="P45" s="118" t="s">
         <v>1225</v>
       </c>
-      <c r="Q45" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R45" s="118">
-        <v>1</v>
+      <c r="Q45" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="R45" s="118" t="s">
+        <v>1410</v>
       </c>
       <c r="S45" s="52" t="s">
         <v>166</v>
@@ -25323,7 +25326,7 @@
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q74 Q76 Q79:Q86">
+  <conditionalFormatting sqref="Q3:Q44 Q76 Q79:Q86 Q46:Q74">
     <cfRule type="cellIs" dxfId="380" priority="292" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -64546,7 +64549,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">TODAY()</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
       <c r="F3" s="59">
         <v>42551</v>
@@ -64895,7 +64898,7 @@
       <c r="G1"/>
       <c r="I1" s="28">
         <f ca="1">TODAY()</f>
-        <v>43699</v>
+        <v>43706</v>
       </c>
       <c r="J1" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
updated OM info with dsc binder info
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076AFDA5-DFCB-47CD-A804-1449367AB1C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95939EC7-6EF5-48BA-B8F7-66BEC092719E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9034" uniqueCount="1411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9042" uniqueCount="1422">
   <si>
     <t>#</t>
   </si>
@@ -4181,9 +4181,6 @@
     <t>digitally in SP</t>
   </si>
   <si>
-    <t>only irrigation in SP</t>
-  </si>
-  <si>
     <t>HVAC only on SP</t>
   </si>
   <si>
@@ -4193,21 +4190,12 @@
     <t>not in SP</t>
   </si>
   <si>
-    <t>only HVAC in SP</t>
-  </si>
-  <si>
     <t>missing plumbing in SP</t>
   </si>
   <si>
-    <t>have restroom OMs only</t>
-  </si>
-  <si>
     <t>HVAC in SP only</t>
   </si>
   <si>
-    <t>only fire suppression in SP</t>
-  </si>
-  <si>
     <t>OM's are saved in SP, but may not be complete (i.e. Electrical seems short)</t>
   </si>
   <si>
@@ -4278,6 +4266,51 @@
   </si>
   <si>
     <t>CM13 minutes combined and on SP (8/29/19)</t>
+  </si>
+  <si>
+    <t>See Hardcopy O&amp;M Binders #47 and #48</t>
+  </si>
+  <si>
+    <t>Hardcopy O&amp;M Binder #1 at DSC</t>
+  </si>
+  <si>
+    <t>only irrigation in SP; Hardcopy O&amp;M Binders 2--7 at DSC</t>
+  </si>
+  <si>
+    <t>only HVAC in SP; Hardcopy O&amp;M Binders 8,11,12,20-24,48-50,52 at DSC</t>
+  </si>
+  <si>
+    <t>have restroom OMs only; hardcopy OM binder #14 (global power)</t>
+  </si>
+  <si>
+    <t>not in SP; HardcopyO&amp;M binder #27 barnhart at DSC</t>
+  </si>
+  <si>
+    <t>not in SP; Hardcopy O&amp;M binders 29/42 at DSC (HVAC only?)</t>
+  </si>
+  <si>
+    <t>Hardcopy O&amp;M binder #10 at DSC -- is a CD Rom)</t>
+  </si>
+  <si>
+    <t>Hardcopy O&amp;M binders #18 at DSC</t>
+  </si>
+  <si>
+    <t>Hardcopy O&amp;M binders #19 at DSC</t>
+  </si>
+  <si>
+    <t>Hardcopy O&amp;M binders #15 at DSC</t>
+  </si>
+  <si>
+    <t>only fire suppression in SP; Hardcopy O&amp;M binders 3,4,5,30</t>
+  </si>
+  <si>
+    <t>plumb _ hvac controls hardcopy O&amp;M binders 29,34 at dsc</t>
+  </si>
+  <si>
+    <t>Harcopy O&amp;M Binder #20 at DSC</t>
+  </si>
+  <si>
+    <t>not in SP; ? Hardcopy o&amp;M binder #28 at dsc?</t>
   </si>
 </sst>
 </file>
@@ -10203,10 +10236,10 @@
   </sheetPr>
   <dimension ref="B1:CD101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1095" topLeftCell="A36" activePane="bottomLeft"/>
-      <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="O52" sqref="O52"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="1110" activePane="bottomLeft"/>
+      <selection activeCell="V1" sqref="I1:V1048576"/>
+      <selection pane="bottomLeft" activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -10219,22 +10252,22 @@
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="7.1328125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.73046875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.59765625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.59765625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.3984375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.73046875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.265625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.86328125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.265625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.265625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.86328125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="11" style="1" customWidth="1"/>
-    <col min="22" max="22" width="15.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.59765625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1328125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.3984375" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.73046875" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="7.265625" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.86328125" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="7.265625" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="7.265625" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="10.86328125" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="11" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="15.59765625" style="1" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="7.265625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.86328125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20.86328125" style="1" customWidth="1"/>
     <col min="25" max="25" width="8.265625" style="1" customWidth="1"/>
     <col min="26" max="26" width="11.86328125" style="1" customWidth="1"/>
     <col min="27" max="27" width="8.265625" style="1" customWidth="1"/>
@@ -10553,7 +10586,7 @@
         <v>166</v>
       </c>
       <c r="R2" s="118" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
       <c r="S2" s="52" t="s">
         <v>166</v>
@@ -10913,7 +10946,7 @@
         <v>170</v>
       </c>
       <c r="X4" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y4" s="118" t="s">
         <v>567</v>
@@ -11084,7 +11117,7 @@
         <v>170</v>
       </c>
       <c r="X5" s="118" t="s">
-        <v>1381</v>
+        <v>1407</v>
       </c>
       <c r="Y5" s="118" t="s">
         <v>567</v>
@@ -11444,7 +11477,7 @@
         <v>170</v>
       </c>
       <c r="X7" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y7" s="118" t="s">
         <v>567</v>
@@ -11619,7 +11652,7 @@
         <v>170</v>
       </c>
       <c r="X8" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y8" s="118" t="s">
         <v>567</v>
@@ -11790,7 +11823,7 @@
         <v>170</v>
       </c>
       <c r="X9" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y9" s="118" t="s">
         <v>567</v>
@@ -11959,7 +11992,7 @@
         <v>170</v>
       </c>
       <c r="X10" s="118" t="s">
-        <v>1381</v>
+        <v>1421</v>
       </c>
       <c r="Y10" s="118" t="s">
         <v>567</v>
@@ -12128,7 +12161,7 @@
         <v>170</v>
       </c>
       <c r="X11" s="118" t="s">
-        <v>1382</v>
+        <v>1410</v>
       </c>
       <c r="Y11" s="118" t="s">
         <v>567</v>
@@ -12301,7 +12334,7 @@
         <v>170</v>
       </c>
       <c r="X12" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y12" s="118" t="s">
         <v>567</v>
@@ -12470,7 +12503,7 @@
         <v>1112</v>
       </c>
       <c r="X13" s="118" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="Y13" s="118" t="s">
         <v>567</v>
@@ -12808,7 +12841,7 @@
         <v>170</v>
       </c>
       <c r="X15" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y15" s="118" t="s">
         <v>567</v>
@@ -12975,7 +13008,7 @@
         <v>170</v>
       </c>
       <c r="X16" s="118" t="s">
-        <v>1384</v>
+        <v>1411</v>
       </c>
       <c r="Y16" s="118" t="s">
         <v>567</v>
@@ -13817,7 +13850,9 @@
       <c r="W21" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="X21" s="118"/>
+      <c r="X21" s="118" t="s">
+        <v>1414</v>
+      </c>
       <c r="Y21" s="118" t="s">
         <v>567</v>
       </c>
@@ -14313,7 +14348,7 @@
         <v>170</v>
       </c>
       <c r="X24" s="118" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="Y24" s="118" t="s">
         <v>567</v>
@@ -14483,7 +14518,9 @@
       <c r="W25" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="X25" s="118"/>
+      <c r="X25" s="118" t="s">
+        <v>1415</v>
+      </c>
       <c r="Y25" s="118" t="s">
         <v>567</v>
       </c>
@@ -14821,7 +14858,9 @@
       <c r="W27" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="X27" s="118"/>
+      <c r="X27" s="118" t="s">
+        <v>1416</v>
+      </c>
       <c r="Y27" s="118" t="s">
         <v>567</v>
       </c>
@@ -15124,7 +15163,7 @@
         <v>1112</v>
       </c>
       <c r="L29" s="52" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="M29" s="52" t="s">
         <v>166</v>
@@ -15157,7 +15196,9 @@
       <c r="W29" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="X29" s="118"/>
+      <c r="X29" s="118" t="s">
+        <v>1417</v>
+      </c>
       <c r="Y29" s="118" t="s">
         <v>567</v>
       </c>
@@ -15327,7 +15368,7 @@
         <v>170</v>
       </c>
       <c r="X30" s="118" t="s">
-        <v>1386</v>
+        <v>1418</v>
       </c>
       <c r="Y30" s="118" t="s">
         <v>567</v>
@@ -15659,7 +15700,7 @@
         <v>1112</v>
       </c>
       <c r="X32" s="118" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
       <c r="Y32" s="52" t="s">
         <v>166</v>
@@ -15796,7 +15837,7 @@
         <v>1112</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
       <c r="M33" s="118" t="s">
         <v>567</v>
@@ -15828,7 +15869,7 @@
         <v>166</v>
       </c>
       <c r="X33" s="118" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="Y33" s="118" t="s">
         <v>567</v>
@@ -16295,7 +16336,7 @@
         <v>166</v>
       </c>
       <c r="L36" s="52" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
       <c r="M36" s="118" t="s">
         <v>567</v>
@@ -16450,7 +16491,7 @@
         <v>166</v>
       </c>
       <c r="H37" s="118" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="I37" s="52" t="s">
         <v>166</v>
@@ -16491,7 +16532,9 @@
       <c r="W37" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="X37" s="118"/>
+      <c r="X37" s="118" t="s">
+        <v>1408</v>
+      </c>
       <c r="Y37" s="118" t="s">
         <v>567</v>
       </c>
@@ -16502,7 +16545,7 @@
         <v>1112</v>
       </c>
       <c r="AB37" s="118" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="AC37" s="118" t="s">
         <v>567</v>
@@ -16623,7 +16666,7 @@
         <v>166</v>
       </c>
       <c r="L38" s="52" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="M38" s="48" t="s">
         <v>170</v>
@@ -16655,13 +16698,13 @@
         <v>166</v>
       </c>
       <c r="X38" s="153" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="Y38" s="52" t="s">
         <v>166</v>
       </c>
       <c r="Z38" s="118" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
       <c r="AA38" s="48" t="s">
         <v>170</v>
@@ -16681,7 +16724,7 @@
         <v>1112</v>
       </c>
       <c r="AH38" s="118" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="AI38" s="150" t="s">
         <v>166</v>
@@ -17007,12 +17050,10 @@
       <c r="V40" s="118">
         <v>1</v>
       </c>
-      <c r="W40" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X40" s="118">
-        <v>1</v>
-      </c>
+      <c r="W40" s="145" t="s">
+        <v>1116</v>
+      </c>
+      <c r="X40" s="118"/>
       <c r="Y40" s="118" t="s">
         <v>567</v>
       </c>
@@ -17876,7 +17917,7 @@
         <v>166</v>
       </c>
       <c r="R45" s="118" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="S45" s="52" t="s">
         <v>166</v>
@@ -18071,7 +18112,7 @@
         <v>170</v>
       </c>
       <c r="X46" s="118" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="Y46" s="118" t="s">
         <v>567</v>
@@ -18240,7 +18281,7 @@
         <v>170</v>
       </c>
       <c r="X47" s="118" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="Y47" s="118" t="s">
         <v>567</v>
@@ -18411,7 +18452,7 @@
         <v>170</v>
       </c>
       <c r="X48" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y48" s="118" t="s">
         <v>567</v>
@@ -18747,7 +18788,7 @@
         <v>170</v>
       </c>
       <c r="X50" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y50" s="118" t="s">
         <v>567</v>
@@ -18950,7 +18991,7 @@
         <v>170</v>
       </c>
       <c r="X51" s="118" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
       <c r="Y51" s="118" t="s">
         <v>567</v>
@@ -19119,7 +19160,7 @@
         <v>170</v>
       </c>
       <c r="X52" s="118" t="s">
-        <v>1381</v>
+        <v>1412</v>
       </c>
       <c r="Y52" s="118" t="s">
         <v>567</v>
@@ -19290,7 +19331,7 @@
         <v>170</v>
       </c>
       <c r="X53" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y53" s="118" t="s">
         <v>567</v>
@@ -19455,7 +19496,7 @@
         <v>170</v>
       </c>
       <c r="X54" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y54" s="118" t="s">
         <v>567</v>
@@ -19632,7 +19673,7 @@
         <v>170</v>
       </c>
       <c r="X55" s="118" t="s">
-        <v>1381</v>
+        <v>1413</v>
       </c>
       <c r="Y55" s="118" t="s">
         <v>567</v>
@@ -19964,7 +20005,7 @@
         <v>170</v>
       </c>
       <c r="X57" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y57" s="118" t="s">
         <v>567</v>
@@ -20129,7 +20170,7 @@
         <v>170</v>
       </c>
       <c r="X58" s="118" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="Y58" s="118" t="s">
         <v>567</v>
@@ -20332,7 +20373,7 @@
         <v>166</v>
       </c>
       <c r="X59" s="118" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="Y59" s="118" t="s">
         <v>567</v>
@@ -20832,7 +20873,9 @@
       <c r="W62" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="X62" s="118"/>
+      <c r="X62" s="118" t="s">
+        <v>1419</v>
+      </c>
       <c r="Y62" s="118" t="s">
         <v>567</v>
       </c>
@@ -21318,11 +21361,11 @@
       <c r="V65" s="118">
         <v>1</v>
       </c>
-      <c r="W65" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X65" s="118">
-        <v>1</v>
+      <c r="W65" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="X65" s="118" t="s">
+        <v>1420</v>
       </c>
       <c r="Y65" s="118" t="s">
         <v>567</v>
@@ -21830,7 +21873,9 @@
       <c r="W68" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="X68" s="118"/>
+      <c r="X68" s="118" t="s">
+        <v>1416</v>
+      </c>
       <c r="Y68" s="118" t="s">
         <v>567</v>
       </c>
@@ -22133,7 +22178,7 @@
         <v>1112</v>
       </c>
       <c r="L70" s="13" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
       <c r="M70" s="118" t="s">
         <v>567</v>
@@ -22791,7 +22836,7 @@
         <v>170</v>
       </c>
       <c r="L74" s="146" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="M74" s="48" t="s">
         <v>170</v>
@@ -23006,7 +23051,7 @@
         <v>166</v>
       </c>
       <c r="R75" s="118" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="S75" s="52" t="s">
         <v>166</v>
@@ -23191,7 +23236,7 @@
         <v>170</v>
       </c>
       <c r="L76" s="146" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
       <c r="M76" s="48" t="s">
         <v>170</v>
@@ -23354,7 +23399,7 @@
         <v>1112</v>
       </c>
       <c r="H77" s="118" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="I77" s="52" t="s">
         <v>166</v>
@@ -23366,7 +23411,7 @@
         <v>166</v>
       </c>
       <c r="L77" s="13" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="M77" s="48" t="s">
         <v>170</v>
@@ -23382,25 +23427,25 @@
         <v>166</v>
       </c>
       <c r="R77" s="118" t="s">
+        <v>1405</v>
+      </c>
+      <c r="S77" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="T77" s="118" t="s">
+        <v>1399</v>
+      </c>
+      <c r="U77" s="118" t="s">
+        <v>567</v>
+      </c>
+      <c r="V77" s="118">
+        <v>1</v>
+      </c>
+      <c r="W77" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="X77" s="118" t="s">
         <v>1409</v>
-      </c>
-      <c r="S77" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T77" s="118" t="s">
-        <v>1403</v>
-      </c>
-      <c r="U77" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="V77" s="118">
-        <v>1</v>
-      </c>
-      <c r="W77" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="X77" s="118" t="s">
-        <v>1378</v>
       </c>
       <c r="Y77" s="118" t="s">
         <v>567</v>
@@ -23539,7 +23584,7 @@
         <v>170</v>
       </c>
       <c r="L78" s="52" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="M78" s="48" t="s">
         <v>170</v>
@@ -23555,7 +23600,7 @@
         <v>166</v>
       </c>
       <c r="R78" s="118" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="S78" s="48" t="s">
         <v>170</v>
@@ -23700,7 +23745,7 @@
         <v>166</v>
       </c>
       <c r="L79" s="153" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
       <c r="M79" s="48" t="s">
         <v>170</v>
@@ -23879,7 +23924,7 @@
         <v>1112</v>
       </c>
       <c r="L80" s="153" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
       <c r="M80" s="48" t="s">
         <v>170</v>
@@ -25033,12 +25078,10 @@
       <c r="V86" s="118">
         <v>1</v>
       </c>
-      <c r="W86" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="X86" s="118">
-        <v>1</v>
-      </c>
+      <c r="W86" s="145" t="s">
+        <v>1116</v>
+      </c>
+      <c r="X86" s="118"/>
       <c r="Y86" s="118" t="s">
         <v>567</v>
       </c>
@@ -26142,7 +26185,7 @@
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W10 W65:W67 W86 W40:W42 W44 W32 W69:W71">
+  <conditionalFormatting sqref="W10 W66:W67 W41:W42 W44 W32 W69:W71">
     <cfRule type="cellIs" dxfId="244" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
@@ -49496,7 +49539,7 @@
       <c r="AN11" s="95"/>
       <c r="AO11" s="94"/>
     </row>
-    <row r="12" spans="2:41" s="99" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:41" s="99" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="94" t="s">
         <v>5</v>
       </c>
@@ -64859,7 +64902,7 @@
   <dimension ref="B1:Y87"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <pane ySplit="6930" activePane="bottomLeft"/>
+      <pane ySplit="7080" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:Y65536"/>
       <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>

</xml_diff>

<commit_message>
Update with meeting minute info
</commit_message>
<xml_diff>
--- a/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
+++ b/resource/SDCCD-Prop-S-N-Closeout-Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95939EC7-6EF5-48BA-B8F7-66BEC092719E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95722767-D8F4-47A8-86B1-15A5686334FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="6135" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9042" uniqueCount="1422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9068" uniqueCount="1426">
   <si>
     <t>#</t>
   </si>
@@ -4277,9 +4277,6 @@
     <t>only irrigation in SP; Hardcopy O&amp;M Binders 2--7 at DSC</t>
   </si>
   <si>
-    <t>only HVAC in SP; Hardcopy O&amp;M Binders 8,11,12,20-24,48-50,52 at DSC</t>
-  </si>
-  <si>
     <t>have restroom OMs only; hardcopy OM binder #14 (global power)</t>
   </si>
   <si>
@@ -4311,6 +4308,21 @@
   </si>
   <si>
     <t>not in SP; ? Hardcopy o&amp;M binder #28 at dsc?</t>
+  </si>
+  <si>
+    <t>8/29/19: only HVAC/Elec/FA/Security in SP; Hardcopy O&amp;M Binders 8,11,12,20-24,48-50,52 at DSC</t>
+  </si>
+  <si>
+    <t>have hardcopy Bldg M prelim fault study</t>
+  </si>
+  <si>
+    <t>have hardcopy Bldg D prelim fault study</t>
+  </si>
+  <si>
+    <t>have hardcopy of soils report only</t>
+  </si>
+  <si>
+    <t>2019-09-17 - CM13 minutes ready - PENDING upload to SP</t>
   </si>
 </sst>
 </file>
@@ -5404,7 +5416,203 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="404">
+  <dxfs count="432">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -8479,7 +8687,7 @@
                   <c:v>Today</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8/29/2019</c:v>
+                  <c:v>9/17/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10237,9 +10445,9 @@
   <dimension ref="B1:CD101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1110" activePane="bottomLeft"/>
-      <selection activeCell="V1" sqref="I1:V1048576"/>
-      <selection pane="bottomLeft" activeCell="X8" sqref="X8"/>
+      <pane ySplit="1140" activePane="bottomLeft"/>
+      <selection activeCell="P1" sqref="E1:P1048576"/>
+      <selection pane="bottomLeft" activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -10248,10 +10456,10 @@
     <col min="2" max="2" width="2.265625" customWidth="1"/>
     <col min="3" max="3" width="6.265625" customWidth="1"/>
     <col min="4" max="4" width="8.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="7.1328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.73046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.265625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="22" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1328125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.73046875" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="5.59765625" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="10.1328125" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="6.59765625" style="1" hidden="1" customWidth="1"/>
@@ -10260,12 +10468,12 @@
     <col min="14" max="14" width="9.73046875" style="1" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="7.265625" style="1" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="10.86328125" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="7.265625" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="7.265625" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="10.86328125" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="11" style="1" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="15.59765625" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="7.265625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.86328125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.265625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.86328125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.59765625" style="1" customWidth="1"/>
     <col min="23" max="23" width="7.265625" style="1" customWidth="1"/>
     <col min="24" max="24" width="20.86328125" style="1" customWidth="1"/>
     <col min="25" max="25" width="8.265625" style="1" customWidth="1"/>
@@ -11097,11 +11305,11 @@
       <c r="P5" s="118" t="s">
         <v>1227</v>
       </c>
-      <c r="Q5" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R5" s="118">
-        <v>1</v>
+      <c r="Q5" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R5" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S5" s="52" t="s">
         <v>166</v>
@@ -11274,11 +11482,11 @@
       <c r="R6" s="118">
         <v>1</v>
       </c>
-      <c r="S6" s="48" t="s">
-        <v>170</v>
+      <c r="S6" s="146" t="s">
+        <v>1112</v>
       </c>
       <c r="T6" s="118" t="s">
-        <v>1314</v>
+        <v>1422</v>
       </c>
       <c r="U6" s="118" t="s">
         <v>567</v>
@@ -11461,11 +11669,11 @@
       <c r="R7" s="118">
         <v>1</v>
       </c>
-      <c r="S7" s="118" t="s">
-        <v>567</v>
+      <c r="S7" s="146" t="s">
+        <v>1112</v>
       </c>
       <c r="T7" s="118" t="s">
-        <v>1313</v>
+        <v>1423</v>
       </c>
       <c r="U7" s="118" t="s">
         <v>567</v>
@@ -11970,11 +12178,11 @@
       <c r="P10" s="118" t="s">
         <v>1234</v>
       </c>
-      <c r="Q10" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R10" s="118">
-        <v>1</v>
+      <c r="Q10" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R10" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S10" s="52" t="s">
         <v>166</v>
@@ -11992,7 +12200,7 @@
         <v>170</v>
       </c>
       <c r="X10" s="118" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="Y10" s="118" t="s">
         <v>567</v>
@@ -12099,7 +12307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:82" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:82" s="18" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13" t="s">
         <v>86</v>
       </c>
@@ -12161,7 +12369,7 @@
         <v>170</v>
       </c>
       <c r="X11" s="118" t="s">
-        <v>1410</v>
+        <v>1421</v>
       </c>
       <c r="Y11" s="118" t="s">
         <v>567</v>
@@ -12481,11 +12689,11 @@
       <c r="P13" s="118" t="s">
         <v>1242</v>
       </c>
-      <c r="Q13" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R13" s="118">
-        <v>1</v>
+      <c r="Q13" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R13" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S13" s="48" t="s">
         <v>170</v>
@@ -12819,11 +13027,11 @@
       <c r="P15" s="118" t="s">
         <v>1245</v>
       </c>
-      <c r="Q15" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R15" s="118">
-        <v>1</v>
+      <c r="Q15" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R15" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S15" s="118" t="s">
         <v>567</v>
@@ -12988,11 +13196,11 @@
       <c r="P16" s="118" t="s">
         <v>1246</v>
       </c>
-      <c r="Q16" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R16" s="118">
-        <v>1</v>
+      <c r="Q16" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R16" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S16" s="52" t="s">
         <v>166</v>
@@ -13008,7 +13216,7 @@
         <v>170</v>
       </c>
       <c r="X16" s="118" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="Y16" s="118" t="s">
         <v>567</v>
@@ -13660,11 +13868,11 @@
       <c r="P20" s="118" t="s">
         <v>1277</v>
       </c>
-      <c r="Q20" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R20" s="118">
-        <v>1</v>
+      <c r="Q20" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R20" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S20" s="52" t="s">
         <v>166</v>
@@ -13831,11 +14039,11 @@
       <c r="P21" s="118" t="s">
         <v>1252</v>
       </c>
-      <c r="Q21" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R21" s="118">
-        <v>1</v>
+      <c r="Q21" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R21" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S21" s="52" t="s">
         <v>166</v>
@@ -13851,7 +14059,7 @@
         <v>170</v>
       </c>
       <c r="X21" s="118" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="Y21" s="118" t="s">
         <v>567</v>
@@ -14004,11 +14212,11 @@
       <c r="P22" s="118" t="s">
         <v>1278</v>
       </c>
-      <c r="Q22" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R22" s="118">
-        <v>1</v>
+      <c r="Q22" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R22" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S22" s="52" t="s">
         <v>166</v>
@@ -14284,7 +14492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B24" s="13" t="s">
         <v>86</v>
       </c>
@@ -14328,11 +14536,11 @@
       <c r="P24" s="118" t="s">
         <v>1254</v>
       </c>
-      <c r="Q24" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R24" s="118">
-        <v>1</v>
+      <c r="Q24" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R24" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S24" s="52" t="s">
         <v>166</v>
@@ -14499,11 +14707,11 @@
       <c r="P25" s="118" t="s">
         <v>1279</v>
       </c>
-      <c r="Q25" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R25" s="118">
-        <v>1</v>
+      <c r="Q25" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R25" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S25" s="52" t="s">
         <v>166</v>
@@ -14519,7 +14727,7 @@
         <v>170</v>
       </c>
       <c r="X25" s="118" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="Y25" s="118" t="s">
         <v>567</v>
@@ -14859,7 +15067,7 @@
         <v>170</v>
       </c>
       <c r="X27" s="118" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="Y27" s="118" t="s">
         <v>567</v>
@@ -14964,7 +15172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B28" s="13" t="s">
         <v>86</v>
       </c>
@@ -15006,11 +15214,11 @@
       <c r="P28" s="118" t="s">
         <v>1244</v>
       </c>
-      <c r="Q28" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R28" s="118">
-        <v>1</v>
+      <c r="Q28" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R28" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S28" s="52" t="s">
         <v>166</v>
@@ -15177,11 +15385,11 @@
       <c r="P29" s="118" t="s">
         <v>1257</v>
       </c>
-      <c r="Q29" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R29" s="118">
-        <v>1</v>
+      <c r="Q29" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R29" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S29" s="52" t="s">
         <v>166</v>
@@ -15197,7 +15405,7 @@
         <v>170</v>
       </c>
       <c r="X29" s="118" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="Y29" s="118" t="s">
         <v>567</v>
@@ -15368,7 +15576,7 @@
         <v>170</v>
       </c>
       <c r="X30" s="118" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="Y30" s="118" t="s">
         <v>567</v>
@@ -15636,7 +15844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:82" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B32" s="13" t="s">
         <v>86</v>
       </c>
@@ -15680,11 +15888,11 @@
       <c r="P32" s="118" t="s">
         <v>1262</v>
       </c>
-      <c r="Q32" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R32" s="118">
-        <v>1</v>
+      <c r="Q32" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R32" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S32" s="52" t="s">
         <v>166</v>
@@ -16183,11 +16391,11 @@
       <c r="P35" s="118" t="s">
         <v>1264</v>
       </c>
-      <c r="Q35" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R35" s="118">
-        <v>1</v>
+      <c r="Q35" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R35" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S35" s="52" t="s">
         <v>166</v>
@@ -18090,11 +18298,11 @@
       <c r="P46" s="118" t="s">
         <v>1232</v>
       </c>
-      <c r="Q46" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R46" s="118">
-        <v>1</v>
+      <c r="Q46" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R46" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S46" s="48" t="s">
         <v>170</v>
@@ -18261,11 +18469,11 @@
       <c r="P47" s="118" t="s">
         <v>1233</v>
       </c>
-      <c r="Q47" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R47" s="118">
-        <v>1</v>
+      <c r="Q47" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R47" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S47" s="52" t="s">
         <v>166</v>
@@ -18768,11 +18976,11 @@
       <c r="P50" s="118" t="s">
         <v>1237</v>
       </c>
-      <c r="Q50" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R50" s="118">
-        <v>1</v>
+      <c r="Q50" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R50" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S50" s="52" t="s">
         <v>166</v>
@@ -18971,11 +19179,11 @@
       <c r="P51" s="118" t="s">
         <v>1235</v>
       </c>
-      <c r="Q51" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R51" s="118">
-        <v>1</v>
+      <c r="Q51" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R51" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S51" s="52" t="s">
         <v>166</v>
@@ -19140,11 +19348,11 @@
       <c r="P52" s="118" t="s">
         <v>1240</v>
       </c>
-      <c r="Q52" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R52" s="118">
-        <v>1</v>
+      <c r="Q52" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R52" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S52" s="48" t="s">
         <v>170</v>
@@ -19160,7 +19368,7 @@
         <v>170</v>
       </c>
       <c r="X52" s="118" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="Y52" s="118" t="s">
         <v>567</v>
@@ -19311,11 +19519,11 @@
       <c r="P53" s="118" t="s">
         <v>1241</v>
       </c>
-      <c r="Q53" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R53" s="118">
-        <v>1</v>
+      <c r="Q53" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R53" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S53" s="52" t="s">
         <v>166</v>
@@ -19673,7 +19881,7 @@
         <v>170</v>
       </c>
       <c r="X55" s="118" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="Y55" s="118" t="s">
         <v>567</v>
@@ -19822,11 +20030,11 @@
       <c r="P56" s="118" t="s">
         <v>1243</v>
       </c>
-      <c r="Q56" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R56" s="118">
-        <v>1</v>
+      <c r="Q56" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R56" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S56" s="52" t="s">
         <v>166</v>
@@ -20874,7 +21082,7 @@
         <v>170</v>
       </c>
       <c r="X62" s="118" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="Y62" s="118" t="s">
         <v>567</v>
@@ -21301,7 +21509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:82" s="18" customFormat="1" ht="7.9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:82" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.35">
       <c r="B65" s="13" t="s">
         <v>4</v>
       </c>
@@ -21345,11 +21553,11 @@
       <c r="P65" s="118" t="s">
         <v>1253</v>
       </c>
-      <c r="Q65" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R65" s="118">
-        <v>1</v>
+      <c r="Q65" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R65" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S65" s="48" t="s">
         <v>170</v>
@@ -21365,7 +21573,7 @@
         <v>170</v>
       </c>
       <c r="X65" s="118" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="Y65" s="118" t="s">
         <v>567</v>
@@ -21874,7 +22082,7 @@
         <v>170</v>
       </c>
       <c r="X68" s="118" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="Y68" s="118" t="s">
         <v>567</v>
@@ -22021,11 +22229,11 @@
       <c r="P69" s="118" t="s">
         <v>1258</v>
       </c>
-      <c r="Q69" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R69" s="118">
-        <v>1</v>
+      <c r="Q69" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R69" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S69" s="146" t="s">
         <v>1112</v>
@@ -22683,11 +22891,11 @@
       <c r="P73" s="118" t="s">
         <v>1261</v>
       </c>
-      <c r="Q73" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R73" s="118">
-        <v>1</v>
+      <c r="Q73" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R73" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S73" s="145" t="s">
         <v>1116</v>
@@ -22854,10 +23062,12 @@
       <c r="R74" s="118">
         <v>1</v>
       </c>
-      <c r="S74" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="T74" s="118"/>
+      <c r="S74" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="T74" s="118" t="s">
+        <v>1424</v>
+      </c>
       <c r="U74" s="118" t="s">
         <v>567</v>
       </c>
@@ -24298,11 +24508,11 @@
       <c r="P82" s="118" t="s">
         <v>1266</v>
       </c>
-      <c r="Q82" s="118" t="s">
-        <v>567</v>
-      </c>
-      <c r="R82" s="118">
-        <v>1</v>
+      <c r="Q82" s="146" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R82" s="118" t="s">
+        <v>1425</v>
       </c>
       <c r="S82" s="48" t="s">
         <v>170</v>
@@ -25232,1741 +25442,1903 @@
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AU39 AU46:AU74 BA14 AW39 AU38:AW38 AU40:AW40 AU2:AW5 AV46:AW55 AV57:AW74 BB4:BB5 BC14:BH14 BI8:BJ8 BI10:BO12 BC2:BL5 BK8:BL9 BB46:BL74 BI14:BL29 R2 AP46:AQ74 AP2:AQ5 AP38:AQ40 AP8:AQ12 AP36:AQ36 AP33:AQ34 AP43:AQ44 AP76:AQ85 AP14:AQ29 AX46:BA46 AX5:AZ5 AX38:BL40 AU34:BL36 AU43:BL44 AX4:BA4 AU8:BH12 AX48:BA74 AX47:AZ47 AU76:BL85 AV14:AZ29 AX2:BB3 AF2:AF86">
-    <cfRule type="cellIs" dxfId="403" priority="357" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="431" priority="386" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI9:BJ9">
-    <cfRule type="cellIs" dxfId="402" priority="356" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="430" priority="385" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO2:BO5 BO8:BO9 BO34:BO36 BO38:BO40 BO43:BO44 BO46:BO74 BO14:BO29 BO76:BO85">
-    <cfRule type="cellIs" dxfId="401" priority="355" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="429" priority="384" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV39 AV56">
-    <cfRule type="cellIs" dxfId="400" priority="354" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="428" priority="383" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM2:BM5 BM8:BM9 BM34:BM36 BM38:BM40 BM43:BM44 BM46:BM74 BM14:BM29 BM76:BM85">
-    <cfRule type="cellIs" dxfId="399" priority="352" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="427" priority="381" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN2:BN5 BN8:BN9 BN34:BN36 BN38:BN40 BN43:BN44 BN46:BN74 BN14:BN29 BN76:BN85">
-    <cfRule type="cellIs" dxfId="398" priority="351" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="426" priority="380" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU14:AU29 BA15:BA29 BB14:BB29 BC15:BH29">
-    <cfRule type="cellIs" dxfId="397" priority="350" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="425" priority="379" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW56">
-    <cfRule type="cellIs" dxfId="396" priority="346" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="424" priority="375" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB30">
-    <cfRule type="cellIs" dxfId="395" priority="336" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="423" priority="365" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 I2:I3 I44 I14 I25 I22:I23 I32:I33 I36 I68:I69">
-    <cfRule type="cellIs" dxfId="394" priority="323" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="422" priority="352" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51 N76:N82 N4 N41:N44 N47 N11:N13 N49 M53:M55 N7:N8 M44 N53:N59 M17:N21 M57:M58 M62 N61:N74 M15:N15 M11:M12 M41:M42 N27 N34:N35 M29:N33 M65:M67 M25:N25 N22:N24 M36:N38 M82 M69:M80">
-    <cfRule type="cellIs" dxfId="393" priority="312" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="421" priority="341" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC2">
-    <cfRule type="cellIs" dxfId="392" priority="309" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="420" priority="338" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD2">
-    <cfRule type="cellIs" dxfId="391" priority="308" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="419" priority="337" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41:K42 K63 K10 K53 K16:K17 K57 K31 K44 K49 K37:K38 K81:K82 K69:K73">
-    <cfRule type="cellIs" dxfId="390" priority="307" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="418" priority="336" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:J85 J43:J44 J38:J40 J18 J33:J34 J46:J74 J2:J3 J20:J29 J36 J8:J12 J14:J15 J5">
-    <cfRule type="cellIs" dxfId="389" priority="306" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="417" priority="335" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L40 L34:L36 L43:L44 L77:L79 L46:L54 L63:L66 L15:L21 L68:L74 L28:L29 L10:L12 L57:L59 L61 L23:L24 L26 L2:L5 L81:L85">
-    <cfRule type="cellIs" dxfId="388" priority="305" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="416" priority="334" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="387" priority="304" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="415" priority="333" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="cellIs" dxfId="386" priority="301" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="414" priority="330" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH86">
-    <cfRule type="cellIs" dxfId="385" priority="300" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="413" priority="329" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2:AN86">
-    <cfRule type="cellIs" dxfId="384" priority="298" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="412" priority="327" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2 AJ44:AJ45 AJ14 AJ61 AJ22:AJ23 AJ63 AJ66 AJ68:AJ69 AJ74:AJ75 AJ71 AJ37 AJ83:AJ86 AJ39:AJ42">
-    <cfRule type="cellIs" dxfId="383" priority="296" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="411" priority="325" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL2:AL86">
-    <cfRule type="cellIs" dxfId="382" priority="294" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="410" priority="323" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O62:O66 O2:O53 O55:O56 O59:O60 O68:O70 O73:O79 O81 O83:O86">
-    <cfRule type="cellIs" dxfId="381" priority="293" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="409" priority="322" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q44 Q76 Q79:Q86 Q46:Q74">
-    <cfRule type="cellIs" dxfId="380" priority="292" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="Q3:Q4 Q76 Q79:Q86 Q48:Q49 Q6:Q9 Q11:Q12 Q54:Q55 Q57:Q64 Q17:Q19 Q14 Q23 Q66:Q68 Q26:Q27 Q30:Q31 Q70:Q72 Q74 Q33:Q34 Q36:Q44">
+    <cfRule type="cellIs" dxfId="408" priority="321" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4 S6:S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S74:S75 S67">
-    <cfRule type="cellIs" dxfId="379" priority="291" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S4 S8 S50 S13 S15 S17 S52 S72 S28 S37:S38 S75 S67">
+    <cfRule type="cellIs" dxfId="407" priority="320" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AE86">
-    <cfRule type="cellIs" dxfId="378" priority="290" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="406" priority="319" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG2:AG5 AG7:AG8 AG10:AG11 AG13:AG86">
-    <cfRule type="cellIs" dxfId="377" priority="289" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="405" priority="318" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AI45 AI2 AI9 AI51 AI13:AI14 AI53:AI55 AI59:AI60 AI20 AI41:AI42 AI22 AI24 AI27 AI65:AI67 AI31 AI74:AI75 AI36:AI37 AI62 AI71 AI69">
-    <cfRule type="cellIs" dxfId="376" priority="288" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="404" priority="317" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK2:AK13 AK15:AK86">
-    <cfRule type="cellIs" dxfId="375" priority="287" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="403" priority="316" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM2:AM86">
-    <cfRule type="cellIs" dxfId="374" priority="286" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="402" priority="315" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="cellIs" dxfId="373" priority="285" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="401" priority="314" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="cellIs" dxfId="372" priority="284" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="400" priority="313" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="371" priority="283" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="399" priority="312" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="370" priority="282" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="398" priority="311" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N45">
-    <cfRule type="cellIs" dxfId="369" priority="281" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="397" priority="310" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
-    <cfRule type="cellIs" dxfId="368" priority="280" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="396" priority="309" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="cellIs" dxfId="367" priority="279" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="395" priority="308" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="366" priority="278" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="394" priority="307" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="cellIs" dxfId="365" priority="277" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="393" priority="306" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="cellIs" dxfId="364" priority="276" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="392" priority="305" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="363" priority="272" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="391" priority="301" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="362" priority="271" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="390" priority="300" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60">
-    <cfRule type="cellIs" dxfId="361" priority="270" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="389" priority="299" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:N14">
-    <cfRule type="cellIs" dxfId="360" priority="269" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="388" priority="298" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="359" priority="268" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="387" priority="297" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="cellIs" dxfId="358" priority="267" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="386" priority="296" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
+    <cfRule type="cellIs" dxfId="385" priority="295" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N28">
+    <cfRule type="cellIs" dxfId="384" priority="294" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M68">
+    <cfRule type="cellIs" dxfId="383" priority="293" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ43">
+    <cfRule type="cellIs" dxfId="382" priority="292" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI43">
+    <cfRule type="cellIs" dxfId="381" priority="291" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ3">
+    <cfRule type="cellIs" dxfId="380" priority="290" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI3">
+    <cfRule type="cellIs" dxfId="379" priority="289" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ4">
+    <cfRule type="cellIs" dxfId="378" priority="288" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI4">
+    <cfRule type="cellIs" dxfId="377" priority="287" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ5">
+    <cfRule type="cellIs" dxfId="376" priority="286" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI5">
+    <cfRule type="cellIs" dxfId="375" priority="285" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ6">
+    <cfRule type="cellIs" dxfId="374" priority="284" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI6">
+    <cfRule type="cellIs" dxfId="373" priority="283" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ7">
+    <cfRule type="cellIs" dxfId="372" priority="282" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI7">
+    <cfRule type="cellIs" dxfId="371" priority="281" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ8:AJ9">
+    <cfRule type="cellIs" dxfId="370" priority="280" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI8">
+    <cfRule type="cellIs" dxfId="369" priority="279" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ46">
+    <cfRule type="cellIs" dxfId="368" priority="278" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI46">
+    <cfRule type="cellIs" dxfId="367" priority="277" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ47">
+    <cfRule type="cellIs" dxfId="366" priority="276" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI47">
+    <cfRule type="cellIs" dxfId="365" priority="275" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ10">
+    <cfRule type="cellIs" dxfId="364" priority="274" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI10">
+    <cfRule type="cellIs" dxfId="363" priority="273" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ48">
+    <cfRule type="cellIs" dxfId="362" priority="272" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI48">
+    <cfRule type="cellIs" dxfId="361" priority="271" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ49">
+    <cfRule type="cellIs" dxfId="360" priority="270" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI49">
+    <cfRule type="cellIs" dxfId="359" priority="269" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ50">
+    <cfRule type="cellIs" dxfId="358" priority="268" stopIfTrue="1" operator="between">
+      <formula>"""Yes"""</formula>
+      <formula>"""Yes"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI50">
     <cfRule type="cellIs" dxfId="357" priority="266" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
+  <conditionalFormatting sqref="AJ11:AJ13">
     <cfRule type="cellIs" dxfId="356" priority="265" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M68">
+  <conditionalFormatting sqref="AI11">
     <cfRule type="cellIs" dxfId="355" priority="264" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ43">
+  <conditionalFormatting sqref="AJ51">
     <cfRule type="cellIs" dxfId="354" priority="263" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI43">
+  <conditionalFormatting sqref="AI52">
     <cfRule type="cellIs" dxfId="353" priority="262" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ3">
+  <conditionalFormatting sqref="AJ52:AJ54">
     <cfRule type="cellIs" dxfId="352" priority="261" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI3">
+  <conditionalFormatting sqref="AJ56">
     <cfRule type="cellIs" dxfId="351" priority="260" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ4">
+  <conditionalFormatting sqref="AI56">
     <cfRule type="cellIs" dxfId="350" priority="259" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI4">
+  <conditionalFormatting sqref="AJ57:AJ58">
     <cfRule type="cellIs" dxfId="349" priority="258" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ5">
+  <conditionalFormatting sqref="AI57:AI58">
     <cfRule type="cellIs" dxfId="348" priority="257" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI5">
+  <conditionalFormatting sqref="AJ15:AJ16">
     <cfRule type="cellIs" dxfId="347" priority="256" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ6">
+  <conditionalFormatting sqref="AI15:AI16">
     <cfRule type="cellIs" dxfId="346" priority="255" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI6">
+  <conditionalFormatting sqref="AJ59:AJ60">
     <cfRule type="cellIs" dxfId="345" priority="254" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ7">
+  <conditionalFormatting sqref="AJ55">
     <cfRule type="cellIs" dxfId="344" priority="253" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI7">
+  <conditionalFormatting sqref="AI19">
     <cfRule type="cellIs" dxfId="343" priority="252" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ8:AJ9">
+  <conditionalFormatting sqref="AJ19">
     <cfRule type="cellIs" dxfId="342" priority="251" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI8">
+  <conditionalFormatting sqref="AI18">
     <cfRule type="cellIs" dxfId="341" priority="250" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ46">
+  <conditionalFormatting sqref="AJ18">
     <cfRule type="cellIs" dxfId="340" priority="249" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI46">
+  <conditionalFormatting sqref="AI17">
     <cfRule type="cellIs" dxfId="339" priority="248" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ47">
+  <conditionalFormatting sqref="AJ17">
     <cfRule type="cellIs" dxfId="338" priority="247" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI47">
+  <conditionalFormatting sqref="AI86">
     <cfRule type="cellIs" dxfId="337" priority="246" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ10">
+  <conditionalFormatting sqref="AI40">
     <cfRule type="cellIs" dxfId="336" priority="245" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI10">
+  <conditionalFormatting sqref="AJ20">
     <cfRule type="cellIs" dxfId="335" priority="244" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ48">
+  <conditionalFormatting sqref="AJ62">
     <cfRule type="cellIs" dxfId="334" priority="243" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI48">
-    <cfRule type="cellIs" dxfId="333" priority="242" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ21">
+    <cfRule type="cellIs" dxfId="333" priority="241" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ49">
-    <cfRule type="cellIs" dxfId="332" priority="241" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ64:AJ65">
+    <cfRule type="cellIs" dxfId="332" priority="239" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI49">
-    <cfRule type="cellIs" dxfId="331" priority="240" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI21">
+    <cfRule type="cellIs" dxfId="331" priority="238" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ50">
-    <cfRule type="cellIs" dxfId="330" priority="239" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI64">
+    <cfRule type="cellIs" dxfId="330" priority="237" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI50">
-    <cfRule type="cellIs" dxfId="329" priority="237" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI23">
+    <cfRule type="cellIs" dxfId="329" priority="236" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11:AJ13">
-    <cfRule type="cellIs" dxfId="328" priority="236" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ24">
+    <cfRule type="cellIs" dxfId="328" priority="235" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI11">
-    <cfRule type="cellIs" dxfId="327" priority="235" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI25">
+    <cfRule type="cellIs" dxfId="327" priority="234" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ51">
-    <cfRule type="cellIs" dxfId="326" priority="234" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ25">
+    <cfRule type="cellIs" dxfId="326" priority="233" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI52">
-    <cfRule type="cellIs" dxfId="325" priority="233" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ67">
+    <cfRule type="cellIs" dxfId="325" priority="232" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ52:AJ54">
-    <cfRule type="cellIs" dxfId="324" priority="232" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI26">
+    <cfRule type="cellIs" dxfId="324" priority="231" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ56">
-    <cfRule type="cellIs" dxfId="323" priority="231" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ26:AJ27">
+    <cfRule type="cellIs" dxfId="323" priority="230" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI56">
-    <cfRule type="cellIs" dxfId="322" priority="230" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI28:AI30">
+    <cfRule type="cellIs" dxfId="322" priority="229" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ57:AJ58">
-    <cfRule type="cellIs" dxfId="321" priority="229" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ28:AJ31">
+    <cfRule type="cellIs" dxfId="321" priority="228" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI57:AI58">
-    <cfRule type="cellIs" dxfId="320" priority="228" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI72">
+    <cfRule type="cellIs" dxfId="320" priority="227" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15:AJ16">
-    <cfRule type="cellIs" dxfId="319" priority="227" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ72">
+    <cfRule type="cellIs" dxfId="319" priority="226" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI15:AI16">
-    <cfRule type="cellIs" dxfId="318" priority="226" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI73">
+    <cfRule type="cellIs" dxfId="318" priority="225" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ59:AJ60">
-    <cfRule type="cellIs" dxfId="317" priority="225" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ73">
+    <cfRule type="cellIs" dxfId="317" priority="224" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ55">
-    <cfRule type="cellIs" dxfId="316" priority="224" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI32">
+    <cfRule type="cellIs" dxfId="316" priority="223" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI19">
-    <cfRule type="cellIs" dxfId="315" priority="223" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ32">
+    <cfRule type="cellIs" dxfId="315" priority="222" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19">
-    <cfRule type="cellIs" dxfId="314" priority="222" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI33">
+    <cfRule type="cellIs" dxfId="314" priority="221" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI18">
-    <cfRule type="cellIs" dxfId="313" priority="221" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ33">
+    <cfRule type="cellIs" dxfId="313" priority="220" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="312" priority="220" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI34:AI35">
+    <cfRule type="cellIs" dxfId="312" priority="219" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI17">
-    <cfRule type="cellIs" dxfId="311" priority="219" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ34:AJ36">
+    <cfRule type="cellIs" dxfId="311" priority="218" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ17">
-    <cfRule type="cellIs" dxfId="310" priority="218" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI61">
+    <cfRule type="cellIs" dxfId="310" priority="217" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI86">
-    <cfRule type="cellIs" dxfId="309" priority="217" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI63">
+    <cfRule type="cellIs" dxfId="309" priority="216" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI40">
-    <cfRule type="cellIs" dxfId="308" priority="216" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ70">
+    <cfRule type="cellIs" dxfId="308" priority="215" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ20">
-    <cfRule type="cellIs" dxfId="307" priority="215" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI70">
+    <cfRule type="cellIs" dxfId="307" priority="214" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ62">
-    <cfRule type="cellIs" dxfId="306" priority="214" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI68">
+    <cfRule type="cellIs" dxfId="306" priority="213" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ21">
+  <conditionalFormatting sqref="AJ76">
     <cfRule type="cellIs" dxfId="305" priority="212" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ64:AJ65">
-    <cfRule type="cellIs" dxfId="304" priority="210" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI76">
+    <cfRule type="cellIs" dxfId="304" priority="211" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI21">
-    <cfRule type="cellIs" dxfId="303" priority="209" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ78">
+    <cfRule type="cellIs" dxfId="303" priority="210" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI64">
-    <cfRule type="cellIs" dxfId="302" priority="208" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI78">
+    <cfRule type="cellIs" dxfId="302" priority="209" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI23">
-    <cfRule type="cellIs" dxfId="301" priority="207" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ38">
+    <cfRule type="cellIs" dxfId="301" priority="208" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ24">
-    <cfRule type="cellIs" dxfId="300" priority="206" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI38">
+    <cfRule type="cellIs" dxfId="300" priority="207" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI25">
-    <cfRule type="cellIs" dxfId="299" priority="205" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ77">
+    <cfRule type="cellIs" dxfId="299" priority="206" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ25">
-    <cfRule type="cellIs" dxfId="298" priority="204" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI77">
+    <cfRule type="cellIs" dxfId="298" priority="205" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ67">
-    <cfRule type="cellIs" dxfId="297" priority="203" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ79">
+    <cfRule type="cellIs" dxfId="297" priority="204" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI26">
-    <cfRule type="cellIs" dxfId="296" priority="202" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI79">
+    <cfRule type="cellIs" dxfId="296" priority="203" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ26:AJ27">
-    <cfRule type="cellIs" dxfId="295" priority="201" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ80">
+    <cfRule type="cellIs" dxfId="295" priority="202" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI28:AI30">
-    <cfRule type="cellIs" dxfId="294" priority="200" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI80">
+    <cfRule type="cellIs" dxfId="294" priority="201" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ28:AJ31">
-    <cfRule type="cellIs" dxfId="293" priority="199" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ81">
+    <cfRule type="cellIs" dxfId="293" priority="200" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI72">
-    <cfRule type="cellIs" dxfId="292" priority="198" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI81">
+    <cfRule type="cellIs" dxfId="292" priority="199" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ72">
-    <cfRule type="cellIs" dxfId="291" priority="197" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AJ82">
+    <cfRule type="cellIs" dxfId="291" priority="198" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI73">
-    <cfRule type="cellIs" dxfId="290" priority="196" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI82">
+    <cfRule type="cellIs" dxfId="290" priority="197" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ73">
-    <cfRule type="cellIs" dxfId="289" priority="195" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI83">
+    <cfRule type="cellIs" dxfId="289" priority="196" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI32">
-    <cfRule type="cellIs" dxfId="288" priority="194" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI84:AI85">
+    <cfRule type="cellIs" dxfId="288" priority="195" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ32">
-    <cfRule type="cellIs" dxfId="287" priority="193" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI39">
+    <cfRule type="cellIs" dxfId="287" priority="194" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI33">
-    <cfRule type="cellIs" dxfId="286" priority="192" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="J31">
+    <cfRule type="cellIs" dxfId="286" priority="193" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ33">
-    <cfRule type="cellIs" dxfId="285" priority="191" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O61">
+    <cfRule type="cellIs" dxfId="285" priority="192" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI34:AI35">
-    <cfRule type="cellIs" dxfId="284" priority="190" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O54">
+    <cfRule type="cellIs" dxfId="284" priority="191" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ34:AJ36">
-    <cfRule type="cellIs" dxfId="283" priority="189" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O57">
+    <cfRule type="cellIs" dxfId="283" priority="190" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI61">
-    <cfRule type="cellIs" dxfId="282" priority="188" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O58">
+    <cfRule type="cellIs" dxfId="282" priority="189" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI63">
-    <cfRule type="cellIs" dxfId="281" priority="187" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O67">
+    <cfRule type="cellIs" dxfId="281" priority="188" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ70">
-    <cfRule type="cellIs" dxfId="280" priority="186" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O71">
+    <cfRule type="cellIs" dxfId="280" priority="187" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI70">
-    <cfRule type="cellIs" dxfId="279" priority="185" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O72">
+    <cfRule type="cellIs" dxfId="279" priority="186" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI68">
-    <cfRule type="cellIs" dxfId="278" priority="184" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O80">
+    <cfRule type="cellIs" dxfId="278" priority="185" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ76">
-    <cfRule type="cellIs" dxfId="277" priority="183" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="O82">
+    <cfRule type="cellIs" dxfId="277" priority="184" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI76">
+  <conditionalFormatting sqref="L62">
     <cfRule type="cellIs" dxfId="276" priority="182" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ78">
-    <cfRule type="cellIs" dxfId="275" priority="181" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="L75">
+    <cfRule type="cellIs" dxfId="275" priority="180" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI78">
-    <cfRule type="cellIs" dxfId="274" priority="180" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AI12">
+    <cfRule type="cellIs" dxfId="274" priority="179" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ38">
-    <cfRule type="cellIs" dxfId="273" priority="179" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="X2">
+    <cfRule type="cellIs" dxfId="273" priority="178" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI38">
-    <cfRule type="cellIs" dxfId="272" priority="178" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="W10 W66:W67 W41:W42 W44 W32 W69:W71">
+    <cfRule type="cellIs" dxfId="272" priority="177" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ77">
-    <cfRule type="cellIs" dxfId="271" priority="177" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AB2">
+    <cfRule type="cellIs" dxfId="271" priority="176" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI77">
-    <cfRule type="cellIs" dxfId="270" priority="176" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
+    <cfRule type="cellIs" dxfId="270" priority="175" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ79">
-    <cfRule type="cellIs" dxfId="269" priority="175" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="Z2">
+    <cfRule type="cellIs" dxfId="269" priority="174" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI79">
-    <cfRule type="cellIs" dxfId="268" priority="174" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y74 Y33:Y37 Y76:Y77 Y39:Y59 Y80:Y86">
+    <cfRule type="cellIs" dxfId="268" priority="173" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ80">
-    <cfRule type="cellIs" dxfId="267" priority="173" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AD2">
+    <cfRule type="cellIs" dxfId="267" priority="172" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI80">
-    <cfRule type="cellIs" dxfId="266" priority="172" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AC2:AC86">
+    <cfRule type="cellIs" dxfId="266" priority="171" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ81">
-    <cfRule type="cellIs" dxfId="265" priority="171" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="V2">
+    <cfRule type="cellIs" dxfId="265" priority="170" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI81">
-    <cfRule type="cellIs" dxfId="264" priority="170" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="U2:U86">
+    <cfRule type="cellIs" dxfId="264" priority="169" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ82">
-    <cfRule type="cellIs" dxfId="263" priority="169" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
+    <cfRule type="cellIs" dxfId="263" priority="168" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI82">
-    <cfRule type="cellIs" dxfId="262" priority="168" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA48">
+    <cfRule type="cellIs" dxfId="262" priority="167" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI83">
-    <cfRule type="cellIs" dxfId="261" priority="167" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA11">
+    <cfRule type="cellIs" dxfId="261" priority="166" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI84:AI85">
-    <cfRule type="cellIs" dxfId="260" priority="166" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA51">
+    <cfRule type="cellIs" dxfId="260" priority="165" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI39">
-    <cfRule type="cellIs" dxfId="259" priority="165" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA52">
+    <cfRule type="cellIs" dxfId="259" priority="164" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
-    <cfRule type="cellIs" dxfId="258" priority="164" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA53">
+    <cfRule type="cellIs" dxfId="258" priority="163" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O61">
-    <cfRule type="cellIs" dxfId="257" priority="163" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA57 AA54:AA55">
+    <cfRule type="cellIs" dxfId="257" priority="162" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O54">
-    <cfRule type="cellIs" dxfId="256" priority="162" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA20">
+    <cfRule type="cellIs" dxfId="256" priority="161" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O57">
-    <cfRule type="cellIs" dxfId="255" priority="161" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA21">
+    <cfRule type="cellIs" dxfId="255" priority="160" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O58">
-    <cfRule type="cellIs" dxfId="254" priority="160" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA66">
+    <cfRule type="cellIs" dxfId="254" priority="159" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O67">
-    <cfRule type="cellIs" dxfId="253" priority="159" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA25">
+    <cfRule type="cellIs" dxfId="253" priority="158" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O71">
-    <cfRule type="cellIs" dxfId="252" priority="158" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA26">
+    <cfRule type="cellIs" dxfId="252" priority="157" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O72">
-    <cfRule type="cellIs" dxfId="251" priority="157" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA28">
+    <cfRule type="cellIs" dxfId="251" priority="156" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="250" priority="156" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA32">
+    <cfRule type="cellIs" dxfId="250" priority="155" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="249" priority="155" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA34">
+    <cfRule type="cellIs" dxfId="249" priority="154" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62">
+  <conditionalFormatting sqref="AA27">
     <cfRule type="cellIs" dxfId="248" priority="153" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L75">
-    <cfRule type="cellIs" dxfId="247" priority="151" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA33 AA31">
+    <cfRule type="cellIs" dxfId="247" priority="152" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI12">
-    <cfRule type="cellIs" dxfId="246" priority="150" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA61 M61">
+    <cfRule type="cellIs" dxfId="246" priority="151" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
-    <cfRule type="cellIs" dxfId="245" priority="149" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA62">
+    <cfRule type="cellIs" dxfId="245" priority="150" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W10 W66:W67 W41:W42 W44 W32 W69:W71">
-    <cfRule type="cellIs" dxfId="244" priority="148" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA63 M63">
+    <cfRule type="cellIs" dxfId="244" priority="149" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2">
-    <cfRule type="cellIs" dxfId="243" priority="147" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA65">
+    <cfRule type="cellIs" dxfId="243" priority="148" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA10 AA44 AA41:AA42 AA12 AA15:AA16 AA69">
-    <cfRule type="cellIs" dxfId="242" priority="146" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA67">
+    <cfRule type="cellIs" dxfId="242" priority="147" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2">
-    <cfRule type="cellIs" dxfId="241" priority="145" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA68">
+    <cfRule type="cellIs" dxfId="241" priority="146" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y13 Y15:Y31 Y61:Y74 Y33:Y37 Y76:Y77 Y39:Y59 Y80:Y86">
-    <cfRule type="cellIs" dxfId="240" priority="144" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA70:AA73">
+    <cfRule type="cellIs" dxfId="240" priority="145" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2">
-    <cfRule type="cellIs" dxfId="239" priority="143" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA77">
+    <cfRule type="cellIs" dxfId="239" priority="144" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC86">
-    <cfRule type="cellIs" dxfId="238" priority="142" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA74 AA38">
+    <cfRule type="cellIs" dxfId="238" priority="143" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2">
-    <cfRule type="cellIs" dxfId="237" priority="141" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="AA37">
+    <cfRule type="cellIs" dxfId="237" priority="142" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U86">
-    <cfRule type="cellIs" dxfId="236" priority="140" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S9">
+    <cfRule type="cellIs" dxfId="236" priority="141" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA7:AA8 AA3:AA4">
-    <cfRule type="cellIs" dxfId="235" priority="139" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S46">
+    <cfRule type="cellIs" dxfId="235" priority="140" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA48">
-    <cfRule type="cellIs" dxfId="234" priority="138" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S48">
+    <cfRule type="cellIs" dxfId="234" priority="139" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA11">
-    <cfRule type="cellIs" dxfId="233" priority="137" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S18">
+    <cfRule type="cellIs" dxfId="233" priority="138" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA51">
-    <cfRule type="cellIs" dxfId="232" priority="136" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S54">
+    <cfRule type="cellIs" dxfId="232" priority="137" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA52">
-    <cfRule type="cellIs" dxfId="231" priority="135" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S55">
+    <cfRule type="cellIs" dxfId="231" priority="136" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA53">
-    <cfRule type="cellIs" dxfId="230" priority="134" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S57">
+    <cfRule type="cellIs" dxfId="230" priority="135" stopIfTrue="1" operator="between">
       <formula>"""Yes"""</formula>
       <formula>"""Yes"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA57 AA54:AA55">
-    <cfRule type="cellIs" dxfId="229" priority="133" stopIfTrue="1" operator="between">
+  <conditionalFormatting sqref="S76">
+    <cfRule type="cellIs" dxfId="229" priority="134" stopIfTrue="1" operator="between">
    